<commit_message>
Upto Group 3 MGT 7
</commit_message>
<xml_diff>
--- a/DataExtraction/Input/Config.xlsx
+++ b/DataExtraction/Input/Config.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
   <si>
     <t>Key</t>
   </si>
@@ -22,13 +22,13 @@
     <t>pdf path</t>
   </si>
   <si>
-    <t>/Users/gundukalyan/PycharmProjects/DataExtraction/Input/Form MGT-7-22092022_signed - Json data L&amp;T.pdf</t>
+    <t>/Users/gundukalyan/Documents/GitHub/mns-json-prep/DataExtraction/Input/Form MGT-7-22092022_signed - Json data L&amp;T.pdf</t>
   </si>
   <si>
     <t>mapping file path</t>
   </si>
   <si>
-    <t>/Users/gundukalyan/PycharmProjects/DataExtraction/Input/MGT7_Newmapping_config-1.xlsx</t>
+    <t>/Users/gundukalyan/Documents/GitHub/mns-json-prep/DataExtraction/Input/MGT7_Newmapping_config.xlsx</t>
   </si>
   <si>
     <t>mapping file sheet name</t>
@@ -56,6 +56,81 @@
   </si>
   <si>
     <t>Group</t>
+  </si>
+  <si>
+    <t>principal_business_activities_field_name</t>
+  </si>
+  <si>
+    <t>principal_business_activities</t>
+  </si>
+  <si>
+    <t>director_shareholdings_field_name</t>
+  </si>
+  <si>
+    <t>director_shareholdings</t>
+  </si>
+  <si>
+    <t>Hold_Sub_Assoc_field_name</t>
+  </si>
+  <si>
+    <t>Holding/ Subsidiary/Associate/  Joint Venture</t>
+  </si>
+  <si>
+    <t>director_remuneration_field_name</t>
+  </si>
+  <si>
+    <t>director_remuneration</t>
+  </si>
+  <si>
+    <t>principal_business_activities_table_name</t>
+  </si>
+  <si>
+    <t>year_field_name</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Hold_Sub_Assoc_column_name</t>
+  </si>
+  <si>
+    <t>HOLD_SUB_ASSOC</t>
+  </si>
+  <si>
+    <t>cin_column_name_in_db</t>
+  </si>
+  <si>
+    <t>cin</t>
+  </si>
+  <si>
+    <t>company_name_column_name_in_db</t>
+  </si>
+  <si>
+    <t>company_name</t>
+  </si>
+  <si>
+    <t>associate_keyword_in_xml</t>
+  </si>
+  <si>
+    <t>ASSOC</t>
+  </si>
+  <si>
+    <t>holding_keyword_in_xml</t>
+  </si>
+  <si>
+    <t>HOLD</t>
+  </si>
+  <si>
+    <t>joint_venture_keyword_in_xml</t>
+  </si>
+  <si>
+    <t>JOINT</t>
+  </si>
+  <si>
+    <t>subsidiary_keyword_in_xml</t>
+  </si>
+  <si>
+    <t>SUBS</t>
   </si>
 </sst>
 </file>
@@ -65,7 +140,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -80,12 +155,6 @@
       <sz val="15"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -114,7 +183,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -197,29 +266,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -236,6 +320,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -259,6 +346,7 @@
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ff89847f"/>
       <rgbColor rgb="fff7f7f6"/>
+      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1407,36 +1495,52 @@
       <c r="E10" s="10"/>
     </row>
     <row r="11" ht="14.6" customHeight="1">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
+      <c r="A11" t="s" s="7">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s" s="7">
+        <v>16</v>
+      </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
     </row>
     <row r="12" ht="14.6" customHeight="1">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
+      <c r="A12" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s" s="9">
+        <v>18</v>
+      </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
     </row>
     <row r="13" ht="14.6" customHeight="1">
-      <c r="A13" s="8"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
     </row>
     <row r="14" ht="14.6" customHeight="1">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
+      <c r="A14" t="s" s="9">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s" s="9">
+        <v>20</v>
+      </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
     </row>
     <row r="15" ht="14.6" customHeight="1">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
+      <c r="A15" t="s" s="7">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s" s="7">
+        <v>22</v>
+      </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -1449,8 +1553,12 @@
       <c r="E16" s="10"/>
     </row>
     <row r="17" ht="14.6" customHeight="1">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
+      <c r="A17" t="s" s="7">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s" s="7">
+        <v>16</v>
+      </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
@@ -1463,8 +1571,12 @@
       <c r="E18" s="10"/>
     </row>
     <row r="19" ht="14.6" customHeight="1">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
+      <c r="A19" t="s" s="7">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s" s="7">
+        <v>25</v>
+      </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -1477,8 +1589,12 @@
       <c r="E20" s="10"/>
     </row>
     <row r="21" ht="14.6" customHeight="1">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
+      <c r="A21" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s" s="7">
+        <v>27</v>
+      </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -1491,15 +1607,23 @@
       <c r="E22" s="10"/>
     </row>
     <row r="23" ht="14.6" customHeight="1">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
+      <c r="A23" t="s" s="7">
+        <v>28</v>
+      </c>
+      <c r="B23" t="s" s="7">
+        <v>29</v>
+      </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
     </row>
     <row r="24" ht="14.6" customHeight="1">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
+      <c r="A24" t="s" s="9">
+        <v>30</v>
+      </c>
+      <c r="B24" t="s" s="9">
+        <v>31</v>
+      </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -1512,29 +1636,45 @@
       <c r="E25" s="8"/>
     </row>
     <row r="26" ht="14.6" customHeight="1">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
+      <c r="A26" t="s" s="11">
+        <v>32</v>
+      </c>
+      <c r="B26" t="s" s="9">
+        <v>33</v>
+      </c>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
     </row>
     <row r="27" ht="14.6" customHeight="1">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
+      <c r="A27" t="s" s="7">
+        <v>34</v>
+      </c>
+      <c r="B27" t="s" s="7">
+        <v>35</v>
+      </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
     </row>
     <row r="28" ht="14.6" customHeight="1">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
+      <c r="A28" t="s" s="9">
+        <v>36</v>
+      </c>
+      <c r="B28" t="s" s="9">
+        <v>37</v>
+      </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
     </row>
     <row r="29" ht="14.6" customHeight="1">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
+      <c r="A29" t="s" s="9">
+        <v>38</v>
+      </c>
+      <c r="B29" t="s" s="7">
+        <v>39</v>
+      </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>

</xml_diff>

<commit_message>
upto director remuneration table update
</commit_message>
<xml_diff>
--- a/DataExtraction/Input/Config.xlsx
+++ b/DataExtraction/Input/Config.xlsx
@@ -40,7 +40,7 @@
     <t>output excel file folder path</t>
   </si>
   <si>
-    <t>/Users/gundukalyan/PycharmProjects/DataExtraction/Output/</t>
+    <t>/Users/gundukalyan/Documents/GitHub/mns-json-prep/DataExtraction/Output/</t>
   </si>
   <si>
     <t>output_sheet_name</t>
@@ -73,7 +73,7 @@
     <t>Hold_Sub_Assoc_field_name</t>
   </si>
   <si>
-    <t>Holding/ Subsidiary/Associate/  Joint Venture</t>
+    <t>Holding/Subsidiary/Associate/Joint Venture</t>
   </si>
   <si>
     <t>director_remuneration_field_name</t>

</xml_diff>

<commit_message>
AOC NBFC 1st phase
</commit_message>
<xml_diff>
--- a/DataExtraction/Input/Config.xlsx
+++ b/DataExtraction/Input/Config.xlsx
@@ -8,12 +8,13 @@
     <sheet name="MGT7" sheetId="1" r:id="rId4"/>
     <sheet name="MSME" sheetId="2" r:id="rId5"/>
     <sheet name="CHG1" sheetId="3" r:id="rId6"/>
+    <sheet name="AOC NBFC" sheetId="4" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="63">
   <si>
     <t>Key</t>
   </si>
@@ -164,6 +165,45 @@
   <si>
     <t>/Users/gundukalyan/Documents/GitHub/mns-json-prep/DataExtraction/Output/CHG1</t>
   </si>
+  <si>
+    <t>/Users/gundukalyan/Documents/GitHub/mns-json-prep/DataExtraction/Input/AOC4_NBFC/FORM NO. AOC-4-NBFC (Ind AS).pdf</t>
+  </si>
+  <si>
+    <t>/Users/gundukalyan/Documents/GitHub/mns-json-prep/DataExtraction/Input/AOC4_NBFC/AOC-4_NBFC_nodes_seperated_config_new.xlsx</t>
+  </si>
+  <si>
+    <t>/Users/gundukalyan/Documents/GitHub/mns-json-prep/DataExtraction/Output/AOC NBFC</t>
+  </si>
+  <si>
+    <t>Previous_year_keyword</t>
+  </si>
+  <si>
+    <t>Previous</t>
+  </si>
+  <si>
+    <t>Current_year_keyword</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>Financial_Parameter_Keyword</t>
+  </si>
+  <si>
+    <t>Financial_Parameter</t>
+  </si>
+  <si>
+    <t>Common_Keyword</t>
+  </si>
+  <si>
+    <t>Common</t>
+  </si>
+  <si>
+    <t>Formula_Keyword</t>
+  </si>
+  <si>
+    <t>formula</t>
+  </si>
 </sst>
 </file>
 
@@ -189,10 +229,9 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="6">
@@ -436,7 +475,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -482,23 +521,20 @@
     <xf numFmtId="49" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -508,6 +544,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1570,7 +1618,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="16.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="59.3516" style="1" customWidth="1"/>
     <col min="2" max="2" width="84.1719" style="1" customWidth="1"/>
@@ -3113,7 +3161,7 @@
       <c r="E30" s="10"/>
     </row>
     <row r="31" ht="14.6" customHeight="1">
-      <c r="A31" s="20"/>
+      <c r="A31" s="9"/>
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
@@ -4100,10 +4148,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="14.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="28.6719" style="21" customWidth="1"/>
-    <col min="2" max="2" width="61.8438" style="21" customWidth="1"/>
-    <col min="3" max="5" width="16.3516" style="21" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="21" customWidth="1"/>
+    <col min="1" max="1" width="28.6719" style="20" customWidth="1"/>
+    <col min="2" max="2" width="61.8438" style="20" customWidth="1"/>
+    <col min="3" max="5" width="16.3516" style="20" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
@@ -4248,8 +4296,8 @@
       <c r="E15" s="10"/>
     </row>
     <row r="16" ht="14.6" customHeight="1">
-      <c r="A16" s="22"/>
-      <c r="B16" s="23"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -4346,7 +4394,7 @@
       <c r="E29" s="10"/>
     </row>
     <row r="30" ht="14.6" customHeight="1">
-      <c r="A30" s="20"/>
+      <c r="A30" s="9"/>
       <c r="B30" s="7"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -5310,6 +5358,1249 @@
       <c r="C167" s="10"/>
       <c r="D167" s="10"/>
       <c r="E167" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E165"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="14.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="28.6719" style="23" customWidth="1"/>
+    <col min="2" max="2" width="61.8438" style="23" customWidth="1"/>
+    <col min="3" max="5" width="16.3516" style="23" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.6" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" ht="14.6" customHeight="1">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" ht="38.6" customHeight="1">
+      <c r="A3" t="s" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s" s="7">
+        <v>50</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" ht="38.6" customHeight="1">
+      <c r="A4" t="s" s="9">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s" s="9">
+        <v>51</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" ht="14.6" customHeight="1">
+      <c r="A5" t="s" s="7">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" ht="26.6" customHeight="1">
+      <c r="A6" t="s" s="9">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s" s="9">
+        <v>52</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" ht="14.6" customHeight="1">
+      <c r="A7" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" ht="14.6" customHeight="1">
+      <c r="A8" t="s" s="9">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s" s="9">
+        <v>12</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" ht="14.6" customHeight="1">
+      <c r="A9" t="s" s="9">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s" s="9">
+        <v>14</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" ht="14.6" customHeight="1">
+      <c r="A10" t="s" s="7">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s" s="7">
+        <v>29</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" ht="26.6" customHeight="1">
+      <c r="A11" t="s" s="9">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s" s="9">
+        <v>31</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+    </row>
+    <row r="12" ht="14.6" customHeight="1">
+      <c r="A12" t="s" s="7">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s" s="24">
+        <v>54</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" ht="14.6" customHeight="1">
+      <c r="A13" t="s" s="7">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s" s="24">
+        <v>56</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" ht="14.6" customHeight="1">
+      <c r="A14" t="s" s="13">
+        <v>57</v>
+      </c>
+      <c r="B14" t="s" s="25">
+        <v>58</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" ht="14.6" customHeight="1">
+      <c r="A15" t="s" s="9">
+        <v>59</v>
+      </c>
+      <c r="B15" t="s" s="26">
+        <v>60</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+    </row>
+    <row r="16" ht="14.6" customHeight="1">
+      <c r="A16" t="s" s="7">
+        <v>61</v>
+      </c>
+      <c r="B16" t="s" s="24">
+        <v>62</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" ht="14.6" customHeight="1">
+      <c r="A17" s="15"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" ht="14.6" customHeight="1">
+      <c r="A18" s="17"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" ht="14.6" customHeight="1">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" ht="14.6" customHeight="1">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" ht="14.6" customHeight="1">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" ht="14.6" customHeight="1">
+      <c r="A22" s="15"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" ht="14.6" customHeight="1">
+      <c r="A23" s="17"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" ht="14.6" customHeight="1">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" ht="14.6" customHeight="1">
+      <c r="A25" s="19"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+    </row>
+    <row r="26" ht="14.6" customHeight="1">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" ht="14.6" customHeight="1">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+    </row>
+    <row r="28" ht="14.6" customHeight="1">
+      <c r="A28" s="9"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" ht="14.6" customHeight="1">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+    </row>
+    <row r="30" ht="14.6" customHeight="1">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+    </row>
+    <row r="31" ht="14.6" customHeight="1">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+    </row>
+    <row r="32" ht="14.6" customHeight="1">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+    </row>
+    <row r="33" ht="14.6" customHeight="1">
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+    </row>
+    <row r="34" ht="14.6" customHeight="1">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+    </row>
+    <row r="35" ht="14.6" customHeight="1">
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+    </row>
+    <row r="36" ht="14.6" customHeight="1">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+    </row>
+    <row r="37" ht="14.6" customHeight="1">
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+    </row>
+    <row r="38" ht="14.6" customHeight="1">
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+    </row>
+    <row r="39" ht="14.6" customHeight="1">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+    </row>
+    <row r="40" ht="14.6" customHeight="1">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+    </row>
+    <row r="41" ht="14.6" customHeight="1">
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+    </row>
+    <row r="42" ht="14.6" customHeight="1">
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+    </row>
+    <row r="43" ht="14.6" customHeight="1">
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+    </row>
+    <row r="44" ht="14.6" customHeight="1">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+    </row>
+    <row r="45" ht="14.6" customHeight="1">
+      <c r="A45" s="9"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+    </row>
+    <row r="46" ht="14.6" customHeight="1">
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+    </row>
+    <row r="47" ht="14.6" customHeight="1">
+      <c r="A47" s="10"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+    </row>
+    <row r="48" ht="14.6" customHeight="1">
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+    </row>
+    <row r="49" ht="14.6" customHeight="1">
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+    </row>
+    <row r="50" ht="14.6" customHeight="1">
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+    </row>
+    <row r="51" ht="14.6" customHeight="1">
+      <c r="A51" s="9"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+    </row>
+    <row r="52" ht="14.6" customHeight="1">
+      <c r="A52" s="7"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+    </row>
+    <row r="53" ht="14.6" customHeight="1">
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+    </row>
+    <row r="54" ht="14.6" customHeight="1">
+      <c r="A54" s="8"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+    </row>
+    <row r="55" ht="14.6" customHeight="1">
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+    </row>
+    <row r="56" ht="14.6" customHeight="1">
+      <c r="A56" s="7"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+    </row>
+    <row r="57" ht="14.6" customHeight="1">
+      <c r="A57" s="10"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+    </row>
+    <row r="58" ht="14.6" customHeight="1">
+      <c r="A58" s="7"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+    </row>
+    <row r="59" ht="14.6" customHeight="1">
+      <c r="A59" s="10"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
+    </row>
+    <row r="60" ht="14.6" customHeight="1">
+      <c r="A60" s="7"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+    </row>
+    <row r="61" ht="14.6" customHeight="1">
+      <c r="A61" s="9"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
+    </row>
+    <row r="62" ht="14.6" customHeight="1">
+      <c r="A62" s="7"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="8"/>
+    </row>
+    <row r="63" ht="14.6" customHeight="1">
+      <c r="A63" s="9"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+    </row>
+    <row r="64" ht="14.6" customHeight="1">
+      <c r="A64" s="8"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
+    </row>
+    <row r="65" ht="14.6" customHeight="1">
+      <c r="A65" s="10"/>
+      <c r="B65" s="10"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+    </row>
+    <row r="66" ht="14.6" customHeight="1">
+      <c r="A66" s="7"/>
+      <c r="B66" s="7"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
+    </row>
+    <row r="67" ht="14.6" customHeight="1">
+      <c r="A67" s="9"/>
+      <c r="B67" s="9"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10"/>
+    </row>
+    <row r="68" ht="14.6" customHeight="1">
+      <c r="A68" s="7"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+    </row>
+    <row r="69" ht="14.6" customHeight="1">
+      <c r="A69" s="9"/>
+      <c r="B69" s="9"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+    </row>
+    <row r="70" ht="14.6" customHeight="1">
+      <c r="A70" s="7"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8"/>
+    </row>
+    <row r="71" ht="14.6" customHeight="1">
+      <c r="A71" s="9"/>
+      <c r="B71" s="9"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="10"/>
+    </row>
+    <row r="72" ht="14.6" customHeight="1">
+      <c r="A72" s="8"/>
+      <c r="B72" s="8"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+    </row>
+    <row r="73" ht="14.6" customHeight="1">
+      <c r="A73" s="9"/>
+      <c r="B73" s="9"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10"/>
+    </row>
+    <row r="74" ht="14.6" customHeight="1">
+      <c r="A74" s="7"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8"/>
+      <c r="E74" s="8"/>
+    </row>
+    <row r="75" ht="14.6" customHeight="1">
+      <c r="A75" s="9"/>
+      <c r="B75" s="9"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="10"/>
+    </row>
+    <row r="76" ht="14.6" customHeight="1">
+      <c r="A76" s="7"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="8"/>
+      <c r="E76" s="8"/>
+    </row>
+    <row r="77" ht="14.6" customHeight="1">
+      <c r="A77" s="9"/>
+      <c r="B77" s="9"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="10"/>
+    </row>
+    <row r="78" ht="14.6" customHeight="1">
+      <c r="A78" s="8"/>
+      <c r="B78" s="8"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
+    </row>
+    <row r="79" ht="14.6" customHeight="1">
+      <c r="A79" s="9"/>
+      <c r="B79" s="9"/>
+      <c r="C79" s="10"/>
+      <c r="D79" s="10"/>
+      <c r="E79" s="10"/>
+    </row>
+    <row r="80" ht="14.6" customHeight="1">
+      <c r="A80" s="7"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="8"/>
+    </row>
+    <row r="81" ht="14.6" customHeight="1">
+      <c r="A81" s="9"/>
+      <c r="B81" s="9"/>
+      <c r="C81" s="10"/>
+      <c r="D81" s="10"/>
+      <c r="E81" s="10"/>
+    </row>
+    <row r="82" ht="14.6" customHeight="1">
+      <c r="A82" s="7"/>
+      <c r="B82" s="7"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="8"/>
+    </row>
+    <row r="83" ht="14.6" customHeight="1">
+      <c r="A83" s="9"/>
+      <c r="B83" s="9"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="10"/>
+      <c r="E83" s="10"/>
+    </row>
+    <row r="84" ht="14.6" customHeight="1">
+      <c r="A84" s="8"/>
+      <c r="B84" s="8"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
+      <c r="E84" s="8"/>
+    </row>
+    <row r="85" ht="14.6" customHeight="1">
+      <c r="A85" s="9"/>
+      <c r="B85" s="10"/>
+      <c r="C85" s="10"/>
+      <c r="D85" s="10"/>
+      <c r="E85" s="10"/>
+    </row>
+    <row r="86" ht="14.6" customHeight="1">
+      <c r="A86" s="7"/>
+      <c r="B86" s="7"/>
+      <c r="C86" s="8"/>
+      <c r="D86" s="8"/>
+      <c r="E86" s="8"/>
+    </row>
+    <row r="87" ht="14.6" customHeight="1">
+      <c r="A87" s="9"/>
+      <c r="B87" s="9"/>
+      <c r="C87" s="10"/>
+      <c r="D87" s="10"/>
+      <c r="E87" s="10"/>
+    </row>
+    <row r="88" ht="14.6" customHeight="1">
+      <c r="A88" s="7"/>
+      <c r="B88" s="7"/>
+      <c r="C88" s="8"/>
+      <c r="D88" s="8"/>
+      <c r="E88" s="8"/>
+    </row>
+    <row r="89" ht="14.6" customHeight="1">
+      <c r="A89" s="9"/>
+      <c r="B89" s="9"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="10"/>
+      <c r="E89" s="10"/>
+    </row>
+    <row r="90" ht="14.6" customHeight="1">
+      <c r="A90" s="7"/>
+      <c r="B90" s="7"/>
+      <c r="C90" s="8"/>
+      <c r="D90" s="8"/>
+      <c r="E90" s="8"/>
+    </row>
+    <row r="91" ht="14.6" customHeight="1">
+      <c r="A91" s="10"/>
+      <c r="B91" s="10"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="10"/>
+      <c r="E91" s="10"/>
+    </row>
+    <row r="92" ht="14.6" customHeight="1">
+      <c r="A92" s="7"/>
+      <c r="B92" s="7"/>
+      <c r="C92" s="8"/>
+      <c r="D92" s="8"/>
+      <c r="E92" s="8"/>
+    </row>
+    <row r="93" ht="14.6" customHeight="1">
+      <c r="A93" s="9"/>
+      <c r="B93" s="9"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="10"/>
+      <c r="E93" s="10"/>
+    </row>
+    <row r="94" ht="14.6" customHeight="1">
+      <c r="A94" s="7"/>
+      <c r="B94" s="7"/>
+      <c r="C94" s="8"/>
+      <c r="D94" s="8"/>
+      <c r="E94" s="8"/>
+    </row>
+    <row r="95" ht="14.6" customHeight="1">
+      <c r="A95" s="10"/>
+      <c r="B95" s="10"/>
+      <c r="C95" s="10"/>
+      <c r="D95" s="10"/>
+      <c r="E95" s="10"/>
+    </row>
+    <row r="96" ht="14.6" customHeight="1">
+      <c r="A96" s="7"/>
+      <c r="B96" s="7"/>
+      <c r="C96" s="8"/>
+      <c r="D96" s="8"/>
+      <c r="E96" s="8"/>
+    </row>
+    <row r="97" ht="14.6" customHeight="1">
+      <c r="A97" s="9"/>
+      <c r="B97" s="9"/>
+      <c r="C97" s="10"/>
+      <c r="D97" s="10"/>
+      <c r="E97" s="10"/>
+    </row>
+    <row r="98" ht="14.6" customHeight="1">
+      <c r="A98" s="7"/>
+      <c r="B98" s="7"/>
+      <c r="C98" s="8"/>
+      <c r="D98" s="8"/>
+      <c r="E98" s="8"/>
+    </row>
+    <row r="99" ht="14.6" customHeight="1">
+      <c r="A99" s="9"/>
+      <c r="B99" s="9"/>
+      <c r="C99" s="10"/>
+      <c r="D99" s="10"/>
+      <c r="E99" s="10"/>
+    </row>
+    <row r="100" ht="14.6" customHeight="1">
+      <c r="A100" s="8"/>
+      <c r="B100" s="8"/>
+      <c r="C100" s="8"/>
+      <c r="D100" s="8"/>
+      <c r="E100" s="8"/>
+    </row>
+    <row r="101" ht="14.6" customHeight="1">
+      <c r="A101" s="9"/>
+      <c r="B101" s="9"/>
+      <c r="C101" s="10"/>
+      <c r="D101" s="10"/>
+      <c r="E101" s="10"/>
+    </row>
+    <row r="102" ht="14.6" customHeight="1">
+      <c r="A102" s="7"/>
+      <c r="B102" s="7"/>
+      <c r="C102" s="8"/>
+      <c r="D102" s="8"/>
+      <c r="E102" s="8"/>
+    </row>
+    <row r="103" ht="14.6" customHeight="1">
+      <c r="A103" s="10"/>
+      <c r="B103" s="10"/>
+      <c r="C103" s="10"/>
+      <c r="D103" s="10"/>
+      <c r="E103" s="10"/>
+    </row>
+    <row r="104" ht="14.6" customHeight="1">
+      <c r="A104" s="7"/>
+      <c r="B104" s="7"/>
+      <c r="C104" s="8"/>
+      <c r="D104" s="8"/>
+      <c r="E104" s="8"/>
+    </row>
+    <row r="105" ht="14.6" customHeight="1">
+      <c r="A105" s="9"/>
+      <c r="B105" s="9"/>
+      <c r="C105" s="10"/>
+      <c r="D105" s="10"/>
+      <c r="E105" s="10"/>
+    </row>
+    <row r="106" ht="14.6" customHeight="1">
+      <c r="A106" s="7"/>
+      <c r="B106" s="7"/>
+      <c r="C106" s="8"/>
+      <c r="D106" s="8"/>
+      <c r="E106" s="8"/>
+    </row>
+    <row r="107" ht="14.6" customHeight="1">
+      <c r="A107" s="10"/>
+      <c r="B107" s="10"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="10"/>
+      <c r="E107" s="10"/>
+    </row>
+    <row r="108" ht="14.6" customHeight="1">
+      <c r="A108" s="7"/>
+      <c r="B108" s="7"/>
+      <c r="C108" s="8"/>
+      <c r="D108" s="8"/>
+      <c r="E108" s="8"/>
+    </row>
+    <row r="109" ht="14.6" customHeight="1">
+      <c r="A109" s="9"/>
+      <c r="B109" s="9"/>
+      <c r="C109" s="10"/>
+      <c r="D109" s="10"/>
+      <c r="E109" s="10"/>
+    </row>
+    <row r="110" ht="14.6" customHeight="1">
+      <c r="A110" s="8"/>
+      <c r="B110" s="8"/>
+      <c r="C110" s="8"/>
+      <c r="D110" s="8"/>
+      <c r="E110" s="8"/>
+    </row>
+    <row r="111" ht="14.6" customHeight="1">
+      <c r="A111" s="9"/>
+      <c r="B111" s="9"/>
+      <c r="C111" s="10"/>
+      <c r="D111" s="10"/>
+      <c r="E111" s="10"/>
+    </row>
+    <row r="112" ht="14.6" customHeight="1">
+      <c r="A112" s="8"/>
+      <c r="B112" s="8"/>
+      <c r="C112" s="8"/>
+      <c r="D112" s="8"/>
+      <c r="E112" s="8"/>
+    </row>
+    <row r="113" ht="14.6" customHeight="1">
+      <c r="A113" s="9"/>
+      <c r="B113" s="9"/>
+      <c r="C113" s="10"/>
+      <c r="D113" s="10"/>
+      <c r="E113" s="10"/>
+    </row>
+    <row r="114" ht="14.6" customHeight="1">
+      <c r="A114" s="7"/>
+      <c r="B114" s="7"/>
+      <c r="C114" s="8"/>
+      <c r="D114" s="8"/>
+      <c r="E114" s="8"/>
+    </row>
+    <row r="115" ht="14.6" customHeight="1">
+      <c r="A115" s="10"/>
+      <c r="B115" s="10"/>
+      <c r="C115" s="10"/>
+      <c r="D115" s="10"/>
+      <c r="E115" s="10"/>
+    </row>
+    <row r="116" ht="14.6" customHeight="1">
+      <c r="A116" s="7"/>
+      <c r="B116" s="7"/>
+      <c r="C116" s="8"/>
+      <c r="D116" s="8"/>
+      <c r="E116" s="8"/>
+    </row>
+    <row r="117" ht="14.6" customHeight="1">
+      <c r="A117" s="9"/>
+      <c r="B117" s="9"/>
+      <c r="C117" s="10"/>
+      <c r="D117" s="10"/>
+      <c r="E117" s="10"/>
+    </row>
+    <row r="118" ht="14.6" customHeight="1">
+      <c r="A118" s="8"/>
+      <c r="B118" s="8"/>
+      <c r="C118" s="8"/>
+      <c r="D118" s="8"/>
+      <c r="E118" s="8"/>
+    </row>
+    <row r="119" ht="14.6" customHeight="1">
+      <c r="A119" s="10"/>
+      <c r="B119" s="10"/>
+      <c r="C119" s="10"/>
+      <c r="D119" s="10"/>
+      <c r="E119" s="10"/>
+    </row>
+    <row r="120" ht="14.6" customHeight="1">
+      <c r="A120" s="7"/>
+      <c r="B120" s="8"/>
+      <c r="C120" s="8"/>
+      <c r="D120" s="8"/>
+      <c r="E120" s="8"/>
+    </row>
+    <row r="121" ht="14.6" customHeight="1">
+      <c r="A121" s="9"/>
+      <c r="B121" s="10"/>
+      <c r="C121" s="10"/>
+      <c r="D121" s="10"/>
+      <c r="E121" s="10"/>
+    </row>
+    <row r="122" ht="14.6" customHeight="1">
+      <c r="A122" s="7"/>
+      <c r="B122" s="7"/>
+      <c r="C122" s="8"/>
+      <c r="D122" s="8"/>
+      <c r="E122" s="8"/>
+    </row>
+    <row r="123" ht="14.6" customHeight="1">
+      <c r="A123" s="10"/>
+      <c r="B123" s="10"/>
+      <c r="C123" s="10"/>
+      <c r="D123" s="10"/>
+      <c r="E123" s="10"/>
+    </row>
+    <row r="124" ht="14.6" customHeight="1">
+      <c r="A124" s="7"/>
+      <c r="B124" s="7"/>
+      <c r="C124" s="8"/>
+      <c r="D124" s="8"/>
+      <c r="E124" s="8"/>
+    </row>
+    <row r="125" ht="14.6" customHeight="1">
+      <c r="A125" s="10"/>
+      <c r="B125" s="10"/>
+      <c r="C125" s="10"/>
+      <c r="D125" s="10"/>
+      <c r="E125" s="10"/>
+    </row>
+    <row r="126" ht="14.6" customHeight="1">
+      <c r="A126" s="8"/>
+      <c r="B126" s="8"/>
+      <c r="C126" s="8"/>
+      <c r="D126" s="8"/>
+      <c r="E126" s="8"/>
+    </row>
+    <row r="127" ht="14.6" customHeight="1">
+      <c r="A127" s="10"/>
+      <c r="B127" s="10"/>
+      <c r="C127" s="10"/>
+      <c r="D127" s="10"/>
+      <c r="E127" s="10"/>
+    </row>
+    <row r="128" ht="14.6" customHeight="1">
+      <c r="A128" s="8"/>
+      <c r="B128" s="8"/>
+      <c r="C128" s="8"/>
+      <c r="D128" s="8"/>
+      <c r="E128" s="8"/>
+    </row>
+    <row r="129" ht="14.6" customHeight="1">
+      <c r="A129" s="9"/>
+      <c r="B129" s="9"/>
+      <c r="C129" s="10"/>
+      <c r="D129" s="10"/>
+      <c r="E129" s="10"/>
+    </row>
+    <row r="130" ht="14.6" customHeight="1">
+      <c r="A130" s="7"/>
+      <c r="B130" s="7"/>
+      <c r="C130" s="8"/>
+      <c r="D130" s="8"/>
+      <c r="E130" s="8"/>
+    </row>
+    <row r="131" ht="14.6" customHeight="1">
+      <c r="A131" s="9"/>
+      <c r="B131" s="9"/>
+      <c r="C131" s="10"/>
+      <c r="D131" s="10"/>
+      <c r="E131" s="10"/>
+    </row>
+    <row r="132" ht="14.6" customHeight="1">
+      <c r="A132" s="7"/>
+      <c r="B132" s="7"/>
+      <c r="C132" s="8"/>
+      <c r="D132" s="8"/>
+      <c r="E132" s="8"/>
+    </row>
+    <row r="133" ht="14.6" customHeight="1">
+      <c r="A133" s="9"/>
+      <c r="B133" s="9"/>
+      <c r="C133" s="10"/>
+      <c r="D133" s="10"/>
+      <c r="E133" s="10"/>
+    </row>
+    <row r="134" ht="14.6" customHeight="1">
+      <c r="A134" s="7"/>
+      <c r="B134" s="7"/>
+      <c r="C134" s="8"/>
+      <c r="D134" s="8"/>
+      <c r="E134" s="8"/>
+    </row>
+    <row r="135" ht="14.6" customHeight="1">
+      <c r="A135" s="9"/>
+      <c r="B135" s="9"/>
+      <c r="C135" s="10"/>
+      <c r="D135" s="10"/>
+      <c r="E135" s="10"/>
+    </row>
+    <row r="136" ht="14.6" customHeight="1">
+      <c r="A136" s="7"/>
+      <c r="B136" s="7"/>
+      <c r="C136" s="8"/>
+      <c r="D136" s="8"/>
+      <c r="E136" s="8"/>
+    </row>
+    <row r="137" ht="14.6" customHeight="1">
+      <c r="A137" s="10"/>
+      <c r="B137" s="10"/>
+      <c r="C137" s="10"/>
+      <c r="D137" s="10"/>
+      <c r="E137" s="10"/>
+    </row>
+    <row r="138" ht="14.6" customHeight="1">
+      <c r="A138" s="7"/>
+      <c r="B138" s="7"/>
+      <c r="C138" s="8"/>
+      <c r="D138" s="8"/>
+      <c r="E138" s="8"/>
+    </row>
+    <row r="139" ht="14.6" customHeight="1">
+      <c r="A139" s="9"/>
+      <c r="B139" s="9"/>
+      <c r="C139" s="10"/>
+      <c r="D139" s="10"/>
+      <c r="E139" s="10"/>
+    </row>
+    <row r="140" ht="14.6" customHeight="1">
+      <c r="A140" s="7"/>
+      <c r="B140" s="7"/>
+      <c r="C140" s="8"/>
+      <c r="D140" s="8"/>
+      <c r="E140" s="8"/>
+    </row>
+    <row r="141" ht="14.6" customHeight="1">
+      <c r="A141" s="9"/>
+      <c r="B141" s="9"/>
+      <c r="C141" s="10"/>
+      <c r="D141" s="10"/>
+      <c r="E141" s="10"/>
+    </row>
+    <row r="142" ht="14.6" customHeight="1">
+      <c r="A142" s="8"/>
+      <c r="B142" s="8"/>
+      <c r="C142" s="8"/>
+      <c r="D142" s="8"/>
+      <c r="E142" s="8"/>
+    </row>
+    <row r="143" ht="14.6" customHeight="1">
+      <c r="A143" s="9"/>
+      <c r="B143" s="9"/>
+      <c r="C143" s="10"/>
+      <c r="D143" s="10"/>
+      <c r="E143" s="10"/>
+    </row>
+    <row r="144" ht="14.6" customHeight="1">
+      <c r="A144" s="7"/>
+      <c r="B144" s="7"/>
+      <c r="C144" s="8"/>
+      <c r="D144" s="8"/>
+      <c r="E144" s="8"/>
+    </row>
+    <row r="145" ht="14.6" customHeight="1">
+      <c r="A145" s="9"/>
+      <c r="B145" s="9"/>
+      <c r="C145" s="10"/>
+      <c r="D145" s="10"/>
+      <c r="E145" s="10"/>
+    </row>
+    <row r="146" ht="14.6" customHeight="1">
+      <c r="A146" s="7"/>
+      <c r="B146" s="7"/>
+      <c r="C146" s="8"/>
+      <c r="D146" s="8"/>
+      <c r="E146" s="8"/>
+    </row>
+    <row r="147" ht="14.6" customHeight="1">
+      <c r="A147" s="9"/>
+      <c r="B147" s="9"/>
+      <c r="C147" s="10"/>
+      <c r="D147" s="10"/>
+      <c r="E147" s="10"/>
+    </row>
+    <row r="148" ht="14.6" customHeight="1">
+      <c r="A148" s="7"/>
+      <c r="B148" s="7"/>
+      <c r="C148" s="8"/>
+      <c r="D148" s="8"/>
+      <c r="E148" s="8"/>
+    </row>
+    <row r="149" ht="14.6" customHeight="1">
+      <c r="A149" s="9"/>
+      <c r="B149" s="9"/>
+      <c r="C149" s="10"/>
+      <c r="D149" s="10"/>
+      <c r="E149" s="10"/>
+    </row>
+    <row r="150" ht="14.6" customHeight="1">
+      <c r="A150" s="8"/>
+      <c r="B150" s="8"/>
+      <c r="C150" s="8"/>
+      <c r="D150" s="8"/>
+      <c r="E150" s="8"/>
+    </row>
+    <row r="151" ht="14.6" customHeight="1">
+      <c r="A151" s="9"/>
+      <c r="B151" s="9"/>
+      <c r="C151" s="10"/>
+      <c r="D151" s="10"/>
+      <c r="E151" s="10"/>
+    </row>
+    <row r="152" ht="14.6" customHeight="1">
+      <c r="A152" s="7"/>
+      <c r="B152" s="7"/>
+      <c r="C152" s="8"/>
+      <c r="D152" s="8"/>
+      <c r="E152" s="8"/>
+    </row>
+    <row r="153" ht="14.6" customHeight="1">
+      <c r="A153" s="9"/>
+      <c r="B153" s="9"/>
+      <c r="C153" s="10"/>
+      <c r="D153" s="10"/>
+      <c r="E153" s="10"/>
+    </row>
+    <row r="154" ht="14.6" customHeight="1">
+      <c r="A154" s="8"/>
+      <c r="B154" s="8"/>
+      <c r="C154" s="8"/>
+      <c r="D154" s="8"/>
+      <c r="E154" s="8"/>
+    </row>
+    <row r="155" ht="14.6" customHeight="1">
+      <c r="A155" s="9"/>
+      <c r="B155" s="9"/>
+      <c r="C155" s="10"/>
+      <c r="D155" s="10"/>
+      <c r="E155" s="10"/>
+    </row>
+    <row r="156" ht="14.6" customHeight="1">
+      <c r="A156" s="7"/>
+      <c r="B156" s="7"/>
+      <c r="C156" s="8"/>
+      <c r="D156" s="8"/>
+      <c r="E156" s="8"/>
+    </row>
+    <row r="157" ht="14.6" customHeight="1">
+      <c r="A157" s="10"/>
+      <c r="B157" s="10"/>
+      <c r="C157" s="10"/>
+      <c r="D157" s="10"/>
+      <c r="E157" s="10"/>
+    </row>
+    <row r="158" ht="14.6" customHeight="1">
+      <c r="A158" s="7"/>
+      <c r="B158" s="7"/>
+      <c r="C158" s="8"/>
+      <c r="D158" s="8"/>
+      <c r="E158" s="8"/>
+    </row>
+    <row r="159" ht="14.6" customHeight="1">
+      <c r="A159" s="9"/>
+      <c r="B159" s="9"/>
+      <c r="C159" s="10"/>
+      <c r="D159" s="10"/>
+      <c r="E159" s="10"/>
+    </row>
+    <row r="160" ht="14.6" customHeight="1">
+      <c r="A160" s="8"/>
+      <c r="B160" s="8"/>
+      <c r="C160" s="8"/>
+      <c r="D160" s="8"/>
+      <c r="E160" s="8"/>
+    </row>
+    <row r="161" ht="14.6" customHeight="1">
+      <c r="A161" s="9"/>
+      <c r="B161" s="9"/>
+      <c r="C161" s="10"/>
+      <c r="D161" s="10"/>
+      <c r="E161" s="10"/>
+    </row>
+    <row r="162" ht="14.6" customHeight="1">
+      <c r="A162" s="7"/>
+      <c r="B162" s="7"/>
+      <c r="C162" s="8"/>
+      <c r="D162" s="8"/>
+      <c r="E162" s="8"/>
+    </row>
+    <row r="163" ht="14.6" customHeight="1">
+      <c r="A163" s="10"/>
+      <c r="B163" s="10"/>
+      <c r="C163" s="10"/>
+      <c r="D163" s="10"/>
+      <c r="E163" s="10"/>
+    </row>
+    <row r="164" ht="14.6" customHeight="1">
+      <c r="A164" s="7"/>
+      <c r="B164" s="7"/>
+      <c r="C164" s="8"/>
+      <c r="D164" s="8"/>
+      <c r="E164" s="8"/>
+    </row>
+    <row r="165" ht="14.6" customHeight="1">
+      <c r="A165" s="9"/>
+      <c r="B165" s="9"/>
+      <c r="C165" s="10"/>
+      <c r="D165" s="10"/>
+      <c r="E165" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
AOC NBFC Version 2
</commit_message>
<xml_diff>
--- a/DataExtraction/Input/Config.xlsx
+++ b/DataExtraction/Input/Config.xlsx
@@ -9,12 +9,13 @@
     <sheet name="MSME" sheetId="2" r:id="rId5"/>
     <sheet name="CHG1" sheetId="3" r:id="rId6"/>
     <sheet name="AOC NBFC" sheetId="4" r:id="rId7"/>
+    <sheet name="AOC NBFC CFS" sheetId="5" r:id="rId8"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="68">
   <si>
     <t>Key</t>
   </si>
@@ -203,6 +204,21 @@
   </si>
   <si>
     <t>formula</t>
+  </si>
+  <si>
+    <t>Constant_Keyword</t>
+  </si>
+  <si>
+    <t>Constant</t>
+  </si>
+  <si>
+    <t>/Users/gundukalyan/Documents/GitHub/mns-json-prep/DataExtraction/Input/AOC4_NBFC_CFS/5.Form AOC-4 CFS NBFC(Ind AS)-26072023_signed.pdf</t>
+  </si>
+  <si>
+    <t>/Users/gundukalyan/Documents/GitHub/mns-json-prep/DataExtraction/Input/AOC4_NBFC_CFS/AOC-4_NBFC_CFS_nodes_seperated_config_new.xlsx</t>
+  </si>
+  <si>
+    <t>/Users/gundukalyan/Documents/GitHub/mns-json-prep/DataExtraction/Output/AOC NBFC CFS</t>
   </si>
 </sst>
 </file>
@@ -475,7 +491,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -556,6 +572,15 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5560,8 +5585,1259 @@
       <c r="E16" s="8"/>
     </row>
     <row r="17" ht="14.6" customHeight="1">
-      <c r="A17" s="15"/>
-      <c r="B17" s="16"/>
+      <c r="A17" t="s" s="27">
+        <v>63</v>
+      </c>
+      <c r="B17" t="s" s="28">
+        <v>64</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" ht="14.6" customHeight="1">
+      <c r="A18" s="17"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" ht="14.6" customHeight="1">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" ht="14.6" customHeight="1">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" ht="14.6" customHeight="1">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" ht="14.6" customHeight="1">
+      <c r="A22" s="15"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" ht="14.6" customHeight="1">
+      <c r="A23" s="17"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" ht="14.6" customHeight="1">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" ht="14.6" customHeight="1">
+      <c r="A25" s="19"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+    </row>
+    <row r="26" ht="14.6" customHeight="1">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" ht="14.6" customHeight="1">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+    </row>
+    <row r="28" ht="14.6" customHeight="1">
+      <c r="A28" s="9"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" ht="14.6" customHeight="1">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+    </row>
+    <row r="30" ht="14.6" customHeight="1">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+    </row>
+    <row r="31" ht="14.6" customHeight="1">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+    </row>
+    <row r="32" ht="14.6" customHeight="1">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+    </row>
+    <row r="33" ht="14.6" customHeight="1">
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+    </row>
+    <row r="34" ht="14.6" customHeight="1">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+    </row>
+    <row r="35" ht="14.6" customHeight="1">
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+    </row>
+    <row r="36" ht="14.6" customHeight="1">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+    </row>
+    <row r="37" ht="14.6" customHeight="1">
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+    </row>
+    <row r="38" ht="14.6" customHeight="1">
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+    </row>
+    <row r="39" ht="14.6" customHeight="1">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+    </row>
+    <row r="40" ht="14.6" customHeight="1">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+    </row>
+    <row r="41" ht="14.6" customHeight="1">
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+    </row>
+    <row r="42" ht="14.6" customHeight="1">
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+    </row>
+    <row r="43" ht="14.6" customHeight="1">
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+    </row>
+    <row r="44" ht="14.6" customHeight="1">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+    </row>
+    <row r="45" ht="14.6" customHeight="1">
+      <c r="A45" s="9"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+    </row>
+    <row r="46" ht="14.6" customHeight="1">
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+    </row>
+    <row r="47" ht="14.6" customHeight="1">
+      <c r="A47" s="10"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+    </row>
+    <row r="48" ht="14.6" customHeight="1">
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+    </row>
+    <row r="49" ht="14.6" customHeight="1">
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+    </row>
+    <row r="50" ht="14.6" customHeight="1">
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+    </row>
+    <row r="51" ht="14.6" customHeight="1">
+      <c r="A51" s="9"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+    </row>
+    <row r="52" ht="14.6" customHeight="1">
+      <c r="A52" s="7"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+    </row>
+    <row r="53" ht="14.6" customHeight="1">
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+    </row>
+    <row r="54" ht="14.6" customHeight="1">
+      <c r="A54" s="8"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+    </row>
+    <row r="55" ht="14.6" customHeight="1">
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+    </row>
+    <row r="56" ht="14.6" customHeight="1">
+      <c r="A56" s="7"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+    </row>
+    <row r="57" ht="14.6" customHeight="1">
+      <c r="A57" s="10"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+    </row>
+    <row r="58" ht="14.6" customHeight="1">
+      <c r="A58" s="7"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+    </row>
+    <row r="59" ht="14.6" customHeight="1">
+      <c r="A59" s="10"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
+    </row>
+    <row r="60" ht="14.6" customHeight="1">
+      <c r="A60" s="7"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+    </row>
+    <row r="61" ht="14.6" customHeight="1">
+      <c r="A61" s="9"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
+    </row>
+    <row r="62" ht="14.6" customHeight="1">
+      <c r="A62" s="7"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="8"/>
+    </row>
+    <row r="63" ht="14.6" customHeight="1">
+      <c r="A63" s="9"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+    </row>
+    <row r="64" ht="14.6" customHeight="1">
+      <c r="A64" s="8"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
+    </row>
+    <row r="65" ht="14.6" customHeight="1">
+      <c r="A65" s="10"/>
+      <c r="B65" s="10"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+    </row>
+    <row r="66" ht="14.6" customHeight="1">
+      <c r="A66" s="7"/>
+      <c r="B66" s="7"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
+    </row>
+    <row r="67" ht="14.6" customHeight="1">
+      <c r="A67" s="9"/>
+      <c r="B67" s="9"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10"/>
+    </row>
+    <row r="68" ht="14.6" customHeight="1">
+      <c r="A68" s="7"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+    </row>
+    <row r="69" ht="14.6" customHeight="1">
+      <c r="A69" s="9"/>
+      <c r="B69" s="9"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+    </row>
+    <row r="70" ht="14.6" customHeight="1">
+      <c r="A70" s="7"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8"/>
+    </row>
+    <row r="71" ht="14.6" customHeight="1">
+      <c r="A71" s="9"/>
+      <c r="B71" s="9"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="10"/>
+    </row>
+    <row r="72" ht="14.6" customHeight="1">
+      <c r="A72" s="8"/>
+      <c r="B72" s="8"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+    </row>
+    <row r="73" ht="14.6" customHeight="1">
+      <c r="A73" s="9"/>
+      <c r="B73" s="9"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10"/>
+    </row>
+    <row r="74" ht="14.6" customHeight="1">
+      <c r="A74" s="7"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8"/>
+      <c r="E74" s="8"/>
+    </row>
+    <row r="75" ht="14.6" customHeight="1">
+      <c r="A75" s="9"/>
+      <c r="B75" s="9"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="10"/>
+    </row>
+    <row r="76" ht="14.6" customHeight="1">
+      <c r="A76" s="7"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="8"/>
+      <c r="E76" s="8"/>
+    </row>
+    <row r="77" ht="14.6" customHeight="1">
+      <c r="A77" s="9"/>
+      <c r="B77" s="9"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="10"/>
+    </row>
+    <row r="78" ht="14.6" customHeight="1">
+      <c r="A78" s="8"/>
+      <c r="B78" s="8"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
+    </row>
+    <row r="79" ht="14.6" customHeight="1">
+      <c r="A79" s="9"/>
+      <c r="B79" s="9"/>
+      <c r="C79" s="10"/>
+      <c r="D79" s="10"/>
+      <c r="E79" s="10"/>
+    </row>
+    <row r="80" ht="14.6" customHeight="1">
+      <c r="A80" s="7"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="8"/>
+    </row>
+    <row r="81" ht="14.6" customHeight="1">
+      <c r="A81" s="9"/>
+      <c r="B81" s="9"/>
+      <c r="C81" s="10"/>
+      <c r="D81" s="10"/>
+      <c r="E81" s="10"/>
+    </row>
+    <row r="82" ht="14.6" customHeight="1">
+      <c r="A82" s="7"/>
+      <c r="B82" s="7"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="8"/>
+    </row>
+    <row r="83" ht="14.6" customHeight="1">
+      <c r="A83" s="9"/>
+      <c r="B83" s="9"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="10"/>
+      <c r="E83" s="10"/>
+    </row>
+    <row r="84" ht="14.6" customHeight="1">
+      <c r="A84" s="8"/>
+      <c r="B84" s="8"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
+      <c r="E84" s="8"/>
+    </row>
+    <row r="85" ht="14.6" customHeight="1">
+      <c r="A85" s="9"/>
+      <c r="B85" s="10"/>
+      <c r="C85" s="10"/>
+      <c r="D85" s="10"/>
+      <c r="E85" s="10"/>
+    </row>
+    <row r="86" ht="14.6" customHeight="1">
+      <c r="A86" s="7"/>
+      <c r="B86" s="7"/>
+      <c r="C86" s="8"/>
+      <c r="D86" s="8"/>
+      <c r="E86" s="8"/>
+    </row>
+    <row r="87" ht="14.6" customHeight="1">
+      <c r="A87" s="9"/>
+      <c r="B87" s="9"/>
+      <c r="C87" s="10"/>
+      <c r="D87" s="10"/>
+      <c r="E87" s="10"/>
+    </row>
+    <row r="88" ht="14.6" customHeight="1">
+      <c r="A88" s="7"/>
+      <c r="B88" s="7"/>
+      <c r="C88" s="8"/>
+      <c r="D88" s="8"/>
+      <c r="E88" s="8"/>
+    </row>
+    <row r="89" ht="14.6" customHeight="1">
+      <c r="A89" s="9"/>
+      <c r="B89" s="9"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="10"/>
+      <c r="E89" s="10"/>
+    </row>
+    <row r="90" ht="14.6" customHeight="1">
+      <c r="A90" s="7"/>
+      <c r="B90" s="7"/>
+      <c r="C90" s="8"/>
+      <c r="D90" s="8"/>
+      <c r="E90" s="8"/>
+    </row>
+    <row r="91" ht="14.6" customHeight="1">
+      <c r="A91" s="10"/>
+      <c r="B91" s="10"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="10"/>
+      <c r="E91" s="10"/>
+    </row>
+    <row r="92" ht="14.6" customHeight="1">
+      <c r="A92" s="7"/>
+      <c r="B92" s="7"/>
+      <c r="C92" s="8"/>
+      <c r="D92" s="8"/>
+      <c r="E92" s="8"/>
+    </row>
+    <row r="93" ht="14.6" customHeight="1">
+      <c r="A93" s="9"/>
+      <c r="B93" s="9"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="10"/>
+      <c r="E93" s="10"/>
+    </row>
+    <row r="94" ht="14.6" customHeight="1">
+      <c r="A94" s="7"/>
+      <c r="B94" s="7"/>
+      <c r="C94" s="8"/>
+      <c r="D94" s="8"/>
+      <c r="E94" s="8"/>
+    </row>
+    <row r="95" ht="14.6" customHeight="1">
+      <c r="A95" s="10"/>
+      <c r="B95" s="10"/>
+      <c r="C95" s="10"/>
+      <c r="D95" s="10"/>
+      <c r="E95" s="10"/>
+    </row>
+    <row r="96" ht="14.6" customHeight="1">
+      <c r="A96" s="7"/>
+      <c r="B96" s="7"/>
+      <c r="C96" s="8"/>
+      <c r="D96" s="8"/>
+      <c r="E96" s="8"/>
+    </row>
+    <row r="97" ht="14.6" customHeight="1">
+      <c r="A97" s="9"/>
+      <c r="B97" s="9"/>
+      <c r="C97" s="10"/>
+      <c r="D97" s="10"/>
+      <c r="E97" s="10"/>
+    </row>
+    <row r="98" ht="14.6" customHeight="1">
+      <c r="A98" s="7"/>
+      <c r="B98" s="7"/>
+      <c r="C98" s="8"/>
+      <c r="D98" s="8"/>
+      <c r="E98" s="8"/>
+    </row>
+    <row r="99" ht="14.6" customHeight="1">
+      <c r="A99" s="9"/>
+      <c r="B99" s="9"/>
+      <c r="C99" s="10"/>
+      <c r="D99" s="10"/>
+      <c r="E99" s="10"/>
+    </row>
+    <row r="100" ht="14.6" customHeight="1">
+      <c r="A100" s="8"/>
+      <c r="B100" s="8"/>
+      <c r="C100" s="8"/>
+      <c r="D100" s="8"/>
+      <c r="E100" s="8"/>
+    </row>
+    <row r="101" ht="14.6" customHeight="1">
+      <c r="A101" s="9"/>
+      <c r="B101" s="9"/>
+      <c r="C101" s="10"/>
+      <c r="D101" s="10"/>
+      <c r="E101" s="10"/>
+    </row>
+    <row r="102" ht="14.6" customHeight="1">
+      <c r="A102" s="7"/>
+      <c r="B102" s="7"/>
+      <c r="C102" s="8"/>
+      <c r="D102" s="8"/>
+      <c r="E102" s="8"/>
+    </row>
+    <row r="103" ht="14.6" customHeight="1">
+      <c r="A103" s="10"/>
+      <c r="B103" s="10"/>
+      <c r="C103" s="10"/>
+      <c r="D103" s="10"/>
+      <c r="E103" s="10"/>
+    </row>
+    <row r="104" ht="14.6" customHeight="1">
+      <c r="A104" s="7"/>
+      <c r="B104" s="7"/>
+      <c r="C104" s="8"/>
+      <c r="D104" s="8"/>
+      <c r="E104" s="8"/>
+    </row>
+    <row r="105" ht="14.6" customHeight="1">
+      <c r="A105" s="9"/>
+      <c r="B105" s="9"/>
+      <c r="C105" s="10"/>
+      <c r="D105" s="10"/>
+      <c r="E105" s="10"/>
+    </row>
+    <row r="106" ht="14.6" customHeight="1">
+      <c r="A106" s="7"/>
+      <c r="B106" s="7"/>
+      <c r="C106" s="8"/>
+      <c r="D106" s="8"/>
+      <c r="E106" s="8"/>
+    </row>
+    <row r="107" ht="14.6" customHeight="1">
+      <c r="A107" s="10"/>
+      <c r="B107" s="10"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="10"/>
+      <c r="E107" s="10"/>
+    </row>
+    <row r="108" ht="14.6" customHeight="1">
+      <c r="A108" s="7"/>
+      <c r="B108" s="7"/>
+      <c r="C108" s="8"/>
+      <c r="D108" s="8"/>
+      <c r="E108" s="8"/>
+    </row>
+    <row r="109" ht="14.6" customHeight="1">
+      <c r="A109" s="9"/>
+      <c r="B109" s="9"/>
+      <c r="C109" s="10"/>
+      <c r="D109" s="10"/>
+      <c r="E109" s="10"/>
+    </row>
+    <row r="110" ht="14.6" customHeight="1">
+      <c r="A110" s="8"/>
+      <c r="B110" s="8"/>
+      <c r="C110" s="8"/>
+      <c r="D110" s="8"/>
+      <c r="E110" s="8"/>
+    </row>
+    <row r="111" ht="14.6" customHeight="1">
+      <c r="A111" s="9"/>
+      <c r="B111" s="9"/>
+      <c r="C111" s="10"/>
+      <c r="D111" s="10"/>
+      <c r="E111" s="10"/>
+    </row>
+    <row r="112" ht="14.6" customHeight="1">
+      <c r="A112" s="8"/>
+      <c r="B112" s="8"/>
+      <c r="C112" s="8"/>
+      <c r="D112" s="8"/>
+      <c r="E112" s="8"/>
+    </row>
+    <row r="113" ht="14.6" customHeight="1">
+      <c r="A113" s="9"/>
+      <c r="B113" s="9"/>
+      <c r="C113" s="10"/>
+      <c r="D113" s="10"/>
+      <c r="E113" s="10"/>
+    </row>
+    <row r="114" ht="14.6" customHeight="1">
+      <c r="A114" s="7"/>
+      <c r="B114" s="7"/>
+      <c r="C114" s="8"/>
+      <c r="D114" s="8"/>
+      <c r="E114" s="8"/>
+    </row>
+    <row r="115" ht="14.6" customHeight="1">
+      <c r="A115" s="10"/>
+      <c r="B115" s="10"/>
+      <c r="C115" s="10"/>
+      <c r="D115" s="10"/>
+      <c r="E115" s="10"/>
+    </row>
+    <row r="116" ht="14.6" customHeight="1">
+      <c r="A116" s="7"/>
+      <c r="B116" s="7"/>
+      <c r="C116" s="8"/>
+      <c r="D116" s="8"/>
+      <c r="E116" s="8"/>
+    </row>
+    <row r="117" ht="14.6" customHeight="1">
+      <c r="A117" s="9"/>
+      <c r="B117" s="9"/>
+      <c r="C117" s="10"/>
+      <c r="D117" s="10"/>
+      <c r="E117" s="10"/>
+    </row>
+    <row r="118" ht="14.6" customHeight="1">
+      <c r="A118" s="8"/>
+      <c r="B118" s="8"/>
+      <c r="C118" s="8"/>
+      <c r="D118" s="8"/>
+      <c r="E118" s="8"/>
+    </row>
+    <row r="119" ht="14.6" customHeight="1">
+      <c r="A119" s="10"/>
+      <c r="B119" s="10"/>
+      <c r="C119" s="10"/>
+      <c r="D119" s="10"/>
+      <c r="E119" s="10"/>
+    </row>
+    <row r="120" ht="14.6" customHeight="1">
+      <c r="A120" s="7"/>
+      <c r="B120" s="8"/>
+      <c r="C120" s="8"/>
+      <c r="D120" s="8"/>
+      <c r="E120" s="8"/>
+    </row>
+    <row r="121" ht="14.6" customHeight="1">
+      <c r="A121" s="9"/>
+      <c r="B121" s="10"/>
+      <c r="C121" s="10"/>
+      <c r="D121" s="10"/>
+      <c r="E121" s="10"/>
+    </row>
+    <row r="122" ht="14.6" customHeight="1">
+      <c r="A122" s="7"/>
+      <c r="B122" s="7"/>
+      <c r="C122" s="8"/>
+      <c r="D122" s="8"/>
+      <c r="E122" s="8"/>
+    </row>
+    <row r="123" ht="14.6" customHeight="1">
+      <c r="A123" s="10"/>
+      <c r="B123" s="10"/>
+      <c r="C123" s="10"/>
+      <c r="D123" s="10"/>
+      <c r="E123" s="10"/>
+    </row>
+    <row r="124" ht="14.6" customHeight="1">
+      <c r="A124" s="7"/>
+      <c r="B124" s="7"/>
+      <c r="C124" s="8"/>
+      <c r="D124" s="8"/>
+      <c r="E124" s="8"/>
+    </row>
+    <row r="125" ht="14.6" customHeight="1">
+      <c r="A125" s="10"/>
+      <c r="B125" s="10"/>
+      <c r="C125" s="10"/>
+      <c r="D125" s="10"/>
+      <c r="E125" s="10"/>
+    </row>
+    <row r="126" ht="14.6" customHeight="1">
+      <c r="A126" s="8"/>
+      <c r="B126" s="8"/>
+      <c r="C126" s="8"/>
+      <c r="D126" s="8"/>
+      <c r="E126" s="8"/>
+    </row>
+    <row r="127" ht="14.6" customHeight="1">
+      <c r="A127" s="10"/>
+      <c r="B127" s="10"/>
+      <c r="C127" s="10"/>
+      <c r="D127" s="10"/>
+      <c r="E127" s="10"/>
+    </row>
+    <row r="128" ht="14.6" customHeight="1">
+      <c r="A128" s="8"/>
+      <c r="B128" s="8"/>
+      <c r="C128" s="8"/>
+      <c r="D128" s="8"/>
+      <c r="E128" s="8"/>
+    </row>
+    <row r="129" ht="14.6" customHeight="1">
+      <c r="A129" s="9"/>
+      <c r="B129" s="9"/>
+      <c r="C129" s="10"/>
+      <c r="D129" s="10"/>
+      <c r="E129" s="10"/>
+    </row>
+    <row r="130" ht="14.6" customHeight="1">
+      <c r="A130" s="7"/>
+      <c r="B130" s="7"/>
+      <c r="C130" s="8"/>
+      <c r="D130" s="8"/>
+      <c r="E130" s="8"/>
+    </row>
+    <row r="131" ht="14.6" customHeight="1">
+      <c r="A131" s="9"/>
+      <c r="B131" s="9"/>
+      <c r="C131" s="10"/>
+      <c r="D131" s="10"/>
+      <c r="E131" s="10"/>
+    </row>
+    <row r="132" ht="14.6" customHeight="1">
+      <c r="A132" s="7"/>
+      <c r="B132" s="7"/>
+      <c r="C132" s="8"/>
+      <c r="D132" s="8"/>
+      <c r="E132" s="8"/>
+    </row>
+    <row r="133" ht="14.6" customHeight="1">
+      <c r="A133" s="9"/>
+      <c r="B133" s="9"/>
+      <c r="C133" s="10"/>
+      <c r="D133" s="10"/>
+      <c r="E133" s="10"/>
+    </row>
+    <row r="134" ht="14.6" customHeight="1">
+      <c r="A134" s="7"/>
+      <c r="B134" s="7"/>
+      <c r="C134" s="8"/>
+      <c r="D134" s="8"/>
+      <c r="E134" s="8"/>
+    </row>
+    <row r="135" ht="14.6" customHeight="1">
+      <c r="A135" s="9"/>
+      <c r="B135" s="9"/>
+      <c r="C135" s="10"/>
+      <c r="D135" s="10"/>
+      <c r="E135" s="10"/>
+    </row>
+    <row r="136" ht="14.6" customHeight="1">
+      <c r="A136" s="7"/>
+      <c r="B136" s="7"/>
+      <c r="C136" s="8"/>
+      <c r="D136" s="8"/>
+      <c r="E136" s="8"/>
+    </row>
+    <row r="137" ht="14.6" customHeight="1">
+      <c r="A137" s="10"/>
+      <c r="B137" s="10"/>
+      <c r="C137" s="10"/>
+      <c r="D137" s="10"/>
+      <c r="E137" s="10"/>
+    </row>
+    <row r="138" ht="14.6" customHeight="1">
+      <c r="A138" s="7"/>
+      <c r="B138" s="7"/>
+      <c r="C138" s="8"/>
+      <c r="D138" s="8"/>
+      <c r="E138" s="8"/>
+    </row>
+    <row r="139" ht="14.6" customHeight="1">
+      <c r="A139" s="9"/>
+      <c r="B139" s="9"/>
+      <c r="C139" s="10"/>
+      <c r="D139" s="10"/>
+      <c r="E139" s="10"/>
+    </row>
+    <row r="140" ht="14.6" customHeight="1">
+      <c r="A140" s="7"/>
+      <c r="B140" s="7"/>
+      <c r="C140" s="8"/>
+      <c r="D140" s="8"/>
+      <c r="E140" s="8"/>
+    </row>
+    <row r="141" ht="14.6" customHeight="1">
+      <c r="A141" s="9"/>
+      <c r="B141" s="9"/>
+      <c r="C141" s="10"/>
+      <c r="D141" s="10"/>
+      <c r="E141" s="10"/>
+    </row>
+    <row r="142" ht="14.6" customHeight="1">
+      <c r="A142" s="8"/>
+      <c r="B142" s="8"/>
+      <c r="C142" s="8"/>
+      <c r="D142" s="8"/>
+      <c r="E142" s="8"/>
+    </row>
+    <row r="143" ht="14.6" customHeight="1">
+      <c r="A143" s="9"/>
+      <c r="B143" s="9"/>
+      <c r="C143" s="10"/>
+      <c r="D143" s="10"/>
+      <c r="E143" s="10"/>
+    </row>
+    <row r="144" ht="14.6" customHeight="1">
+      <c r="A144" s="7"/>
+      <c r="B144" s="7"/>
+      <c r="C144" s="8"/>
+      <c r="D144" s="8"/>
+      <c r="E144" s="8"/>
+    </row>
+    <row r="145" ht="14.6" customHeight="1">
+      <c r="A145" s="9"/>
+      <c r="B145" s="9"/>
+      <c r="C145" s="10"/>
+      <c r="D145" s="10"/>
+      <c r="E145" s="10"/>
+    </row>
+    <row r="146" ht="14.6" customHeight="1">
+      <c r="A146" s="7"/>
+      <c r="B146" s="7"/>
+      <c r="C146" s="8"/>
+      <c r="D146" s="8"/>
+      <c r="E146" s="8"/>
+    </row>
+    <row r="147" ht="14.6" customHeight="1">
+      <c r="A147" s="9"/>
+      <c r="B147" s="9"/>
+      <c r="C147" s="10"/>
+      <c r="D147" s="10"/>
+      <c r="E147" s="10"/>
+    </row>
+    <row r="148" ht="14.6" customHeight="1">
+      <c r="A148" s="7"/>
+      <c r="B148" s="7"/>
+      <c r="C148" s="8"/>
+      <c r="D148" s="8"/>
+      <c r="E148" s="8"/>
+    </row>
+    <row r="149" ht="14.6" customHeight="1">
+      <c r="A149" s="9"/>
+      <c r="B149" s="9"/>
+      <c r="C149" s="10"/>
+      <c r="D149" s="10"/>
+      <c r="E149" s="10"/>
+    </row>
+    <row r="150" ht="14.6" customHeight="1">
+      <c r="A150" s="8"/>
+      <c r="B150" s="8"/>
+      <c r="C150" s="8"/>
+      <c r="D150" s="8"/>
+      <c r="E150" s="8"/>
+    </row>
+    <row r="151" ht="14.6" customHeight="1">
+      <c r="A151" s="9"/>
+      <c r="B151" s="9"/>
+      <c r="C151" s="10"/>
+      <c r="D151" s="10"/>
+      <c r="E151" s="10"/>
+    </row>
+    <row r="152" ht="14.6" customHeight="1">
+      <c r="A152" s="7"/>
+      <c r="B152" s="7"/>
+      <c r="C152" s="8"/>
+      <c r="D152" s="8"/>
+      <c r="E152" s="8"/>
+    </row>
+    <row r="153" ht="14.6" customHeight="1">
+      <c r="A153" s="9"/>
+      <c r="B153" s="9"/>
+      <c r="C153" s="10"/>
+      <c r="D153" s="10"/>
+      <c r="E153" s="10"/>
+    </row>
+    <row r="154" ht="14.6" customHeight="1">
+      <c r="A154" s="8"/>
+      <c r="B154" s="8"/>
+      <c r="C154" s="8"/>
+      <c r="D154" s="8"/>
+      <c r="E154" s="8"/>
+    </row>
+    <row r="155" ht="14.6" customHeight="1">
+      <c r="A155" s="9"/>
+      <c r="B155" s="9"/>
+      <c r="C155" s="10"/>
+      <c r="D155" s="10"/>
+      <c r="E155" s="10"/>
+    </row>
+    <row r="156" ht="14.6" customHeight="1">
+      <c r="A156" s="7"/>
+      <c r="B156" s="7"/>
+      <c r="C156" s="8"/>
+      <c r="D156" s="8"/>
+      <c r="E156" s="8"/>
+    </row>
+    <row r="157" ht="14.6" customHeight="1">
+      <c r="A157" s="10"/>
+      <c r="B157" s="10"/>
+      <c r="C157" s="10"/>
+      <c r="D157" s="10"/>
+      <c r="E157" s="10"/>
+    </row>
+    <row r="158" ht="14.6" customHeight="1">
+      <c r="A158" s="7"/>
+      <c r="B158" s="7"/>
+      <c r="C158" s="8"/>
+      <c r="D158" s="8"/>
+      <c r="E158" s="8"/>
+    </row>
+    <row r="159" ht="14.6" customHeight="1">
+      <c r="A159" s="9"/>
+      <c r="B159" s="9"/>
+      <c r="C159" s="10"/>
+      <c r="D159" s="10"/>
+      <c r="E159" s="10"/>
+    </row>
+    <row r="160" ht="14.6" customHeight="1">
+      <c r="A160" s="8"/>
+      <c r="B160" s="8"/>
+      <c r="C160" s="8"/>
+      <c r="D160" s="8"/>
+      <c r="E160" s="8"/>
+    </row>
+    <row r="161" ht="14.6" customHeight="1">
+      <c r="A161" s="9"/>
+      <c r="B161" s="9"/>
+      <c r="C161" s="10"/>
+      <c r="D161" s="10"/>
+      <c r="E161" s="10"/>
+    </row>
+    <row r="162" ht="14.6" customHeight="1">
+      <c r="A162" s="7"/>
+      <c r="B162" s="7"/>
+      <c r="C162" s="8"/>
+      <c r="D162" s="8"/>
+      <c r="E162" s="8"/>
+    </row>
+    <row r="163" ht="14.6" customHeight="1">
+      <c r="A163" s="10"/>
+      <c r="B163" s="10"/>
+      <c r="C163" s="10"/>
+      <c r="D163" s="10"/>
+      <c r="E163" s="10"/>
+    </row>
+    <row r="164" ht="14.6" customHeight="1">
+      <c r="A164" s="7"/>
+      <c r="B164" s="7"/>
+      <c r="C164" s="8"/>
+      <c r="D164" s="8"/>
+      <c r="E164" s="8"/>
+    </row>
+    <row r="165" ht="14.6" customHeight="1">
+      <c r="A165" s="9"/>
+      <c r="B165" s="9"/>
+      <c r="C165" s="10"/>
+      <c r="D165" s="10"/>
+      <c r="E165" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E165"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="14.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="28.6719" style="29" customWidth="1"/>
+    <col min="2" max="2" width="61.8438" style="29" customWidth="1"/>
+    <col min="3" max="5" width="16.3516" style="29" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.6" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" ht="14.6" customHeight="1">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" ht="38.6" customHeight="1">
+      <c r="A3" t="s" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s" s="7">
+        <v>65</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" ht="38.6" customHeight="1">
+      <c r="A4" t="s" s="9">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s" s="9">
+        <v>66</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" ht="14.6" customHeight="1">
+      <c r="A5" t="s" s="7">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" ht="26.6" customHeight="1">
+      <c r="A6" t="s" s="9">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s" s="9">
+        <v>67</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" ht="14.6" customHeight="1">
+      <c r="A7" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" ht="14.6" customHeight="1">
+      <c r="A8" t="s" s="9">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s" s="9">
+        <v>12</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" ht="14.6" customHeight="1">
+      <c r="A9" t="s" s="9">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s" s="9">
+        <v>14</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" ht="14.6" customHeight="1">
+      <c r="A10" t="s" s="7">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s" s="7">
+        <v>29</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" ht="26.6" customHeight="1">
+      <c r="A11" t="s" s="9">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s" s="9">
+        <v>31</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+    </row>
+    <row r="12" ht="14.6" customHeight="1">
+      <c r="A12" t="s" s="7">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s" s="24">
+        <v>54</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" ht="14.6" customHeight="1">
+      <c r="A13" t="s" s="7">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s" s="24">
+        <v>56</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" ht="14.6" customHeight="1">
+      <c r="A14" t="s" s="13">
+        <v>57</v>
+      </c>
+      <c r="B14" t="s" s="25">
+        <v>58</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" ht="14.6" customHeight="1">
+      <c r="A15" t="s" s="9">
+        <v>59</v>
+      </c>
+      <c r="B15" t="s" s="26">
+        <v>60</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+    </row>
+    <row r="16" ht="14.6" customHeight="1">
+      <c r="A16" t="s" s="7">
+        <v>61</v>
+      </c>
+      <c r="B16" t="s" s="24">
+        <v>62</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" ht="14.6" customHeight="1">
+      <c r="A17" t="s" s="27">
+        <v>63</v>
+      </c>
+      <c r="B17" t="s" s="28">
+        <v>64</v>
+      </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>

</xml_diff>

<commit_message>
AOC NBFC n NBFC CFS After feedback points
</commit_message>
<xml_diff>
--- a/DataExtraction/Input/Config.xlsx
+++ b/DataExtraction/Input/Config.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="70">
   <si>
     <t>Key</t>
   </si>
@@ -212,6 +212,12 @@
     <t>Constant</t>
   </si>
   <si>
+    <t>Additional_Auditor_Table_Name</t>
+  </si>
+  <si>
+    <t>additional_auditor_details</t>
+  </si>
+  <si>
     <t>/Users/gundukalyan/Documents/GitHub/mns-json-prep/DataExtraction/Input/AOC4_NBFC_CFS/5.Form AOC-4 CFS NBFC(Ind AS)-26072023_signed.pdf</t>
   </si>
   <si>
@@ -228,7 +234,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -246,6 +252,11 @@
     </font>
     <font>
       <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -491,7 +502,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -577,6 +588,12 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -5595,9 +5612,13 @@
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
     </row>
-    <row r="18" ht="14.6" customHeight="1">
-      <c r="A18" s="17"/>
-      <c r="B18" s="18"/>
+    <row r="18" ht="15.35" customHeight="1">
+      <c r="A18" t="s" s="29">
+        <v>65</v>
+      </c>
+      <c r="B18" t="s" s="30">
+        <v>66</v>
+      </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -6653,10 +6674,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="14.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="28.6719" style="29" customWidth="1"/>
-    <col min="2" max="2" width="61.8438" style="29" customWidth="1"/>
-    <col min="3" max="5" width="16.3516" style="29" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="29" customWidth="1"/>
+    <col min="1" max="1" width="28.6719" style="31" customWidth="1"/>
+    <col min="2" max="2" width="61.8438" style="31" customWidth="1"/>
+    <col min="3" max="5" width="16.3516" style="31" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
@@ -6682,7 +6703,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -6693,7 +6714,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -6715,7 +6736,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s" s="9">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -6842,9 +6863,13 @@
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
     </row>
-    <row r="18" ht="14.6" customHeight="1">
-      <c r="A18" s="17"/>
-      <c r="B18" s="18"/>
+    <row r="18" ht="15.35" customHeight="1">
+      <c r="A18" t="s" s="29">
+        <v>65</v>
+      </c>
+      <c r="B18" t="s" s="30">
+        <v>66</v>
+      </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>

</xml_diff>

<commit_message>
form 8 interim Dev complete with testing
</commit_message>
<xml_diff>
--- a/DataExtraction/Input/Config.xlsx
+++ b/DataExtraction/Input/Config.xlsx
@@ -9820,7 +9820,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E186"/>
+  <dimension ref="A1:E185"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -9948,128 +9948,128 @@
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" ht="26.6" customHeight="1">
-      <c r="A13" t="s" s="9">
-        <v>30</v>
-      </c>
-      <c r="B13" t="s" s="9">
-        <v>31</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
+    <row r="13" ht="15.35" customHeight="1">
+      <c r="A13" s="21"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
     </row>
     <row r="14" ht="15.35" customHeight="1">
-      <c r="A14" s="21"/>
-      <c r="B14" s="22"/>
+      <c r="A14" t="s" s="29">
+        <v>125</v>
+      </c>
+      <c r="B14" t="s" s="29">
+        <v>126</v>
+      </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
     </row>
     <row r="15" ht="15.35" customHeight="1">
-      <c r="A15" t="s" s="29">
-        <v>125</v>
-      </c>
-      <c r="B15" t="s" s="29">
-        <v>126</v>
+      <c r="A15" t="s" s="21">
+        <v>127</v>
+      </c>
+      <c r="B15" t="s" s="7">
+        <v>128</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
     </row>
     <row r="16" ht="15.35" customHeight="1">
-      <c r="A16" t="s" s="21">
-        <v>127</v>
-      </c>
-      <c r="B16" t="s" s="7">
-        <v>128</v>
-      </c>
+      <c r="A16" s="29"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
     </row>
     <row r="17" ht="15.35" customHeight="1">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" t="s" s="29">
+        <v>129</v>
+      </c>
+      <c r="B17" t="s" s="29">
+        <v>130</v>
+      </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
     </row>
     <row r="18" ht="15.35" customHeight="1">
-      <c r="A18" t="s" s="29">
-        <v>129</v>
-      </c>
-      <c r="B18" t="s" s="29">
-        <v>130</v>
-      </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="A18" t="s" s="23">
+        <v>54</v>
+      </c>
+      <c r="B18" t="s" s="9">
+        <v>55</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
     </row>
     <row r="19" ht="15.35" customHeight="1">
-      <c r="A19" t="s" s="23">
-        <v>54</v>
-      </c>
-      <c r="B19" t="s" s="9">
-        <v>55</v>
-      </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
+      <c r="A19" t="s" s="22">
+        <v>56</v>
+      </c>
+      <c r="B19" t="s" s="22">
+        <v>57</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
     </row>
     <row r="20" ht="15.35" customHeight="1">
-      <c r="A20" t="s" s="22">
-        <v>56</v>
-      </c>
-      <c r="B20" t="s" s="22">
-        <v>57</v>
-      </c>
+      <c r="A20" s="21"/>
+      <c r="B20" s="22"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
     </row>
     <row r="21" ht="15.35" customHeight="1">
-      <c r="A21" s="21"/>
-      <c r="B21" s="22"/>
+      <c r="A21" t="s" s="9">
+        <v>62</v>
+      </c>
+      <c r="B21" t="s" s="22">
+        <v>131</v>
+      </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
     </row>
     <row r="22" ht="15.35" customHeight="1">
-      <c r="A22" t="s" s="9">
-        <v>62</v>
+      <c r="A22" t="s" s="7">
+        <v>64</v>
       </c>
       <c r="B22" t="s" s="22">
-        <v>131</v>
+        <v>65</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
     </row>
     <row r="23" ht="15.35" customHeight="1">
-      <c r="A23" t="s" s="7">
-        <v>64</v>
-      </c>
-      <c r="B23" t="s" s="22">
-        <v>65</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
     </row>
     <row r="24" ht="15.35" customHeight="1">
-      <c r="A24" s="7"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
+      <c r="A24" t="s" s="21">
+        <v>132</v>
+      </c>
+      <c r="B24" t="s" s="22">
+        <v>133</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
     </row>
     <row r="25" ht="15.35" customHeight="1">
       <c r="A25" t="s" s="21">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B25" t="s" s="22">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
@@ -10077,39 +10077,39 @@
     </row>
     <row r="26" ht="15.35" customHeight="1">
       <c r="A26" t="s" s="21">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B26" t="s" s="22">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
     </row>
     <row r="27" ht="15.35" customHeight="1">
-      <c r="A27" t="s" s="21">
-        <v>136</v>
-      </c>
-      <c r="B27" t="s" s="22">
-        <v>137</v>
-      </c>
+      <c r="A27" s="21"/>
+      <c r="B27" s="22"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
     </row>
     <row r="28" ht="15.35" customHeight="1">
-      <c r="A28" s="21"/>
-      <c r="B28" s="22"/>
+      <c r="A28" t="s" s="29">
+        <v>138</v>
+      </c>
+      <c r="B28" t="s" s="29">
+        <v>139</v>
+      </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
     </row>
     <row r="29" ht="15.35" customHeight="1">
       <c r="A29" t="s" s="29">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B29" t="s" s="29">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -10117,1162 +10117,1151 @@
     </row>
     <row r="30" ht="15.35" customHeight="1">
       <c r="A30" t="s" s="29">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B30" t="s" s="29">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
     </row>
     <row r="31" ht="15.35" customHeight="1">
-      <c r="A31" t="s" s="29">
-        <v>142</v>
-      </c>
-      <c r="B31" t="s" s="29">
-        <v>143</v>
-      </c>
+      <c r="A31" s="21"/>
+      <c r="B31" s="22"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
     </row>
     <row r="32" ht="15.35" customHeight="1">
-      <c r="A32" s="21"/>
-      <c r="B32" s="22"/>
+      <c r="A32" t="s" s="46">
+        <v>144</v>
+      </c>
+      <c r="B32" t="s" s="25">
+        <v>145</v>
+      </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" ht="15.35" customHeight="1">
-      <c r="A33" t="s" s="46">
-        <v>144</v>
-      </c>
-      <c r="B33" t="s" s="25">
+    <row r="33" ht="14.6" customHeight="1">
+      <c r="A33" t="s" s="13">
+        <v>146</v>
+      </c>
+      <c r="B33" t="s" s="47">
         <v>145</v>
       </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
     </row>
     <row r="34" ht="14.6" customHeight="1">
-      <c r="A34" t="s" s="13">
-        <v>146</v>
-      </c>
-      <c r="B34" t="s" s="47">
-        <v>145</v>
+      <c r="A34" t="s" s="24">
+        <v>147</v>
+      </c>
+      <c r="B34" t="s" s="25">
+        <v>59</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
     </row>
     <row r="35" ht="14.6" customHeight="1">
-      <c r="A35" t="s" s="24">
-        <v>147</v>
-      </c>
-      <c r="B35" t="s" s="25">
-        <v>59</v>
-      </c>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
+      <c r="A35" s="48"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
     </row>
     <row r="36" ht="14.6" customHeight="1">
-      <c r="A36" s="48"/>
-      <c r="B36" s="49"/>
+      <c r="A36" t="s" s="26">
+        <v>60</v>
+      </c>
+      <c r="B36" t="s" s="27">
+        <v>61</v>
+      </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
     </row>
     <row r="37" ht="14.6" customHeight="1">
-      <c r="A37" t="s" s="26">
-        <v>60</v>
-      </c>
-      <c r="B37" t="s" s="27">
-        <v>61</v>
-      </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
+      <c r="A37" t="s" s="7">
+        <v>52</v>
+      </c>
+      <c r="B37" t="s" s="22">
+        <v>53</v>
+      </c>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
     </row>
     <row r="38" ht="14.6" customHeight="1">
-      <c r="A38" t="s" s="7">
-        <v>52</v>
-      </c>
-      <c r="B38" t="s" s="22">
-        <v>53</v>
-      </c>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
+      <c r="A38" s="29"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
     </row>
     <row r="39" ht="14.6" customHeight="1">
-      <c r="A39" s="29"/>
-      <c r="B39" s="29"/>
+      <c r="A39" t="s" s="29">
+        <v>120</v>
+      </c>
+      <c r="B39" t="s" s="29">
+        <v>121</v>
+      </c>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
     </row>
     <row r="40" ht="14.6" customHeight="1">
-      <c r="A40" t="s" s="29">
-        <v>120</v>
-      </c>
-      <c r="B40" t="s" s="29">
-        <v>121</v>
-      </c>
+      <c r="A40" s="50"/>
+      <c r="B40" s="51"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
     </row>
     <row r="41" ht="14.6" customHeight="1">
-      <c r="A41" s="50"/>
-      <c r="B41" s="51"/>
+      <c r="A41" t="s" s="52">
+        <v>148</v>
+      </c>
+      <c r="B41" s="53">
+        <v>0</v>
+      </c>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" ht="14.6" customHeight="1">
-      <c r="A42" t="s" s="52">
-        <v>148</v>
-      </c>
-      <c r="B42" s="53">
-        <v>0</v>
-      </c>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
+      <c r="A42" t="s" s="54">
+        <v>149</v>
+      </c>
+      <c r="B42" s="55">
+        <v>1</v>
+      </c>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
     </row>
     <row r="43" ht="14.6" customHeight="1">
-      <c r="A43" t="s" s="54">
-        <v>149</v>
-      </c>
-      <c r="B43" s="55">
-        <v>1</v>
+      <c r="A43" t="s" s="56">
+        <v>150</v>
+      </c>
+      <c r="B43" s="57">
+        <v>2</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
     </row>
     <row r="44" ht="14.6" customHeight="1">
-      <c r="A44" t="s" s="56">
-        <v>150</v>
-      </c>
-      <c r="B44" s="57">
-        <v>2</v>
-      </c>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
+      <c r="A44" t="s" s="58">
+        <v>151</v>
+      </c>
+      <c r="B44" s="59">
+        <v>3</v>
+      </c>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
     </row>
     <row r="45" ht="14.6" customHeight="1">
-      <c r="A45" t="s" s="58">
-        <v>151</v>
-      </c>
-      <c r="B45" s="59">
-        <v>3</v>
-      </c>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
+      <c r="A45" t="s" s="60">
+        <v>152</v>
+      </c>
+      <c r="B45" s="61">
+        <v>4</v>
+      </c>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
     </row>
     <row r="46" ht="14.6" customHeight="1">
-      <c r="A46" t="s" s="60">
-        <v>152</v>
-      </c>
-      <c r="B46" s="61">
-        <v>4</v>
-      </c>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
+      <c r="A46" t="s" s="58">
+        <v>153</v>
+      </c>
+      <c r="B46" s="59">
+        <v>5</v>
+      </c>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
     </row>
     <row r="47" ht="14.6" customHeight="1">
-      <c r="A47" t="s" s="58">
-        <v>153</v>
-      </c>
-      <c r="B47" s="59">
-        <v>5</v>
-      </c>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
+      <c r="A47" t="s" s="62">
+        <v>154</v>
+      </c>
+      <c r="B47" s="63">
+        <v>6</v>
+      </c>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
     </row>
     <row r="48" ht="14.6" customHeight="1">
-      <c r="A48" t="s" s="62">
-        <v>154</v>
-      </c>
-      <c r="B48" s="63">
-        <v>6</v>
-      </c>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
+      <c r="A48" s="9"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
     </row>
     <row r="49" ht="14.6" customHeight="1">
       <c r="A49" s="9"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
     </row>
     <row r="50" ht="14.6" customHeight="1">
-      <c r="A50" s="9"/>
-      <c r="B50" s="9"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
     </row>
     <row r="51" ht="14.6" customHeight="1">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
+      <c r="A51" s="10"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
     </row>
     <row r="52" ht="14.6" customHeight="1">
-      <c r="A52" s="10"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
+      <c r="A52" s="7"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
     </row>
     <row r="53" ht="14.6" customHeight="1">
-      <c r="A53" s="7"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
     </row>
     <row r="54" ht="14.6" customHeight="1">
-      <c r="A54" s="9"/>
-      <c r="B54" s="9"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
+      <c r="A54" s="8"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
     </row>
     <row r="55" ht="14.6" customHeight="1">
-      <c r="A55" s="8"/>
-      <c r="B55" s="8"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
     </row>
     <row r="56" ht="14.6" customHeight="1">
-      <c r="A56" s="9"/>
-      <c r="B56" s="9"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
+      <c r="A56" s="8"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
     </row>
     <row r="57" ht="14.6" customHeight="1">
-      <c r="A57" s="8"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
     </row>
     <row r="58" ht="14.6" customHeight="1">
-      <c r="A58" s="9"/>
-      <c r="B58" s="9"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
+      <c r="A58" s="8"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
     </row>
     <row r="59" ht="14.6" customHeight="1">
-      <c r="A59" s="8"/>
-      <c r="B59" s="8"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
+      <c r="A59" s="10"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
     </row>
     <row r="60" ht="14.6" customHeight="1">
-      <c r="A60" s="10"/>
-      <c r="B60" s="10"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="10"/>
+      <c r="A60" s="7"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
     </row>
     <row r="61" ht="14.6" customHeight="1">
-      <c r="A61" s="7"/>
-      <c r="B61" s="7"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
+      <c r="A61" s="10"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
     </row>
     <row r="62" ht="14.6" customHeight="1">
-      <c r="A62" s="10"/>
-      <c r="B62" s="10"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="10"/>
+      <c r="A62" s="7"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="8"/>
     </row>
     <row r="63" ht="14.6" customHeight="1">
-      <c r="A63" s="7"/>
-      <c r="B63" s="7"/>
-      <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8"/>
+      <c r="A63" s="9"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
     </row>
     <row r="64" ht="14.6" customHeight="1">
-      <c r="A64" s="9"/>
-      <c r="B64" s="9"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
+      <c r="A64" s="8"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
     </row>
     <row r="65" ht="14.6" customHeight="1">
-      <c r="A65" s="8"/>
-      <c r="B65" s="8"/>
-      <c r="C65" s="8"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="8"/>
+      <c r="A65" s="9"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
     </row>
     <row r="66" ht="14.6" customHeight="1">
-      <c r="A66" s="9"/>
-      <c r="B66" s="9"/>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
-      <c r="E66" s="10"/>
+      <c r="A66" s="7"/>
+      <c r="B66" s="7"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
     </row>
     <row r="67" ht="14.6" customHeight="1">
-      <c r="A67" s="7"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="8"/>
-      <c r="D67" s="8"/>
-      <c r="E67" s="8"/>
+      <c r="A67" s="10"/>
+      <c r="B67" s="10"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10"/>
     </row>
     <row r="68" ht="14.6" customHeight="1">
-      <c r="A68" s="10"/>
-      <c r="B68" s="10"/>
-      <c r="C68" s="10"/>
-      <c r="D68" s="10"/>
-      <c r="E68" s="10"/>
+      <c r="A68" s="8"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
     </row>
     <row r="69" ht="14.6" customHeight="1">
-      <c r="A69" s="8"/>
-      <c r="B69" s="8"/>
-      <c r="C69" s="8"/>
-      <c r="D69" s="8"/>
-      <c r="E69" s="8"/>
+      <c r="A69" s="9"/>
+      <c r="B69" s="9"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
     </row>
     <row r="70" ht="14.6" customHeight="1">
-      <c r="A70" s="9"/>
-      <c r="B70" s="9"/>
-      <c r="C70" s="10"/>
-      <c r="D70" s="10"/>
-      <c r="E70" s="10"/>
+      <c r="A70" s="7"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8"/>
     </row>
     <row r="71" ht="14.6" customHeight="1">
-      <c r="A71" s="7"/>
-      <c r="B71" s="7"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="8"/>
-      <c r="E71" s="8"/>
+      <c r="A71" s="9"/>
+      <c r="B71" s="9"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="10"/>
     </row>
     <row r="72" ht="14.6" customHeight="1">
-      <c r="A72" s="9"/>
-      <c r="B72" s="9"/>
-      <c r="C72" s="10"/>
-      <c r="D72" s="10"/>
-      <c r="E72" s="10"/>
+      <c r="A72" s="7"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
     </row>
     <row r="73" ht="14.6" customHeight="1">
-      <c r="A73" s="7"/>
-      <c r="B73" s="7"/>
-      <c r="C73" s="8"/>
-      <c r="D73" s="8"/>
-      <c r="E73" s="8"/>
+      <c r="A73" s="9"/>
+      <c r="B73" s="9"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10"/>
     </row>
     <row r="74" ht="14.6" customHeight="1">
-      <c r="A74" s="9"/>
-      <c r="B74" s="9"/>
-      <c r="C74" s="10"/>
-      <c r="D74" s="10"/>
-      <c r="E74" s="10"/>
+      <c r="A74" s="8"/>
+      <c r="B74" s="8"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8"/>
+      <c r="E74" s="8"/>
     </row>
     <row r="75" ht="14.6" customHeight="1">
-      <c r="A75" s="8"/>
-      <c r="B75" s="8"/>
-      <c r="C75" s="8"/>
-      <c r="D75" s="8"/>
-      <c r="E75" s="8"/>
+      <c r="A75" s="9"/>
+      <c r="B75" s="9"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="10"/>
     </row>
     <row r="76" ht="14.6" customHeight="1">
-      <c r="A76" s="9"/>
-      <c r="B76" s="9"/>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10"/>
-      <c r="E76" s="10"/>
+      <c r="A76" s="7"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="8"/>
+      <c r="E76" s="8"/>
     </row>
     <row r="77" ht="14.6" customHeight="1">
-      <c r="A77" s="7"/>
-      <c r="B77" s="7"/>
-      <c r="C77" s="8"/>
-      <c r="D77" s="8"/>
-      <c r="E77" s="8"/>
+      <c r="A77" s="10"/>
+      <c r="B77" s="10"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="10"/>
     </row>
     <row r="78" ht="14.6" customHeight="1">
-      <c r="A78" s="10"/>
-      <c r="B78" s="10"/>
-      <c r="C78" s="10"/>
-      <c r="D78" s="10"/>
-      <c r="E78" s="10"/>
+      <c r="A78" s="7"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
     </row>
     <row r="79" ht="14.6" customHeight="1">
-      <c r="A79" s="7"/>
-      <c r="B79" s="7"/>
-      <c r="C79" s="8"/>
-      <c r="D79" s="8"/>
-      <c r="E79" s="8"/>
+      <c r="A79" s="10"/>
+      <c r="B79" s="10"/>
+      <c r="C79" s="10"/>
+      <c r="D79" s="10"/>
+      <c r="E79" s="10"/>
     </row>
     <row r="80" ht="14.6" customHeight="1">
-      <c r="A80" s="10"/>
-      <c r="B80" s="10"/>
-      <c r="C80" s="10"/>
-      <c r="D80" s="10"/>
-      <c r="E80" s="10"/>
+      <c r="A80" s="7"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="8"/>
     </row>
     <row r="81" ht="14.6" customHeight="1">
-      <c r="A81" s="7"/>
-      <c r="B81" s="7"/>
-      <c r="C81" s="8"/>
-      <c r="D81" s="8"/>
-      <c r="E81" s="8"/>
+      <c r="A81" s="9"/>
+      <c r="B81" s="10"/>
+      <c r="C81" s="10"/>
+      <c r="D81" s="10"/>
+      <c r="E81" s="10"/>
     </row>
     <row r="82" ht="14.6" customHeight="1">
-      <c r="A82" s="9"/>
-      <c r="B82" s="10"/>
-      <c r="C82" s="10"/>
-      <c r="D82" s="10"/>
-      <c r="E82" s="10"/>
+      <c r="A82" s="7"/>
+      <c r="B82" s="8"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="8"/>
     </row>
     <row r="83" ht="14.6" customHeight="1">
-      <c r="A83" s="7"/>
-      <c r="B83" s="8"/>
-      <c r="C83" s="8"/>
-      <c r="D83" s="8"/>
-      <c r="E83" s="8"/>
+      <c r="A83" s="9"/>
+      <c r="B83" s="10"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="10"/>
+      <c r="E83" s="10"/>
     </row>
     <row r="84" ht="14.6" customHeight="1">
-      <c r="A84" s="9"/>
-      <c r="B84" s="10"/>
-      <c r="C84" s="10"/>
-      <c r="D84" s="10"/>
-      <c r="E84" s="10"/>
+      <c r="A84" s="8"/>
+      <c r="B84" s="8"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
+      <c r="E84" s="8"/>
     </row>
     <row r="85" ht="14.6" customHeight="1">
-      <c r="A85" s="8"/>
-      <c r="B85" s="8"/>
-      <c r="C85" s="8"/>
-      <c r="D85" s="8"/>
-      <c r="E85" s="8"/>
+      <c r="A85" s="10"/>
+      <c r="B85" s="10"/>
+      <c r="C85" s="10"/>
+      <c r="D85" s="10"/>
+      <c r="E85" s="10"/>
     </row>
     <row r="86" ht="14.6" customHeight="1">
-      <c r="A86" s="10"/>
-      <c r="B86" s="10"/>
-      <c r="C86" s="10"/>
-      <c r="D86" s="10"/>
-      <c r="E86" s="10"/>
+      <c r="A86" s="7"/>
+      <c r="B86" s="7"/>
+      <c r="C86" s="8"/>
+      <c r="D86" s="8"/>
+      <c r="E86" s="8"/>
     </row>
     <row r="87" ht="14.6" customHeight="1">
-      <c r="A87" s="7"/>
-      <c r="B87" s="7"/>
-      <c r="C87" s="8"/>
-      <c r="D87" s="8"/>
-      <c r="E87" s="8"/>
+      <c r="A87" s="9"/>
+      <c r="B87" s="9"/>
+      <c r="C87" s="10"/>
+      <c r="D87" s="10"/>
+      <c r="E87" s="10"/>
     </row>
     <row r="88" ht="14.6" customHeight="1">
-      <c r="A88" s="9"/>
-      <c r="B88" s="9"/>
-      <c r="C88" s="10"/>
-      <c r="D88" s="10"/>
-      <c r="E88" s="10"/>
+      <c r="A88" s="7"/>
+      <c r="B88" s="7"/>
+      <c r="C88" s="8"/>
+      <c r="D88" s="8"/>
+      <c r="E88" s="8"/>
     </row>
     <row r="89" ht="14.6" customHeight="1">
-      <c r="A89" s="7"/>
-      <c r="B89" s="7"/>
-      <c r="C89" s="8"/>
-      <c r="D89" s="8"/>
-      <c r="E89" s="8"/>
+      <c r="A89" s="9"/>
+      <c r="B89" s="9"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="10"/>
+      <c r="E89" s="10"/>
     </row>
     <row r="90" ht="14.6" customHeight="1">
-      <c r="A90" s="9"/>
-      <c r="B90" s="9"/>
-      <c r="C90" s="10"/>
-      <c r="D90" s="10"/>
-      <c r="E90" s="10"/>
+      <c r="A90" s="7"/>
+      <c r="B90" s="7"/>
+      <c r="C90" s="8"/>
+      <c r="D90" s="8"/>
+      <c r="E90" s="8"/>
     </row>
     <row r="91" ht="14.6" customHeight="1">
-      <c r="A91" s="7"/>
-      <c r="B91" s="7"/>
-      <c r="C91" s="8"/>
-      <c r="D91" s="8"/>
-      <c r="E91" s="8"/>
+      <c r="A91" s="9"/>
+      <c r="B91" s="9"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="10"/>
+      <c r="E91" s="10"/>
     </row>
     <row r="92" ht="14.6" customHeight="1">
-      <c r="A92" s="9"/>
-      <c r="B92" s="9"/>
-      <c r="C92" s="10"/>
-      <c r="D92" s="10"/>
-      <c r="E92" s="10"/>
+      <c r="A92" s="8"/>
+      <c r="B92" s="8"/>
+      <c r="C92" s="8"/>
+      <c r="D92" s="8"/>
+      <c r="E92" s="8"/>
     </row>
     <row r="93" ht="14.6" customHeight="1">
-      <c r="A93" s="8"/>
-      <c r="B93" s="8"/>
-      <c r="C93" s="8"/>
-      <c r="D93" s="8"/>
-      <c r="E93" s="8"/>
+      <c r="A93" s="9"/>
+      <c r="B93" s="9"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="10"/>
+      <c r="E93" s="10"/>
     </row>
     <row r="94" ht="14.6" customHeight="1">
-      <c r="A94" s="9"/>
-      <c r="B94" s="9"/>
-      <c r="C94" s="10"/>
-      <c r="D94" s="10"/>
-      <c r="E94" s="10"/>
+      <c r="A94" s="7"/>
+      <c r="B94" s="7"/>
+      <c r="C94" s="8"/>
+      <c r="D94" s="8"/>
+      <c r="E94" s="8"/>
     </row>
     <row r="95" ht="14.6" customHeight="1">
-      <c r="A95" s="7"/>
-      <c r="B95" s="7"/>
-      <c r="C95" s="8"/>
-      <c r="D95" s="8"/>
-      <c r="E95" s="8"/>
+      <c r="A95" s="9"/>
+      <c r="B95" s="9"/>
+      <c r="C95" s="10"/>
+      <c r="D95" s="10"/>
+      <c r="E95" s="10"/>
     </row>
     <row r="96" ht="14.6" customHeight="1">
-      <c r="A96" s="9"/>
-      <c r="B96" s="9"/>
-      <c r="C96" s="10"/>
-      <c r="D96" s="10"/>
-      <c r="E96" s="10"/>
+      <c r="A96" s="7"/>
+      <c r="B96" s="7"/>
+      <c r="C96" s="8"/>
+      <c r="D96" s="8"/>
+      <c r="E96" s="8"/>
     </row>
     <row r="97" ht="14.6" customHeight="1">
-      <c r="A97" s="7"/>
-      <c r="B97" s="7"/>
-      <c r="C97" s="8"/>
-      <c r="D97" s="8"/>
-      <c r="E97" s="8"/>
+      <c r="A97" s="9"/>
+      <c r="B97" s="9"/>
+      <c r="C97" s="10"/>
+      <c r="D97" s="10"/>
+      <c r="E97" s="10"/>
     </row>
     <row r="98" ht="14.6" customHeight="1">
-      <c r="A98" s="9"/>
-      <c r="B98" s="9"/>
-      <c r="C98" s="10"/>
-      <c r="D98" s="10"/>
-      <c r="E98" s="10"/>
+      <c r="A98" s="8"/>
+      <c r="B98" s="8"/>
+      <c r="C98" s="8"/>
+      <c r="D98" s="8"/>
+      <c r="E98" s="8"/>
     </row>
     <row r="99" ht="14.6" customHeight="1">
-      <c r="A99" s="8"/>
-      <c r="B99" s="8"/>
-      <c r="C99" s="8"/>
-      <c r="D99" s="8"/>
-      <c r="E99" s="8"/>
+      <c r="A99" s="9"/>
+      <c r="B99" s="9"/>
+      <c r="C99" s="10"/>
+      <c r="D99" s="10"/>
+      <c r="E99" s="10"/>
     </row>
     <row r="100" ht="14.6" customHeight="1">
-      <c r="A100" s="9"/>
-      <c r="B100" s="9"/>
-      <c r="C100" s="10"/>
-      <c r="D100" s="10"/>
-      <c r="E100" s="10"/>
+      <c r="A100" s="7"/>
+      <c r="B100" s="7"/>
+      <c r="C100" s="8"/>
+      <c r="D100" s="8"/>
+      <c r="E100" s="8"/>
     </row>
     <row r="101" ht="14.6" customHeight="1">
-      <c r="A101" s="7"/>
-      <c r="B101" s="7"/>
-      <c r="C101" s="8"/>
-      <c r="D101" s="8"/>
-      <c r="E101" s="8"/>
+      <c r="A101" s="9"/>
+      <c r="B101" s="9"/>
+      <c r="C101" s="10"/>
+      <c r="D101" s="10"/>
+      <c r="E101" s="10"/>
     </row>
     <row r="102" ht="14.6" customHeight="1">
-      <c r="A102" s="9"/>
-      <c r="B102" s="9"/>
-      <c r="C102" s="10"/>
-      <c r="D102" s="10"/>
-      <c r="E102" s="10"/>
+      <c r="A102" s="7"/>
+      <c r="B102" s="7"/>
+      <c r="C102" s="8"/>
+      <c r="D102" s="8"/>
+      <c r="E102" s="8"/>
     </row>
     <row r="103" ht="14.6" customHeight="1">
-      <c r="A103" s="7"/>
-      <c r="B103" s="7"/>
-      <c r="C103" s="8"/>
-      <c r="D103" s="8"/>
-      <c r="E103" s="8"/>
+      <c r="A103" s="9"/>
+      <c r="B103" s="9"/>
+      <c r="C103" s="10"/>
+      <c r="D103" s="10"/>
+      <c r="E103" s="10"/>
     </row>
     <row r="104" ht="14.6" customHeight="1">
-      <c r="A104" s="9"/>
-      <c r="B104" s="9"/>
-      <c r="C104" s="10"/>
-      <c r="D104" s="10"/>
-      <c r="E104" s="10"/>
+      <c r="A104" s="8"/>
+      <c r="B104" s="8"/>
+      <c r="C104" s="8"/>
+      <c r="D104" s="8"/>
+      <c r="E104" s="8"/>
     </row>
     <row r="105" ht="14.6" customHeight="1">
-      <c r="A105" s="8"/>
-      <c r="B105" s="8"/>
-      <c r="C105" s="8"/>
-      <c r="D105" s="8"/>
-      <c r="E105" s="8"/>
+      <c r="A105" s="9"/>
+      <c r="B105" s="10"/>
+      <c r="C105" s="10"/>
+      <c r="D105" s="10"/>
+      <c r="E105" s="10"/>
     </row>
     <row r="106" ht="14.6" customHeight="1">
-      <c r="A106" s="9"/>
-      <c r="B106" s="10"/>
-      <c r="C106" s="10"/>
-      <c r="D106" s="10"/>
-      <c r="E106" s="10"/>
+      <c r="A106" s="7"/>
+      <c r="B106" s="7"/>
+      <c r="C106" s="8"/>
+      <c r="D106" s="8"/>
+      <c r="E106" s="8"/>
     </row>
     <row r="107" ht="14.6" customHeight="1">
-      <c r="A107" s="7"/>
-      <c r="B107" s="7"/>
-      <c r="C107" s="8"/>
-      <c r="D107" s="8"/>
-      <c r="E107" s="8"/>
+      <c r="A107" s="9"/>
+      <c r="B107" s="9"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="10"/>
+      <c r="E107" s="10"/>
     </row>
     <row r="108" ht="14.6" customHeight="1">
-      <c r="A108" s="9"/>
-      <c r="B108" s="9"/>
-      <c r="C108" s="10"/>
-      <c r="D108" s="10"/>
-      <c r="E108" s="10"/>
+      <c r="A108" s="7"/>
+      <c r="B108" s="7"/>
+      <c r="C108" s="8"/>
+      <c r="D108" s="8"/>
+      <c r="E108" s="8"/>
     </row>
     <row r="109" ht="14.6" customHeight="1">
-      <c r="A109" s="7"/>
-      <c r="B109" s="7"/>
-      <c r="C109" s="8"/>
-      <c r="D109" s="8"/>
-      <c r="E109" s="8"/>
+      <c r="A109" s="9"/>
+      <c r="B109" s="9"/>
+      <c r="C109" s="10"/>
+      <c r="D109" s="10"/>
+      <c r="E109" s="10"/>
     </row>
     <row r="110" ht="14.6" customHeight="1">
-      <c r="A110" s="9"/>
-      <c r="B110" s="9"/>
-      <c r="C110" s="10"/>
-      <c r="D110" s="10"/>
-      <c r="E110" s="10"/>
+      <c r="A110" s="7"/>
+      <c r="B110" s="7"/>
+      <c r="C110" s="8"/>
+      <c r="D110" s="8"/>
+      <c r="E110" s="8"/>
     </row>
     <row r="111" ht="14.6" customHeight="1">
-      <c r="A111" s="7"/>
-      <c r="B111" s="7"/>
-      <c r="C111" s="8"/>
-      <c r="D111" s="8"/>
-      <c r="E111" s="8"/>
+      <c r="A111" s="10"/>
+      <c r="B111" s="10"/>
+      <c r="C111" s="10"/>
+      <c r="D111" s="10"/>
+      <c r="E111" s="10"/>
     </row>
     <row r="112" ht="14.6" customHeight="1">
-      <c r="A112" s="10"/>
-      <c r="B112" s="10"/>
-      <c r="C112" s="10"/>
-      <c r="D112" s="10"/>
-      <c r="E112" s="10"/>
+      <c r="A112" s="7"/>
+      <c r="B112" s="7"/>
+      <c r="C112" s="8"/>
+      <c r="D112" s="8"/>
+      <c r="E112" s="8"/>
     </row>
     <row r="113" ht="14.6" customHeight="1">
-      <c r="A113" s="7"/>
-      <c r="B113" s="7"/>
-      <c r="C113" s="8"/>
-      <c r="D113" s="8"/>
-      <c r="E113" s="8"/>
+      <c r="A113" s="9"/>
+      <c r="B113" s="9"/>
+      <c r="C113" s="10"/>
+      <c r="D113" s="10"/>
+      <c r="E113" s="10"/>
     </row>
     <row r="114" ht="14.6" customHeight="1">
-      <c r="A114" s="9"/>
-      <c r="B114" s="9"/>
-      <c r="C114" s="10"/>
-      <c r="D114" s="10"/>
-      <c r="E114" s="10"/>
+      <c r="A114" s="7"/>
+      <c r="B114" s="7"/>
+      <c r="C114" s="8"/>
+      <c r="D114" s="8"/>
+      <c r="E114" s="8"/>
     </row>
     <row r="115" ht="14.6" customHeight="1">
-      <c r="A115" s="7"/>
-      <c r="B115" s="7"/>
-      <c r="C115" s="8"/>
-      <c r="D115" s="8"/>
-      <c r="E115" s="8"/>
+      <c r="A115" s="10"/>
+      <c r="B115" s="10"/>
+      <c r="C115" s="10"/>
+      <c r="D115" s="10"/>
+      <c r="E115" s="10"/>
     </row>
     <row r="116" ht="14.6" customHeight="1">
-      <c r="A116" s="10"/>
-      <c r="B116" s="10"/>
-      <c r="C116" s="10"/>
-      <c r="D116" s="10"/>
-      <c r="E116" s="10"/>
+      <c r="A116" s="7"/>
+      <c r="B116" s="7"/>
+      <c r="C116" s="8"/>
+      <c r="D116" s="8"/>
+      <c r="E116" s="8"/>
     </row>
     <row r="117" ht="14.6" customHeight="1">
-      <c r="A117" s="7"/>
-      <c r="B117" s="7"/>
-      <c r="C117" s="8"/>
-      <c r="D117" s="8"/>
-      <c r="E117" s="8"/>
+      <c r="A117" s="9"/>
+      <c r="B117" s="9"/>
+      <c r="C117" s="10"/>
+      <c r="D117" s="10"/>
+      <c r="E117" s="10"/>
     </row>
     <row r="118" ht="14.6" customHeight="1">
-      <c r="A118" s="9"/>
-      <c r="B118" s="9"/>
-      <c r="C118" s="10"/>
-      <c r="D118" s="10"/>
-      <c r="E118" s="10"/>
+      <c r="A118" s="7"/>
+      <c r="B118" s="7"/>
+      <c r="C118" s="8"/>
+      <c r="D118" s="8"/>
+      <c r="E118" s="8"/>
     </row>
     <row r="119" ht="14.6" customHeight="1">
-      <c r="A119" s="7"/>
-      <c r="B119" s="7"/>
-      <c r="C119" s="8"/>
-      <c r="D119" s="8"/>
-      <c r="E119" s="8"/>
+      <c r="A119" s="9"/>
+      <c r="B119" s="9"/>
+      <c r="C119" s="10"/>
+      <c r="D119" s="10"/>
+      <c r="E119" s="10"/>
     </row>
     <row r="120" ht="14.6" customHeight="1">
-      <c r="A120" s="9"/>
-      <c r="B120" s="9"/>
-      <c r="C120" s="10"/>
-      <c r="D120" s="10"/>
-      <c r="E120" s="10"/>
+      <c r="A120" s="8"/>
+      <c r="B120" s="8"/>
+      <c r="C120" s="8"/>
+      <c r="D120" s="8"/>
+      <c r="E120" s="8"/>
     </row>
     <row r="121" ht="14.6" customHeight="1">
-      <c r="A121" s="8"/>
-      <c r="B121" s="8"/>
-      <c r="C121" s="8"/>
-      <c r="D121" s="8"/>
-      <c r="E121" s="8"/>
+      <c r="A121" s="9"/>
+      <c r="B121" s="9"/>
+      <c r="C121" s="10"/>
+      <c r="D121" s="10"/>
+      <c r="E121" s="10"/>
     </row>
     <row r="122" ht="14.6" customHeight="1">
-      <c r="A122" s="9"/>
-      <c r="B122" s="9"/>
-      <c r="C122" s="10"/>
-      <c r="D122" s="10"/>
-      <c r="E122" s="10"/>
+      <c r="A122" s="7"/>
+      <c r="B122" s="7"/>
+      <c r="C122" s="8"/>
+      <c r="D122" s="8"/>
+      <c r="E122" s="8"/>
     </row>
     <row r="123" ht="14.6" customHeight="1">
-      <c r="A123" s="7"/>
-      <c r="B123" s="7"/>
-      <c r="C123" s="8"/>
-      <c r="D123" s="8"/>
-      <c r="E123" s="8"/>
+      <c r="A123" s="10"/>
+      <c r="B123" s="10"/>
+      <c r="C123" s="10"/>
+      <c r="D123" s="10"/>
+      <c r="E123" s="10"/>
     </row>
     <row r="124" ht="14.6" customHeight="1">
-      <c r="A124" s="10"/>
-      <c r="B124" s="10"/>
-      <c r="C124" s="10"/>
-      <c r="D124" s="10"/>
-      <c r="E124" s="10"/>
+      <c r="A124" s="7"/>
+      <c r="B124" s="7"/>
+      <c r="C124" s="8"/>
+      <c r="D124" s="8"/>
+      <c r="E124" s="8"/>
     </row>
     <row r="125" ht="14.6" customHeight="1">
-      <c r="A125" s="7"/>
-      <c r="B125" s="7"/>
-      <c r="C125" s="8"/>
-      <c r="D125" s="8"/>
-      <c r="E125" s="8"/>
+      <c r="A125" s="9"/>
+      <c r="B125" s="9"/>
+      <c r="C125" s="10"/>
+      <c r="D125" s="10"/>
+      <c r="E125" s="10"/>
     </row>
     <row r="126" ht="14.6" customHeight="1">
-      <c r="A126" s="9"/>
-      <c r="B126" s="9"/>
-      <c r="C126" s="10"/>
-      <c r="D126" s="10"/>
-      <c r="E126" s="10"/>
+      <c r="A126" s="7"/>
+      <c r="B126" s="7"/>
+      <c r="C126" s="8"/>
+      <c r="D126" s="8"/>
+      <c r="E126" s="8"/>
     </row>
     <row r="127" ht="14.6" customHeight="1">
-      <c r="A127" s="7"/>
-      <c r="B127" s="7"/>
-      <c r="C127" s="8"/>
-      <c r="D127" s="8"/>
-      <c r="E127" s="8"/>
+      <c r="A127" s="10"/>
+      <c r="B127" s="10"/>
+      <c r="C127" s="10"/>
+      <c r="D127" s="10"/>
+      <c r="E127" s="10"/>
     </row>
     <row r="128" ht="14.6" customHeight="1">
-      <c r="A128" s="10"/>
-      <c r="B128" s="10"/>
-      <c r="C128" s="10"/>
-      <c r="D128" s="10"/>
-      <c r="E128" s="10"/>
+      <c r="A128" s="7"/>
+      <c r="B128" s="7"/>
+      <c r="C128" s="8"/>
+      <c r="D128" s="8"/>
+      <c r="E128" s="8"/>
     </row>
     <row r="129" ht="14.6" customHeight="1">
-      <c r="A129" s="7"/>
-      <c r="B129" s="7"/>
-      <c r="C129" s="8"/>
-      <c r="D129" s="8"/>
-      <c r="E129" s="8"/>
+      <c r="A129" s="9"/>
+      <c r="B129" s="9"/>
+      <c r="C129" s="10"/>
+      <c r="D129" s="10"/>
+      <c r="E129" s="10"/>
     </row>
     <row r="130" ht="14.6" customHeight="1">
-      <c r="A130" s="9"/>
-      <c r="B130" s="9"/>
-      <c r="C130" s="10"/>
-      <c r="D130" s="10"/>
-      <c r="E130" s="10"/>
+      <c r="A130" s="8"/>
+      <c r="B130" s="8"/>
+      <c r="C130" s="8"/>
+      <c r="D130" s="8"/>
+      <c r="E130" s="8"/>
     </row>
     <row r="131" ht="14.6" customHeight="1">
-      <c r="A131" s="8"/>
-      <c r="B131" s="8"/>
-      <c r="C131" s="8"/>
-      <c r="D131" s="8"/>
-      <c r="E131" s="8"/>
+      <c r="A131" s="9"/>
+      <c r="B131" s="9"/>
+      <c r="C131" s="10"/>
+      <c r="D131" s="10"/>
+      <c r="E131" s="10"/>
     </row>
     <row r="132" ht="14.6" customHeight="1">
-      <c r="A132" s="9"/>
-      <c r="B132" s="9"/>
-      <c r="C132" s="10"/>
-      <c r="D132" s="10"/>
-      <c r="E132" s="10"/>
+      <c r="A132" s="8"/>
+      <c r="B132" s="8"/>
+      <c r="C132" s="8"/>
+      <c r="D132" s="8"/>
+      <c r="E132" s="8"/>
     </row>
     <row r="133" ht="14.6" customHeight="1">
-      <c r="A133" s="8"/>
-      <c r="B133" s="8"/>
-      <c r="C133" s="8"/>
-      <c r="D133" s="8"/>
-      <c r="E133" s="8"/>
+      <c r="A133" s="9"/>
+      <c r="B133" s="9"/>
+      <c r="C133" s="10"/>
+      <c r="D133" s="10"/>
+      <c r="E133" s="10"/>
     </row>
     <row r="134" ht="14.6" customHeight="1">
-      <c r="A134" s="9"/>
-      <c r="B134" s="9"/>
-      <c r="C134" s="10"/>
-      <c r="D134" s="10"/>
-      <c r="E134" s="10"/>
+      <c r="A134" s="7"/>
+      <c r="B134" s="7"/>
+      <c r="C134" s="8"/>
+      <c r="D134" s="8"/>
+      <c r="E134" s="8"/>
     </row>
     <row r="135" ht="14.6" customHeight="1">
-      <c r="A135" s="7"/>
-      <c r="B135" s="7"/>
-      <c r="C135" s="8"/>
-      <c r="D135" s="8"/>
-      <c r="E135" s="8"/>
+      <c r="A135" s="10"/>
+      <c r="B135" s="10"/>
+      <c r="C135" s="10"/>
+      <c r="D135" s="10"/>
+      <c r="E135" s="10"/>
     </row>
     <row r="136" ht="14.6" customHeight="1">
-      <c r="A136" s="10"/>
-      <c r="B136" s="10"/>
-      <c r="C136" s="10"/>
-      <c r="D136" s="10"/>
-      <c r="E136" s="10"/>
+      <c r="A136" s="7"/>
+      <c r="B136" s="7"/>
+      <c r="C136" s="8"/>
+      <c r="D136" s="8"/>
+      <c r="E136" s="8"/>
     </row>
     <row r="137" ht="14.6" customHeight="1">
-      <c r="A137" s="7"/>
-      <c r="B137" s="7"/>
-      <c r="C137" s="8"/>
-      <c r="D137" s="8"/>
-      <c r="E137" s="8"/>
+      <c r="A137" s="9"/>
+      <c r="B137" s="9"/>
+      <c r="C137" s="10"/>
+      <c r="D137" s="10"/>
+      <c r="E137" s="10"/>
     </row>
     <row r="138" ht="14.6" customHeight="1">
-      <c r="A138" s="9"/>
-      <c r="B138" s="9"/>
-      <c r="C138" s="10"/>
-      <c r="D138" s="10"/>
-      <c r="E138" s="10"/>
+      <c r="A138" s="8"/>
+      <c r="B138" s="8"/>
+      <c r="C138" s="8"/>
+      <c r="D138" s="8"/>
+      <c r="E138" s="8"/>
     </row>
     <row r="139" ht="14.6" customHeight="1">
-      <c r="A139" s="8"/>
-      <c r="B139" s="8"/>
-      <c r="C139" s="8"/>
-      <c r="D139" s="8"/>
-      <c r="E139" s="8"/>
+      <c r="A139" s="10"/>
+      <c r="B139" s="10"/>
+      <c r="C139" s="10"/>
+      <c r="D139" s="10"/>
+      <c r="E139" s="10"/>
     </row>
     <row r="140" ht="14.6" customHeight="1">
-      <c r="A140" s="10"/>
-      <c r="B140" s="10"/>
-      <c r="C140" s="10"/>
-      <c r="D140" s="10"/>
-      <c r="E140" s="10"/>
+      <c r="A140" s="7"/>
+      <c r="B140" s="8"/>
+      <c r="C140" s="8"/>
+      <c r="D140" s="8"/>
+      <c r="E140" s="8"/>
     </row>
     <row r="141" ht="14.6" customHeight="1">
-      <c r="A141" s="7"/>
-      <c r="B141" s="8"/>
-      <c r="C141" s="8"/>
-      <c r="D141" s="8"/>
-      <c r="E141" s="8"/>
+      <c r="A141" s="9"/>
+      <c r="B141" s="10"/>
+      <c r="C141" s="10"/>
+      <c r="D141" s="10"/>
+      <c r="E141" s="10"/>
     </row>
     <row r="142" ht="14.6" customHeight="1">
-      <c r="A142" s="9"/>
-      <c r="B142" s="10"/>
-      <c r="C142" s="10"/>
-      <c r="D142" s="10"/>
-      <c r="E142" s="10"/>
+      <c r="A142" s="7"/>
+      <c r="B142" s="7"/>
+      <c r="C142" s="8"/>
+      <c r="D142" s="8"/>
+      <c r="E142" s="8"/>
     </row>
     <row r="143" ht="14.6" customHeight="1">
-      <c r="A143" s="7"/>
-      <c r="B143" s="7"/>
-      <c r="C143" s="8"/>
-      <c r="D143" s="8"/>
-      <c r="E143" s="8"/>
+      <c r="A143" s="10"/>
+      <c r="B143" s="10"/>
+      <c r="C143" s="10"/>
+      <c r="D143" s="10"/>
+      <c r="E143" s="10"/>
     </row>
     <row r="144" ht="14.6" customHeight="1">
-      <c r="A144" s="10"/>
-      <c r="B144" s="10"/>
-      <c r="C144" s="10"/>
-      <c r="D144" s="10"/>
-      <c r="E144" s="10"/>
+      <c r="A144" s="7"/>
+      <c r="B144" s="7"/>
+      <c r="C144" s="8"/>
+      <c r="D144" s="8"/>
+      <c r="E144" s="8"/>
     </row>
     <row r="145" ht="14.6" customHeight="1">
-      <c r="A145" s="7"/>
-      <c r="B145" s="7"/>
-      <c r="C145" s="8"/>
-      <c r="D145" s="8"/>
-      <c r="E145" s="8"/>
+      <c r="A145" s="10"/>
+      <c r="B145" s="10"/>
+      <c r="C145" s="10"/>
+      <c r="D145" s="10"/>
+      <c r="E145" s="10"/>
     </row>
     <row r="146" ht="14.6" customHeight="1">
-      <c r="A146" s="10"/>
-      <c r="B146" s="10"/>
-      <c r="C146" s="10"/>
-      <c r="D146" s="10"/>
-      <c r="E146" s="10"/>
+      <c r="A146" s="8"/>
+      <c r="B146" s="8"/>
+      <c r="C146" s="8"/>
+      <c r="D146" s="8"/>
+      <c r="E146" s="8"/>
     </row>
     <row r="147" ht="14.6" customHeight="1">
-      <c r="A147" s="8"/>
-      <c r="B147" s="8"/>
-      <c r="C147" s="8"/>
-      <c r="D147" s="8"/>
-      <c r="E147" s="8"/>
+      <c r="A147" s="10"/>
+      <c r="B147" s="10"/>
+      <c r="C147" s="10"/>
+      <c r="D147" s="10"/>
+      <c r="E147" s="10"/>
     </row>
     <row r="148" ht="14.6" customHeight="1">
-      <c r="A148" s="10"/>
-      <c r="B148" s="10"/>
-      <c r="C148" s="10"/>
-      <c r="D148" s="10"/>
-      <c r="E148" s="10"/>
+      <c r="A148" s="8"/>
+      <c r="B148" s="8"/>
+      <c r="C148" s="8"/>
+      <c r="D148" s="8"/>
+      <c r="E148" s="8"/>
     </row>
     <row r="149" ht="14.6" customHeight="1">
-      <c r="A149" s="8"/>
-      <c r="B149" s="8"/>
-      <c r="C149" s="8"/>
-      <c r="D149" s="8"/>
-      <c r="E149" s="8"/>
+      <c r="A149" s="9"/>
+      <c r="B149" s="9"/>
+      <c r="C149" s="10"/>
+      <c r="D149" s="10"/>
+      <c r="E149" s="10"/>
     </row>
     <row r="150" ht="14.6" customHeight="1">
-      <c r="A150" s="9"/>
-      <c r="B150" s="9"/>
-      <c r="C150" s="10"/>
-      <c r="D150" s="10"/>
-      <c r="E150" s="10"/>
+      <c r="A150" s="7"/>
+      <c r="B150" s="7"/>
+      <c r="C150" s="8"/>
+      <c r="D150" s="8"/>
+      <c r="E150" s="8"/>
     </row>
     <row r="151" ht="14.6" customHeight="1">
-      <c r="A151" s="7"/>
-      <c r="B151" s="7"/>
-      <c r="C151" s="8"/>
-      <c r="D151" s="8"/>
-      <c r="E151" s="8"/>
+      <c r="A151" s="9"/>
+      <c r="B151" s="9"/>
+      <c r="C151" s="10"/>
+      <c r="D151" s="10"/>
+      <c r="E151" s="10"/>
     </row>
     <row r="152" ht="14.6" customHeight="1">
-      <c r="A152" s="9"/>
-      <c r="B152" s="9"/>
-      <c r="C152" s="10"/>
-      <c r="D152" s="10"/>
-      <c r="E152" s="10"/>
+      <c r="A152" s="7"/>
+      <c r="B152" s="7"/>
+      <c r="C152" s="8"/>
+      <c r="D152" s="8"/>
+      <c r="E152" s="8"/>
     </row>
     <row r="153" ht="14.6" customHeight="1">
-      <c r="A153" s="7"/>
-      <c r="B153" s="7"/>
-      <c r="C153" s="8"/>
-      <c r="D153" s="8"/>
-      <c r="E153" s="8"/>
+      <c r="A153" s="9"/>
+      <c r="B153" s="9"/>
+      <c r="C153" s="10"/>
+      <c r="D153" s="10"/>
+      <c r="E153" s="10"/>
     </row>
     <row r="154" ht="14.6" customHeight="1">
-      <c r="A154" s="9"/>
-      <c r="B154" s="9"/>
-      <c r="C154" s="10"/>
-      <c r="D154" s="10"/>
-      <c r="E154" s="10"/>
+      <c r="A154" s="7"/>
+      <c r="B154" s="7"/>
+      <c r="C154" s="8"/>
+      <c r="D154" s="8"/>
+      <c r="E154" s="8"/>
     </row>
     <row r="155" ht="14.6" customHeight="1">
-      <c r="A155" s="7"/>
-      <c r="B155" s="7"/>
-      <c r="C155" s="8"/>
-      <c r="D155" s="8"/>
-      <c r="E155" s="8"/>
+      <c r="A155" s="9"/>
+      <c r="B155" s="9"/>
+      <c r="C155" s="10"/>
+      <c r="D155" s="10"/>
+      <c r="E155" s="10"/>
     </row>
     <row r="156" ht="14.6" customHeight="1">
-      <c r="A156" s="9"/>
-      <c r="B156" s="9"/>
-      <c r="C156" s="10"/>
-      <c r="D156" s="10"/>
-      <c r="E156" s="10"/>
+      <c r="A156" s="7"/>
+      <c r="B156" s="7"/>
+      <c r="C156" s="8"/>
+      <c r="D156" s="8"/>
+      <c r="E156" s="8"/>
     </row>
     <row r="157" ht="14.6" customHeight="1">
-      <c r="A157" s="7"/>
-      <c r="B157" s="7"/>
-      <c r="C157" s="8"/>
-      <c r="D157" s="8"/>
-      <c r="E157" s="8"/>
+      <c r="A157" s="10"/>
+      <c r="B157" s="10"/>
+      <c r="C157" s="10"/>
+      <c r="D157" s="10"/>
+      <c r="E157" s="10"/>
     </row>
     <row r="158" ht="14.6" customHeight="1">
-      <c r="A158" s="10"/>
-      <c r="B158" s="10"/>
-      <c r="C158" s="10"/>
-      <c r="D158" s="10"/>
-      <c r="E158" s="10"/>
+      <c r="A158" s="7"/>
+      <c r="B158" s="7"/>
+      <c r="C158" s="8"/>
+      <c r="D158" s="8"/>
+      <c r="E158" s="8"/>
     </row>
     <row r="159" ht="14.6" customHeight="1">
-      <c r="A159" s="7"/>
-      <c r="B159" s="7"/>
-      <c r="C159" s="8"/>
-      <c r="D159" s="8"/>
-      <c r="E159" s="8"/>
+      <c r="A159" s="9"/>
+      <c r="B159" s="9"/>
+      <c r="C159" s="10"/>
+      <c r="D159" s="10"/>
+      <c r="E159" s="10"/>
     </row>
     <row r="160" ht="14.6" customHeight="1">
-      <c r="A160" s="9"/>
-      <c r="B160" s="9"/>
-      <c r="C160" s="10"/>
-      <c r="D160" s="10"/>
-      <c r="E160" s="10"/>
+      <c r="A160" s="7"/>
+      <c r="B160" s="7"/>
+      <c r="C160" s="8"/>
+      <c r="D160" s="8"/>
+      <c r="E160" s="8"/>
     </row>
     <row r="161" ht="14.6" customHeight="1">
-      <c r="A161" s="7"/>
-      <c r="B161" s="7"/>
-      <c r="C161" s="8"/>
-      <c r="D161" s="8"/>
-      <c r="E161" s="8"/>
+      <c r="A161" s="9"/>
+      <c r="B161" s="9"/>
+      <c r="C161" s="10"/>
+      <c r="D161" s="10"/>
+      <c r="E161" s="10"/>
     </row>
     <row r="162" ht="14.6" customHeight="1">
-      <c r="A162" s="9"/>
-      <c r="B162" s="9"/>
-      <c r="C162" s="10"/>
-      <c r="D162" s="10"/>
-      <c r="E162" s="10"/>
+      <c r="A162" s="8"/>
+      <c r="B162" s="8"/>
+      <c r="C162" s="8"/>
+      <c r="D162" s="8"/>
+      <c r="E162" s="8"/>
     </row>
     <row r="163" ht="14.6" customHeight="1">
-      <c r="A163" s="8"/>
-      <c r="B163" s="8"/>
-      <c r="C163" s="8"/>
-      <c r="D163" s="8"/>
-      <c r="E163" s="8"/>
+      <c r="A163" s="9"/>
+      <c r="B163" s="9"/>
+      <c r="C163" s="10"/>
+      <c r="D163" s="10"/>
+      <c r="E163" s="10"/>
     </row>
     <row r="164" ht="14.6" customHeight="1">
-      <c r="A164" s="9"/>
-      <c r="B164" s="9"/>
-      <c r="C164" s="10"/>
-      <c r="D164" s="10"/>
-      <c r="E164" s="10"/>
+      <c r="A164" s="7"/>
+      <c r="B164" s="7"/>
+      <c r="C164" s="8"/>
+      <c r="D164" s="8"/>
+      <c r="E164" s="8"/>
     </row>
     <row r="165" ht="14.6" customHeight="1">
-      <c r="A165" s="7"/>
-      <c r="B165" s="7"/>
-      <c r="C165" s="8"/>
-      <c r="D165" s="8"/>
-      <c r="E165" s="8"/>
+      <c r="A165" s="9"/>
+      <c r="B165" s="9"/>
+      <c r="C165" s="10"/>
+      <c r="D165" s="10"/>
+      <c r="E165" s="10"/>
     </row>
     <row r="166" ht="14.6" customHeight="1">
-      <c r="A166" s="9"/>
-      <c r="B166" s="9"/>
-      <c r="C166" s="10"/>
-      <c r="D166" s="10"/>
-      <c r="E166" s="10"/>
+      <c r="A166" s="7"/>
+      <c r="B166" s="7"/>
+      <c r="C166" s="8"/>
+      <c r="D166" s="8"/>
+      <c r="E166" s="8"/>
     </row>
     <row r="167" ht="14.6" customHeight="1">
-      <c r="A167" s="7"/>
-      <c r="B167" s="7"/>
-      <c r="C167" s="8"/>
-      <c r="D167" s="8"/>
-      <c r="E167" s="8"/>
+      <c r="A167" s="9"/>
+      <c r="B167" s="9"/>
+      <c r="C167" s="10"/>
+      <c r="D167" s="10"/>
+      <c r="E167" s="10"/>
     </row>
     <row r="168" ht="14.6" customHeight="1">
-      <c r="A168" s="9"/>
-      <c r="B168" s="9"/>
-      <c r="C168" s="10"/>
-      <c r="D168" s="10"/>
-      <c r="E168" s="10"/>
+      <c r="A168" s="7"/>
+      <c r="B168" s="7"/>
+      <c r="C168" s="8"/>
+      <c r="D168" s="8"/>
+      <c r="E168" s="8"/>
     </row>
     <row r="169" ht="14.6" customHeight="1">
-      <c r="A169" s="7"/>
-      <c r="B169" s="7"/>
-      <c r="C169" s="8"/>
-      <c r="D169" s="8"/>
-      <c r="E169" s="8"/>
+      <c r="A169" s="9"/>
+      <c r="B169" s="9"/>
+      <c r="C169" s="10"/>
+      <c r="D169" s="10"/>
+      <c r="E169" s="10"/>
     </row>
     <row r="170" ht="14.6" customHeight="1">
-      <c r="A170" s="9"/>
-      <c r="B170" s="9"/>
-      <c r="C170" s="10"/>
-      <c r="D170" s="10"/>
-      <c r="E170" s="10"/>
+      <c r="A170" s="8"/>
+      <c r="B170" s="8"/>
+      <c r="C170" s="8"/>
+      <c r="D170" s="8"/>
+      <c r="E170" s="8"/>
     </row>
     <row r="171" ht="14.6" customHeight="1">
-      <c r="A171" s="8"/>
-      <c r="B171" s="8"/>
-      <c r="C171" s="8"/>
-      <c r="D171" s="8"/>
-      <c r="E171" s="8"/>
+      <c r="A171" s="9"/>
+      <c r="B171" s="9"/>
+      <c r="C171" s="10"/>
+      <c r="D171" s="10"/>
+      <c r="E171" s="10"/>
     </row>
     <row r="172" ht="14.6" customHeight="1">
-      <c r="A172" s="9"/>
-      <c r="B172" s="9"/>
-      <c r="C172" s="10"/>
-      <c r="D172" s="10"/>
-      <c r="E172" s="10"/>
+      <c r="A172" s="7"/>
+      <c r="B172" s="7"/>
+      <c r="C172" s="8"/>
+      <c r="D172" s="8"/>
+      <c r="E172" s="8"/>
     </row>
     <row r="173" ht="14.6" customHeight="1">
-      <c r="A173" s="7"/>
-      <c r="B173" s="7"/>
-      <c r="C173" s="8"/>
-      <c r="D173" s="8"/>
-      <c r="E173" s="8"/>
+      <c r="A173" s="9"/>
+      <c r="B173" s="9"/>
+      <c r="C173" s="10"/>
+      <c r="D173" s="10"/>
+      <c r="E173" s="10"/>
     </row>
     <row r="174" ht="14.6" customHeight="1">
-      <c r="A174" s="9"/>
-      <c r="B174" s="9"/>
-      <c r="C174" s="10"/>
-      <c r="D174" s="10"/>
-      <c r="E174" s="10"/>
+      <c r="A174" s="8"/>
+      <c r="B174" s="8"/>
+      <c r="C174" s="8"/>
+      <c r="D174" s="8"/>
+      <c r="E174" s="8"/>
     </row>
     <row r="175" ht="14.6" customHeight="1">
-      <c r="A175" s="8"/>
-      <c r="B175" s="8"/>
-      <c r="C175" s="8"/>
-      <c r="D175" s="8"/>
-      <c r="E175" s="8"/>
+      <c r="A175" s="9"/>
+      <c r="B175" s="9"/>
+      <c r="C175" s="10"/>
+      <c r="D175" s="10"/>
+      <c r="E175" s="10"/>
     </row>
     <row r="176" ht="14.6" customHeight="1">
-      <c r="A176" s="9"/>
-      <c r="B176" s="9"/>
-      <c r="C176" s="10"/>
-      <c r="D176" s="10"/>
-      <c r="E176" s="10"/>
+      <c r="A176" s="7"/>
+      <c r="B176" s="7"/>
+      <c r="C176" s="8"/>
+      <c r="D176" s="8"/>
+      <c r="E176" s="8"/>
     </row>
     <row r="177" ht="14.6" customHeight="1">
-      <c r="A177" s="7"/>
-      <c r="B177" s="7"/>
-      <c r="C177" s="8"/>
-      <c r="D177" s="8"/>
-      <c r="E177" s="8"/>
+      <c r="A177" s="10"/>
+      <c r="B177" s="10"/>
+      <c r="C177" s="10"/>
+      <c r="D177" s="10"/>
+      <c r="E177" s="10"/>
     </row>
     <row r="178" ht="14.6" customHeight="1">
-      <c r="A178" s="10"/>
-      <c r="B178" s="10"/>
-      <c r="C178" s="10"/>
-      <c r="D178" s="10"/>
-      <c r="E178" s="10"/>
+      <c r="A178" s="7"/>
+      <c r="B178" s="7"/>
+      <c r="C178" s="8"/>
+      <c r="D178" s="8"/>
+      <c r="E178" s="8"/>
     </row>
     <row r="179" ht="14.6" customHeight="1">
-      <c r="A179" s="7"/>
-      <c r="B179" s="7"/>
-      <c r="C179" s="8"/>
-      <c r="D179" s="8"/>
-      <c r="E179" s="8"/>
+      <c r="A179" s="9"/>
+      <c r="B179" s="9"/>
+      <c r="C179" s="10"/>
+      <c r="D179" s="10"/>
+      <c r="E179" s="10"/>
     </row>
     <row r="180" ht="14.6" customHeight="1">
-      <c r="A180" s="9"/>
-      <c r="B180" s="9"/>
-      <c r="C180" s="10"/>
-      <c r="D180" s="10"/>
-      <c r="E180" s="10"/>
+      <c r="A180" s="8"/>
+      <c r="B180" s="8"/>
+      <c r="C180" s="8"/>
+      <c r="D180" s="8"/>
+      <c r="E180" s="8"/>
     </row>
     <row r="181" ht="14.6" customHeight="1">
-      <c r="A181" s="8"/>
-      <c r="B181" s="8"/>
-      <c r="C181" s="8"/>
-      <c r="D181" s="8"/>
-      <c r="E181" s="8"/>
+      <c r="A181" s="9"/>
+      <c r="B181" s="9"/>
+      <c r="C181" s="10"/>
+      <c r="D181" s="10"/>
+      <c r="E181" s="10"/>
     </row>
     <row r="182" ht="14.6" customHeight="1">
-      <c r="A182" s="9"/>
-      <c r="B182" s="9"/>
-      <c r="C182" s="10"/>
-      <c r="D182" s="10"/>
-      <c r="E182" s="10"/>
+      <c r="A182" s="7"/>
+      <c r="B182" s="7"/>
+      <c r="C182" s="8"/>
+      <c r="D182" s="8"/>
+      <c r="E182" s="8"/>
     </row>
     <row r="183" ht="14.6" customHeight="1">
-      <c r="A183" s="7"/>
-      <c r="B183" s="7"/>
-      <c r="C183" s="8"/>
-      <c r="D183" s="8"/>
-      <c r="E183" s="8"/>
+      <c r="A183" s="10"/>
+      <c r="B183" s="10"/>
+      <c r="C183" s="10"/>
+      <c r="D183" s="10"/>
+      <c r="E183" s="10"/>
     </row>
     <row r="184" ht="14.6" customHeight="1">
-      <c r="A184" s="10"/>
-      <c r="B184" s="10"/>
-      <c r="C184" s="10"/>
-      <c r="D184" s="10"/>
-      <c r="E184" s="10"/>
+      <c r="A184" s="7"/>
+      <c r="B184" s="7"/>
+      <c r="C184" s="8"/>
+      <c r="D184" s="8"/>
+      <c r="E184" s="8"/>
     </row>
     <row r="185" ht="14.6" customHeight="1">
-      <c r="A185" s="7"/>
-      <c r="B185" s="7"/>
-      <c r="C185" s="8"/>
-      <c r="D185" s="8"/>
-      <c r="E185" s="8"/>
-    </row>
-    <row r="186" ht="14.6" customHeight="1">
-      <c r="A186" s="9"/>
-      <c r="B186" s="9"/>
-      <c r="C186" s="10"/>
-      <c r="D186" s="10"/>
-      <c r="E186" s="10"/>
+      <c r="A185" s="9"/>
+      <c r="B185" s="9"/>
+      <c r="C185" s="10"/>
+      <c r="D185" s="10"/>
+      <c r="E185" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
Form 8 Annual Dev
</commit_message>
<xml_diff>
--- a/DataExtraction/Input/Config.xlsx
+++ b/DataExtraction/Input/Config.xlsx
@@ -12,13 +12,14 @@
     <sheet name="AOC NBFC CFS" sheetId="5" r:id="rId8"/>
     <sheet name="DIR" sheetId="6" r:id="rId9"/>
     <sheet name="Form_8_Interim" sheetId="7" r:id="rId10"/>
-    <sheet name="Sheet 1" sheetId="8" r:id="rId11"/>
+    <sheet name="Form_8_annual" sheetId="8" r:id="rId11"/>
+    <sheet name="Sheet 1" sheetId="9" r:id="rId12"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="196">
   <si>
     <t>Key</t>
   </si>
@@ -483,6 +484,126 @@
   </si>
   <si>
     <t>column_json_node_index</t>
+  </si>
+  <si>
+    <t>/Users/gundukalyan/Documents/GitHub/mns-json-prep/DataExtraction/Input/LLP/Form_8_annual/LLP Form8-11012022_signed_1 (1).pdf</t>
+  </si>
+  <si>
+    <t>/Users/gundukalyan/Documents/GitHub/mns-json-prep/DataExtraction/Input/LLP/Form_8_annual/FORM-8(ANNUAL)_nodes_config.xlsx</t>
+  </si>
+  <si>
+    <t>/Users/gundukalyan/Documents/GitHub/mns-json-prep/DataExtraction/Output/LLP/Form_8_annual</t>
+  </si>
+  <si>
+    <t>Document_type</t>
+  </si>
+  <si>
+    <t>annual_keyword_in_xml</t>
+  </si>
+  <si>
+    <t>ANNU</t>
+  </si>
+  <si>
+    <t>year_index</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>year_column_name</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>stated_on</t>
+  </si>
+  <si>
+    <t>auditor_type_field_name</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>auditor_type_column_name</t>
+  </si>
+  <si>
+    <t>financials_auditor_column_name</t>
+  </si>
+  <si>
+    <t>financials_auditor</t>
+  </si>
+  <si>
+    <t>auditor_type_value_to_check</t>
+  </si>
+  <si>
+    <t>AUDR</t>
+  </si>
+  <si>
+    <t>auditor_name_field_name</t>
+  </si>
+  <si>
+    <t>auditor_name</t>
+  </si>
+  <si>
+    <t>auditor_name_column_name</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>membership_number_field_name</t>
+  </si>
+  <si>
+    <t>membership_number</t>
+  </si>
+  <si>
+    <t>membership_number_column_name</t>
+  </si>
+  <si>
+    <t>line_1_field_name</t>
+  </si>
+  <si>
+    <t>line_1</t>
+  </si>
+  <si>
+    <t>line_2_field_name</t>
+  </si>
+  <si>
+    <t>line_2</t>
+  </si>
+  <si>
+    <t>city_field_name</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>district_field_name</t>
+  </si>
+  <si>
+    <t>district</t>
+  </si>
+  <si>
+    <t>state_field_name</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>pincode_field_name</t>
+  </si>
+  <si>
+    <t>pincode</t>
+  </si>
+  <si>
+    <t>address_column_name</t>
+  </si>
+  <si>
+    <t>address</t>
   </si>
   <si>
     <t>Table 1</t>
@@ -571,7 +692,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -866,6 +987,102 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="19"/>
       </left>
       <right style="thin">
@@ -975,7 +1192,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1171,28 +1388,94 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="30" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="31" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="32" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="33" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="34" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="35" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="36" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -11277,6 +11560,1525 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:E191"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="14.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="48" style="64" customWidth="1"/>
+    <col min="2" max="2" width="61.8516" style="64" customWidth="1"/>
+    <col min="3" max="5" width="16.3516" style="64" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="64" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.6" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" ht="14.6" customHeight="1">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" ht="38.6" customHeight="1">
+      <c r="A3" t="s" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s" s="7">
+        <v>155</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" ht="26.6" customHeight="1">
+      <c r="A4" t="s" s="9">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s" s="9">
+        <v>156</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" ht="14.6" customHeight="1">
+      <c r="A5" t="s" s="7">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" ht="14.6" customHeight="1">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" ht="26.6" customHeight="1">
+      <c r="A7" t="s" s="9">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s" s="9">
+        <v>157</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" ht="14.6" customHeight="1">
+      <c r="A8" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" ht="14.6" customHeight="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" ht="14.6" customHeight="1">
+      <c r="A10" t="s" s="9">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s" s="9">
+        <v>12</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+    </row>
+    <row r="11" ht="14.6" customHeight="1">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+    </row>
+    <row r="12" ht="14.6" customHeight="1">
+      <c r="A12" t="s" s="7">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s" s="7">
+        <v>29</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" ht="15.35" customHeight="1">
+      <c r="A13" s="21"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" ht="15.35" customHeight="1">
+      <c r="A14" t="s" s="29">
+        <v>125</v>
+      </c>
+      <c r="B14" t="s" s="29">
+        <v>158</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" ht="15.35" customHeight="1">
+      <c r="A15" t="s" s="21">
+        <v>159</v>
+      </c>
+      <c r="B15" t="s" s="7">
+        <v>160</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" ht="15.35" customHeight="1">
+      <c r="A16" s="21"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" ht="15.35" customHeight="1">
+      <c r="A17" t="s" s="52">
+        <v>148</v>
+      </c>
+      <c r="B17" s="53">
+        <v>0</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" ht="15.35" customHeight="1">
+      <c r="A18" t="s" s="54">
+        <v>149</v>
+      </c>
+      <c r="B18" s="55">
+        <v>1</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" ht="15.35" customHeight="1">
+      <c r="A19" t="s" s="54">
+        <v>161</v>
+      </c>
+      <c r="B19" s="57">
+        <v>2</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" ht="15.35" customHeight="1">
+      <c r="A20" t="s" s="56">
+        <v>150</v>
+      </c>
+      <c r="B20" s="65">
+        <v>3</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" ht="15.35" customHeight="1">
+      <c r="A21" t="s" s="58">
+        <v>151</v>
+      </c>
+      <c r="B21" s="61">
+        <v>4</v>
+      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" ht="15.35" customHeight="1">
+      <c r="A22" t="s" s="60">
+        <v>152</v>
+      </c>
+      <c r="B22" s="59">
+        <v>5</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" ht="15.35" customHeight="1">
+      <c r="A23" t="s" s="58">
+        <v>153</v>
+      </c>
+      <c r="B23" s="63">
+        <v>6</v>
+      </c>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" ht="15.35" customHeight="1">
+      <c r="A24" t="s" s="62">
+        <v>154</v>
+      </c>
+      <c r="B24" t="s" s="22">
+        <v>162</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" ht="15.35" customHeight="1">
+      <c r="A25" s="21"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" ht="15.35" customHeight="1">
+      <c r="A26" t="s" s="9">
+        <v>69</v>
+      </c>
+      <c r="B26" t="s" s="29">
+        <v>70</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" ht="15.35" customHeight="1">
+      <c r="A27" t="s" s="7">
+        <v>71</v>
+      </c>
+      <c r="B27" t="s" s="29">
+        <v>72</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" ht="15.35" customHeight="1">
+      <c r="A28" t="s" s="7">
+        <v>75</v>
+      </c>
+      <c r="B28" t="s" s="29">
+        <v>76</v>
+      </c>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+    </row>
+    <row r="29" ht="15.35" customHeight="1">
+      <c r="A29" t="s" s="7">
+        <v>77</v>
+      </c>
+      <c r="B29" t="s" s="29">
+        <v>163</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" ht="15.35" customHeight="1">
+      <c r="A30" s="21"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+    </row>
+    <row r="31" ht="15.35" customHeight="1">
+      <c r="A31" t="s" s="21">
+        <v>164</v>
+      </c>
+      <c r="B31" t="s" s="22">
+        <v>165</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+    </row>
+    <row r="32" ht="15.35" customHeight="1">
+      <c r="A32" t="s" s="21">
+        <v>52</v>
+      </c>
+      <c r="B32" t="s" s="29">
+        <v>166</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+    </row>
+    <row r="33" ht="15.35" customHeight="1">
+      <c r="A33" t="s" s="29">
+        <v>167</v>
+      </c>
+      <c r="B33" t="s" s="29">
+        <v>168</v>
+      </c>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" ht="15.35" customHeight="1">
+      <c r="A34" t="s" s="29">
+        <v>169</v>
+      </c>
+      <c r="B34" t="s" s="29">
+        <v>168</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+    </row>
+    <row r="35" ht="15.35" customHeight="1">
+      <c r="A35" t="s" s="43">
+        <v>170</v>
+      </c>
+      <c r="B35" t="s" s="43">
+        <v>171</v>
+      </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+    </row>
+    <row r="36" ht="15.35" customHeight="1">
+      <c r="A36" t="s" s="29">
+        <v>172</v>
+      </c>
+      <c r="B36" t="s" s="29">
+        <v>173</v>
+      </c>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+    </row>
+    <row r="37" ht="15.35" customHeight="1">
+      <c r="A37" s="21"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+    </row>
+    <row r="38" ht="15.35" customHeight="1">
+      <c r="A38" t="s" s="66">
+        <v>174</v>
+      </c>
+      <c r="B38" t="s" s="67">
+        <v>175</v>
+      </c>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+    </row>
+    <row r="39" ht="14.6" customHeight="1">
+      <c r="A39" t="s" s="68">
+        <v>176</v>
+      </c>
+      <c r="B39" t="s" s="47">
+        <v>177</v>
+      </c>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+    </row>
+    <row r="40" ht="14.6" customHeight="1">
+      <c r="A40" t="s" s="69">
+        <v>178</v>
+      </c>
+      <c r="B40" t="s" s="67">
+        <v>179</v>
+      </c>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+    </row>
+    <row r="41" ht="14.6" customHeight="1">
+      <c r="A41" t="s" s="70">
+        <v>180</v>
+      </c>
+      <c r="B41" t="s" s="71">
+        <v>145</v>
+      </c>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+    </row>
+    <row r="42" ht="14.6" customHeight="1">
+      <c r="A42" t="s" s="72">
+        <v>181</v>
+      </c>
+      <c r="B42" t="s" s="73">
+        <v>182</v>
+      </c>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+    </row>
+    <row r="43" ht="14.6" customHeight="1">
+      <c r="A43" t="s" s="29">
+        <v>183</v>
+      </c>
+      <c r="B43" t="s" s="29">
+        <v>184</v>
+      </c>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+    </row>
+    <row r="44" ht="14.6" customHeight="1">
+      <c r="A44" t="s" s="29">
+        <v>185</v>
+      </c>
+      <c r="B44" t="s" s="29">
+        <v>186</v>
+      </c>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+    </row>
+    <row r="45" ht="14.6" customHeight="1">
+      <c r="A45" t="s" s="29">
+        <v>187</v>
+      </c>
+      <c r="B45" t="s" s="29">
+        <v>188</v>
+      </c>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+    </row>
+    <row r="46" ht="14.6" customHeight="1">
+      <c r="A46" t="s" s="69">
+        <v>189</v>
+      </c>
+      <c r="B46" t="s" s="67">
+        <v>190</v>
+      </c>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+    </row>
+    <row r="47" ht="14.6" customHeight="1">
+      <c r="A47" t="s" s="74">
+        <v>191</v>
+      </c>
+      <c r="B47" t="s" s="75">
+        <v>192</v>
+      </c>
+      <c r="C47" s="76"/>
+      <c r="D47" s="76"/>
+      <c r="E47" s="77"/>
+    </row>
+    <row r="48" ht="14.6" customHeight="1">
+      <c r="A48" t="s" s="78">
+        <v>193</v>
+      </c>
+      <c r="B48" t="s" s="79">
+        <v>194</v>
+      </c>
+      <c r="C48" s="80"/>
+      <c r="D48" s="80"/>
+      <c r="E48" s="81"/>
+    </row>
+    <row r="49" ht="14.6" customHeight="1">
+      <c r="A49" s="82"/>
+      <c r="B49" s="80"/>
+      <c r="C49" s="80"/>
+      <c r="D49" s="80"/>
+      <c r="E49" s="81"/>
+    </row>
+    <row r="50" ht="14.6" customHeight="1">
+      <c r="A50" s="82"/>
+      <c r="B50" s="80"/>
+      <c r="C50" s="80"/>
+      <c r="D50" s="80"/>
+      <c r="E50" s="81"/>
+    </row>
+    <row r="51" ht="14.6" customHeight="1">
+      <c r="A51" s="82"/>
+      <c r="B51" s="80"/>
+      <c r="C51" s="80"/>
+      <c r="D51" s="80"/>
+      <c r="E51" s="81"/>
+    </row>
+    <row r="52" ht="14.6" customHeight="1">
+      <c r="A52" s="82"/>
+      <c r="B52" s="80"/>
+      <c r="C52" s="80"/>
+      <c r="D52" s="80"/>
+      <c r="E52" s="81"/>
+    </row>
+    <row r="53" ht="14.6" customHeight="1">
+      <c r="A53" s="83"/>
+      <c r="B53" s="84"/>
+      <c r="C53" s="84"/>
+      <c r="D53" s="84"/>
+      <c r="E53" s="85"/>
+    </row>
+    <row r="54" ht="14.6" customHeight="1">
+      <c r="A54" s="9"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+    </row>
+    <row r="55" ht="14.6" customHeight="1">
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+    </row>
+    <row r="56" ht="14.6" customHeight="1">
+      <c r="A56" s="7"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+    </row>
+    <row r="57" ht="14.6" customHeight="1">
+      <c r="A57" s="10"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+    </row>
+    <row r="58" ht="14.6" customHeight="1">
+      <c r="A58" s="7"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+    </row>
+    <row r="59" ht="14.6" customHeight="1">
+      <c r="A59" s="9"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
+    </row>
+    <row r="60" ht="14.6" customHeight="1">
+      <c r="A60" s="8"/>
+      <c r="B60" s="8"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+    </row>
+    <row r="61" ht="14.6" customHeight="1">
+      <c r="A61" s="9"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
+    </row>
+    <row r="62" ht="14.6" customHeight="1">
+      <c r="A62" s="8"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="8"/>
+    </row>
+    <row r="63" ht="14.6" customHeight="1">
+      <c r="A63" s="9"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+    </row>
+    <row r="64" ht="14.6" customHeight="1">
+      <c r="A64" s="8"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
+    </row>
+    <row r="65" ht="14.6" customHeight="1">
+      <c r="A65" s="10"/>
+      <c r="B65" s="10"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+    </row>
+    <row r="66" ht="14.6" customHeight="1">
+      <c r="A66" s="7"/>
+      <c r="B66" s="7"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
+    </row>
+    <row r="67" ht="14.6" customHeight="1">
+      <c r="A67" s="10"/>
+      <c r="B67" s="10"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10"/>
+    </row>
+    <row r="68" ht="14.6" customHeight="1">
+      <c r="A68" s="7"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+    </row>
+    <row r="69" ht="14.6" customHeight="1">
+      <c r="A69" s="9"/>
+      <c r="B69" s="9"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+    </row>
+    <row r="70" ht="14.6" customHeight="1">
+      <c r="A70" s="8"/>
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8"/>
+    </row>
+    <row r="71" ht="14.6" customHeight="1">
+      <c r="A71" s="9"/>
+      <c r="B71" s="9"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="10"/>
+    </row>
+    <row r="72" ht="14.6" customHeight="1">
+      <c r="A72" s="7"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+    </row>
+    <row r="73" ht="14.6" customHeight="1">
+      <c r="A73" s="10"/>
+      <c r="B73" s="10"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10"/>
+    </row>
+    <row r="74" ht="14.6" customHeight="1">
+      <c r="A74" s="8"/>
+      <c r="B74" s="8"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8"/>
+      <c r="E74" s="8"/>
+    </row>
+    <row r="75" ht="14.6" customHeight="1">
+      <c r="A75" s="9"/>
+      <c r="B75" s="9"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="10"/>
+    </row>
+    <row r="76" ht="14.6" customHeight="1">
+      <c r="A76" s="7"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="8"/>
+      <c r="E76" s="8"/>
+    </row>
+    <row r="77" ht="14.6" customHeight="1">
+      <c r="A77" s="9"/>
+      <c r="B77" s="9"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="10"/>
+    </row>
+    <row r="78" ht="14.6" customHeight="1">
+      <c r="A78" s="7"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
+    </row>
+    <row r="79" ht="14.6" customHeight="1">
+      <c r="A79" s="9"/>
+      <c r="B79" s="9"/>
+      <c r="C79" s="10"/>
+      <c r="D79" s="10"/>
+      <c r="E79" s="10"/>
+    </row>
+    <row r="80" ht="14.6" customHeight="1">
+      <c r="A80" s="8"/>
+      <c r="B80" s="8"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="8"/>
+    </row>
+    <row r="81" ht="14.6" customHeight="1">
+      <c r="A81" s="9"/>
+      <c r="B81" s="9"/>
+      <c r="C81" s="10"/>
+      <c r="D81" s="10"/>
+      <c r="E81" s="10"/>
+    </row>
+    <row r="82" ht="14.6" customHeight="1">
+      <c r="A82" s="7"/>
+      <c r="B82" s="7"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="8"/>
+    </row>
+    <row r="83" ht="14.6" customHeight="1">
+      <c r="A83" s="10"/>
+      <c r="B83" s="10"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="10"/>
+      <c r="E83" s="10"/>
+    </row>
+    <row r="84" ht="14.6" customHeight="1">
+      <c r="A84" s="7"/>
+      <c r="B84" s="7"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
+      <c r="E84" s="8"/>
+    </row>
+    <row r="85" ht="14.6" customHeight="1">
+      <c r="A85" s="10"/>
+      <c r="B85" s="10"/>
+      <c r="C85" s="10"/>
+      <c r="D85" s="10"/>
+      <c r="E85" s="10"/>
+    </row>
+    <row r="86" ht="14.6" customHeight="1">
+      <c r="A86" s="7"/>
+      <c r="B86" s="7"/>
+      <c r="C86" s="8"/>
+      <c r="D86" s="8"/>
+      <c r="E86" s="8"/>
+    </row>
+    <row r="87" ht="14.6" customHeight="1">
+      <c r="A87" s="9"/>
+      <c r="B87" s="10"/>
+      <c r="C87" s="10"/>
+      <c r="D87" s="10"/>
+      <c r="E87" s="10"/>
+    </row>
+    <row r="88" ht="14.6" customHeight="1">
+      <c r="A88" s="7"/>
+      <c r="B88" s="8"/>
+      <c r="C88" s="8"/>
+      <c r="D88" s="8"/>
+      <c r="E88" s="8"/>
+    </row>
+    <row r="89" ht="14.6" customHeight="1">
+      <c r="A89" s="9"/>
+      <c r="B89" s="10"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="10"/>
+      <c r="E89" s="10"/>
+    </row>
+    <row r="90" ht="14.6" customHeight="1">
+      <c r="A90" s="8"/>
+      <c r="B90" s="8"/>
+      <c r="C90" s="8"/>
+      <c r="D90" s="8"/>
+      <c r="E90" s="8"/>
+    </row>
+    <row r="91" ht="14.6" customHeight="1">
+      <c r="A91" s="10"/>
+      <c r="B91" s="10"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="10"/>
+      <c r="E91" s="10"/>
+    </row>
+    <row r="92" ht="14.6" customHeight="1">
+      <c r="A92" s="7"/>
+      <c r="B92" s="7"/>
+      <c r="C92" s="8"/>
+      <c r="D92" s="8"/>
+      <c r="E92" s="8"/>
+    </row>
+    <row r="93" ht="14.6" customHeight="1">
+      <c r="A93" s="9"/>
+      <c r="B93" s="9"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="10"/>
+      <c r="E93" s="10"/>
+    </row>
+    <row r="94" ht="14.6" customHeight="1">
+      <c r="A94" s="7"/>
+      <c r="B94" s="7"/>
+      <c r="C94" s="8"/>
+      <c r="D94" s="8"/>
+      <c r="E94" s="8"/>
+    </row>
+    <row r="95" ht="14.6" customHeight="1">
+      <c r="A95" s="9"/>
+      <c r="B95" s="9"/>
+      <c r="C95" s="10"/>
+      <c r="D95" s="10"/>
+      <c r="E95" s="10"/>
+    </row>
+    <row r="96" ht="14.6" customHeight="1">
+      <c r="A96" s="7"/>
+      <c r="B96" s="7"/>
+      <c r="C96" s="8"/>
+      <c r="D96" s="8"/>
+      <c r="E96" s="8"/>
+    </row>
+    <row r="97" ht="14.6" customHeight="1">
+      <c r="A97" s="9"/>
+      <c r="B97" s="9"/>
+      <c r="C97" s="10"/>
+      <c r="D97" s="10"/>
+      <c r="E97" s="10"/>
+    </row>
+    <row r="98" ht="14.6" customHeight="1">
+      <c r="A98" s="8"/>
+      <c r="B98" s="8"/>
+      <c r="C98" s="8"/>
+      <c r="D98" s="8"/>
+      <c r="E98" s="8"/>
+    </row>
+    <row r="99" ht="14.6" customHeight="1">
+      <c r="A99" s="9"/>
+      <c r="B99" s="9"/>
+      <c r="C99" s="10"/>
+      <c r="D99" s="10"/>
+      <c r="E99" s="10"/>
+    </row>
+    <row r="100" ht="14.6" customHeight="1">
+      <c r="A100" s="7"/>
+      <c r="B100" s="7"/>
+      <c r="C100" s="8"/>
+      <c r="D100" s="8"/>
+      <c r="E100" s="8"/>
+    </row>
+    <row r="101" ht="14.6" customHeight="1">
+      <c r="A101" s="9"/>
+      <c r="B101" s="9"/>
+      <c r="C101" s="10"/>
+      <c r="D101" s="10"/>
+      <c r="E101" s="10"/>
+    </row>
+    <row r="102" ht="14.6" customHeight="1">
+      <c r="A102" s="7"/>
+      <c r="B102" s="7"/>
+      <c r="C102" s="8"/>
+      <c r="D102" s="8"/>
+      <c r="E102" s="8"/>
+    </row>
+    <row r="103" ht="14.6" customHeight="1">
+      <c r="A103" s="9"/>
+      <c r="B103" s="9"/>
+      <c r="C103" s="10"/>
+      <c r="D103" s="10"/>
+      <c r="E103" s="10"/>
+    </row>
+    <row r="104" ht="14.6" customHeight="1">
+      <c r="A104" s="8"/>
+      <c r="B104" s="8"/>
+      <c r="C104" s="8"/>
+      <c r="D104" s="8"/>
+      <c r="E104" s="8"/>
+    </row>
+    <row r="105" ht="14.6" customHeight="1">
+      <c r="A105" s="9"/>
+      <c r="B105" s="9"/>
+      <c r="C105" s="10"/>
+      <c r="D105" s="10"/>
+      <c r="E105" s="10"/>
+    </row>
+    <row r="106" ht="14.6" customHeight="1">
+      <c r="A106" s="7"/>
+      <c r="B106" s="7"/>
+      <c r="C106" s="8"/>
+      <c r="D106" s="8"/>
+      <c r="E106" s="8"/>
+    </row>
+    <row r="107" ht="14.6" customHeight="1">
+      <c r="A107" s="9"/>
+      <c r="B107" s="9"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="10"/>
+      <c r="E107" s="10"/>
+    </row>
+    <row r="108" ht="14.6" customHeight="1">
+      <c r="A108" s="7"/>
+      <c r="B108" s="7"/>
+      <c r="C108" s="8"/>
+      <c r="D108" s="8"/>
+      <c r="E108" s="8"/>
+    </row>
+    <row r="109" ht="14.6" customHeight="1">
+      <c r="A109" s="9"/>
+      <c r="B109" s="9"/>
+      <c r="C109" s="10"/>
+      <c r="D109" s="10"/>
+      <c r="E109" s="10"/>
+    </row>
+    <row r="110" ht="14.6" customHeight="1">
+      <c r="A110" s="8"/>
+      <c r="B110" s="8"/>
+      <c r="C110" s="8"/>
+      <c r="D110" s="8"/>
+      <c r="E110" s="8"/>
+    </row>
+    <row r="111" ht="14.6" customHeight="1">
+      <c r="A111" s="9"/>
+      <c r="B111" s="10"/>
+      <c r="C111" s="10"/>
+      <c r="D111" s="10"/>
+      <c r="E111" s="10"/>
+    </row>
+    <row r="112" ht="14.6" customHeight="1">
+      <c r="A112" s="7"/>
+      <c r="B112" s="7"/>
+      <c r="C112" s="8"/>
+      <c r="D112" s="8"/>
+      <c r="E112" s="8"/>
+    </row>
+    <row r="113" ht="14.6" customHeight="1">
+      <c r="A113" s="9"/>
+      <c r="B113" s="9"/>
+      <c r="C113" s="10"/>
+      <c r="D113" s="10"/>
+      <c r="E113" s="10"/>
+    </row>
+    <row r="114" ht="14.6" customHeight="1">
+      <c r="A114" s="7"/>
+      <c r="B114" s="7"/>
+      <c r="C114" s="8"/>
+      <c r="D114" s="8"/>
+      <c r="E114" s="8"/>
+    </row>
+    <row r="115" ht="14.6" customHeight="1">
+      <c r="A115" s="9"/>
+      <c r="B115" s="9"/>
+      <c r="C115" s="10"/>
+      <c r="D115" s="10"/>
+      <c r="E115" s="10"/>
+    </row>
+    <row r="116" ht="14.6" customHeight="1">
+      <c r="A116" s="7"/>
+      <c r="B116" s="7"/>
+      <c r="C116" s="8"/>
+      <c r="D116" s="8"/>
+      <c r="E116" s="8"/>
+    </row>
+    <row r="117" ht="14.6" customHeight="1">
+      <c r="A117" s="10"/>
+      <c r="B117" s="10"/>
+      <c r="C117" s="10"/>
+      <c r="D117" s="10"/>
+      <c r="E117" s="10"/>
+    </row>
+    <row r="118" ht="14.6" customHeight="1">
+      <c r="A118" s="7"/>
+      <c r="B118" s="7"/>
+      <c r="C118" s="8"/>
+      <c r="D118" s="8"/>
+      <c r="E118" s="8"/>
+    </row>
+    <row r="119" ht="14.6" customHeight="1">
+      <c r="A119" s="9"/>
+      <c r="B119" s="9"/>
+      <c r="C119" s="10"/>
+      <c r="D119" s="10"/>
+      <c r="E119" s="10"/>
+    </row>
+    <row r="120" ht="14.6" customHeight="1">
+      <c r="A120" s="7"/>
+      <c r="B120" s="7"/>
+      <c r="C120" s="8"/>
+      <c r="D120" s="8"/>
+      <c r="E120" s="8"/>
+    </row>
+    <row r="121" ht="14.6" customHeight="1">
+      <c r="A121" s="10"/>
+      <c r="B121" s="10"/>
+      <c r="C121" s="10"/>
+      <c r="D121" s="10"/>
+      <c r="E121" s="10"/>
+    </row>
+    <row r="122" ht="14.6" customHeight="1">
+      <c r="A122" s="7"/>
+      <c r="B122" s="7"/>
+      <c r="C122" s="8"/>
+      <c r="D122" s="8"/>
+      <c r="E122" s="8"/>
+    </row>
+    <row r="123" ht="14.6" customHeight="1">
+      <c r="A123" s="9"/>
+      <c r="B123" s="9"/>
+      <c r="C123" s="10"/>
+      <c r="D123" s="10"/>
+      <c r="E123" s="10"/>
+    </row>
+    <row r="124" ht="14.6" customHeight="1">
+      <c r="A124" s="7"/>
+      <c r="B124" s="7"/>
+      <c r="C124" s="8"/>
+      <c r="D124" s="8"/>
+      <c r="E124" s="8"/>
+    </row>
+    <row r="125" ht="14.6" customHeight="1">
+      <c r="A125" s="9"/>
+      <c r="B125" s="9"/>
+      <c r="C125" s="10"/>
+      <c r="D125" s="10"/>
+      <c r="E125" s="10"/>
+    </row>
+    <row r="126" ht="14.6" customHeight="1">
+      <c r="A126" s="8"/>
+      <c r="B126" s="8"/>
+      <c r="C126" s="8"/>
+      <c r="D126" s="8"/>
+      <c r="E126" s="8"/>
+    </row>
+    <row r="127" ht="14.6" customHeight="1">
+      <c r="A127" s="9"/>
+      <c r="B127" s="9"/>
+      <c r="C127" s="10"/>
+      <c r="D127" s="10"/>
+      <c r="E127" s="10"/>
+    </row>
+    <row r="128" ht="14.6" customHeight="1">
+      <c r="A128" s="7"/>
+      <c r="B128" s="7"/>
+      <c r="C128" s="8"/>
+      <c r="D128" s="8"/>
+      <c r="E128" s="8"/>
+    </row>
+    <row r="129" ht="14.6" customHeight="1">
+      <c r="A129" s="10"/>
+      <c r="B129" s="10"/>
+      <c r="C129" s="10"/>
+      <c r="D129" s="10"/>
+      <c r="E129" s="10"/>
+    </row>
+    <row r="130" ht="14.6" customHeight="1">
+      <c r="A130" s="7"/>
+      <c r="B130" s="7"/>
+      <c r="C130" s="8"/>
+      <c r="D130" s="8"/>
+      <c r="E130" s="8"/>
+    </row>
+    <row r="131" ht="14.6" customHeight="1">
+      <c r="A131" s="9"/>
+      <c r="B131" s="9"/>
+      <c r="C131" s="10"/>
+      <c r="D131" s="10"/>
+      <c r="E131" s="10"/>
+    </row>
+    <row r="132" ht="14.6" customHeight="1">
+      <c r="A132" s="7"/>
+      <c r="B132" s="7"/>
+      <c r="C132" s="8"/>
+      <c r="D132" s="8"/>
+      <c r="E132" s="8"/>
+    </row>
+    <row r="133" ht="14.6" customHeight="1">
+      <c r="A133" s="10"/>
+      <c r="B133" s="10"/>
+      <c r="C133" s="10"/>
+      <c r="D133" s="10"/>
+      <c r="E133" s="10"/>
+    </row>
+    <row r="134" ht="14.6" customHeight="1">
+      <c r="A134" s="7"/>
+      <c r="B134" s="7"/>
+      <c r="C134" s="8"/>
+      <c r="D134" s="8"/>
+      <c r="E134" s="8"/>
+    </row>
+    <row r="135" ht="14.6" customHeight="1">
+      <c r="A135" s="9"/>
+      <c r="B135" s="9"/>
+      <c r="C135" s="10"/>
+      <c r="D135" s="10"/>
+      <c r="E135" s="10"/>
+    </row>
+    <row r="136" ht="14.6" customHeight="1">
+      <c r="A136" s="8"/>
+      <c r="B136" s="8"/>
+      <c r="C136" s="8"/>
+      <c r="D136" s="8"/>
+      <c r="E136" s="8"/>
+    </row>
+    <row r="137" ht="14.6" customHeight="1">
+      <c r="A137" s="9"/>
+      <c r="B137" s="9"/>
+      <c r="C137" s="10"/>
+      <c r="D137" s="10"/>
+      <c r="E137" s="10"/>
+    </row>
+    <row r="138" ht="14.6" customHeight="1">
+      <c r="A138" s="8"/>
+      <c r="B138" s="8"/>
+      <c r="C138" s="8"/>
+      <c r="D138" s="8"/>
+      <c r="E138" s="8"/>
+    </row>
+    <row r="139" ht="14.6" customHeight="1">
+      <c r="A139" s="9"/>
+      <c r="B139" s="9"/>
+      <c r="C139" s="10"/>
+      <c r="D139" s="10"/>
+      <c r="E139" s="10"/>
+    </row>
+    <row r="140" ht="14.6" customHeight="1">
+      <c r="A140" s="7"/>
+      <c r="B140" s="7"/>
+      <c r="C140" s="8"/>
+      <c r="D140" s="8"/>
+      <c r="E140" s="8"/>
+    </row>
+    <row r="141" ht="14.6" customHeight="1">
+      <c r="A141" s="10"/>
+      <c r="B141" s="10"/>
+      <c r="C141" s="10"/>
+      <c r="D141" s="10"/>
+      <c r="E141" s="10"/>
+    </row>
+    <row r="142" ht="14.6" customHeight="1">
+      <c r="A142" s="7"/>
+      <c r="B142" s="7"/>
+      <c r="C142" s="8"/>
+      <c r="D142" s="8"/>
+      <c r="E142" s="8"/>
+    </row>
+    <row r="143" ht="14.6" customHeight="1">
+      <c r="A143" s="9"/>
+      <c r="B143" s="9"/>
+      <c r="C143" s="10"/>
+      <c r="D143" s="10"/>
+      <c r="E143" s="10"/>
+    </row>
+    <row r="144" ht="14.6" customHeight="1">
+      <c r="A144" s="8"/>
+      <c r="B144" s="8"/>
+      <c r="C144" s="8"/>
+      <c r="D144" s="8"/>
+      <c r="E144" s="8"/>
+    </row>
+    <row r="145" ht="14.6" customHeight="1">
+      <c r="A145" s="10"/>
+      <c r="B145" s="10"/>
+      <c r="C145" s="10"/>
+      <c r="D145" s="10"/>
+      <c r="E145" s="10"/>
+    </row>
+    <row r="146" ht="14.6" customHeight="1">
+      <c r="A146" s="7"/>
+      <c r="B146" s="8"/>
+      <c r="C146" s="8"/>
+      <c r="D146" s="8"/>
+      <c r="E146" s="8"/>
+    </row>
+    <row r="147" ht="14.6" customHeight="1">
+      <c r="A147" s="9"/>
+      <c r="B147" s="10"/>
+      <c r="C147" s="10"/>
+      <c r="D147" s="10"/>
+      <c r="E147" s="10"/>
+    </row>
+    <row r="148" ht="14.6" customHeight="1">
+      <c r="A148" s="7"/>
+      <c r="B148" s="7"/>
+      <c r="C148" s="8"/>
+      <c r="D148" s="8"/>
+      <c r="E148" s="8"/>
+    </row>
+    <row r="149" ht="14.6" customHeight="1">
+      <c r="A149" s="10"/>
+      <c r="B149" s="10"/>
+      <c r="C149" s="10"/>
+      <c r="D149" s="10"/>
+      <c r="E149" s="10"/>
+    </row>
+    <row r="150" ht="14.6" customHeight="1">
+      <c r="A150" s="7"/>
+      <c r="B150" s="7"/>
+      <c r="C150" s="8"/>
+      <c r="D150" s="8"/>
+      <c r="E150" s="8"/>
+    </row>
+    <row r="151" ht="14.6" customHeight="1">
+      <c r="A151" s="10"/>
+      <c r="B151" s="10"/>
+      <c r="C151" s="10"/>
+      <c r="D151" s="10"/>
+      <c r="E151" s="10"/>
+    </row>
+    <row r="152" ht="14.6" customHeight="1">
+      <c r="A152" s="8"/>
+      <c r="B152" s="8"/>
+      <c r="C152" s="8"/>
+      <c r="D152" s="8"/>
+      <c r="E152" s="8"/>
+    </row>
+    <row r="153" ht="14.6" customHeight="1">
+      <c r="A153" s="10"/>
+      <c r="B153" s="10"/>
+      <c r="C153" s="10"/>
+      <c r="D153" s="10"/>
+      <c r="E153" s="10"/>
+    </row>
+    <row r="154" ht="14.6" customHeight="1">
+      <c r="A154" s="8"/>
+      <c r="B154" s="8"/>
+      <c r="C154" s="8"/>
+      <c r="D154" s="8"/>
+      <c r="E154" s="8"/>
+    </row>
+    <row r="155" ht="14.6" customHeight="1">
+      <c r="A155" s="9"/>
+      <c r="B155" s="9"/>
+      <c r="C155" s="10"/>
+      <c r="D155" s="10"/>
+      <c r="E155" s="10"/>
+    </row>
+    <row r="156" ht="14.6" customHeight="1">
+      <c r="A156" s="7"/>
+      <c r="B156" s="7"/>
+      <c r="C156" s="8"/>
+      <c r="D156" s="8"/>
+      <c r="E156" s="8"/>
+    </row>
+    <row r="157" ht="14.6" customHeight="1">
+      <c r="A157" s="9"/>
+      <c r="B157" s="9"/>
+      <c r="C157" s="10"/>
+      <c r="D157" s="10"/>
+      <c r="E157" s="10"/>
+    </row>
+    <row r="158" ht="14.6" customHeight="1">
+      <c r="A158" s="7"/>
+      <c r="B158" s="7"/>
+      <c r="C158" s="8"/>
+      <c r="D158" s="8"/>
+      <c r="E158" s="8"/>
+    </row>
+    <row r="159" ht="14.6" customHeight="1">
+      <c r="A159" s="9"/>
+      <c r="B159" s="9"/>
+      <c r="C159" s="10"/>
+      <c r="D159" s="10"/>
+      <c r="E159" s="10"/>
+    </row>
+    <row r="160" ht="14.6" customHeight="1">
+      <c r="A160" s="7"/>
+      <c r="B160" s="7"/>
+      <c r="C160" s="8"/>
+      <c r="D160" s="8"/>
+      <c r="E160" s="8"/>
+    </row>
+    <row r="161" ht="14.6" customHeight="1">
+      <c r="A161" s="9"/>
+      <c r="B161" s="9"/>
+      <c r="C161" s="10"/>
+      <c r="D161" s="10"/>
+      <c r="E161" s="10"/>
+    </row>
+    <row r="162" ht="14.6" customHeight="1">
+      <c r="A162" s="7"/>
+      <c r="B162" s="7"/>
+      <c r="C162" s="8"/>
+      <c r="D162" s="8"/>
+      <c r="E162" s="8"/>
+    </row>
+    <row r="163" ht="14.6" customHeight="1">
+      <c r="A163" s="10"/>
+      <c r="B163" s="10"/>
+      <c r="C163" s="10"/>
+      <c r="D163" s="10"/>
+      <c r="E163" s="10"/>
+    </row>
+    <row r="164" ht="14.6" customHeight="1">
+      <c r="A164" s="7"/>
+      <c r="B164" s="7"/>
+      <c r="C164" s="8"/>
+      <c r="D164" s="8"/>
+      <c r="E164" s="8"/>
+    </row>
+    <row r="165" ht="14.6" customHeight="1">
+      <c r="A165" s="9"/>
+      <c r="B165" s="9"/>
+      <c r="C165" s="10"/>
+      <c r="D165" s="10"/>
+      <c r="E165" s="10"/>
+    </row>
+    <row r="166" ht="14.6" customHeight="1">
+      <c r="A166" s="7"/>
+      <c r="B166" s="7"/>
+      <c r="C166" s="8"/>
+      <c r="D166" s="8"/>
+      <c r="E166" s="8"/>
+    </row>
+    <row r="167" ht="14.6" customHeight="1">
+      <c r="A167" s="9"/>
+      <c r="B167" s="9"/>
+      <c r="C167" s="10"/>
+      <c r="D167" s="10"/>
+      <c r="E167" s="10"/>
+    </row>
+    <row r="168" ht="14.6" customHeight="1">
+      <c r="A168" s="8"/>
+      <c r="B168" s="8"/>
+      <c r="C168" s="8"/>
+      <c r="D168" s="8"/>
+      <c r="E168" s="8"/>
+    </row>
+    <row r="169" ht="14.6" customHeight="1">
+      <c r="A169" s="9"/>
+      <c r="B169" s="9"/>
+      <c r="C169" s="10"/>
+      <c r="D169" s="10"/>
+      <c r="E169" s="10"/>
+    </row>
+    <row r="170" ht="14.6" customHeight="1">
+      <c r="A170" s="7"/>
+      <c r="B170" s="7"/>
+      <c r="C170" s="8"/>
+      <c r="D170" s="8"/>
+      <c r="E170" s="8"/>
+    </row>
+    <row r="171" ht="14.6" customHeight="1">
+      <c r="A171" s="9"/>
+      <c r="B171" s="9"/>
+      <c r="C171" s="10"/>
+      <c r="D171" s="10"/>
+      <c r="E171" s="10"/>
+    </row>
+    <row r="172" ht="14.6" customHeight="1">
+      <c r="A172" s="7"/>
+      <c r="B172" s="7"/>
+      <c r="C172" s="8"/>
+      <c r="D172" s="8"/>
+      <c r="E172" s="8"/>
+    </row>
+    <row r="173" ht="14.6" customHeight="1">
+      <c r="A173" s="9"/>
+      <c r="B173" s="9"/>
+      <c r="C173" s="10"/>
+      <c r="D173" s="10"/>
+      <c r="E173" s="10"/>
+    </row>
+    <row r="174" ht="14.6" customHeight="1">
+      <c r="A174" s="7"/>
+      <c r="B174" s="7"/>
+      <c r="C174" s="8"/>
+      <c r="D174" s="8"/>
+      <c r="E174" s="8"/>
+    </row>
+    <row r="175" ht="14.6" customHeight="1">
+      <c r="A175" s="9"/>
+      <c r="B175" s="9"/>
+      <c r="C175" s="10"/>
+      <c r="D175" s="10"/>
+      <c r="E175" s="10"/>
+    </row>
+    <row r="176" ht="14.6" customHeight="1">
+      <c r="A176" s="8"/>
+      <c r="B176" s="8"/>
+      <c r="C176" s="8"/>
+      <c r="D176" s="8"/>
+      <c r="E176" s="8"/>
+    </row>
+    <row r="177" ht="14.6" customHeight="1">
+      <c r="A177" s="9"/>
+      <c r="B177" s="9"/>
+      <c r="C177" s="10"/>
+      <c r="D177" s="10"/>
+      <c r="E177" s="10"/>
+    </row>
+    <row r="178" ht="14.6" customHeight="1">
+      <c r="A178" s="7"/>
+      <c r="B178" s="7"/>
+      <c r="C178" s="8"/>
+      <c r="D178" s="8"/>
+      <c r="E178" s="8"/>
+    </row>
+    <row r="179" ht="14.6" customHeight="1">
+      <c r="A179" s="9"/>
+      <c r="B179" s="9"/>
+      <c r="C179" s="10"/>
+      <c r="D179" s="10"/>
+      <c r="E179" s="10"/>
+    </row>
+    <row r="180" ht="14.6" customHeight="1">
+      <c r="A180" s="8"/>
+      <c r="B180" s="8"/>
+      <c r="C180" s="8"/>
+      <c r="D180" s="8"/>
+      <c r="E180" s="8"/>
+    </row>
+    <row r="181" ht="14.6" customHeight="1">
+      <c r="A181" s="9"/>
+      <c r="B181" s="9"/>
+      <c r="C181" s="10"/>
+      <c r="D181" s="10"/>
+      <c r="E181" s="10"/>
+    </row>
+    <row r="182" ht="14.6" customHeight="1">
+      <c r="A182" s="7"/>
+      <c r="B182" s="7"/>
+      <c r="C182" s="8"/>
+      <c r="D182" s="8"/>
+      <c r="E182" s="8"/>
+    </row>
+    <row r="183" ht="14.6" customHeight="1">
+      <c r="A183" s="10"/>
+      <c r="B183" s="10"/>
+      <c r="C183" s="10"/>
+      <c r="D183" s="10"/>
+      <c r="E183" s="10"/>
+    </row>
+    <row r="184" ht="14.6" customHeight="1">
+      <c r="A184" s="7"/>
+      <c r="B184" s="7"/>
+      <c r="C184" s="8"/>
+      <c r="D184" s="8"/>
+      <c r="E184" s="8"/>
+    </row>
+    <row r="185" ht="14.6" customHeight="1">
+      <c r="A185" s="9"/>
+      <c r="B185" s="9"/>
+      <c r="C185" s="10"/>
+      <c r="D185" s="10"/>
+      <c r="E185" s="10"/>
+    </row>
+    <row r="186" ht="14.6" customHeight="1">
+      <c r="A186" s="8"/>
+      <c r="B186" s="8"/>
+      <c r="C186" s="8"/>
+      <c r="D186" s="8"/>
+      <c r="E186" s="8"/>
+    </row>
+    <row r="187" ht="14.6" customHeight="1">
+      <c r="A187" s="9"/>
+      <c r="B187" s="9"/>
+      <c r="C187" s="10"/>
+      <c r="D187" s="10"/>
+      <c r="E187" s="10"/>
+    </row>
+    <row r="188" ht="14.6" customHeight="1">
+      <c r="A188" s="7"/>
+      <c r="B188" s="7"/>
+      <c r="C188" s="8"/>
+      <c r="D188" s="8"/>
+      <c r="E188" s="8"/>
+    </row>
+    <row r="189" ht="14.6" customHeight="1">
+      <c r="A189" s="10"/>
+      <c r="B189" s="10"/>
+      <c r="C189" s="10"/>
+      <c r="D189" s="10"/>
+      <c r="E189" s="10"/>
+    </row>
+    <row r="190" ht="14.6" customHeight="1">
+      <c r="A190" s="7"/>
+      <c r="B190" s="7"/>
+      <c r="C190" s="8"/>
+      <c r="D190" s="8"/>
+      <c r="E190" s="8"/>
+    </row>
+    <row r="191" ht="14.6" customHeight="1">
+      <c r="A191" s="9"/>
+      <c r="B191" s="9"/>
+      <c r="C191" s="10"/>
+      <c r="D191" s="10"/>
+      <c r="E191" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A2:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
@@ -11285,88 +13087,88 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="14.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="64" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="64" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="86" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="86" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.55" customHeight="1">
-      <c r="A1" t="s" s="65">
-        <v>155</v>
-      </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
+      <c r="A1" t="s" s="87">
+        <v>195</v>
+      </c>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
     </row>
     <row r="2" ht="14.15" customHeight="1">
-      <c r="A2" s="66"/>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
+      <c r="A2" s="88"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
     </row>
     <row r="3" ht="14.15" customHeight="1">
-      <c r="A3" s="67"/>
-      <c r="B3" s="68"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
+      <c r="A3" s="89"/>
+      <c r="B3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
     </row>
     <row r="4" ht="13.95" customHeight="1">
-      <c r="A4" s="70"/>
-      <c r="B4" s="71"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
+      <c r="A4" s="92"/>
+      <c r="B4" s="93"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
     </row>
     <row r="5" ht="13.95" customHeight="1">
-      <c r="A5" s="70"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
+      <c r="A5" s="92"/>
+      <c r="B5" s="93"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
     </row>
     <row r="6" ht="13.95" customHeight="1">
-      <c r="A6" s="70"/>
-      <c r="B6" s="71"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
+      <c r="A6" s="92"/>
+      <c r="B6" s="93"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="94"/>
+      <c r="E6" s="94"/>
     </row>
     <row r="7" ht="13.95" customHeight="1">
-      <c r="A7" s="70"/>
-      <c r="B7" s="71"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
+      <c r="A7" s="92"/>
+      <c r="B7" s="93"/>
+      <c r="C7" s="94"/>
+      <c r="D7" s="94"/>
+      <c r="E7" s="94"/>
     </row>
     <row r="8" ht="13.95" customHeight="1">
-      <c r="A8" s="70"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
+      <c r="A8" s="92"/>
+      <c r="B8" s="93"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="94"/>
     </row>
     <row r="9" ht="13.95" customHeight="1">
-      <c r="A9" s="70"/>
-      <c r="B9" s="71"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
+      <c r="A9" s="92"/>
+      <c r="B9" s="93"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="94"/>
+      <c r="E9" s="94"/>
     </row>
     <row r="10" ht="13.95" customHeight="1">
-      <c r="A10" s="70"/>
-      <c r="B10" s="71"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
+      <c r="A10" s="92"/>
+      <c r="B10" s="93"/>
+      <c r="C10" s="94"/>
+      <c r="D10" s="94"/>
+      <c r="E10" s="94"/>
     </row>
     <row r="11" ht="13.95" customHeight="1">
-      <c r="A11" s="70"/>
-      <c r="B11" s="71"/>
-      <c r="C11" s="72"/>
-      <c r="D11" s="72"/>
-      <c r="E11" s="72"/>
+      <c r="A11" s="92"/>
+      <c r="B11" s="93"/>
+      <c r="C11" s="94"/>
+      <c r="D11" s="94"/>
+      <c r="E11" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
DIR SQL Query update
</commit_message>
<xml_diff>
--- a/DataExtraction/Input/Config.xlsx
+++ b/DataExtraction/Input/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="242">
   <si>
     <t>Key</t>
   </si>
@@ -290,6 +290,18 @@
     <t>/Users/gundukalyan/Documents/GitHub/mns-json-prep/DataExtraction/Output/DIR</t>
   </si>
   <si>
+    <t>din_column_name_in_db</t>
+  </si>
+  <si>
+    <t>din</t>
+  </si>
+  <si>
+    <t>designation_after_event_column_name_in_db</t>
+  </si>
+  <si>
+    <t>designation_after_event</t>
+  </si>
+  <si>
     <t>activity_abbreviation_list</t>
   </si>
   <si>
@@ -348,9 +360,6 @@
   </si>
   <si>
     <t>designation_column_name</t>
-  </si>
-  <si>
-    <t>designation_after_event</t>
   </si>
   <si>
     <t>appointment_keyword</t>
@@ -685,9 +694,6 @@
   </si>
   <si>
     <t>din_column_name</t>
-  </si>
-  <si>
-    <t>din</t>
   </si>
   <si>
     <t>pan_column_name</t>
@@ -4133,7 +4139,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -4144,7 +4150,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -4173,7 +4179,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s" s="9">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -4228,7 +4234,7 @@
     </row>
     <row r="13" ht="14.6" customHeight="1">
       <c r="A13" t="s" s="7">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B13" t="s" s="7">
         <v>29</v>
@@ -4246,7 +4252,7 @@
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" t="s" s="52">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B15" s="94">
         <v>0</v>
@@ -4257,7 +4263,7 @@
     </row>
     <row r="16" ht="15.35" customHeight="1">
       <c r="A16" t="s" s="95">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B16" s="59">
         <v>2</v>
@@ -4268,7 +4274,7 @@
     </row>
     <row r="17" ht="15.35" customHeight="1">
       <c r="A17" t="s" s="96">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B17" s="59">
         <v>3</v>
@@ -4279,7 +4285,7 @@
     </row>
     <row r="18" ht="15.35" customHeight="1">
       <c r="A18" t="s" s="58">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B18" s="61">
         <v>4</v>
@@ -4290,7 +4296,7 @@
     </row>
     <row r="19" ht="15.35" customHeight="1">
       <c r="A19" t="s" s="60">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B19" s="63">
         <v>6</v>
@@ -4301,7 +4307,7 @@
     </row>
     <row r="20" ht="15.35" customHeight="1">
       <c r="A20" t="s" s="58">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B20" s="59">
         <v>7</v>
@@ -4312,7 +4318,7 @@
     </row>
     <row r="21" ht="15.35" customHeight="1">
       <c r="A21" t="s" s="62">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B21" s="63">
         <v>8</v>
@@ -4330,10 +4336,10 @@
     </row>
     <row r="23" ht="15.35" customHeight="1">
       <c r="A23" t="s" s="9">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B23" t="s" s="29">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -4341,10 +4347,10 @@
     </row>
     <row r="24" ht="15.35" customHeight="1">
       <c r="A24" t="s" s="29">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B24" t="s" s="29">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -4370,10 +4376,10 @@
     </row>
     <row r="27" ht="15.35" customHeight="1">
       <c r="A27" t="s" s="29">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B27" t="s" s="29">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -4388,10 +4394,10 @@
     </row>
     <row r="29" ht="15.35" customHeight="1">
       <c r="A29" t="s" s="29">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B29" t="s" s="29">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -4399,10 +4405,10 @@
     </row>
     <row r="30" ht="15.35" customHeight="1">
       <c r="A30" t="s" s="29">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B30" t="s" s="29">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -4417,10 +4423,10 @@
     </row>
     <row r="32" ht="15.35" customHeight="1">
       <c r="A32" t="s" s="29">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B32" t="s" s="29">
-        <v>214</v>
+        <v>90</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
@@ -4428,10 +4434,10 @@
     </row>
     <row r="33" ht="15.35" customHeight="1">
       <c r="A33" t="s" s="43">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B33" t="s" s="43">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
@@ -4446,10 +4452,10 @@
     </row>
     <row r="35" ht="15.35" customHeight="1">
       <c r="A35" t="s" s="97">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B35" t="s" s="97">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -4457,10 +4463,10 @@
     </row>
     <row r="36" ht="14.6" customHeight="1">
       <c r="A36" t="s" s="70">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B36" t="s" s="71">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
@@ -4475,10 +4481,10 @@
     </row>
     <row r="38" ht="14.6" customHeight="1">
       <c r="A38" t="s" s="26">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B38" t="s" s="73">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
@@ -4486,10 +4492,10 @@
     </row>
     <row r="39" ht="14.6" customHeight="1">
       <c r="A39" t="s" s="29">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B39" t="s" s="29">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
@@ -4504,10 +4510,10 @@
     </row>
     <row r="41" ht="14.6" customHeight="1">
       <c r="A41" t="s" s="29">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B41" t="s" s="29">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
@@ -4515,10 +4521,10 @@
     </row>
     <row r="42" ht="14.6" customHeight="1">
       <c r="A42" t="s" s="98">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B42" t="s" s="98">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
@@ -4533,10 +4539,10 @@
     </row>
     <row r="44" ht="14.6" customHeight="1">
       <c r="A44" t="s" s="29">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B44" t="s" s="29">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
@@ -4544,10 +4550,10 @@
     </row>
     <row r="45" ht="14.6" customHeight="1">
       <c r="A45" t="s" s="69">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B45" t="s" s="67">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
@@ -4555,10 +4561,10 @@
     </row>
     <row r="46" ht="14.6" customHeight="1">
       <c r="A46" t="s" s="99">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B46" t="s" s="100">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C46" s="101"/>
       <c r="D46" s="101"/>
@@ -4573,10 +4579,10 @@
     </row>
     <row r="48" ht="14.6" customHeight="1">
       <c r="A48" t="s" s="9">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B48" t="s" s="9">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
@@ -4584,10 +4590,10 @@
     </row>
     <row r="49" ht="14.6" customHeight="1">
       <c r="A49" t="s" s="7">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B49" t="s" s="7">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
@@ -4595,10 +4601,10 @@
     </row>
     <row r="50" ht="14.6" customHeight="1">
       <c r="A50" t="s" s="9">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B50" t="s" s="9">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
@@ -5616,7 +5622,7 @@
   <sheetData>
     <row r="1" ht="15.55" customHeight="1">
       <c r="A1" t="s" s="104">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B1" s="104"/>
       <c r="C1" s="104"/>
@@ -10718,7 +10724,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E164"/>
+  <dimension ref="A1:E166"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -10827,53 +10833,53 @@
     </row>
     <row r="10" ht="26.6" customHeight="1">
       <c r="A10" t="s" s="9">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="B10" t="s" s="9">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
     </row>
-    <row r="11" ht="15.35" customHeight="1">
-      <c r="A11" t="s" s="21">
-        <v>89</v>
-      </c>
-      <c r="B11" t="s" s="36">
-        <v>90</v>
-      </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" ht="14.6" customHeight="1">
-      <c r="A12" t="s" s="7">
+    <row r="11" ht="26.6" customHeight="1">
+      <c r="A11" t="s" s="9">
         <v>91</v>
       </c>
-      <c r="B12" t="s" s="37">
+      <c r="B11" t="s" s="9">
         <v>92</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+    </row>
+    <row r="12" ht="26.6" customHeight="1">
+      <c r="A12" t="s" s="9">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s" s="9">
+        <v>31</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
     </row>
-    <row r="13" ht="14.6" customHeight="1">
-      <c r="A13" t="s" s="7">
+    <row r="13" ht="15.35" customHeight="1">
+      <c r="A13" t="s" s="21">
         <v>93</v>
       </c>
-      <c r="B13" t="s" s="38">
+      <c r="B13" t="s" s="36">
         <v>94</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" ht="15.35" customHeight="1">
-      <c r="A14" t="s" s="23">
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" ht="14.6" customHeight="1">
+      <c r="A14" t="s" s="7">
         <v>95</v>
       </c>
-      <c r="B14" t="s" s="9">
+      <c r="B14" t="s" s="37">
         <v>96</v>
       </c>
       <c r="C14" s="10"/>
@@ -10881,169 +10887,177 @@
       <c r="E14" s="10"/>
     </row>
     <row r="15" ht="14.6" customHeight="1">
-      <c r="A15" t="s" s="22">
+      <c r="A15" t="s" s="7">
         <v>97</v>
       </c>
-      <c r="B15" t="s" s="29">
+      <c r="B15" t="s" s="38">
         <v>98</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" ht="14.6" customHeight="1">
-      <c r="A16" t="s" s="13">
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+    </row>
+    <row r="16" ht="15.35" customHeight="1">
+      <c r="A16" t="s" s="23">
         <v>99</v>
       </c>
-      <c r="B16" t="s" s="39">
+      <c r="B16" t="s" s="9">
         <v>100</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
     </row>
-    <row r="17" ht="15.35" customHeight="1">
-      <c r="A17" t="s" s="9">
+    <row r="17" ht="14.6" customHeight="1">
+      <c r="A17" t="s" s="22">
         <v>101</v>
       </c>
-      <c r="B17" t="s" s="23">
+      <c r="B17" t="s" s="29">
         <v>102</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" ht="15.35" customHeight="1">
-      <c r="A18" t="s" s="7">
+    <row r="18" ht="14.6" customHeight="1">
+      <c r="A18" t="s" s="13">
         <v>103</v>
       </c>
-      <c r="B18" t="s" s="21">
-        <v>92</v>
+      <c r="B18" t="s" s="39">
+        <v>104</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
     </row>
     <row r="19" ht="15.35" customHeight="1">
-      <c r="A19" t="s" s="7">
-        <v>104</v>
-      </c>
-      <c r="B19" t="s" s="21">
-        <v>94</v>
+      <c r="A19" t="s" s="9">
+        <v>105</v>
+      </c>
+      <c r="B19" t="s" s="23">
+        <v>106</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
     </row>
     <row r="20" ht="15.35" customHeight="1">
-      <c r="A20" t="s" s="9">
-        <v>105</v>
-      </c>
-      <c r="B20" t="s" s="23">
+      <c r="A20" t="s" s="7">
+        <v>107</v>
+      </c>
+      <c r="B20" t="s" s="21">
         <v>96</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
     </row>
-    <row r="21" ht="14.6" customHeight="1">
-      <c r="A21" t="s" s="24">
-        <v>106</v>
-      </c>
-      <c r="B21" t="s" s="40">
-        <v>107</v>
+    <row r="21" ht="15.35" customHeight="1">
+      <c r="A21" t="s" s="7">
+        <v>108</v>
+      </c>
+      <c r="B21" t="s" s="21">
+        <v>98</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" ht="14.6" customHeight="1">
-      <c r="A22" t="s" s="26">
-        <v>108</v>
-      </c>
-      <c r="B22" t="s" s="41">
+    <row r="22" ht="15.35" customHeight="1">
+      <c r="A22" t="s" s="9">
         <v>109</v>
+      </c>
+      <c r="B22" t="s" s="23">
+        <v>100</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" ht="15.35" customHeight="1">
-      <c r="A23" t="s" s="21">
+    <row r="23" ht="14.6" customHeight="1">
+      <c r="A23" t="s" s="24">
         <v>110</v>
       </c>
-      <c r="B23" t="s" s="21">
+      <c r="B23" t="s" s="40">
         <v>111</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" ht="15.35" customHeight="1">
-      <c r="A24" t="s" s="42">
+    <row r="24" ht="14.6" customHeight="1">
+      <c r="A24" t="s" s="26">
         <v>112</v>
       </c>
-      <c r="B24" t="s" s="23">
-        <v>113</v>
+      <c r="B24" t="s" s="41">
+        <v>92</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
     </row>
-    <row r="25" ht="14.6" customHeight="1">
-      <c r="A25" t="s" s="43">
+    <row r="25" ht="15.35" customHeight="1">
+      <c r="A25" t="s" s="21">
+        <v>113</v>
+      </c>
+      <c r="B25" t="s" s="21">
         <v>114</v>
-      </c>
-      <c r="B25" t="s" s="43">
-        <v>115</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" ht="14.6" customHeight="1">
-      <c r="A26" t="s" s="44">
+    <row r="26" ht="15.35" customHeight="1">
+      <c r="A26" t="s" s="42">
+        <v>115</v>
+      </c>
+      <c r="B26" t="s" s="23">
         <v>116</v>
-      </c>
-      <c r="B26" t="s" s="44">
-        <v>117</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
     </row>
     <row r="27" ht="14.6" customHeight="1">
-      <c r="A27" t="s" s="44">
+      <c r="A27" t="s" s="43">
+        <v>117</v>
+      </c>
+      <c r="B27" t="s" s="43">
         <v>118</v>
-      </c>
-      <c r="B27" t="s" s="43">
-        <v>119</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
     </row>
     <row r="28" ht="14.6" customHeight="1">
-      <c r="A28" t="s" s="9">
+      <c r="A28" t="s" s="44">
+        <v>119</v>
+      </c>
+      <c r="B28" t="s" s="44">
         <v>120</v>
-      </c>
-      <c r="B28" t="s" s="9">
-        <v>121</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
     </row>
     <row r="29" ht="14.6" customHeight="1">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
+      <c r="A29" t="s" s="44">
+        <v>121</v>
+      </c>
+      <c r="B29" t="s" s="43">
+        <v>122</v>
+      </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
     </row>
     <row r="30" ht="14.6" customHeight="1">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
+      <c r="A30" t="s" s="9">
+        <v>123</v>
+      </c>
+      <c r="B30" t="s" s="9">
+        <v>124</v>
+      </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
@@ -11056,15 +11070,15 @@
       <c r="E31" s="8"/>
     </row>
     <row r="32" ht="14.6" customHeight="1">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
     </row>
     <row r="33" ht="14.6" customHeight="1">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
@@ -11098,15 +11112,15 @@
       <c r="E37" s="8"/>
     </row>
     <row r="38" ht="14.6" customHeight="1">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="9"/>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
     </row>
     <row r="39" ht="14.6" customHeight="1">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
@@ -11126,15 +11140,15 @@
       <c r="E41" s="8"/>
     </row>
     <row r="42" ht="14.6" customHeight="1">
-      <c r="A42" s="9"/>
-      <c r="B42" s="9"/>
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
     </row>
     <row r="43" ht="14.6" customHeight="1">
-      <c r="A43" s="8"/>
-      <c r="B43" s="8"/>
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
@@ -11147,36 +11161,36 @@
       <c r="E44" s="10"/>
     </row>
     <row r="45" ht="14.6" customHeight="1">
-      <c r="A45" s="7"/>
-      <c r="B45" s="7"/>
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
     </row>
     <row r="46" ht="14.6" customHeight="1">
-      <c r="A46" s="10"/>
-      <c r="B46" s="10"/>
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
       <c r="C46" s="10"/>
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
     </row>
     <row r="47" ht="14.6" customHeight="1">
-      <c r="A47" s="8"/>
-      <c r="B47" s="8"/>
+      <c r="A47" s="7"/>
+      <c r="B47" s="7"/>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
     </row>
     <row r="48" ht="14.6" customHeight="1">
-      <c r="A48" s="9"/>
-      <c r="B48" s="9"/>
+      <c r="A48" s="10"/>
+      <c r="B48" s="10"/>
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
     </row>
     <row r="49" ht="14.6" customHeight="1">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
+      <c r="A49" s="8"/>
+      <c r="B49" s="8"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
@@ -11203,8 +11217,8 @@
       <c r="E52" s="10"/>
     </row>
     <row r="53" ht="14.6" customHeight="1">
-      <c r="A53" s="8"/>
-      <c r="B53" s="8"/>
+      <c r="A53" s="7"/>
+      <c r="B53" s="7"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
       <c r="E53" s="8"/>
@@ -11217,15 +11231,15 @@
       <c r="E54" s="10"/>
     </row>
     <row r="55" ht="14.6" customHeight="1">
-      <c r="A55" s="7"/>
-      <c r="B55" s="7"/>
+      <c r="A55" s="8"/>
+      <c r="B55" s="8"/>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
       <c r="E55" s="8"/>
     </row>
     <row r="56" ht="14.6" customHeight="1">
-      <c r="A56" s="10"/>
-      <c r="B56" s="10"/>
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>
       <c r="E56" s="10"/>
@@ -11252,7 +11266,7 @@
       <c r="E59" s="8"/>
     </row>
     <row r="60" ht="14.6" customHeight="1">
-      <c r="A60" s="9"/>
+      <c r="A60" s="10"/>
       <c r="B60" s="10"/>
       <c r="C60" s="10"/>
       <c r="D60" s="10"/>
@@ -11260,7 +11274,7 @@
     </row>
     <row r="61" ht="14.6" customHeight="1">
       <c r="A61" s="7"/>
-      <c r="B61" s="8"/>
+      <c r="B61" s="7"/>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
       <c r="E61" s="8"/>
@@ -11273,29 +11287,29 @@
       <c r="E62" s="10"/>
     </row>
     <row r="63" ht="14.6" customHeight="1">
-      <c r="A63" s="8"/>
+      <c r="A63" s="7"/>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
       <c r="E63" s="8"/>
     </row>
     <row r="64" ht="14.6" customHeight="1">
-      <c r="A64" s="10"/>
+      <c r="A64" s="9"/>
       <c r="B64" s="10"/>
       <c r="C64" s="10"/>
       <c r="D64" s="10"/>
       <c r="E64" s="10"/>
     </row>
     <row r="65" ht="14.6" customHeight="1">
-      <c r="A65" s="7"/>
-      <c r="B65" s="7"/>
+      <c r="A65" s="8"/>
+      <c r="B65" s="8"/>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
       <c r="E65" s="8"/>
     </row>
     <row r="66" ht="14.6" customHeight="1">
-      <c r="A66" s="9"/>
-      <c r="B66" s="9"/>
+      <c r="A66" s="10"/>
+      <c r="B66" s="10"/>
       <c r="C66" s="10"/>
       <c r="D66" s="10"/>
       <c r="E66" s="10"/>
@@ -11329,8 +11343,8 @@
       <c r="E70" s="10"/>
     </row>
     <row r="71" ht="14.6" customHeight="1">
-      <c r="A71" s="8"/>
-      <c r="B71" s="8"/>
+      <c r="A71" s="7"/>
+      <c r="B71" s="7"/>
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
       <c r="E71" s="8"/>
@@ -11343,8 +11357,8 @@
       <c r="E72" s="10"/>
     </row>
     <row r="73" ht="14.6" customHeight="1">
-      <c r="A73" s="7"/>
-      <c r="B73" s="7"/>
+      <c r="A73" s="8"/>
+      <c r="B73" s="8"/>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
       <c r="E73" s="8"/>
@@ -11371,8 +11385,8 @@
       <c r="E76" s="10"/>
     </row>
     <row r="77" ht="14.6" customHeight="1">
-      <c r="A77" s="8"/>
-      <c r="B77" s="8"/>
+      <c r="A77" s="7"/>
+      <c r="B77" s="7"/>
       <c r="C77" s="8"/>
       <c r="D77" s="8"/>
       <c r="E77" s="8"/>
@@ -11385,8 +11399,8 @@
       <c r="E78" s="10"/>
     </row>
     <row r="79" ht="14.6" customHeight="1">
-      <c r="A79" s="7"/>
-      <c r="B79" s="7"/>
+      <c r="A79" s="8"/>
+      <c r="B79" s="8"/>
       <c r="C79" s="8"/>
       <c r="D79" s="8"/>
       <c r="E79" s="8"/>
@@ -11413,29 +11427,29 @@
       <c r="E82" s="10"/>
     </row>
     <row r="83" ht="14.6" customHeight="1">
-      <c r="A83" s="8"/>
-      <c r="B83" s="8"/>
+      <c r="A83" s="7"/>
+      <c r="B83" s="7"/>
       <c r="C83" s="8"/>
       <c r="D83" s="8"/>
       <c r="E83" s="8"/>
     </row>
     <row r="84" ht="14.6" customHeight="1">
       <c r="A84" s="9"/>
-      <c r="B84" s="10"/>
+      <c r="B84" s="9"/>
       <c r="C84" s="10"/>
       <c r="D84" s="10"/>
       <c r="E84" s="10"/>
     </row>
     <row r="85" ht="14.6" customHeight="1">
-      <c r="A85" s="7"/>
-      <c r="B85" s="7"/>
+      <c r="A85" s="8"/>
+      <c r="B85" s="8"/>
       <c r="C85" s="8"/>
       <c r="D85" s="8"/>
       <c r="E85" s="8"/>
     </row>
     <row r="86" ht="14.6" customHeight="1">
       <c r="A86" s="9"/>
-      <c r="B86" s="9"/>
+      <c r="B86" s="10"/>
       <c r="C86" s="10"/>
       <c r="D86" s="10"/>
       <c r="E86" s="10"/>
@@ -11462,8 +11476,8 @@
       <c r="E89" s="8"/>
     </row>
     <row r="90" ht="14.6" customHeight="1">
-      <c r="A90" s="10"/>
-      <c r="B90" s="10"/>
+      <c r="A90" s="9"/>
+      <c r="B90" s="9"/>
       <c r="C90" s="10"/>
       <c r="D90" s="10"/>
       <c r="E90" s="10"/>
@@ -11476,8 +11490,8 @@
       <c r="E91" s="8"/>
     </row>
     <row r="92" ht="14.6" customHeight="1">
-      <c r="A92" s="9"/>
-      <c r="B92" s="9"/>
+      <c r="A92" s="10"/>
+      <c r="B92" s="10"/>
       <c r="C92" s="10"/>
       <c r="D92" s="10"/>
       <c r="E92" s="10"/>
@@ -11490,8 +11504,8 @@
       <c r="E93" s="8"/>
     </row>
     <row r="94" ht="14.6" customHeight="1">
-      <c r="A94" s="10"/>
-      <c r="B94" s="10"/>
+      <c r="A94" s="9"/>
+      <c r="B94" s="9"/>
       <c r="C94" s="10"/>
       <c r="D94" s="10"/>
       <c r="E94" s="10"/>
@@ -11504,8 +11518,8 @@
       <c r="E95" s="8"/>
     </row>
     <row r="96" ht="14.6" customHeight="1">
-      <c r="A96" s="9"/>
-      <c r="B96" s="9"/>
+      <c r="A96" s="10"/>
+      <c r="B96" s="10"/>
       <c r="C96" s="10"/>
       <c r="D96" s="10"/>
       <c r="E96" s="10"/>
@@ -11525,8 +11539,8 @@
       <c r="E98" s="10"/>
     </row>
     <row r="99" ht="14.6" customHeight="1">
-      <c r="A99" s="8"/>
-      <c r="B99" s="8"/>
+      <c r="A99" s="7"/>
+      <c r="B99" s="7"/>
       <c r="C99" s="8"/>
       <c r="D99" s="8"/>
       <c r="E99" s="8"/>
@@ -11539,15 +11553,15 @@
       <c r="E100" s="10"/>
     </row>
     <row r="101" ht="14.6" customHeight="1">
-      <c r="A101" s="7"/>
-      <c r="B101" s="7"/>
+      <c r="A101" s="8"/>
+      <c r="B101" s="8"/>
       <c r="C101" s="8"/>
       <c r="D101" s="8"/>
       <c r="E101" s="8"/>
     </row>
     <row r="102" ht="14.6" customHeight="1">
-      <c r="A102" s="10"/>
-      <c r="B102" s="10"/>
+      <c r="A102" s="9"/>
+      <c r="B102" s="9"/>
       <c r="C102" s="10"/>
       <c r="D102" s="10"/>
       <c r="E102" s="10"/>
@@ -11560,8 +11574,8 @@
       <c r="E103" s="8"/>
     </row>
     <row r="104" ht="14.6" customHeight="1">
-      <c r="A104" s="9"/>
-      <c r="B104" s="9"/>
+      <c r="A104" s="10"/>
+      <c r="B104" s="10"/>
       <c r="C104" s="10"/>
       <c r="D104" s="10"/>
       <c r="E104" s="10"/>
@@ -11574,8 +11588,8 @@
       <c r="E105" s="8"/>
     </row>
     <row r="106" ht="14.6" customHeight="1">
-      <c r="A106" s="10"/>
-      <c r="B106" s="10"/>
+      <c r="A106" s="9"/>
+      <c r="B106" s="9"/>
       <c r="C106" s="10"/>
       <c r="D106" s="10"/>
       <c r="E106" s="10"/>
@@ -11588,15 +11602,15 @@
       <c r="E107" s="8"/>
     </row>
     <row r="108" ht="14.6" customHeight="1">
-      <c r="A108" s="9"/>
-      <c r="B108" s="9"/>
+      <c r="A108" s="10"/>
+      <c r="B108" s="10"/>
       <c r="C108" s="10"/>
       <c r="D108" s="10"/>
       <c r="E108" s="10"/>
     </row>
     <row r="109" ht="14.6" customHeight="1">
-      <c r="A109" s="8"/>
-      <c r="B109" s="8"/>
+      <c r="A109" s="7"/>
+      <c r="B109" s="7"/>
       <c r="C109" s="8"/>
       <c r="D109" s="8"/>
       <c r="E109" s="8"/>
@@ -11623,15 +11637,15 @@
       <c r="E112" s="10"/>
     </row>
     <row r="113" ht="14.6" customHeight="1">
-      <c r="A113" s="7"/>
-      <c r="B113" s="7"/>
+      <c r="A113" s="8"/>
+      <c r="B113" s="8"/>
       <c r="C113" s="8"/>
       <c r="D113" s="8"/>
       <c r="E113" s="8"/>
     </row>
     <row r="114" ht="14.6" customHeight="1">
-      <c r="A114" s="10"/>
-      <c r="B114" s="10"/>
+      <c r="A114" s="9"/>
+      <c r="B114" s="9"/>
       <c r="C114" s="10"/>
       <c r="D114" s="10"/>
       <c r="E114" s="10"/>
@@ -11644,35 +11658,35 @@
       <c r="E115" s="8"/>
     </row>
     <row r="116" ht="14.6" customHeight="1">
-      <c r="A116" s="9"/>
-      <c r="B116" s="9"/>
+      <c r="A116" s="10"/>
+      <c r="B116" s="10"/>
       <c r="C116" s="10"/>
       <c r="D116" s="10"/>
       <c r="E116" s="10"/>
     </row>
     <row r="117" ht="14.6" customHeight="1">
-      <c r="A117" s="8"/>
-      <c r="B117" s="8"/>
+      <c r="A117" s="7"/>
+      <c r="B117" s="7"/>
       <c r="C117" s="8"/>
       <c r="D117" s="8"/>
       <c r="E117" s="8"/>
     </row>
     <row r="118" ht="14.6" customHeight="1">
-      <c r="A118" s="10"/>
-      <c r="B118" s="10"/>
+      <c r="A118" s="9"/>
+      <c r="B118" s="9"/>
       <c r="C118" s="10"/>
       <c r="D118" s="10"/>
       <c r="E118" s="10"/>
     </row>
     <row r="119" ht="14.6" customHeight="1">
-      <c r="A119" s="7"/>
+      <c r="A119" s="8"/>
       <c r="B119" s="8"/>
       <c r="C119" s="8"/>
       <c r="D119" s="8"/>
       <c r="E119" s="8"/>
     </row>
     <row r="120" ht="14.6" customHeight="1">
-      <c r="A120" s="9"/>
+      <c r="A120" s="10"/>
       <c r="B120" s="10"/>
       <c r="C120" s="10"/>
       <c r="D120" s="10"/>
@@ -11680,13 +11694,13 @@
     </row>
     <row r="121" ht="14.6" customHeight="1">
       <c r="A121" s="7"/>
-      <c r="B121" s="7"/>
+      <c r="B121" s="8"/>
       <c r="C121" s="8"/>
       <c r="D121" s="8"/>
       <c r="E121" s="8"/>
     </row>
     <row r="122" ht="14.6" customHeight="1">
-      <c r="A122" s="10"/>
+      <c r="A122" s="9"/>
       <c r="B122" s="10"/>
       <c r="C122" s="10"/>
       <c r="D122" s="10"/>
@@ -11707,8 +11721,8 @@
       <c r="E124" s="10"/>
     </row>
     <row r="125" ht="14.6" customHeight="1">
-      <c r="A125" s="8"/>
-      <c r="B125" s="8"/>
+      <c r="A125" s="7"/>
+      <c r="B125" s="7"/>
       <c r="C125" s="8"/>
       <c r="D125" s="8"/>
       <c r="E125" s="8"/>
@@ -11728,15 +11742,15 @@
       <c r="E127" s="8"/>
     </row>
     <row r="128" ht="14.6" customHeight="1">
-      <c r="A128" s="9"/>
-      <c r="B128" s="9"/>
+      <c r="A128" s="10"/>
+      <c r="B128" s="10"/>
       <c r="C128" s="10"/>
       <c r="D128" s="10"/>
       <c r="E128" s="10"/>
     </row>
     <row r="129" ht="14.6" customHeight="1">
-      <c r="A129" s="7"/>
-      <c r="B129" s="7"/>
+      <c r="A129" s="8"/>
+      <c r="B129" s="8"/>
       <c r="C129" s="8"/>
       <c r="D129" s="8"/>
       <c r="E129" s="8"/>
@@ -11784,8 +11798,8 @@
       <c r="E135" s="8"/>
     </row>
     <row r="136" ht="14.6" customHeight="1">
-      <c r="A136" s="10"/>
-      <c r="B136" s="10"/>
+      <c r="A136" s="9"/>
+      <c r="B136" s="9"/>
       <c r="C136" s="10"/>
       <c r="D136" s="10"/>
       <c r="E136" s="10"/>
@@ -11798,8 +11812,8 @@
       <c r="E137" s="8"/>
     </row>
     <row r="138" ht="14.6" customHeight="1">
-      <c r="A138" s="9"/>
-      <c r="B138" s="9"/>
+      <c r="A138" s="10"/>
+      <c r="B138" s="10"/>
       <c r="C138" s="10"/>
       <c r="D138" s="10"/>
       <c r="E138" s="10"/>
@@ -11819,8 +11833,8 @@
       <c r="E140" s="10"/>
     </row>
     <row r="141" ht="14.6" customHeight="1">
-      <c r="A141" s="8"/>
-      <c r="B141" s="8"/>
+      <c r="A141" s="7"/>
+      <c r="B141" s="7"/>
       <c r="C141" s="8"/>
       <c r="D141" s="8"/>
       <c r="E141" s="8"/>
@@ -11833,8 +11847,8 @@
       <c r="E142" s="10"/>
     </row>
     <row r="143" ht="14.6" customHeight="1">
-      <c r="A143" s="7"/>
-      <c r="B143" s="7"/>
+      <c r="A143" s="8"/>
+      <c r="B143" s="8"/>
       <c r="C143" s="8"/>
       <c r="D143" s="8"/>
       <c r="E143" s="8"/>
@@ -11875,8 +11889,8 @@
       <c r="E148" s="10"/>
     </row>
     <row r="149" ht="14.6" customHeight="1">
-      <c r="A149" s="8"/>
-      <c r="B149" s="8"/>
+      <c r="A149" s="7"/>
+      <c r="B149" s="7"/>
       <c r="C149" s="8"/>
       <c r="D149" s="8"/>
       <c r="E149" s="8"/>
@@ -11889,8 +11903,8 @@
       <c r="E150" s="10"/>
     </row>
     <row r="151" ht="14.6" customHeight="1">
-      <c r="A151" s="7"/>
-      <c r="B151" s="7"/>
+      <c r="A151" s="8"/>
+      <c r="B151" s="8"/>
       <c r="C151" s="8"/>
       <c r="D151" s="8"/>
       <c r="E151" s="8"/>
@@ -11903,8 +11917,8 @@
       <c r="E152" s="10"/>
     </row>
     <row r="153" ht="14.6" customHeight="1">
-      <c r="A153" s="8"/>
-      <c r="B153" s="8"/>
+      <c r="A153" s="7"/>
+      <c r="B153" s="7"/>
       <c r="C153" s="8"/>
       <c r="D153" s="8"/>
       <c r="E153" s="8"/>
@@ -11917,15 +11931,15 @@
       <c r="E154" s="10"/>
     </row>
     <row r="155" ht="14.6" customHeight="1">
-      <c r="A155" s="7"/>
-      <c r="B155" s="7"/>
+      <c r="A155" s="8"/>
+      <c r="B155" s="8"/>
       <c r="C155" s="8"/>
       <c r="D155" s="8"/>
       <c r="E155" s="8"/>
     </row>
     <row r="156" ht="14.6" customHeight="1">
-      <c r="A156" s="10"/>
-      <c r="B156" s="10"/>
+      <c r="A156" s="9"/>
+      <c r="B156" s="9"/>
       <c r="C156" s="10"/>
       <c r="D156" s="10"/>
       <c r="E156" s="10"/>
@@ -11938,15 +11952,15 @@
       <c r="E157" s="8"/>
     </row>
     <row r="158" ht="14.6" customHeight="1">
-      <c r="A158" s="9"/>
-      <c r="B158" s="9"/>
+      <c r="A158" s="10"/>
+      <c r="B158" s="10"/>
       <c r="C158" s="10"/>
       <c r="D158" s="10"/>
       <c r="E158" s="10"/>
     </row>
     <row r="159" ht="14.6" customHeight="1">
-      <c r="A159" s="8"/>
-      <c r="B159" s="8"/>
+      <c r="A159" s="7"/>
+      <c r="B159" s="7"/>
       <c r="C159" s="8"/>
       <c r="D159" s="8"/>
       <c r="E159" s="8"/>
@@ -11959,15 +11973,15 @@
       <c r="E160" s="10"/>
     </row>
     <row r="161" ht="14.6" customHeight="1">
-      <c r="A161" s="7"/>
-      <c r="B161" s="7"/>
+      <c r="A161" s="8"/>
+      <c r="B161" s="8"/>
       <c r="C161" s="8"/>
       <c r="D161" s="8"/>
       <c r="E161" s="8"/>
     </row>
     <row r="162" ht="14.6" customHeight="1">
-      <c r="A162" s="10"/>
-      <c r="B162" s="10"/>
+      <c r="A162" s="9"/>
+      <c r="B162" s="9"/>
       <c r="C162" s="10"/>
       <c r="D162" s="10"/>
       <c r="E162" s="10"/>
@@ -11980,11 +11994,25 @@
       <c r="E163" s="8"/>
     </row>
     <row r="164" ht="14.6" customHeight="1">
-      <c r="A164" s="9"/>
-      <c r="B164" s="9"/>
+      <c r="A164" s="10"/>
+      <c r="B164" s="10"/>
       <c r="C164" s="10"/>
       <c r="D164" s="10"/>
       <c r="E164" s="10"/>
+    </row>
+    <row r="165" ht="14.6" customHeight="1">
+      <c r="A165" s="7"/>
+      <c r="B165" s="7"/>
+      <c r="C165" s="8"/>
+      <c r="D165" s="8"/>
+      <c r="E165" s="8"/>
+    </row>
+    <row r="166" ht="14.6" customHeight="1">
+      <c r="A166" s="9"/>
+      <c r="B166" s="9"/>
+      <c r="C166" s="10"/>
+      <c r="D166" s="10"/>
+      <c r="E166" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -12035,7 +12063,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -12046,7 +12074,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -12075,7 +12103,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s" s="9">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -12137,10 +12165,10 @@
     </row>
     <row r="14" ht="15.35" customHeight="1">
       <c r="A14" t="s" s="29">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B14" t="s" s="29">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -12148,10 +12176,10 @@
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" t="s" s="21">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B15" t="s" s="7">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -12166,10 +12194,10 @@
     </row>
     <row r="17" ht="15.35" customHeight="1">
       <c r="A17" t="s" s="29">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B17" t="s" s="29">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -12209,7 +12237,7 @@
         <v>62</v>
       </c>
       <c r="B21" t="s" s="22">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -12235,10 +12263,10 @@
     </row>
     <row r="24" ht="15.35" customHeight="1">
       <c r="A24" t="s" s="21">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B24" t="s" s="22">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -12246,10 +12274,10 @@
     </row>
     <row r="25" ht="15.35" customHeight="1">
       <c r="A25" t="s" s="21">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B25" t="s" s="22">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
@@ -12257,10 +12285,10 @@
     </row>
     <row r="26" ht="15.35" customHeight="1">
       <c r="A26" t="s" s="21">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B26" t="s" s="22">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
@@ -12275,10 +12303,10 @@
     </row>
     <row r="28" ht="15.35" customHeight="1">
       <c r="A28" t="s" s="29">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B28" t="s" s="29">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -12286,10 +12314,10 @@
     </row>
     <row r="29" ht="15.35" customHeight="1">
       <c r="A29" t="s" s="29">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B29" t="s" s="29">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -12297,10 +12325,10 @@
     </row>
     <row r="30" ht="15.35" customHeight="1">
       <c r="A30" t="s" s="29">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B30" t="s" s="29">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -12315,10 +12343,10 @@
     </row>
     <row r="32" ht="15.35" customHeight="1">
       <c r="A32" t="s" s="46">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B32" t="s" s="25">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
@@ -12326,10 +12354,10 @@
     </row>
     <row r="33" ht="14.6" customHeight="1">
       <c r="A33" t="s" s="13">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B33" t="s" s="47">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -12337,7 +12365,7 @@
     </row>
     <row r="34" ht="14.6" customHeight="1">
       <c r="A34" t="s" s="24">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B34" t="s" s="25">
         <v>59</v>
@@ -12384,10 +12412,10 @@
     </row>
     <row r="39" ht="14.6" customHeight="1">
       <c r="A39" t="s" s="29">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B39" t="s" s="29">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
@@ -12402,7 +12430,7 @@
     </row>
     <row r="41" ht="14.6" customHeight="1">
       <c r="A41" t="s" s="52">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B41" s="53">
         <v>0</v>
@@ -12413,7 +12441,7 @@
     </row>
     <row r="42" ht="14.6" customHeight="1">
       <c r="A42" t="s" s="54">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B42" s="55">
         <v>1</v>
@@ -12424,7 +12452,7 @@
     </row>
     <row r="43" ht="14.6" customHeight="1">
       <c r="A43" t="s" s="56">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B43" s="57">
         <v>2</v>
@@ -12435,7 +12463,7 @@
     </row>
     <row r="44" ht="14.6" customHeight="1">
       <c r="A44" t="s" s="58">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B44" s="59">
         <v>3</v>
@@ -12446,7 +12474,7 @@
     </row>
     <row r="45" ht="14.6" customHeight="1">
       <c r="A45" t="s" s="60">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B45" s="61">
         <v>4</v>
@@ -12457,7 +12485,7 @@
     </row>
     <row r="46" ht="14.6" customHeight="1">
       <c r="A46" t="s" s="58">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B46" s="59">
         <v>5</v>
@@ -12468,7 +12496,7 @@
     </row>
     <row r="47" ht="14.6" customHeight="1">
       <c r="A47" t="s" s="62">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B47" s="63">
         <v>6</v>
@@ -13492,7 +13520,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -13503,7 +13531,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -13532,7 +13560,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s" s="9">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -13594,10 +13622,10 @@
     </row>
     <row r="14" ht="15.35" customHeight="1">
       <c r="A14" t="s" s="29">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B14" t="s" s="29">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -13605,10 +13633,10 @@
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" t="s" s="21">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B15" t="s" s="7">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -13623,7 +13651,7 @@
     </row>
     <row r="17" ht="15.35" customHeight="1">
       <c r="A17" t="s" s="52">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B17" s="53">
         <v>0</v>
@@ -13634,7 +13662,7 @@
     </row>
     <row r="18" ht="15.35" customHeight="1">
       <c r="A18" t="s" s="54">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B18" s="55">
         <v>1</v>
@@ -13645,7 +13673,7 @@
     </row>
     <row r="19" ht="15.35" customHeight="1">
       <c r="A19" t="s" s="54">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B19" s="57">
         <v>2</v>
@@ -13656,7 +13684,7 @@
     </row>
     <row r="20" ht="15.35" customHeight="1">
       <c r="A20" t="s" s="56">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B20" s="65">
         <v>3</v>
@@ -13667,7 +13695,7 @@
     </row>
     <row r="21" ht="15.35" customHeight="1">
       <c r="A21" t="s" s="58">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B21" s="61">
         <v>4</v>
@@ -13678,7 +13706,7 @@
     </row>
     <row r="22" ht="15.35" customHeight="1">
       <c r="A22" t="s" s="60">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B22" s="59">
         <v>5</v>
@@ -13689,7 +13717,7 @@
     </row>
     <row r="23" ht="15.35" customHeight="1">
       <c r="A23" t="s" s="58">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B23" s="63">
         <v>6</v>
@@ -13700,10 +13728,10 @@
     </row>
     <row r="24" ht="15.35" customHeight="1">
       <c r="A24" t="s" s="62">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B24" t="s" s="22">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -13754,7 +13782,7 @@
         <v>77</v>
       </c>
       <c r="B29" t="s" s="29">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -13769,10 +13797,10 @@
     </row>
     <row r="31" ht="15.35" customHeight="1">
       <c r="A31" t="s" s="21">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B31" t="s" s="22">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
@@ -13783,7 +13811,7 @@
         <v>52</v>
       </c>
       <c r="B32" t="s" s="29">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
@@ -13791,10 +13819,10 @@
     </row>
     <row r="33" ht="15.35" customHeight="1">
       <c r="A33" t="s" s="29">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B33" t="s" s="29">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
@@ -13802,10 +13830,10 @@
     </row>
     <row r="34" ht="15.35" customHeight="1">
       <c r="A34" t="s" s="29">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B34" t="s" s="29">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
@@ -13813,10 +13841,10 @@
     </row>
     <row r="35" ht="15.35" customHeight="1">
       <c r="A35" t="s" s="43">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B35" t="s" s="43">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -13824,10 +13852,10 @@
     </row>
     <row r="36" ht="15.35" customHeight="1">
       <c r="A36" t="s" s="29">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B36" t="s" s="29">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
@@ -13842,10 +13870,10 @@
     </row>
     <row r="38" ht="15.35" customHeight="1">
       <c r="A38" t="s" s="66">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B38" t="s" s="67">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
@@ -13853,10 +13881,10 @@
     </row>
     <row r="39" ht="14.6" customHeight="1">
       <c r="A39" t="s" s="68">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B39" t="s" s="47">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
@@ -13864,10 +13892,10 @@
     </row>
     <row r="40" ht="14.6" customHeight="1">
       <c r="A40" t="s" s="69">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B40" t="s" s="67">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
@@ -13875,10 +13903,10 @@
     </row>
     <row r="41" ht="14.6" customHeight="1">
       <c r="A41" t="s" s="70">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B41" t="s" s="71">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
@@ -13886,10 +13914,10 @@
     </row>
     <row r="42" ht="14.6" customHeight="1">
       <c r="A42" t="s" s="72">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B42" t="s" s="73">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
@@ -13897,10 +13925,10 @@
     </row>
     <row r="43" ht="14.6" customHeight="1">
       <c r="A43" t="s" s="29">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B43" t="s" s="29">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
@@ -13908,10 +13936,10 @@
     </row>
     <row r="44" ht="14.6" customHeight="1">
       <c r="A44" t="s" s="29">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B44" t="s" s="29">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
@@ -13919,10 +13947,10 @@
     </row>
     <row r="45" ht="14.6" customHeight="1">
       <c r="A45" t="s" s="29">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B45" t="s" s="29">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
@@ -13930,10 +13958,10 @@
     </row>
     <row r="46" ht="14.6" customHeight="1">
       <c r="A46" t="s" s="69">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B46" t="s" s="67">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
@@ -13941,10 +13969,10 @@
     </row>
     <row r="47" ht="14.6" customHeight="1">
       <c r="A47" t="s" s="74">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B47" t="s" s="75">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C47" s="76"/>
       <c r="D47" s="76"/>
@@ -13952,10 +13980,10 @@
     </row>
     <row r="48" ht="14.6" customHeight="1">
       <c r="A48" t="s" s="78">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B48" t="s" s="79">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C48" s="80"/>
       <c r="D48" s="80"/>
@@ -15011,7 +15039,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -15022,7 +15050,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -15051,7 +15079,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s" s="9">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -15095,7 +15123,7 @@
     </row>
     <row r="12" ht="14.6" customHeight="1">
       <c r="A12" t="s" s="7">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B12" t="s" s="7">
         <v>29</v>
@@ -15113,7 +15141,7 @@
     </row>
     <row r="14" ht="15.35" customHeight="1">
       <c r="A14" t="s" s="52">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B14" s="53">
         <v>0</v>
@@ -15124,7 +15152,7 @@
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" t="s" s="54">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B15" s="57">
         <v>1</v>
@@ -15135,7 +15163,7 @@
     </row>
     <row r="16" ht="15.35" customHeight="1">
       <c r="A16" t="s" s="56">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B16" s="65">
         <v>2</v>
@@ -15146,7 +15174,7 @@
     </row>
     <row r="17" ht="15.35" customHeight="1">
       <c r="A17" t="s" s="58">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B17" s="59">
         <v>3</v>
@@ -15157,7 +15185,7 @@
     </row>
     <row r="18" ht="15.35" customHeight="1">
       <c r="A18" t="s" s="60">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B18" s="61">
         <v>4</v>
@@ -15168,7 +15196,7 @@
     </row>
     <row r="19" ht="15.35" customHeight="1">
       <c r="A19" t="s" s="58">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B19" s="59">
         <v>5</v>
@@ -15179,7 +15207,7 @@
     </row>
     <row r="20" ht="15.35" customHeight="1">
       <c r="A20" t="s" s="62">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B20" s="63">
         <v>6</v>
@@ -15197,10 +15225,10 @@
     </row>
     <row r="22" ht="15.35" customHeight="1">
       <c r="A22" t="s" s="9">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B22" t="s" s="29">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>

</xml_diff>

<commit_message>
DIR 2 Feedback points
updated with din check in query instead of name and added cin check for attachment
</commit_message>
<xml_diff>
--- a/DataExtraction/Input/Config.xlsx
+++ b/DataExtraction/Input/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="247">
   <si>
     <t>Key</t>
   </si>
@@ -294,6 +294,24 @@
   </si>
   <si>
     <t>din</t>
+  </si>
+  <si>
+    <t>pan_column_name_in_db</t>
+  </si>
+  <si>
+    <t>pan</t>
+  </si>
+  <si>
+    <t>phone_number_column_name_in_db</t>
+  </si>
+  <si>
+    <t>phone_number</t>
+  </si>
+  <si>
+    <t>email_column_name_in_db</t>
+  </si>
+  <si>
+    <t>email</t>
   </si>
   <si>
     <t>designation_after_event_column_name_in_db</t>
@@ -697,9 +715,6 @@
   </si>
   <si>
     <t>pan_column_name</t>
-  </si>
-  <si>
-    <t>pan</t>
   </si>
   <si>
     <t>financial_year_column_name</t>
@@ -4139,7 +4154,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -4150,7 +4165,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -4179,7 +4194,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s" s="9">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -4234,7 +4249,7 @@
     </row>
     <row r="13" ht="14.6" customHeight="1">
       <c r="A13" t="s" s="7">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="B13" t="s" s="7">
         <v>29</v>
@@ -4252,7 +4267,7 @@
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" t="s" s="52">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B15" s="94">
         <v>0</v>
@@ -4263,7 +4278,7 @@
     </row>
     <row r="16" ht="15.35" customHeight="1">
       <c r="A16" t="s" s="95">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B16" s="59">
         <v>2</v>
@@ -4274,7 +4289,7 @@
     </row>
     <row r="17" ht="15.35" customHeight="1">
       <c r="A17" t="s" s="96">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B17" s="59">
         <v>3</v>
@@ -4285,7 +4300,7 @@
     </row>
     <row r="18" ht="15.35" customHeight="1">
       <c r="A18" t="s" s="58">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B18" s="61">
         <v>4</v>
@@ -4296,7 +4311,7 @@
     </row>
     <row r="19" ht="15.35" customHeight="1">
       <c r="A19" t="s" s="60">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="B19" s="63">
         <v>6</v>
@@ -4307,7 +4322,7 @@
     </row>
     <row r="20" ht="15.35" customHeight="1">
       <c r="A20" t="s" s="58">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="B20" s="59">
         <v>7</v>
@@ -4318,7 +4333,7 @@
     </row>
     <row r="21" ht="15.35" customHeight="1">
       <c r="A21" t="s" s="62">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B21" s="63">
         <v>8</v>
@@ -4336,10 +4351,10 @@
     </row>
     <row r="23" ht="15.35" customHeight="1">
       <c r="A23" t="s" s="9">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="B23" t="s" s="29">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -4347,10 +4362,10 @@
     </row>
     <row r="24" ht="15.35" customHeight="1">
       <c r="A24" t="s" s="29">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="B24" t="s" s="29">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -4376,10 +4391,10 @@
     </row>
     <row r="27" ht="15.35" customHeight="1">
       <c r="A27" t="s" s="29">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="B27" t="s" s="29">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -4394,10 +4409,10 @@
     </row>
     <row r="29" ht="15.35" customHeight="1">
       <c r="A29" t="s" s="29">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="B29" t="s" s="29">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -4405,10 +4420,10 @@
     </row>
     <row r="30" ht="15.35" customHeight="1">
       <c r="A30" t="s" s="29">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="B30" t="s" s="29">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -4423,7 +4438,7 @@
     </row>
     <row r="32" ht="15.35" customHeight="1">
       <c r="A32" t="s" s="29">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="B32" t="s" s="29">
         <v>90</v>
@@ -4434,10 +4449,10 @@
     </row>
     <row r="33" ht="15.35" customHeight="1">
       <c r="A33" t="s" s="43">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="B33" t="s" s="43">
-        <v>218</v>
+        <v>92</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
@@ -4452,10 +4467,10 @@
     </row>
     <row r="35" ht="15.35" customHeight="1">
       <c r="A35" t="s" s="97">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="B35" t="s" s="97">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -4463,10 +4478,10 @@
     </row>
     <row r="36" ht="14.6" customHeight="1">
       <c r="A36" t="s" s="70">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="B36" t="s" s="71">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
@@ -4481,10 +4496,10 @@
     </row>
     <row r="38" ht="14.6" customHeight="1">
       <c r="A38" t="s" s="26">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="B38" t="s" s="73">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
@@ -4492,10 +4507,10 @@
     </row>
     <row r="39" ht="14.6" customHeight="1">
       <c r="A39" t="s" s="29">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="B39" t="s" s="29">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
@@ -4510,10 +4525,10 @@
     </row>
     <row r="41" ht="14.6" customHeight="1">
       <c r="A41" t="s" s="29">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="B41" t="s" s="29">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
@@ -4521,10 +4536,10 @@
     </row>
     <row r="42" ht="14.6" customHeight="1">
       <c r="A42" t="s" s="98">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="B42" t="s" s="98">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
@@ -4539,10 +4554,10 @@
     </row>
     <row r="44" ht="14.6" customHeight="1">
       <c r="A44" t="s" s="29">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="B44" t="s" s="29">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
@@ -4550,10 +4565,10 @@
     </row>
     <row r="45" ht="14.6" customHeight="1">
       <c r="A45" t="s" s="69">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="B45" t="s" s="67">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
@@ -4561,10 +4576,10 @@
     </row>
     <row r="46" ht="14.6" customHeight="1">
       <c r="A46" t="s" s="99">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="B46" t="s" s="100">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="C46" s="101"/>
       <c r="D46" s="101"/>
@@ -4579,10 +4594,10 @@
     </row>
     <row r="48" ht="14.6" customHeight="1">
       <c r="A48" t="s" s="9">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="B48" t="s" s="9">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
@@ -4590,10 +4605,10 @@
     </row>
     <row r="49" ht="14.6" customHeight="1">
       <c r="A49" t="s" s="7">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="B49" t="s" s="7">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
@@ -4601,10 +4616,10 @@
     </row>
     <row r="50" ht="14.6" customHeight="1">
       <c r="A50" t="s" s="9">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="B50" t="s" s="9">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
@@ -5622,7 +5637,7 @@
   <sheetData>
     <row r="1" ht="15.55" customHeight="1">
       <c r="A1" t="s" s="104">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="B1" s="104"/>
       <c r="C1" s="104"/>
@@ -10724,7 +10739,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E166"/>
+  <dimension ref="A1:E169"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -10855,75 +10870,75 @@
     </row>
     <row r="12" ht="26.6" customHeight="1">
       <c r="A12" t="s" s="9">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="B12" t="s" s="9">
-        <v>31</v>
+        <v>94</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
     </row>
-    <row r="13" ht="15.35" customHeight="1">
-      <c r="A13" t="s" s="21">
-        <v>93</v>
-      </c>
-      <c r="B13" t="s" s="36">
-        <v>94</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" ht="14.6" customHeight="1">
-      <c r="A14" t="s" s="7">
+    <row r="13" ht="26.6" customHeight="1">
+      <c r="A13" t="s" s="9">
         <v>95</v>
       </c>
-      <c r="B14" t="s" s="37">
+      <c r="B13" t="s" s="9">
         <v>96</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" ht="26.6" customHeight="1">
+      <c r="A14" t="s" s="9">
+        <v>97</v>
+      </c>
+      <c r="B14" t="s" s="9">
+        <v>98</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
     </row>
-    <row r="15" ht="14.6" customHeight="1">
-      <c r="A15" t="s" s="7">
-        <v>97</v>
-      </c>
-      <c r="B15" t="s" s="38">
-        <v>98</v>
+    <row r="15" ht="26.6" customHeight="1">
+      <c r="A15" t="s" s="9">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s" s="9">
+        <v>31</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
     </row>
     <row r="16" ht="15.35" customHeight="1">
-      <c r="A16" t="s" s="23">
+      <c r="A16" t="s" s="21">
         <v>99</v>
       </c>
-      <c r="B16" t="s" s="9">
+      <c r="B16" t="s" s="36">
         <v>100</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
     </row>
     <row r="17" ht="14.6" customHeight="1">
-      <c r="A17" t="s" s="22">
+      <c r="A17" t="s" s="7">
         <v>101</v>
       </c>
-      <c r="B17" t="s" s="29">
+      <c r="B17" t="s" s="37">
         <v>102</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
     </row>
     <row r="18" ht="14.6" customHeight="1">
-      <c r="A18" t="s" s="13">
+      <c r="A18" t="s" s="7">
         <v>103</v>
       </c>
-      <c r="B18" t="s" s="39">
+      <c r="B18" t="s" s="38">
         <v>104</v>
       </c>
       <c r="C18" s="10"/>
@@ -10931,1088 +10946,1121 @@
       <c r="E18" s="10"/>
     </row>
     <row r="19" ht="15.35" customHeight="1">
-      <c r="A19" t="s" s="9">
+      <c r="A19" t="s" s="23">
         <v>105</v>
       </c>
-      <c r="B19" t="s" s="23">
+      <c r="B19" t="s" s="9">
         <v>106</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" ht="15.35" customHeight="1">
-      <c r="A20" t="s" s="7">
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" ht="14.6" customHeight="1">
+      <c r="A20" t="s" s="22">
         <v>107</v>
       </c>
-      <c r="B20" t="s" s="21">
-        <v>96</v>
-      </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-    </row>
-    <row r="21" ht="15.35" customHeight="1">
-      <c r="A21" t="s" s="7">
+      <c r="B20" t="s" s="29">
         <v>108</v>
       </c>
-      <c r="B21" t="s" s="21">
-        <v>98</v>
-      </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" ht="14.6" customHeight="1">
+      <c r="A21" t="s" s="13">
+        <v>109</v>
+      </c>
+      <c r="B21" t="s" s="39">
+        <v>110</v>
+      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
     </row>
     <row r="22" ht="15.35" customHeight="1">
       <c r="A22" t="s" s="9">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B22" t="s" s="23">
-        <v>100</v>
-      </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-    </row>
-    <row r="23" ht="14.6" customHeight="1">
-      <c r="A23" t="s" s="24">
-        <v>110</v>
-      </c>
-      <c r="B23" t="s" s="40">
-        <v>111</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" ht="14.6" customHeight="1">
-      <c r="A24" t="s" s="26">
         <v>112</v>
       </c>
-      <c r="B24" t="s" s="41">
-        <v>92</v>
-      </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" ht="15.35" customHeight="1">
+      <c r="A23" t="s" s="7">
+        <v>113</v>
+      </c>
+      <c r="B23" t="s" s="21">
+        <v>102</v>
+      </c>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" ht="15.35" customHeight="1">
+      <c r="A24" t="s" s="7">
+        <v>114</v>
+      </c>
+      <c r="B24" t="s" s="21">
+        <v>104</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
     </row>
     <row r="25" ht="15.35" customHeight="1">
-      <c r="A25" t="s" s="21">
-        <v>113</v>
-      </c>
-      <c r="B25" t="s" s="21">
-        <v>114</v>
-      </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" ht="15.35" customHeight="1">
-      <c r="A26" t="s" s="42">
+      <c r="A25" t="s" s="9">
         <v>115</v>
       </c>
-      <c r="B26" t="s" s="23">
+      <c r="B25" t="s" s="23">
+        <v>106</v>
+      </c>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+    </row>
+    <row r="26" ht="14.6" customHeight="1">
+      <c r="A26" t="s" s="24">
         <v>116</v>
       </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
+      <c r="B26" t="s" s="40">
+        <v>117</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
     </row>
     <row r="27" ht="14.6" customHeight="1">
-      <c r="A27" t="s" s="43">
-        <v>117</v>
-      </c>
-      <c r="B27" t="s" s="43">
+      <c r="A27" t="s" s="26">
         <v>118</v>
       </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-    </row>
-    <row r="28" ht="14.6" customHeight="1">
-      <c r="A28" t="s" s="44">
+      <c r="B27" t="s" s="41">
+        <v>98</v>
+      </c>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+    </row>
+    <row r="28" ht="15.35" customHeight="1">
+      <c r="A28" t="s" s="21">
         <v>119</v>
       </c>
-      <c r="B28" t="s" s="44">
+      <c r="B28" t="s" s="21">
         <v>120</v>
       </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-    </row>
-    <row r="29" ht="14.6" customHeight="1">
-      <c r="A29" t="s" s="44">
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" ht="15.35" customHeight="1">
+      <c r="A29" t="s" s="42">
         <v>121</v>
       </c>
-      <c r="B29" t="s" s="43">
+      <c r="B29" t="s" s="23">
         <v>122</v>
       </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
     </row>
     <row r="30" ht="14.6" customHeight="1">
-      <c r="A30" t="s" s="9">
+      <c r="A30" t="s" s="43">
         <v>123</v>
       </c>
-      <c r="B30" t="s" s="9">
+      <c r="B30" t="s" s="43">
         <v>124</v>
       </c>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
     </row>
     <row r="31" ht="14.6" customHeight="1">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
+      <c r="A31" t="s" s="44">
+        <v>125</v>
+      </c>
+      <c r="B31" t="s" s="44">
+        <v>126</v>
+      </c>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
     </row>
     <row r="32" ht="14.6" customHeight="1">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
+      <c r="A32" t="s" s="44">
+        <v>127</v>
+      </c>
+      <c r="B32" t="s" s="43">
+        <v>128</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
     </row>
     <row r="33" ht="14.6" customHeight="1">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
+      <c r="A33" t="s" s="9">
+        <v>129</v>
+      </c>
+      <c r="B33" t="s" s="9">
+        <v>130</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
     </row>
     <row r="34" ht="14.6" customHeight="1">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
     </row>
     <row r="35" ht="14.6" customHeight="1">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
     </row>
     <row r="36" ht="14.6" customHeight="1">
-      <c r="A36" s="9"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
     </row>
     <row r="37" ht="14.6" customHeight="1">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
     </row>
     <row r="38" ht="14.6" customHeight="1">
-      <c r="A38" s="9"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
     </row>
     <row r="39" ht="14.6" customHeight="1">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
     </row>
     <row r="40" ht="14.6" customHeight="1">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
     </row>
     <row r="41" ht="14.6" customHeight="1">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
     </row>
     <row r="42" ht="14.6" customHeight="1">
-      <c r="A42" s="10"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
     </row>
     <row r="43" ht="14.6" customHeight="1">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
     </row>
     <row r="44" ht="14.6" customHeight="1">
-      <c r="A44" s="9"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
     </row>
     <row r="45" ht="14.6" customHeight="1">
-      <c r="A45" s="8"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
+      <c r="A45" s="10"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
     </row>
     <row r="46" ht="14.6" customHeight="1">
-      <c r="A46" s="9"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
     </row>
     <row r="47" ht="14.6" customHeight="1">
-      <c r="A47" s="7"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
+      <c r="A47" s="9"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
     </row>
     <row r="48" ht="14.6" customHeight="1">
-      <c r="A48" s="10"/>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
     </row>
     <row r="49" ht="14.6" customHeight="1">
-      <c r="A49" s="8"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
     </row>
     <row r="50" ht="14.6" customHeight="1">
-      <c r="A50" s="9"/>
-      <c r="B50" s="9"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
     </row>
     <row r="51" ht="14.6" customHeight="1">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
+      <c r="A51" s="10"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
     </row>
     <row r="52" ht="14.6" customHeight="1">
-      <c r="A52" s="9"/>
-      <c r="B52" s="9"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
     </row>
     <row r="53" ht="14.6" customHeight="1">
-      <c r="A53" s="7"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
     </row>
     <row r="54" ht="14.6" customHeight="1">
-      <c r="A54" s="9"/>
-      <c r="B54" s="9"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
+      <c r="A54" s="7"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
     </row>
     <row r="55" ht="14.6" customHeight="1">
-      <c r="A55" s="8"/>
-      <c r="B55" s="8"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
     </row>
     <row r="56" ht="14.6" customHeight="1">
-      <c r="A56" s="9"/>
-      <c r="B56" s="9"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
+      <c r="A56" s="7"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
     </row>
     <row r="57" ht="14.6" customHeight="1">
-      <c r="A57" s="7"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
     </row>
     <row r="58" ht="14.6" customHeight="1">
-      <c r="A58" s="10"/>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
+      <c r="A58" s="8"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
     </row>
     <row r="59" ht="14.6" customHeight="1">
-      <c r="A59" s="7"/>
-      <c r="B59" s="7"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
+      <c r="A59" s="9"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
     </row>
     <row r="60" ht="14.6" customHeight="1">
-      <c r="A60" s="10"/>
-      <c r="B60" s="10"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="10"/>
+      <c r="A60" s="7"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
     </row>
     <row r="61" ht="14.6" customHeight="1">
-      <c r="A61" s="7"/>
-      <c r="B61" s="7"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
+      <c r="A61" s="10"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
     </row>
     <row r="62" ht="14.6" customHeight="1">
-      <c r="A62" s="9"/>
-      <c r="B62" s="10"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="10"/>
+      <c r="A62" s="7"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="8"/>
     </row>
     <row r="63" ht="14.6" customHeight="1">
-      <c r="A63" s="7"/>
-      <c r="B63" s="8"/>
-      <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8"/>
+      <c r="A63" s="10"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
     </row>
     <row r="64" ht="14.6" customHeight="1">
-      <c r="A64" s="9"/>
-      <c r="B64" s="10"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
+      <c r="A64" s="7"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
     </row>
     <row r="65" ht="14.6" customHeight="1">
-      <c r="A65" s="8"/>
-      <c r="B65" s="8"/>
-      <c r="C65" s="8"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="8"/>
+      <c r="A65" s="9"/>
+      <c r="B65" s="10"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
     </row>
     <row r="66" ht="14.6" customHeight="1">
-      <c r="A66" s="10"/>
-      <c r="B66" s="10"/>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
-      <c r="E66" s="10"/>
+      <c r="A66" s="7"/>
+      <c r="B66" s="8"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
     </row>
     <row r="67" ht="14.6" customHeight="1">
-      <c r="A67" s="7"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="8"/>
-      <c r="D67" s="8"/>
-      <c r="E67" s="8"/>
+      <c r="A67" s="9"/>
+      <c r="B67" s="10"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10"/>
     </row>
     <row r="68" ht="14.6" customHeight="1">
-      <c r="A68" s="9"/>
-      <c r="B68" s="9"/>
-      <c r="C68" s="10"/>
-      <c r="D68" s="10"/>
-      <c r="E68" s="10"/>
+      <c r="A68" s="8"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
     </row>
     <row r="69" ht="14.6" customHeight="1">
-      <c r="A69" s="7"/>
-      <c r="B69" s="7"/>
-      <c r="C69" s="8"/>
-      <c r="D69" s="8"/>
-      <c r="E69" s="8"/>
+      <c r="A69" s="10"/>
+      <c r="B69" s="10"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
     </row>
     <row r="70" ht="14.6" customHeight="1">
-      <c r="A70" s="9"/>
-      <c r="B70" s="9"/>
-      <c r="C70" s="10"/>
-      <c r="D70" s="10"/>
-      <c r="E70" s="10"/>
+      <c r="A70" s="7"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8"/>
     </row>
     <row r="71" ht="14.6" customHeight="1">
-      <c r="A71" s="7"/>
-      <c r="B71" s="7"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="8"/>
-      <c r="E71" s="8"/>
+      <c r="A71" s="9"/>
+      <c r="B71" s="9"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="10"/>
     </row>
     <row r="72" ht="14.6" customHeight="1">
-      <c r="A72" s="9"/>
-      <c r="B72" s="9"/>
-      <c r="C72" s="10"/>
-      <c r="D72" s="10"/>
-      <c r="E72" s="10"/>
+      <c r="A72" s="7"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
     </row>
     <row r="73" ht="14.6" customHeight="1">
-      <c r="A73" s="8"/>
-      <c r="B73" s="8"/>
-      <c r="C73" s="8"/>
-      <c r="D73" s="8"/>
-      <c r="E73" s="8"/>
+      <c r="A73" s="9"/>
+      <c r="B73" s="9"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10"/>
     </row>
     <row r="74" ht="14.6" customHeight="1">
-      <c r="A74" s="9"/>
-      <c r="B74" s="9"/>
-      <c r="C74" s="10"/>
-      <c r="D74" s="10"/>
-      <c r="E74" s="10"/>
+      <c r="A74" s="7"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8"/>
+      <c r="E74" s="8"/>
     </row>
     <row r="75" ht="14.6" customHeight="1">
-      <c r="A75" s="7"/>
-      <c r="B75" s="7"/>
-      <c r="C75" s="8"/>
-      <c r="D75" s="8"/>
-      <c r="E75" s="8"/>
+      <c r="A75" s="9"/>
+      <c r="B75" s="9"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="10"/>
     </row>
     <row r="76" ht="14.6" customHeight="1">
-      <c r="A76" s="9"/>
-      <c r="B76" s="9"/>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10"/>
-      <c r="E76" s="10"/>
+      <c r="A76" s="8"/>
+      <c r="B76" s="8"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="8"/>
+      <c r="E76" s="8"/>
     </row>
     <row r="77" ht="14.6" customHeight="1">
-      <c r="A77" s="7"/>
-      <c r="B77" s="7"/>
-      <c r="C77" s="8"/>
-      <c r="D77" s="8"/>
-      <c r="E77" s="8"/>
+      <c r="A77" s="9"/>
+      <c r="B77" s="9"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="10"/>
     </row>
     <row r="78" ht="14.6" customHeight="1">
-      <c r="A78" s="9"/>
-      <c r="B78" s="9"/>
-      <c r="C78" s="10"/>
-      <c r="D78" s="10"/>
-      <c r="E78" s="10"/>
+      <c r="A78" s="7"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
     </row>
     <row r="79" ht="14.6" customHeight="1">
-      <c r="A79" s="8"/>
-      <c r="B79" s="8"/>
-      <c r="C79" s="8"/>
-      <c r="D79" s="8"/>
-      <c r="E79" s="8"/>
+      <c r="A79" s="9"/>
+      <c r="B79" s="9"/>
+      <c r="C79" s="10"/>
+      <c r="D79" s="10"/>
+      <c r="E79" s="10"/>
     </row>
     <row r="80" ht="14.6" customHeight="1">
-      <c r="A80" s="9"/>
-      <c r="B80" s="9"/>
-      <c r="C80" s="10"/>
-      <c r="D80" s="10"/>
-      <c r="E80" s="10"/>
+      <c r="A80" s="7"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="8"/>
     </row>
     <row r="81" ht="14.6" customHeight="1">
-      <c r="A81" s="7"/>
-      <c r="B81" s="7"/>
-      <c r="C81" s="8"/>
-      <c r="D81" s="8"/>
-      <c r="E81" s="8"/>
+      <c r="A81" s="9"/>
+      <c r="B81" s="9"/>
+      <c r="C81" s="10"/>
+      <c r="D81" s="10"/>
+      <c r="E81" s="10"/>
     </row>
     <row r="82" ht="14.6" customHeight="1">
-      <c r="A82" s="9"/>
-      <c r="B82" s="9"/>
-      <c r="C82" s="10"/>
-      <c r="D82" s="10"/>
-      <c r="E82" s="10"/>
+      <c r="A82" s="8"/>
+      <c r="B82" s="8"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="8"/>
     </row>
     <row r="83" ht="14.6" customHeight="1">
-      <c r="A83" s="7"/>
-      <c r="B83" s="7"/>
-      <c r="C83" s="8"/>
-      <c r="D83" s="8"/>
-      <c r="E83" s="8"/>
+      <c r="A83" s="9"/>
+      <c r="B83" s="9"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="10"/>
+      <c r="E83" s="10"/>
     </row>
     <row r="84" ht="14.6" customHeight="1">
-      <c r="A84" s="9"/>
-      <c r="B84" s="9"/>
-      <c r="C84" s="10"/>
-      <c r="D84" s="10"/>
-      <c r="E84" s="10"/>
+      <c r="A84" s="7"/>
+      <c r="B84" s="7"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
+      <c r="E84" s="8"/>
     </row>
     <row r="85" ht="14.6" customHeight="1">
-      <c r="A85" s="8"/>
-      <c r="B85" s="8"/>
-      <c r="C85" s="8"/>
-      <c r="D85" s="8"/>
-      <c r="E85" s="8"/>
+      <c r="A85" s="9"/>
+      <c r="B85" s="9"/>
+      <c r="C85" s="10"/>
+      <c r="D85" s="10"/>
+      <c r="E85" s="10"/>
     </row>
     <row r="86" ht="14.6" customHeight="1">
-      <c r="A86" s="9"/>
-      <c r="B86" s="10"/>
-      <c r="C86" s="10"/>
-      <c r="D86" s="10"/>
-      <c r="E86" s="10"/>
+      <c r="A86" s="7"/>
+      <c r="B86" s="7"/>
+      <c r="C86" s="8"/>
+      <c r="D86" s="8"/>
+      <c r="E86" s="8"/>
     </row>
     <row r="87" ht="14.6" customHeight="1">
-      <c r="A87" s="7"/>
-      <c r="B87" s="7"/>
-      <c r="C87" s="8"/>
-      <c r="D87" s="8"/>
-      <c r="E87" s="8"/>
+      <c r="A87" s="9"/>
+      <c r="B87" s="9"/>
+      <c r="C87" s="10"/>
+      <c r="D87" s="10"/>
+      <c r="E87" s="10"/>
     </row>
     <row r="88" ht="14.6" customHeight="1">
-      <c r="A88" s="9"/>
-      <c r="B88" s="9"/>
-      <c r="C88" s="10"/>
-      <c r="D88" s="10"/>
-      <c r="E88" s="10"/>
+      <c r="A88" s="8"/>
+      <c r="B88" s="8"/>
+      <c r="C88" s="8"/>
+      <c r="D88" s="8"/>
+      <c r="E88" s="8"/>
     </row>
     <row r="89" ht="14.6" customHeight="1">
-      <c r="A89" s="7"/>
-      <c r="B89" s="7"/>
-      <c r="C89" s="8"/>
-      <c r="D89" s="8"/>
-      <c r="E89" s="8"/>
+      <c r="A89" s="9"/>
+      <c r="B89" s="10"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="10"/>
+      <c r="E89" s="10"/>
     </row>
     <row r="90" ht="14.6" customHeight="1">
-      <c r="A90" s="9"/>
-      <c r="B90" s="9"/>
-      <c r="C90" s="10"/>
-      <c r="D90" s="10"/>
-      <c r="E90" s="10"/>
+      <c r="A90" s="7"/>
+      <c r="B90" s="7"/>
+      <c r="C90" s="8"/>
+      <c r="D90" s="8"/>
+      <c r="E90" s="8"/>
     </row>
     <row r="91" ht="14.6" customHeight="1">
-      <c r="A91" s="7"/>
-      <c r="B91" s="7"/>
-      <c r="C91" s="8"/>
-      <c r="D91" s="8"/>
-      <c r="E91" s="8"/>
+      <c r="A91" s="9"/>
+      <c r="B91" s="9"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="10"/>
+      <c r="E91" s="10"/>
     </row>
     <row r="92" ht="14.6" customHeight="1">
-      <c r="A92" s="10"/>
-      <c r="B92" s="10"/>
-      <c r="C92" s="10"/>
-      <c r="D92" s="10"/>
-      <c r="E92" s="10"/>
+      <c r="A92" s="7"/>
+      <c r="B92" s="7"/>
+      <c r="C92" s="8"/>
+      <c r="D92" s="8"/>
+      <c r="E92" s="8"/>
     </row>
     <row r="93" ht="14.6" customHeight="1">
-      <c r="A93" s="7"/>
-      <c r="B93" s="7"/>
-      <c r="C93" s="8"/>
-      <c r="D93" s="8"/>
-      <c r="E93" s="8"/>
+      <c r="A93" s="9"/>
+      <c r="B93" s="9"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="10"/>
+      <c r="E93" s="10"/>
     </row>
     <row r="94" ht="14.6" customHeight="1">
-      <c r="A94" s="9"/>
-      <c r="B94" s="9"/>
-      <c r="C94" s="10"/>
-      <c r="D94" s="10"/>
-      <c r="E94" s="10"/>
+      <c r="A94" s="7"/>
+      <c r="B94" s="7"/>
+      <c r="C94" s="8"/>
+      <c r="D94" s="8"/>
+      <c r="E94" s="8"/>
     </row>
     <row r="95" ht="14.6" customHeight="1">
-      <c r="A95" s="7"/>
-      <c r="B95" s="7"/>
-      <c r="C95" s="8"/>
-      <c r="D95" s="8"/>
-      <c r="E95" s="8"/>
+      <c r="A95" s="10"/>
+      <c r="B95" s="10"/>
+      <c r="C95" s="10"/>
+      <c r="D95" s="10"/>
+      <c r="E95" s="10"/>
     </row>
     <row r="96" ht="14.6" customHeight="1">
-      <c r="A96" s="10"/>
-      <c r="B96" s="10"/>
-      <c r="C96" s="10"/>
-      <c r="D96" s="10"/>
-      <c r="E96" s="10"/>
+      <c r="A96" s="7"/>
+      <c r="B96" s="7"/>
+      <c r="C96" s="8"/>
+      <c r="D96" s="8"/>
+      <c r="E96" s="8"/>
     </row>
     <row r="97" ht="14.6" customHeight="1">
-      <c r="A97" s="7"/>
-      <c r="B97" s="7"/>
-      <c r="C97" s="8"/>
-      <c r="D97" s="8"/>
-      <c r="E97" s="8"/>
+      <c r="A97" s="9"/>
+      <c r="B97" s="9"/>
+      <c r="C97" s="10"/>
+      <c r="D97" s="10"/>
+      <c r="E97" s="10"/>
     </row>
     <row r="98" ht="14.6" customHeight="1">
-      <c r="A98" s="9"/>
-      <c r="B98" s="9"/>
-      <c r="C98" s="10"/>
-      <c r="D98" s="10"/>
-      <c r="E98" s="10"/>
+      <c r="A98" s="7"/>
+      <c r="B98" s="7"/>
+      <c r="C98" s="8"/>
+      <c r="D98" s="8"/>
+      <c r="E98" s="8"/>
     </row>
     <row r="99" ht="14.6" customHeight="1">
-      <c r="A99" s="7"/>
-      <c r="B99" s="7"/>
-      <c r="C99" s="8"/>
-      <c r="D99" s="8"/>
-      <c r="E99" s="8"/>
+      <c r="A99" s="10"/>
+      <c r="B99" s="10"/>
+      <c r="C99" s="10"/>
+      <c r="D99" s="10"/>
+      <c r="E99" s="10"/>
     </row>
     <row r="100" ht="14.6" customHeight="1">
-      <c r="A100" s="9"/>
-      <c r="B100" s="9"/>
-      <c r="C100" s="10"/>
-      <c r="D100" s="10"/>
-      <c r="E100" s="10"/>
+      <c r="A100" s="7"/>
+      <c r="B100" s="7"/>
+      <c r="C100" s="8"/>
+      <c r="D100" s="8"/>
+      <c r="E100" s="8"/>
     </row>
     <row r="101" ht="14.6" customHeight="1">
-      <c r="A101" s="8"/>
-      <c r="B101" s="8"/>
-      <c r="C101" s="8"/>
-      <c r="D101" s="8"/>
-      <c r="E101" s="8"/>
+      <c r="A101" s="9"/>
+      <c r="B101" s="9"/>
+      <c r="C101" s="10"/>
+      <c r="D101" s="10"/>
+      <c r="E101" s="10"/>
     </row>
     <row r="102" ht="14.6" customHeight="1">
-      <c r="A102" s="9"/>
-      <c r="B102" s="9"/>
-      <c r="C102" s="10"/>
-      <c r="D102" s="10"/>
-      <c r="E102" s="10"/>
+      <c r="A102" s="7"/>
+      <c r="B102" s="7"/>
+      <c r="C102" s="8"/>
+      <c r="D102" s="8"/>
+      <c r="E102" s="8"/>
     </row>
     <row r="103" ht="14.6" customHeight="1">
-      <c r="A103" s="7"/>
-      <c r="B103" s="7"/>
-      <c r="C103" s="8"/>
-      <c r="D103" s="8"/>
-      <c r="E103" s="8"/>
+      <c r="A103" s="9"/>
+      <c r="B103" s="9"/>
+      <c r="C103" s="10"/>
+      <c r="D103" s="10"/>
+      <c r="E103" s="10"/>
     </row>
     <row r="104" ht="14.6" customHeight="1">
-      <c r="A104" s="10"/>
-      <c r="B104" s="10"/>
-      <c r="C104" s="10"/>
-      <c r="D104" s="10"/>
-      <c r="E104" s="10"/>
+      <c r="A104" s="8"/>
+      <c r="B104" s="8"/>
+      <c r="C104" s="8"/>
+      <c r="D104" s="8"/>
+      <c r="E104" s="8"/>
     </row>
     <row r="105" ht="14.6" customHeight="1">
-      <c r="A105" s="7"/>
-      <c r="B105" s="7"/>
-      <c r="C105" s="8"/>
-      <c r="D105" s="8"/>
-      <c r="E105" s="8"/>
+      <c r="A105" s="9"/>
+      <c r="B105" s="9"/>
+      <c r="C105" s="10"/>
+      <c r="D105" s="10"/>
+      <c r="E105" s="10"/>
     </row>
     <row r="106" ht="14.6" customHeight="1">
-      <c r="A106" s="9"/>
-      <c r="B106" s="9"/>
-      <c r="C106" s="10"/>
-      <c r="D106" s="10"/>
-      <c r="E106" s="10"/>
+      <c r="A106" s="7"/>
+      <c r="B106" s="7"/>
+      <c r="C106" s="8"/>
+      <c r="D106" s="8"/>
+      <c r="E106" s="8"/>
     </row>
     <row r="107" ht="14.6" customHeight="1">
-      <c r="A107" s="7"/>
-      <c r="B107" s="7"/>
-      <c r="C107" s="8"/>
-      <c r="D107" s="8"/>
-      <c r="E107" s="8"/>
+      <c r="A107" s="10"/>
+      <c r="B107" s="10"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="10"/>
+      <c r="E107" s="10"/>
     </row>
     <row r="108" ht="14.6" customHeight="1">
-      <c r="A108" s="10"/>
-      <c r="B108" s="10"/>
-      <c r="C108" s="10"/>
-      <c r="D108" s="10"/>
-      <c r="E108" s="10"/>
+      <c r="A108" s="7"/>
+      <c r="B108" s="7"/>
+      <c r="C108" s="8"/>
+      <c r="D108" s="8"/>
+      <c r="E108" s="8"/>
     </row>
     <row r="109" ht="14.6" customHeight="1">
-      <c r="A109" s="7"/>
-      <c r="B109" s="7"/>
-      <c r="C109" s="8"/>
-      <c r="D109" s="8"/>
-      <c r="E109" s="8"/>
+      <c r="A109" s="9"/>
+      <c r="B109" s="9"/>
+      <c r="C109" s="10"/>
+      <c r="D109" s="10"/>
+      <c r="E109" s="10"/>
     </row>
     <row r="110" ht="14.6" customHeight="1">
-      <c r="A110" s="9"/>
-      <c r="B110" s="9"/>
-      <c r="C110" s="10"/>
-      <c r="D110" s="10"/>
-      <c r="E110" s="10"/>
+      <c r="A110" s="7"/>
+      <c r="B110" s="7"/>
+      <c r="C110" s="8"/>
+      <c r="D110" s="8"/>
+      <c r="E110" s="8"/>
     </row>
     <row r="111" ht="14.6" customHeight="1">
-      <c r="A111" s="8"/>
-      <c r="B111" s="8"/>
-      <c r="C111" s="8"/>
-      <c r="D111" s="8"/>
-      <c r="E111" s="8"/>
+      <c r="A111" s="10"/>
+      <c r="B111" s="10"/>
+      <c r="C111" s="10"/>
+      <c r="D111" s="10"/>
+      <c r="E111" s="10"/>
     </row>
     <row r="112" ht="14.6" customHeight="1">
-      <c r="A112" s="9"/>
-      <c r="B112" s="9"/>
-      <c r="C112" s="10"/>
-      <c r="D112" s="10"/>
-      <c r="E112" s="10"/>
+      <c r="A112" s="7"/>
+      <c r="B112" s="7"/>
+      <c r="C112" s="8"/>
+      <c r="D112" s="8"/>
+      <c r="E112" s="8"/>
     </row>
     <row r="113" ht="14.6" customHeight="1">
-      <c r="A113" s="8"/>
-      <c r="B113" s="8"/>
-      <c r="C113" s="8"/>
-      <c r="D113" s="8"/>
-      <c r="E113" s="8"/>
+      <c r="A113" s="9"/>
+      <c r="B113" s="9"/>
+      <c r="C113" s="10"/>
+      <c r="D113" s="10"/>
+      <c r="E113" s="10"/>
     </row>
     <row r="114" ht="14.6" customHeight="1">
-      <c r="A114" s="9"/>
-      <c r="B114" s="9"/>
-      <c r="C114" s="10"/>
-      <c r="D114" s="10"/>
-      <c r="E114" s="10"/>
+      <c r="A114" s="8"/>
+      <c r="B114" s="8"/>
+      <c r="C114" s="8"/>
+      <c r="D114" s="8"/>
+      <c r="E114" s="8"/>
     </row>
     <row r="115" ht="14.6" customHeight="1">
-      <c r="A115" s="7"/>
-      <c r="B115" s="7"/>
-      <c r="C115" s="8"/>
-      <c r="D115" s="8"/>
-      <c r="E115" s="8"/>
+      <c r="A115" s="9"/>
+      <c r="B115" s="9"/>
+      <c r="C115" s="10"/>
+      <c r="D115" s="10"/>
+      <c r="E115" s="10"/>
     </row>
     <row r="116" ht="14.6" customHeight="1">
-      <c r="A116" s="10"/>
-      <c r="B116" s="10"/>
-      <c r="C116" s="10"/>
-      <c r="D116" s="10"/>
-      <c r="E116" s="10"/>
+      <c r="A116" s="8"/>
+      <c r="B116" s="8"/>
+      <c r="C116" s="8"/>
+      <c r="D116" s="8"/>
+      <c r="E116" s="8"/>
     </row>
     <row r="117" ht="14.6" customHeight="1">
-      <c r="A117" s="7"/>
-      <c r="B117" s="7"/>
-      <c r="C117" s="8"/>
-      <c r="D117" s="8"/>
-      <c r="E117" s="8"/>
+      <c r="A117" s="9"/>
+      <c r="B117" s="9"/>
+      <c r="C117" s="10"/>
+      <c r="D117" s="10"/>
+      <c r="E117" s="10"/>
     </row>
     <row r="118" ht="14.6" customHeight="1">
-      <c r="A118" s="9"/>
-      <c r="B118" s="9"/>
-      <c r="C118" s="10"/>
-      <c r="D118" s="10"/>
-      <c r="E118" s="10"/>
+      <c r="A118" s="7"/>
+      <c r="B118" s="7"/>
+      <c r="C118" s="8"/>
+      <c r="D118" s="8"/>
+      <c r="E118" s="8"/>
     </row>
     <row r="119" ht="14.6" customHeight="1">
-      <c r="A119" s="8"/>
-      <c r="B119" s="8"/>
-      <c r="C119" s="8"/>
-      <c r="D119" s="8"/>
-      <c r="E119" s="8"/>
+      <c r="A119" s="10"/>
+      <c r="B119" s="10"/>
+      <c r="C119" s="10"/>
+      <c r="D119" s="10"/>
+      <c r="E119" s="10"/>
     </row>
     <row r="120" ht="14.6" customHeight="1">
-      <c r="A120" s="10"/>
-      <c r="B120" s="10"/>
-      <c r="C120" s="10"/>
-      <c r="D120" s="10"/>
-      <c r="E120" s="10"/>
+      <c r="A120" s="7"/>
+      <c r="B120" s="7"/>
+      <c r="C120" s="8"/>
+      <c r="D120" s="8"/>
+      <c r="E120" s="8"/>
     </row>
     <row r="121" ht="14.6" customHeight="1">
-      <c r="A121" s="7"/>
-      <c r="B121" s="8"/>
-      <c r="C121" s="8"/>
-      <c r="D121" s="8"/>
-      <c r="E121" s="8"/>
+      <c r="A121" s="9"/>
+      <c r="B121" s="9"/>
+      <c r="C121" s="10"/>
+      <c r="D121" s="10"/>
+      <c r="E121" s="10"/>
     </row>
     <row r="122" ht="14.6" customHeight="1">
-      <c r="A122" s="9"/>
-      <c r="B122" s="10"/>
-      <c r="C122" s="10"/>
-      <c r="D122" s="10"/>
-      <c r="E122" s="10"/>
+      <c r="A122" s="8"/>
+      <c r="B122" s="8"/>
+      <c r="C122" s="8"/>
+      <c r="D122" s="8"/>
+      <c r="E122" s="8"/>
     </row>
     <row r="123" ht="14.6" customHeight="1">
-      <c r="A123" s="7"/>
-      <c r="B123" s="7"/>
-      <c r="C123" s="8"/>
-      <c r="D123" s="8"/>
-      <c r="E123" s="8"/>
+      <c r="A123" s="10"/>
+      <c r="B123" s="10"/>
+      <c r="C123" s="10"/>
+      <c r="D123" s="10"/>
+      <c r="E123" s="10"/>
     </row>
     <row r="124" ht="14.6" customHeight="1">
-      <c r="A124" s="10"/>
-      <c r="B124" s="10"/>
-      <c r="C124" s="10"/>
-      <c r="D124" s="10"/>
-      <c r="E124" s="10"/>
+      <c r="A124" s="7"/>
+      <c r="B124" s="8"/>
+      <c r="C124" s="8"/>
+      <c r="D124" s="8"/>
+      <c r="E124" s="8"/>
     </row>
     <row r="125" ht="14.6" customHeight="1">
-      <c r="A125" s="7"/>
-      <c r="B125" s="7"/>
-      <c r="C125" s="8"/>
-      <c r="D125" s="8"/>
-      <c r="E125" s="8"/>
+      <c r="A125" s="9"/>
+      <c r="B125" s="10"/>
+      <c r="C125" s="10"/>
+      <c r="D125" s="10"/>
+      <c r="E125" s="10"/>
     </row>
     <row r="126" ht="14.6" customHeight="1">
-      <c r="A126" s="10"/>
-      <c r="B126" s="10"/>
-      <c r="C126" s="10"/>
-      <c r="D126" s="10"/>
-      <c r="E126" s="10"/>
+      <c r="A126" s="7"/>
+      <c r="B126" s="7"/>
+      <c r="C126" s="8"/>
+      <c r="D126" s="8"/>
+      <c r="E126" s="8"/>
     </row>
     <row r="127" ht="14.6" customHeight="1">
-      <c r="A127" s="8"/>
-      <c r="B127" s="8"/>
-      <c r="C127" s="8"/>
-      <c r="D127" s="8"/>
-      <c r="E127" s="8"/>
+      <c r="A127" s="10"/>
+      <c r="B127" s="10"/>
+      <c r="C127" s="10"/>
+      <c r="D127" s="10"/>
+      <c r="E127" s="10"/>
     </row>
     <row r="128" ht="14.6" customHeight="1">
-      <c r="A128" s="10"/>
-      <c r="B128" s="10"/>
-      <c r="C128" s="10"/>
-      <c r="D128" s="10"/>
-      <c r="E128" s="10"/>
+      <c r="A128" s="7"/>
+      <c r="B128" s="7"/>
+      <c r="C128" s="8"/>
+      <c r="D128" s="8"/>
+      <c r="E128" s="8"/>
     </row>
     <row r="129" ht="14.6" customHeight="1">
-      <c r="A129" s="8"/>
-      <c r="B129" s="8"/>
-      <c r="C129" s="8"/>
-      <c r="D129" s="8"/>
-      <c r="E129" s="8"/>
+      <c r="A129" s="10"/>
+      <c r="B129" s="10"/>
+      <c r="C129" s="10"/>
+      <c r="D129" s="10"/>
+      <c r="E129" s="10"/>
     </row>
     <row r="130" ht="14.6" customHeight="1">
-      <c r="A130" s="9"/>
-      <c r="B130" s="9"/>
-      <c r="C130" s="10"/>
-      <c r="D130" s="10"/>
-      <c r="E130" s="10"/>
+      <c r="A130" s="8"/>
+      <c r="B130" s="8"/>
+      <c r="C130" s="8"/>
+      <c r="D130" s="8"/>
+      <c r="E130" s="8"/>
     </row>
     <row r="131" ht="14.6" customHeight="1">
-      <c r="A131" s="7"/>
-      <c r="B131" s="7"/>
-      <c r="C131" s="8"/>
-      <c r="D131" s="8"/>
-      <c r="E131" s="8"/>
+      <c r="A131" s="10"/>
+      <c r="B131" s="10"/>
+      <c r="C131" s="10"/>
+      <c r="D131" s="10"/>
+      <c r="E131" s="10"/>
     </row>
     <row r="132" ht="14.6" customHeight="1">
-      <c r="A132" s="9"/>
-      <c r="B132" s="9"/>
-      <c r="C132" s="10"/>
-      <c r="D132" s="10"/>
-      <c r="E132" s="10"/>
+      <c r="A132" s="8"/>
+      <c r="B132" s="8"/>
+      <c r="C132" s="8"/>
+      <c r="D132" s="8"/>
+      <c r="E132" s="8"/>
     </row>
     <row r="133" ht="14.6" customHeight="1">
-      <c r="A133" s="7"/>
-      <c r="B133" s="7"/>
-      <c r="C133" s="8"/>
-      <c r="D133" s="8"/>
-      <c r="E133" s="8"/>
+      <c r="A133" s="9"/>
+      <c r="B133" s="9"/>
+      <c r="C133" s="10"/>
+      <c r="D133" s="10"/>
+      <c r="E133" s="10"/>
     </row>
     <row r="134" ht="14.6" customHeight="1">
-      <c r="A134" s="9"/>
-      <c r="B134" s="9"/>
-      <c r="C134" s="10"/>
-      <c r="D134" s="10"/>
-      <c r="E134" s="10"/>
+      <c r="A134" s="7"/>
+      <c r="B134" s="7"/>
+      <c r="C134" s="8"/>
+      <c r="D134" s="8"/>
+      <c r="E134" s="8"/>
     </row>
     <row r="135" ht="14.6" customHeight="1">
-      <c r="A135" s="7"/>
-      <c r="B135" s="7"/>
-      <c r="C135" s="8"/>
-      <c r="D135" s="8"/>
-      <c r="E135" s="8"/>
+      <c r="A135" s="9"/>
+      <c r="B135" s="9"/>
+      <c r="C135" s="10"/>
+      <c r="D135" s="10"/>
+      <c r="E135" s="10"/>
     </row>
     <row r="136" ht="14.6" customHeight="1">
-      <c r="A136" s="9"/>
-      <c r="B136" s="9"/>
-      <c r="C136" s="10"/>
-      <c r="D136" s="10"/>
-      <c r="E136" s="10"/>
+      <c r="A136" s="7"/>
+      <c r="B136" s="7"/>
+      <c r="C136" s="8"/>
+      <c r="D136" s="8"/>
+      <c r="E136" s="8"/>
     </row>
     <row r="137" ht="14.6" customHeight="1">
-      <c r="A137" s="7"/>
-      <c r="B137" s="7"/>
-      <c r="C137" s="8"/>
-      <c r="D137" s="8"/>
-      <c r="E137" s="8"/>
+      <c r="A137" s="9"/>
+      <c r="B137" s="9"/>
+      <c r="C137" s="10"/>
+      <c r="D137" s="10"/>
+      <c r="E137" s="10"/>
     </row>
     <row r="138" ht="14.6" customHeight="1">
-      <c r="A138" s="10"/>
-      <c r="B138" s="10"/>
-      <c r="C138" s="10"/>
-      <c r="D138" s="10"/>
-      <c r="E138" s="10"/>
+      <c r="A138" s="7"/>
+      <c r="B138" s="7"/>
+      <c r="C138" s="8"/>
+      <c r="D138" s="8"/>
+      <c r="E138" s="8"/>
     </row>
     <row r="139" ht="14.6" customHeight="1">
-      <c r="A139" s="7"/>
-      <c r="B139" s="7"/>
-      <c r="C139" s="8"/>
-      <c r="D139" s="8"/>
-      <c r="E139" s="8"/>
+      <c r="A139" s="9"/>
+      <c r="B139" s="9"/>
+      <c r="C139" s="10"/>
+      <c r="D139" s="10"/>
+      <c r="E139" s="10"/>
     </row>
     <row r="140" ht="14.6" customHeight="1">
-      <c r="A140" s="9"/>
-      <c r="B140" s="9"/>
-      <c r="C140" s="10"/>
-      <c r="D140" s="10"/>
-      <c r="E140" s="10"/>
+      <c r="A140" s="7"/>
+      <c r="B140" s="7"/>
+      <c r="C140" s="8"/>
+      <c r="D140" s="8"/>
+      <c r="E140" s="8"/>
     </row>
     <row r="141" ht="14.6" customHeight="1">
-      <c r="A141" s="7"/>
-      <c r="B141" s="7"/>
-      <c r="C141" s="8"/>
-      <c r="D141" s="8"/>
-      <c r="E141" s="8"/>
+      <c r="A141" s="10"/>
+      <c r="B141" s="10"/>
+      <c r="C141" s="10"/>
+      <c r="D141" s="10"/>
+      <c r="E141" s="10"/>
     </row>
     <row r="142" ht="14.6" customHeight="1">
-      <c r="A142" s="9"/>
-      <c r="B142" s="9"/>
-      <c r="C142" s="10"/>
-      <c r="D142" s="10"/>
-      <c r="E142" s="10"/>
+      <c r="A142" s="7"/>
+      <c r="B142" s="7"/>
+      <c r="C142" s="8"/>
+      <c r="D142" s="8"/>
+      <c r="E142" s="8"/>
     </row>
     <row r="143" ht="14.6" customHeight="1">
-      <c r="A143" s="8"/>
-      <c r="B143" s="8"/>
-      <c r="C143" s="8"/>
-      <c r="D143" s="8"/>
-      <c r="E143" s="8"/>
+      <c r="A143" s="9"/>
+      <c r="B143" s="9"/>
+      <c r="C143" s="10"/>
+      <c r="D143" s="10"/>
+      <c r="E143" s="10"/>
     </row>
     <row r="144" ht="14.6" customHeight="1">
-      <c r="A144" s="9"/>
-      <c r="B144" s="9"/>
-      <c r="C144" s="10"/>
-      <c r="D144" s="10"/>
-      <c r="E144" s="10"/>
+      <c r="A144" s="7"/>
+      <c r="B144" s="7"/>
+      <c r="C144" s="8"/>
+      <c r="D144" s="8"/>
+      <c r="E144" s="8"/>
     </row>
     <row r="145" ht="14.6" customHeight="1">
-      <c r="A145" s="7"/>
-      <c r="B145" s="7"/>
-      <c r="C145" s="8"/>
-      <c r="D145" s="8"/>
-      <c r="E145" s="8"/>
+      <c r="A145" s="9"/>
+      <c r="B145" s="9"/>
+      <c r="C145" s="10"/>
+      <c r="D145" s="10"/>
+      <c r="E145" s="10"/>
     </row>
     <row r="146" ht="14.6" customHeight="1">
-      <c r="A146" s="9"/>
-      <c r="B146" s="9"/>
-      <c r="C146" s="10"/>
-      <c r="D146" s="10"/>
-      <c r="E146" s="10"/>
+      <c r="A146" s="8"/>
+      <c r="B146" s="8"/>
+      <c r="C146" s="8"/>
+      <c r="D146" s="8"/>
+      <c r="E146" s="8"/>
     </row>
     <row r="147" ht="14.6" customHeight="1">
-      <c r="A147" s="7"/>
-      <c r="B147" s="7"/>
-      <c r="C147" s="8"/>
-      <c r="D147" s="8"/>
-      <c r="E147" s="8"/>
+      <c r="A147" s="9"/>
+      <c r="B147" s="9"/>
+      <c r="C147" s="10"/>
+      <c r="D147" s="10"/>
+      <c r="E147" s="10"/>
     </row>
     <row r="148" ht="14.6" customHeight="1">
-      <c r="A148" s="9"/>
-      <c r="B148" s="9"/>
-      <c r="C148" s="10"/>
-      <c r="D148" s="10"/>
-      <c r="E148" s="10"/>
+      <c r="A148" s="7"/>
+      <c r="B148" s="7"/>
+      <c r="C148" s="8"/>
+      <c r="D148" s="8"/>
+      <c r="E148" s="8"/>
     </row>
     <row r="149" ht="14.6" customHeight="1">
-      <c r="A149" s="7"/>
-      <c r="B149" s="7"/>
-      <c r="C149" s="8"/>
-      <c r="D149" s="8"/>
-      <c r="E149" s="8"/>
+      <c r="A149" s="9"/>
+      <c r="B149" s="9"/>
+      <c r="C149" s="10"/>
+      <c r="D149" s="10"/>
+      <c r="E149" s="10"/>
     </row>
     <row r="150" ht="14.6" customHeight="1">
-      <c r="A150" s="9"/>
-      <c r="B150" s="9"/>
-      <c r="C150" s="10"/>
-      <c r="D150" s="10"/>
-      <c r="E150" s="10"/>
+      <c r="A150" s="7"/>
+      <c r="B150" s="7"/>
+      <c r="C150" s="8"/>
+      <c r="D150" s="8"/>
+      <c r="E150" s="8"/>
     </row>
     <row r="151" ht="14.6" customHeight="1">
-      <c r="A151" s="8"/>
-      <c r="B151" s="8"/>
-      <c r="C151" s="8"/>
-      <c r="D151" s="8"/>
-      <c r="E151" s="8"/>
+      <c r="A151" s="9"/>
+      <c r="B151" s="9"/>
+      <c r="C151" s="10"/>
+      <c r="D151" s="10"/>
+      <c r="E151" s="10"/>
     </row>
     <row r="152" ht="14.6" customHeight="1">
-      <c r="A152" s="9"/>
-      <c r="B152" s="9"/>
-      <c r="C152" s="10"/>
-      <c r="D152" s="10"/>
-      <c r="E152" s="10"/>
+      <c r="A152" s="7"/>
+      <c r="B152" s="7"/>
+      <c r="C152" s="8"/>
+      <c r="D152" s="8"/>
+      <c r="E152" s="8"/>
     </row>
     <row r="153" ht="14.6" customHeight="1">
-      <c r="A153" s="7"/>
-      <c r="B153" s="7"/>
-      <c r="C153" s="8"/>
-      <c r="D153" s="8"/>
-      <c r="E153" s="8"/>
+      <c r="A153" s="9"/>
+      <c r="B153" s="9"/>
+      <c r="C153" s="10"/>
+      <c r="D153" s="10"/>
+      <c r="E153" s="10"/>
     </row>
     <row r="154" ht="14.6" customHeight="1">
-      <c r="A154" s="9"/>
-      <c r="B154" s="9"/>
-      <c r="C154" s="10"/>
-      <c r="D154" s="10"/>
-      <c r="E154" s="10"/>
+      <c r="A154" s="8"/>
+      <c r="B154" s="8"/>
+      <c r="C154" s="8"/>
+      <c r="D154" s="8"/>
+      <c r="E154" s="8"/>
     </row>
     <row r="155" ht="14.6" customHeight="1">
-      <c r="A155" s="8"/>
-      <c r="B155" s="8"/>
-      <c r="C155" s="8"/>
-      <c r="D155" s="8"/>
-      <c r="E155" s="8"/>
+      <c r="A155" s="9"/>
+      <c r="B155" s="9"/>
+      <c r="C155" s="10"/>
+      <c r="D155" s="10"/>
+      <c r="E155" s="10"/>
     </row>
     <row r="156" ht="14.6" customHeight="1">
-      <c r="A156" s="9"/>
-      <c r="B156" s="9"/>
-      <c r="C156" s="10"/>
-      <c r="D156" s="10"/>
-      <c r="E156" s="10"/>
+      <c r="A156" s="7"/>
+      <c r="B156" s="7"/>
+      <c r="C156" s="8"/>
+      <c r="D156" s="8"/>
+      <c r="E156" s="8"/>
     </row>
     <row r="157" ht="14.6" customHeight="1">
-      <c r="A157" s="7"/>
-      <c r="B157" s="7"/>
-      <c r="C157" s="8"/>
-      <c r="D157" s="8"/>
-      <c r="E157" s="8"/>
+      <c r="A157" s="9"/>
+      <c r="B157" s="9"/>
+      <c r="C157" s="10"/>
+      <c r="D157" s="10"/>
+      <c r="E157" s="10"/>
     </row>
     <row r="158" ht="14.6" customHeight="1">
-      <c r="A158" s="10"/>
-      <c r="B158" s="10"/>
-      <c r="C158" s="10"/>
-      <c r="D158" s="10"/>
-      <c r="E158" s="10"/>
+      <c r="A158" s="8"/>
+      <c r="B158" s="8"/>
+      <c r="C158" s="8"/>
+      <c r="D158" s="8"/>
+      <c r="E158" s="8"/>
     </row>
     <row r="159" ht="14.6" customHeight="1">
-      <c r="A159" s="7"/>
-      <c r="B159" s="7"/>
-      <c r="C159" s="8"/>
-      <c r="D159" s="8"/>
-      <c r="E159" s="8"/>
+      <c r="A159" s="9"/>
+      <c r="B159" s="9"/>
+      <c r="C159" s="10"/>
+      <c r="D159" s="10"/>
+      <c r="E159" s="10"/>
     </row>
     <row r="160" ht="14.6" customHeight="1">
-      <c r="A160" s="9"/>
-      <c r="B160" s="9"/>
-      <c r="C160" s="10"/>
-      <c r="D160" s="10"/>
-      <c r="E160" s="10"/>
+      <c r="A160" s="7"/>
+      <c r="B160" s="7"/>
+      <c r="C160" s="8"/>
+      <c r="D160" s="8"/>
+      <c r="E160" s="8"/>
     </row>
     <row r="161" ht="14.6" customHeight="1">
-      <c r="A161" s="8"/>
-      <c r="B161" s="8"/>
-      <c r="C161" s="8"/>
-      <c r="D161" s="8"/>
-      <c r="E161" s="8"/>
+      <c r="A161" s="10"/>
+      <c r="B161" s="10"/>
+      <c r="C161" s="10"/>
+      <c r="D161" s="10"/>
+      <c r="E161" s="10"/>
     </row>
     <row r="162" ht="14.6" customHeight="1">
-      <c r="A162" s="9"/>
-      <c r="B162" s="9"/>
-      <c r="C162" s="10"/>
-      <c r="D162" s="10"/>
-      <c r="E162" s="10"/>
+      <c r="A162" s="7"/>
+      <c r="B162" s="7"/>
+      <c r="C162" s="8"/>
+      <c r="D162" s="8"/>
+      <c r="E162" s="8"/>
     </row>
     <row r="163" ht="14.6" customHeight="1">
-      <c r="A163" s="7"/>
-      <c r="B163" s="7"/>
-      <c r="C163" s="8"/>
-      <c r="D163" s="8"/>
-      <c r="E163" s="8"/>
+      <c r="A163" s="9"/>
+      <c r="B163" s="9"/>
+      <c r="C163" s="10"/>
+      <c r="D163" s="10"/>
+      <c r="E163" s="10"/>
     </row>
     <row r="164" ht="14.6" customHeight="1">
-      <c r="A164" s="10"/>
-      <c r="B164" s="10"/>
-      <c r="C164" s="10"/>
-      <c r="D164" s="10"/>
-      <c r="E164" s="10"/>
+      <c r="A164" s="8"/>
+      <c r="B164" s="8"/>
+      <c r="C164" s="8"/>
+      <c r="D164" s="8"/>
+      <c r="E164" s="8"/>
     </row>
     <row r="165" ht="14.6" customHeight="1">
-      <c r="A165" s="7"/>
-      <c r="B165" s="7"/>
-      <c r="C165" s="8"/>
-      <c r="D165" s="8"/>
-      <c r="E165" s="8"/>
+      <c r="A165" s="9"/>
+      <c r="B165" s="9"/>
+      <c r="C165" s="10"/>
+      <c r="D165" s="10"/>
+      <c r="E165" s="10"/>
     </row>
     <row r="166" ht="14.6" customHeight="1">
-      <c r="A166" s="9"/>
-      <c r="B166" s="9"/>
-      <c r="C166" s="10"/>
-      <c r="D166" s="10"/>
-      <c r="E166" s="10"/>
+      <c r="A166" s="7"/>
+      <c r="B166" s="7"/>
+      <c r="C166" s="8"/>
+      <c r="D166" s="8"/>
+      <c r="E166" s="8"/>
+    </row>
+    <row r="167" ht="14.6" customHeight="1">
+      <c r="A167" s="10"/>
+      <c r="B167" s="10"/>
+      <c r="C167" s="10"/>
+      <c r="D167" s="10"/>
+      <c r="E167" s="10"/>
+    </row>
+    <row r="168" ht="14.6" customHeight="1">
+      <c r="A168" s="7"/>
+      <c r="B168" s="7"/>
+      <c r="C168" s="8"/>
+      <c r="D168" s="8"/>
+      <c r="E168" s="8"/>
+    </row>
+    <row r="169" ht="14.6" customHeight="1">
+      <c r="A169" s="9"/>
+      <c r="B169" s="9"/>
+      <c r="C169" s="10"/>
+      <c r="D169" s="10"/>
+      <c r="E169" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -12063,7 +12111,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -12074,7 +12122,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -12103,7 +12151,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s" s="9">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -12165,10 +12213,10 @@
     </row>
     <row r="14" ht="15.35" customHeight="1">
       <c r="A14" t="s" s="29">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B14" t="s" s="29">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -12176,10 +12224,10 @@
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" t="s" s="21">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B15" t="s" s="7">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -12194,10 +12242,10 @@
     </row>
     <row r="17" ht="15.35" customHeight="1">
       <c r="A17" t="s" s="29">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B17" t="s" s="29">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -12237,7 +12285,7 @@
         <v>62</v>
       </c>
       <c r="B21" t="s" s="22">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -12263,10 +12311,10 @@
     </row>
     <row r="24" ht="15.35" customHeight="1">
       <c r="A24" t="s" s="21">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B24" t="s" s="22">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -12274,10 +12322,10 @@
     </row>
     <row r="25" ht="15.35" customHeight="1">
       <c r="A25" t="s" s="21">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B25" t="s" s="22">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
@@ -12285,10 +12333,10 @@
     </row>
     <row r="26" ht="15.35" customHeight="1">
       <c r="A26" t="s" s="21">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B26" t="s" s="22">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
@@ -12303,10 +12351,10 @@
     </row>
     <row r="28" ht="15.35" customHeight="1">
       <c r="A28" t="s" s="29">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B28" t="s" s="29">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -12314,10 +12362,10 @@
     </row>
     <row r="29" ht="15.35" customHeight="1">
       <c r="A29" t="s" s="29">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="B29" t="s" s="29">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -12325,10 +12373,10 @@
     </row>
     <row r="30" ht="15.35" customHeight="1">
       <c r="A30" t="s" s="29">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="B30" t="s" s="29">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -12343,10 +12391,10 @@
     </row>
     <row r="32" ht="15.35" customHeight="1">
       <c r="A32" t="s" s="46">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B32" t="s" s="25">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
@@ -12354,10 +12402,10 @@
     </row>
     <row r="33" ht="14.6" customHeight="1">
       <c r="A33" t="s" s="13">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="B33" t="s" s="47">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -12365,7 +12413,7 @@
     </row>
     <row r="34" ht="14.6" customHeight="1">
       <c r="A34" t="s" s="24">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B34" t="s" s="25">
         <v>59</v>
@@ -12412,10 +12460,10 @@
     </row>
     <row r="39" ht="14.6" customHeight="1">
       <c r="A39" t="s" s="29">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B39" t="s" s="29">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
@@ -12430,7 +12478,7 @@
     </row>
     <row r="41" ht="14.6" customHeight="1">
       <c r="A41" t="s" s="52">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B41" s="53">
         <v>0</v>
@@ -12441,7 +12489,7 @@
     </row>
     <row r="42" ht="14.6" customHeight="1">
       <c r="A42" t="s" s="54">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B42" s="55">
         <v>1</v>
@@ -12452,7 +12500,7 @@
     </row>
     <row r="43" ht="14.6" customHeight="1">
       <c r="A43" t="s" s="56">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B43" s="57">
         <v>2</v>
@@ -12463,7 +12511,7 @@
     </row>
     <row r="44" ht="14.6" customHeight="1">
       <c r="A44" t="s" s="58">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B44" s="59">
         <v>3</v>
@@ -12474,7 +12522,7 @@
     </row>
     <row r="45" ht="14.6" customHeight="1">
       <c r="A45" t="s" s="60">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="B45" s="61">
         <v>4</v>
@@ -12485,7 +12533,7 @@
     </row>
     <row r="46" ht="14.6" customHeight="1">
       <c r="A46" t="s" s="58">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="B46" s="59">
         <v>5</v>
@@ -12496,7 +12544,7 @@
     </row>
     <row r="47" ht="14.6" customHeight="1">
       <c r="A47" t="s" s="62">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B47" s="63">
         <v>6</v>
@@ -13520,7 +13568,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -13531,7 +13579,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -13560,7 +13608,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s" s="9">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -13622,10 +13670,10 @@
     </row>
     <row r="14" ht="15.35" customHeight="1">
       <c r="A14" t="s" s="29">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B14" t="s" s="29">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -13633,10 +13681,10 @@
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" t="s" s="21">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B15" t="s" s="7">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -13651,7 +13699,7 @@
     </row>
     <row r="17" ht="15.35" customHeight="1">
       <c r="A17" t="s" s="52">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B17" s="53">
         <v>0</v>
@@ -13662,7 +13710,7 @@
     </row>
     <row r="18" ht="15.35" customHeight="1">
       <c r="A18" t="s" s="54">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B18" s="55">
         <v>1</v>
@@ -13673,7 +13721,7 @@
     </row>
     <row r="19" ht="15.35" customHeight="1">
       <c r="A19" t="s" s="54">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B19" s="57">
         <v>2</v>
@@ -13684,7 +13732,7 @@
     </row>
     <row r="20" ht="15.35" customHeight="1">
       <c r="A20" t="s" s="56">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B20" s="65">
         <v>3</v>
@@ -13695,7 +13743,7 @@
     </row>
     <row r="21" ht="15.35" customHeight="1">
       <c r="A21" t="s" s="58">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B21" s="61">
         <v>4</v>
@@ -13706,7 +13754,7 @@
     </row>
     <row r="22" ht="15.35" customHeight="1">
       <c r="A22" t="s" s="60">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="B22" s="59">
         <v>5</v>
@@ -13717,7 +13765,7 @@
     </row>
     <row r="23" ht="15.35" customHeight="1">
       <c r="A23" t="s" s="58">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="B23" s="63">
         <v>6</v>
@@ -13728,10 +13776,10 @@
     </row>
     <row r="24" ht="15.35" customHeight="1">
       <c r="A24" t="s" s="62">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B24" t="s" s="22">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -13782,7 +13830,7 @@
         <v>77</v>
       </c>
       <c r="B29" t="s" s="29">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -13797,10 +13845,10 @@
     </row>
     <row r="31" ht="15.35" customHeight="1">
       <c r="A31" t="s" s="21">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="B31" t="s" s="22">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
@@ -13811,7 +13859,7 @@
         <v>52</v>
       </c>
       <c r="B32" t="s" s="29">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
@@ -13819,10 +13867,10 @@
     </row>
     <row r="33" ht="15.35" customHeight="1">
       <c r="A33" t="s" s="29">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B33" t="s" s="29">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
@@ -13830,10 +13878,10 @@
     </row>
     <row r="34" ht="15.35" customHeight="1">
       <c r="A34" t="s" s="29">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="B34" t="s" s="29">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
@@ -13841,10 +13889,10 @@
     </row>
     <row r="35" ht="15.35" customHeight="1">
       <c r="A35" t="s" s="43">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B35" t="s" s="43">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -13852,10 +13900,10 @@
     </row>
     <row r="36" ht="15.35" customHeight="1">
       <c r="A36" t="s" s="29">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="B36" t="s" s="29">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
@@ -13870,10 +13918,10 @@
     </row>
     <row r="38" ht="15.35" customHeight="1">
       <c r="A38" t="s" s="66">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="B38" t="s" s="67">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
@@ -13881,10 +13929,10 @@
     </row>
     <row r="39" ht="14.6" customHeight="1">
       <c r="A39" t="s" s="68">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="B39" t="s" s="47">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
@@ -13892,10 +13940,10 @@
     </row>
     <row r="40" ht="14.6" customHeight="1">
       <c r="A40" t="s" s="69">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="B40" t="s" s="67">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
@@ -13903,10 +13951,10 @@
     </row>
     <row r="41" ht="14.6" customHeight="1">
       <c r="A41" t="s" s="70">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="B41" t="s" s="71">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
@@ -13914,10 +13962,10 @@
     </row>
     <row r="42" ht="14.6" customHeight="1">
       <c r="A42" t="s" s="72">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B42" t="s" s="73">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
@@ -13925,10 +13973,10 @@
     </row>
     <row r="43" ht="14.6" customHeight="1">
       <c r="A43" t="s" s="29">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="B43" t="s" s="29">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
@@ -13936,10 +13984,10 @@
     </row>
     <row r="44" ht="14.6" customHeight="1">
       <c r="A44" t="s" s="29">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="B44" t="s" s="29">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
@@ -13947,10 +13995,10 @@
     </row>
     <row r="45" ht="14.6" customHeight="1">
       <c r="A45" t="s" s="29">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B45" t="s" s="29">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
@@ -13958,10 +14006,10 @@
     </row>
     <row r="46" ht="14.6" customHeight="1">
       <c r="A46" t="s" s="69">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B46" t="s" s="67">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
@@ -13969,10 +14017,10 @@
     </row>
     <row r="47" ht="14.6" customHeight="1">
       <c r="A47" t="s" s="74">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="B47" t="s" s="75">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="C47" s="76"/>
       <c r="D47" s="76"/>
@@ -13980,10 +14028,10 @@
     </row>
     <row r="48" ht="14.6" customHeight="1">
       <c r="A48" t="s" s="78">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="B48" t="s" s="79">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="C48" s="80"/>
       <c r="D48" s="80"/>
@@ -15039,7 +15087,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -15050,7 +15098,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -15079,7 +15127,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s" s="9">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -15123,7 +15171,7 @@
     </row>
     <row r="12" ht="14.6" customHeight="1">
       <c r="A12" t="s" s="7">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="B12" t="s" s="7">
         <v>29</v>
@@ -15141,7 +15189,7 @@
     </row>
     <row r="14" ht="15.35" customHeight="1">
       <c r="A14" t="s" s="52">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B14" s="53">
         <v>0</v>
@@ -15152,7 +15200,7 @@
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" t="s" s="54">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B15" s="57">
         <v>1</v>
@@ -15163,7 +15211,7 @@
     </row>
     <row r="16" ht="15.35" customHeight="1">
       <c r="A16" t="s" s="56">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B16" s="65">
         <v>2</v>
@@ -15174,7 +15222,7 @@
     </row>
     <row r="17" ht="15.35" customHeight="1">
       <c r="A17" t="s" s="58">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B17" s="59">
         <v>3</v>
@@ -15185,7 +15233,7 @@
     </row>
     <row r="18" ht="15.35" customHeight="1">
       <c r="A18" t="s" s="60">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="B18" s="61">
         <v>4</v>
@@ -15196,7 +15244,7 @@
     </row>
     <row r="19" ht="15.35" customHeight="1">
       <c r="A19" t="s" s="58">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="B19" s="59">
         <v>5</v>
@@ -15207,7 +15255,7 @@
     </row>
     <row r="20" ht="15.35" customHeight="1">
       <c r="A20" t="s" s="62">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B20" s="63">
         <v>6</v>
@@ -15225,10 +15273,10 @@
     </row>
     <row r="22" ht="15.35" customHeight="1">
       <c r="A22" t="s" s="9">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="B22" t="s" s="29">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>

</xml_diff>

<commit_message>
MGT 7 Company Address update
</commit_message>
<xml_diff>
--- a/DataExtraction/Input/Config.xlsx
+++ b/DataExtraction/Input/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="253">
   <si>
     <t>Key</t>
   </si>
@@ -141,6 +141,24 @@
   </si>
   <si>
     <t>SUBS</t>
+  </si>
+  <si>
+    <t>total_equity_shares_column_name</t>
+  </si>
+  <si>
+    <t>total_equity_shares</t>
+  </si>
+  <si>
+    <t>total_preference_shares_column_name</t>
+  </si>
+  <si>
+    <t>total_preference_shares</t>
+  </si>
+  <si>
+    <t>registered_full_address_column_name</t>
+  </si>
+  <si>
+    <t>registered_full_address</t>
   </si>
   <si>
     <t>/Users/gundukalyan/Documents/GitHub/mns-json-prep/DataExtraction/Input/MSME/0_Form MSME FORM I-14092023_signed_1 - Copy.pdf</t>
@@ -810,12 +828,12 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -1484,6 +1502,9 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1511,19 +1532,19 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1535,19 +1556,16 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1565,7 +1583,7 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1586,10 +1604,10 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1646,34 +1664,34 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1682,10 +1700,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1709,22 +1727,22 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1739,16 +1757,16 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="34" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -3154,15 +3172,23 @@
       <c r="E30" s="10"/>
     </row>
     <row r="31" ht="14.6" customHeight="1">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
+      <c r="A31" t="s" s="7">
+        <v>40</v>
+      </c>
+      <c r="B31" t="s" s="7">
+        <v>41</v>
+      </c>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
     </row>
     <row r="32" ht="14.6" customHeight="1">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
+      <c r="A32" t="s" s="9">
+        <v>42</v>
+      </c>
+      <c r="B32" t="s" s="9">
+        <v>43</v>
+      </c>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
@@ -3175,8 +3201,12 @@
       <c r="E33" s="8"/>
     </row>
     <row r="34" ht="14.6" customHeight="1">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9"/>
+      <c r="A34" t="s" s="12">
+        <v>44</v>
+      </c>
+      <c r="B34" t="s" s="12">
+        <v>45</v>
+      </c>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
@@ -4154,7 +4184,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -4165,7 +4195,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -4194,7 +4224,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s" s="9">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -4249,7 +4279,7 @@
     </row>
     <row r="13" ht="14.6" customHeight="1">
       <c r="A13" t="s" s="7">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="B13" t="s" s="7">
         <v>29</v>
@@ -4259,15 +4289,15 @@
       <c r="E13" s="8"/>
     </row>
     <row r="14" ht="15.35" customHeight="1">
-      <c r="A14" s="21"/>
-      <c r="B14" s="22"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" t="s" s="52">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B15" s="94">
         <v>0</v>
@@ -4278,7 +4308,7 @@
     </row>
     <row r="16" ht="15.35" customHeight="1">
       <c r="A16" t="s" s="95">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B16" s="59">
         <v>2</v>
@@ -4289,7 +4319,7 @@
     </row>
     <row r="17" ht="15.35" customHeight="1">
       <c r="A17" t="s" s="96">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="B17" s="59">
         <v>3</v>
@@ -4300,7 +4330,7 @@
     </row>
     <row r="18" ht="15.35" customHeight="1">
       <c r="A18" t="s" s="58">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="B18" s="61">
         <v>4</v>
@@ -4311,7 +4341,7 @@
     </row>
     <row r="19" ht="15.35" customHeight="1">
       <c r="A19" t="s" s="60">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B19" s="63">
         <v>6</v>
@@ -4322,7 +4352,7 @@
     </row>
     <row r="20" ht="15.35" customHeight="1">
       <c r="A20" t="s" s="58">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B20" s="59">
         <v>7</v>
@@ -4333,7 +4363,7 @@
     </row>
     <row r="21" ht="15.35" customHeight="1">
       <c r="A21" t="s" s="62">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B21" s="63">
         <v>8</v>
@@ -4343,39 +4373,39 @@
       <c r="E21" s="8"/>
     </row>
     <row r="22" ht="15.35" customHeight="1">
-      <c r="A22" s="21"/>
-      <c r="B22" s="22"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="23"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
     </row>
     <row r="23" ht="15.35" customHeight="1">
       <c r="A23" t="s" s="9">
-        <v>212</v>
-      </c>
-      <c r="B23" t="s" s="29">
-        <v>213</v>
+        <v>218</v>
+      </c>
+      <c r="B23" t="s" s="30">
+        <v>219</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
     </row>
     <row r="24" ht="15.35" customHeight="1">
-      <c r="A24" t="s" s="29">
-        <v>214</v>
-      </c>
-      <c r="B24" t="s" s="29">
-        <v>215</v>
+      <c r="A24" t="s" s="30">
+        <v>220</v>
+      </c>
+      <c r="B24" t="s" s="30">
+        <v>221</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
     </row>
     <row r="25" ht="15.35" customHeight="1">
-      <c r="A25" t="s" s="29">
+      <c r="A25" t="s" s="30">
         <v>23</v>
       </c>
-      <c r="B25" t="s" s="29">
+      <c r="B25" t="s" s="30">
         <v>16</v>
       </c>
       <c r="C25" s="8"/>
@@ -4383,65 +4413,65 @@
       <c r="E25" s="8"/>
     </row>
     <row r="26" ht="15.35" customHeight="1">
-      <c r="A26" s="29"/>
-      <c r="B26" s="29"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="30"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
     </row>
     <row r="27" ht="15.35" customHeight="1">
-      <c r="A27" t="s" s="29">
-        <v>216</v>
-      </c>
-      <c r="B27" t="s" s="29">
-        <v>217</v>
+      <c r="A27" t="s" s="30">
+        <v>222</v>
+      </c>
+      <c r="B27" t="s" s="30">
+        <v>223</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
     </row>
     <row r="28" ht="15.35" customHeight="1">
-      <c r="A28" s="29"/>
-      <c r="B28" s="29"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
     </row>
     <row r="29" ht="15.35" customHeight="1">
-      <c r="A29" t="s" s="29">
-        <v>218</v>
-      </c>
-      <c r="B29" t="s" s="29">
-        <v>219</v>
+      <c r="A29" t="s" s="30">
+        <v>224</v>
+      </c>
+      <c r="B29" t="s" s="30">
+        <v>225</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
     </row>
     <row r="30" ht="15.35" customHeight="1">
-      <c r="A30" t="s" s="29">
-        <v>220</v>
-      </c>
-      <c r="B30" t="s" s="29">
-        <v>221</v>
+      <c r="A30" t="s" s="30">
+        <v>226</v>
+      </c>
+      <c r="B30" t="s" s="30">
+        <v>227</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
     </row>
     <row r="31" ht="15.35" customHeight="1">
-      <c r="A31" s="29"/>
-      <c r="B31" s="29"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="30"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
     </row>
     <row r="32" ht="15.35" customHeight="1">
-      <c r="A32" t="s" s="29">
-        <v>222</v>
-      </c>
-      <c r="B32" t="s" s="29">
-        <v>90</v>
+      <c r="A32" t="s" s="30">
+        <v>228</v>
+      </c>
+      <c r="B32" t="s" s="30">
+        <v>96</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
@@ -4449,28 +4479,28 @@
     </row>
     <row r="33" ht="15.35" customHeight="1">
       <c r="A33" t="s" s="43">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="B33" t="s" s="43">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
     </row>
     <row r="34" ht="15.35" customHeight="1">
-      <c r="A34" s="29"/>
-      <c r="B34" s="29"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="30"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
     </row>
     <row r="35" ht="15.35" customHeight="1">
       <c r="A35" t="s" s="97">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="B35" t="s" s="97">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -4478,10 +4508,10 @@
     </row>
     <row r="36" ht="14.6" customHeight="1">
       <c r="A36" t="s" s="70">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B36" t="s" s="71">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
@@ -4495,40 +4525,40 @@
       <c r="E37" s="8"/>
     </row>
     <row r="38" ht="14.6" customHeight="1">
-      <c r="A38" t="s" s="26">
-        <v>226</v>
+      <c r="A38" t="s" s="27">
+        <v>232</v>
       </c>
       <c r="B38" t="s" s="73">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
     </row>
     <row r="39" ht="14.6" customHeight="1">
-      <c r="A39" t="s" s="29">
-        <v>228</v>
-      </c>
-      <c r="B39" t="s" s="29">
-        <v>229</v>
+      <c r="A39" t="s" s="30">
+        <v>234</v>
+      </c>
+      <c r="B39" t="s" s="30">
+        <v>235</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
     </row>
     <row r="40" ht="14.6" customHeight="1">
-      <c r="A40" s="29"/>
-      <c r="B40" s="29"/>
+      <c r="A40" s="30"/>
+      <c r="B40" s="30"/>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
     </row>
     <row r="41" ht="14.6" customHeight="1">
-      <c r="A41" t="s" s="29">
-        <v>230</v>
-      </c>
-      <c r="B41" t="s" s="29">
-        <v>231</v>
+      <c r="A41" t="s" s="30">
+        <v>236</v>
+      </c>
+      <c r="B41" t="s" s="30">
+        <v>237</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
@@ -4536,28 +4566,28 @@
     </row>
     <row r="42" ht="14.6" customHeight="1">
       <c r="A42" t="s" s="98">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="B42" t="s" s="98">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
     </row>
     <row r="43" ht="14.6" customHeight="1">
-      <c r="A43" s="29"/>
-      <c r="B43" s="29"/>
+      <c r="A43" s="30"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
     </row>
     <row r="44" ht="14.6" customHeight="1">
-      <c r="A44" t="s" s="29">
-        <v>234</v>
-      </c>
-      <c r="B44" t="s" s="29">
-        <v>235</v>
+      <c r="A44" t="s" s="30">
+        <v>240</v>
+      </c>
+      <c r="B44" t="s" s="30">
+        <v>241</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
@@ -4565,10 +4595,10 @@
     </row>
     <row r="45" ht="14.6" customHeight="1">
       <c r="A45" t="s" s="69">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="B45" t="s" s="67">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
@@ -4576,10 +4606,10 @@
     </row>
     <row r="46" ht="14.6" customHeight="1">
       <c r="A46" t="s" s="99">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B46" t="s" s="100">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="C46" s="101"/>
       <c r="D46" s="101"/>
@@ -4594,10 +4624,10 @@
     </row>
     <row r="48" ht="14.6" customHeight="1">
       <c r="A48" t="s" s="9">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="B48" t="s" s="9">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
@@ -4605,10 +4635,10 @@
     </row>
     <row r="49" ht="14.6" customHeight="1">
       <c r="A49" t="s" s="7">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="B49" t="s" s="7">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
@@ -4616,10 +4646,10 @@
     </row>
     <row r="50" ht="14.6" customHeight="1">
       <c r="A50" t="s" s="9">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="B50" t="s" s="9">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
@@ -5637,7 +5667,7 @@
   <sheetData>
     <row r="1" ht="15.55" customHeight="1">
       <c r="A1" t="s" s="104">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="B1" s="104"/>
       <c r="C1" s="104"/>
@@ -5737,10 +5767,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="14.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="24.5" style="12" customWidth="1"/>
-    <col min="2" max="2" width="61.8516" style="12" customWidth="1"/>
-    <col min="3" max="5" width="16.3516" style="12" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="12" customWidth="1"/>
+    <col min="1" max="1" width="24.5" style="13" customWidth="1"/>
+    <col min="2" max="2" width="61.8516" style="13" customWidth="1"/>
+    <col min="3" max="5" width="16.3516" style="13" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
@@ -5766,7 +5796,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -5777,7 +5807,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -5806,7 +5836,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s" s="9">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -5890,21 +5920,21 @@
     </row>
     <row r="16" ht="26.6" customHeight="1">
       <c r="A16" t="s" s="7">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s" s="7">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
     </row>
     <row r="17" ht="14.6" customHeight="1">
-      <c r="A17" t="s" s="13">
-        <v>45</v>
-      </c>
-      <c r="B17" t="s" s="14">
-        <v>46</v>
+      <c r="A17" t="s" s="14">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s" s="15">
+        <v>52</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -5925,15 +5955,15 @@
       <c r="E19" s="8"/>
     </row>
     <row r="20" ht="14.6" customHeight="1">
-      <c r="A20" s="15"/>
-      <c r="B20" s="16"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
     </row>
     <row r="21" ht="14.6" customHeight="1">
-      <c r="A21" s="17"/>
-      <c r="B21" s="18"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="19"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -5960,15 +5990,15 @@
       <c r="E24" s="10"/>
     </row>
     <row r="25" ht="14.6" customHeight="1">
-      <c r="A25" s="15"/>
-      <c r="B25" s="16"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
     </row>
     <row r="26" ht="14.6" customHeight="1">
-      <c r="A26" s="17"/>
-      <c r="B26" s="18"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="19"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -5981,7 +6011,7 @@
       <c r="E27" s="8"/>
     </row>
     <row r="28" ht="14.6" customHeight="1">
-      <c r="A28" s="19"/>
+      <c r="A28" s="20"/>
       <c r="B28" s="9"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
@@ -6987,10 +7017,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="14.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="28.6719" style="20" customWidth="1"/>
-    <col min="2" max="2" width="61.8516" style="20" customWidth="1"/>
-    <col min="3" max="5" width="16.3516" style="20" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="20" customWidth="1"/>
+    <col min="1" max="1" width="28.6719" style="21" customWidth="1"/>
+    <col min="2" max="2" width="61.8516" style="21" customWidth="1"/>
+    <col min="3" max="5" width="16.3516" style="21" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
@@ -7016,7 +7046,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -7027,7 +7057,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -7056,7 +7086,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s" s="9">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -7125,11 +7155,11 @@
       <c r="E13" s="10"/>
     </row>
     <row r="14" ht="15.35" customHeight="1">
-      <c r="A14" t="s" s="21">
-        <v>50</v>
-      </c>
-      <c r="B14" t="s" s="22">
-        <v>51</v>
+      <c r="A14" t="s" s="22">
+        <v>56</v>
+      </c>
+      <c r="B14" t="s" s="23">
+        <v>57</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -7137,54 +7167,54 @@
     </row>
     <row r="15" ht="14.6" customHeight="1">
       <c r="A15" t="s" s="7">
-        <v>52</v>
-      </c>
-      <c r="B15" t="s" s="22">
-        <v>53</v>
+        <v>58</v>
+      </c>
+      <c r="B15" t="s" s="23">
+        <v>59</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
     </row>
     <row r="16" ht="30.35" customHeight="1">
-      <c r="A16" t="s" s="23">
-        <v>54</v>
+      <c r="A16" t="s" s="24">
+        <v>60</v>
       </c>
       <c r="B16" t="s" s="9">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
     </row>
     <row r="17" ht="14.6" customHeight="1">
-      <c r="A17" t="s" s="22">
-        <v>56</v>
-      </c>
-      <c r="B17" t="s" s="22">
-        <v>57</v>
+      <c r="A17" t="s" s="23">
+        <v>62</v>
+      </c>
+      <c r="B17" t="s" s="23">
+        <v>63</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
     </row>
     <row r="18" ht="14.6" customHeight="1">
-      <c r="A18" t="s" s="24">
-        <v>58</v>
-      </c>
-      <c r="B18" t="s" s="25">
-        <v>59</v>
+      <c r="A18" t="s" s="25">
+        <v>64</v>
+      </c>
+      <c r="B18" t="s" s="26">
+        <v>65</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
     </row>
     <row r="19" ht="14.6" customHeight="1">
-      <c r="A19" t="s" s="26">
-        <v>60</v>
-      </c>
-      <c r="B19" t="s" s="27">
-        <v>61</v>
+      <c r="A19" t="s" s="27">
+        <v>66</v>
+      </c>
+      <c r="B19" t="s" s="28">
+        <v>67</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -7192,10 +7222,10 @@
     </row>
     <row r="20" ht="14.6" customHeight="1">
       <c r="A20" t="s" s="9">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B20" t="s" s="9">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -7203,10 +7233,10 @@
     </row>
     <row r="21" ht="14.6" customHeight="1">
       <c r="A21" t="s" s="7">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B21" t="s" s="7">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -7220,15 +7250,15 @@
       <c r="E22" s="10"/>
     </row>
     <row r="23" ht="14.6" customHeight="1">
-      <c r="A23" s="15"/>
-      <c r="B23" s="16"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="17"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
     </row>
     <row r="24" ht="14.6" customHeight="1">
-      <c r="A24" s="17"/>
-      <c r="B24" s="18"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="19"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -7241,7 +7271,7 @@
       <c r="E25" s="8"/>
     </row>
     <row r="26" ht="14.6" customHeight="1">
-      <c r="A26" s="19"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="9"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -8247,10 +8277,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="14.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="28.6719" style="28" customWidth="1"/>
-    <col min="2" max="2" width="61.8516" style="28" customWidth="1"/>
-    <col min="3" max="5" width="16.3516" style="28" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="28" customWidth="1"/>
+    <col min="1" max="1" width="28.6719" style="29" customWidth="1"/>
+    <col min="2" max="2" width="61.8516" style="29" customWidth="1"/>
+    <col min="3" max="5" width="16.3516" style="29" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
@@ -8276,7 +8306,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -8287,7 +8317,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -8309,7 +8339,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s" s="9">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -8372,10 +8402,10 @@
     </row>
     <row r="12" ht="14.6" customHeight="1">
       <c r="A12" t="s" s="7">
-        <v>69</v>
-      </c>
-      <c r="B12" t="s" s="29">
-        <v>70</v>
+        <v>75</v>
+      </c>
+      <c r="B12" t="s" s="30">
+        <v>76</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -8383,21 +8413,21 @@
     </row>
     <row r="13" ht="14.6" customHeight="1">
       <c r="A13" t="s" s="7">
-        <v>71</v>
-      </c>
-      <c r="B13" t="s" s="29">
-        <v>72</v>
+        <v>77</v>
+      </c>
+      <c r="B13" t="s" s="30">
+        <v>78</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
     </row>
     <row r="14" ht="14.6" customHeight="1">
-      <c r="A14" t="s" s="13">
-        <v>73</v>
-      </c>
-      <c r="B14" t="s" s="30">
-        <v>74</v>
+      <c r="A14" t="s" s="14">
+        <v>79</v>
+      </c>
+      <c r="B14" t="s" s="31">
+        <v>80</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -8405,10 +8435,10 @@
     </row>
     <row r="15" ht="14.6" customHeight="1">
       <c r="A15" t="s" s="9">
-        <v>75</v>
-      </c>
-      <c r="B15" t="s" s="31">
-        <v>76</v>
+        <v>81</v>
+      </c>
+      <c r="B15" t="s" s="12">
+        <v>82</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -8416,21 +8446,21 @@
     </row>
     <row r="16" ht="14.6" customHeight="1">
       <c r="A16" t="s" s="7">
-        <v>77</v>
-      </c>
-      <c r="B16" t="s" s="29">
-        <v>78</v>
+        <v>83</v>
+      </c>
+      <c r="B16" t="s" s="30">
+        <v>84</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
     </row>
     <row r="17" ht="14.6" customHeight="1">
-      <c r="A17" t="s" s="24">
-        <v>79</v>
+      <c r="A17" t="s" s="25">
+        <v>85</v>
       </c>
       <c r="B17" t="s" s="32">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -8438,10 +8468,10 @@
     </row>
     <row r="18" ht="15.35" customHeight="1">
       <c r="A18" t="s" s="33">
-        <v>81</v>
-      </c>
-      <c r="B18" t="s" s="27">
-        <v>82</v>
+        <v>87</v>
+      </c>
+      <c r="B18" t="s" s="28">
+        <v>88</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -8469,15 +8499,15 @@
       <c r="E21" s="10"/>
     </row>
     <row r="22" ht="14.6" customHeight="1">
-      <c r="A22" s="15"/>
-      <c r="B22" s="16"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="17"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
     </row>
     <row r="23" ht="14.6" customHeight="1">
-      <c r="A23" s="17"/>
-      <c r="B23" s="18"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="19"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -8490,7 +8520,7 @@
       <c r="E24" s="8"/>
     </row>
     <row r="25" ht="14.6" customHeight="1">
-      <c r="A25" s="19"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="9"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -9525,7 +9555,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -9536,7 +9566,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -9558,7 +9588,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s" s="9">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -9621,10 +9651,10 @@
     </row>
     <row r="12" ht="14.6" customHeight="1">
       <c r="A12" t="s" s="7">
-        <v>69</v>
-      </c>
-      <c r="B12" t="s" s="29">
-        <v>70</v>
+        <v>75</v>
+      </c>
+      <c r="B12" t="s" s="30">
+        <v>76</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -9632,21 +9662,21 @@
     </row>
     <row r="13" ht="14.6" customHeight="1">
       <c r="A13" t="s" s="7">
-        <v>71</v>
-      </c>
-      <c r="B13" t="s" s="29">
-        <v>72</v>
+        <v>77</v>
+      </c>
+      <c r="B13" t="s" s="30">
+        <v>78</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
     </row>
     <row r="14" ht="14.6" customHeight="1">
-      <c r="A14" t="s" s="13">
-        <v>73</v>
-      </c>
-      <c r="B14" t="s" s="30">
-        <v>74</v>
+      <c r="A14" t="s" s="14">
+        <v>79</v>
+      </c>
+      <c r="B14" t="s" s="31">
+        <v>80</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -9654,10 +9684,10 @@
     </row>
     <row r="15" ht="14.6" customHeight="1">
       <c r="A15" t="s" s="9">
-        <v>75</v>
-      </c>
-      <c r="B15" t="s" s="31">
-        <v>76</v>
+        <v>81</v>
+      </c>
+      <c r="B15" t="s" s="12">
+        <v>82</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -9665,21 +9695,21 @@
     </row>
     <row r="16" ht="14.6" customHeight="1">
       <c r="A16" t="s" s="7">
-        <v>77</v>
-      </c>
-      <c r="B16" t="s" s="29">
-        <v>78</v>
+        <v>83</v>
+      </c>
+      <c r="B16" t="s" s="30">
+        <v>84</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
     </row>
     <row r="17" ht="14.6" customHeight="1">
-      <c r="A17" t="s" s="24">
-        <v>79</v>
+      <c r="A17" t="s" s="25">
+        <v>85</v>
       </c>
       <c r="B17" t="s" s="32">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -9687,10 +9717,10 @@
     </row>
     <row r="18" ht="15.35" customHeight="1">
       <c r="A18" t="s" s="33">
-        <v>81</v>
-      </c>
-      <c r="B18" t="s" s="27">
-        <v>82</v>
+        <v>87</v>
+      </c>
+      <c r="B18" t="s" s="28">
+        <v>88</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -9718,15 +9748,15 @@
       <c r="E21" s="10"/>
     </row>
     <row r="22" ht="14.6" customHeight="1">
-      <c r="A22" s="15"/>
-      <c r="B22" s="16"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="17"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
     </row>
     <row r="23" ht="14.6" customHeight="1">
-      <c r="A23" s="17"/>
-      <c r="B23" s="18"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="19"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -9739,7 +9769,7 @@
       <c r="E24" s="8"/>
     </row>
     <row r="25" ht="14.6" customHeight="1">
-      <c r="A25" s="19"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="9"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -10774,7 +10804,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -10785,7 +10815,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -10807,7 +10837,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s" s="9">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -10848,10 +10878,10 @@
     </row>
     <row r="10" ht="26.6" customHeight="1">
       <c r="A10" t="s" s="9">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B10" t="s" s="9">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -10859,10 +10889,10 @@
     </row>
     <row r="11" ht="26.6" customHeight="1">
       <c r="A11" t="s" s="9">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B11" t="s" s="9">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -10870,10 +10900,10 @@
     </row>
     <row r="12" ht="26.6" customHeight="1">
       <c r="A12" t="s" s="9">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s" s="9">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -10881,10 +10911,10 @@
     </row>
     <row r="13" ht="26.6" customHeight="1">
       <c r="A13" t="s" s="9">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B13" t="s" s="9">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -10892,10 +10922,10 @@
     </row>
     <row r="14" ht="26.6" customHeight="1">
       <c r="A14" t="s" s="9">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B14" t="s" s="9">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -10913,11 +10943,11 @@
       <c r="E15" s="10"/>
     </row>
     <row r="16" ht="15.35" customHeight="1">
-      <c r="A16" t="s" s="21">
-        <v>99</v>
+      <c r="A16" t="s" s="22">
+        <v>105</v>
       </c>
       <c r="B16" t="s" s="36">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -10925,10 +10955,10 @@
     </row>
     <row r="17" ht="14.6" customHeight="1">
       <c r="A17" t="s" s="7">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B17" t="s" s="37">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -10936,43 +10966,43 @@
     </row>
     <row r="18" ht="14.6" customHeight="1">
       <c r="A18" t="s" s="7">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B18" t="s" s="38">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
     </row>
     <row r="19" ht="15.35" customHeight="1">
-      <c r="A19" t="s" s="23">
-        <v>105</v>
+      <c r="A19" t="s" s="24">
+        <v>111</v>
       </c>
       <c r="B19" t="s" s="9">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
     </row>
     <row r="20" ht="14.6" customHeight="1">
-      <c r="A20" t="s" s="22">
-        <v>107</v>
-      </c>
-      <c r="B20" t="s" s="29">
-        <v>108</v>
+      <c r="A20" t="s" s="23">
+        <v>113</v>
+      </c>
+      <c r="B20" t="s" s="30">
+        <v>114</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
     </row>
     <row r="21" ht="14.6" customHeight="1">
-      <c r="A21" t="s" s="13">
-        <v>109</v>
+      <c r="A21" t="s" s="14">
+        <v>115</v>
       </c>
       <c r="B21" t="s" s="39">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -10980,10 +11010,10 @@
     </row>
     <row r="22" ht="15.35" customHeight="1">
       <c r="A22" t="s" s="9">
-        <v>111</v>
-      </c>
-      <c r="B22" t="s" s="23">
-        <v>112</v>
+        <v>117</v>
+      </c>
+      <c r="B22" t="s" s="24">
+        <v>118</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -10991,10 +11021,10 @@
     </row>
     <row r="23" ht="15.35" customHeight="1">
       <c r="A23" t="s" s="7">
-        <v>113</v>
-      </c>
-      <c r="B23" t="s" s="21">
-        <v>102</v>
+        <v>119</v>
+      </c>
+      <c r="B23" t="s" s="22">
+        <v>108</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
@@ -11002,10 +11032,10 @@
     </row>
     <row r="24" ht="15.35" customHeight="1">
       <c r="A24" t="s" s="7">
-        <v>114</v>
-      </c>
-      <c r="B24" t="s" s="21">
-        <v>104</v>
+        <v>120</v>
+      </c>
+      <c r="B24" t="s" s="22">
+        <v>110</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -11013,43 +11043,43 @@
     </row>
     <row r="25" ht="15.35" customHeight="1">
       <c r="A25" t="s" s="9">
-        <v>115</v>
-      </c>
-      <c r="B25" t="s" s="23">
-        <v>106</v>
+        <v>121</v>
+      </c>
+      <c r="B25" t="s" s="24">
+        <v>112</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
     </row>
     <row r="26" ht="14.6" customHeight="1">
-      <c r="A26" t="s" s="24">
-        <v>116</v>
+      <c r="A26" t="s" s="25">
+        <v>122</v>
       </c>
       <c r="B26" t="s" s="40">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
     </row>
     <row r="27" ht="14.6" customHeight="1">
-      <c r="A27" t="s" s="26">
-        <v>118</v>
+      <c r="A27" t="s" s="27">
+        <v>124</v>
       </c>
       <c r="B27" t="s" s="41">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
     </row>
     <row r="28" ht="15.35" customHeight="1">
-      <c r="A28" t="s" s="21">
-        <v>119</v>
-      </c>
-      <c r="B28" t="s" s="21">
-        <v>120</v>
+      <c r="A28" t="s" s="22">
+        <v>125</v>
+      </c>
+      <c r="B28" t="s" s="22">
+        <v>126</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -11057,10 +11087,10 @@
     </row>
     <row r="29" ht="15.35" customHeight="1">
       <c r="A29" t="s" s="42">
-        <v>121</v>
-      </c>
-      <c r="B29" t="s" s="23">
-        <v>122</v>
+        <v>127</v>
+      </c>
+      <c r="B29" t="s" s="24">
+        <v>128</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
@@ -11068,10 +11098,10 @@
     </row>
     <row r="30" ht="14.6" customHeight="1">
       <c r="A30" t="s" s="43">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B30" t="s" s="43">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -11079,10 +11109,10 @@
     </row>
     <row r="31" ht="14.6" customHeight="1">
       <c r="A31" t="s" s="44">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B31" t="s" s="44">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
@@ -11090,10 +11120,10 @@
     </row>
     <row r="32" ht="14.6" customHeight="1">
       <c r="A32" t="s" s="44">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B32" t="s" s="43">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
@@ -11101,10 +11131,10 @@
     </row>
     <row r="33" ht="14.6" customHeight="1">
       <c r="A33" t="s" s="9">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B33" t="s" s="9">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -12111,7 +12141,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -12122,7 +12152,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -12151,7 +12181,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s" s="9">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -12205,87 +12235,87 @@
       <c r="E12" s="8"/>
     </row>
     <row r="13" ht="15.35" customHeight="1">
-      <c r="A13" s="21"/>
-      <c r="B13" s="22"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
     </row>
     <row r="14" ht="15.35" customHeight="1">
-      <c r="A14" t="s" s="29">
-        <v>134</v>
-      </c>
-      <c r="B14" t="s" s="29">
-        <v>135</v>
+      <c r="A14" t="s" s="30">
+        <v>140</v>
+      </c>
+      <c r="B14" t="s" s="30">
+        <v>141</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
     </row>
     <row r="15" ht="15.35" customHeight="1">
-      <c r="A15" t="s" s="21">
-        <v>136</v>
+      <c r="A15" t="s" s="22">
+        <v>142</v>
       </c>
       <c r="B15" t="s" s="7">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
     </row>
     <row r="16" ht="15.35" customHeight="1">
-      <c r="A16" s="29"/>
-      <c r="B16" s="29"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
     </row>
     <row r="17" ht="15.35" customHeight="1">
-      <c r="A17" t="s" s="29">
-        <v>138</v>
-      </c>
-      <c r="B17" t="s" s="29">
-        <v>139</v>
+      <c r="A17" t="s" s="30">
+        <v>144</v>
+      </c>
+      <c r="B17" t="s" s="30">
+        <v>145</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
     </row>
     <row r="18" ht="15.35" customHeight="1">
-      <c r="A18" t="s" s="23">
-        <v>54</v>
+      <c r="A18" t="s" s="24">
+        <v>60</v>
       </c>
       <c r="B18" t="s" s="9">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
     </row>
     <row r="19" ht="15.35" customHeight="1">
-      <c r="A19" t="s" s="22">
-        <v>56</v>
-      </c>
-      <c r="B19" t="s" s="22">
-        <v>57</v>
+      <c r="A19" t="s" s="23">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s" s="23">
+        <v>63</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
     </row>
     <row r="20" ht="15.35" customHeight="1">
-      <c r="A20" s="21"/>
-      <c r="B20" s="22"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
     </row>
     <row r="21" ht="15.35" customHeight="1">
       <c r="A21" t="s" s="9">
-        <v>62</v>
-      </c>
-      <c r="B21" t="s" s="22">
-        <v>140</v>
+        <v>68</v>
+      </c>
+      <c r="B21" t="s" s="23">
+        <v>146</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -12293,10 +12323,10 @@
     </row>
     <row r="22" ht="15.35" customHeight="1">
       <c r="A22" t="s" s="7">
-        <v>64</v>
-      </c>
-      <c r="B22" t="s" s="22">
-        <v>65</v>
+        <v>70</v>
+      </c>
+      <c r="B22" t="s" s="23">
+        <v>71</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -12304,119 +12334,119 @@
     </row>
     <row r="23" ht="15.35" customHeight="1">
       <c r="A23" s="7"/>
-      <c r="B23" s="22"/>
+      <c r="B23" s="23"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
     </row>
     <row r="24" ht="15.35" customHeight="1">
-      <c r="A24" t="s" s="21">
-        <v>141</v>
-      </c>
-      <c r="B24" t="s" s="22">
-        <v>142</v>
+      <c r="A24" t="s" s="22">
+        <v>147</v>
+      </c>
+      <c r="B24" t="s" s="23">
+        <v>148</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
     </row>
     <row r="25" ht="15.35" customHeight="1">
-      <c r="A25" t="s" s="21">
-        <v>143</v>
-      </c>
-      <c r="B25" t="s" s="22">
-        <v>144</v>
+      <c r="A25" t="s" s="22">
+        <v>149</v>
+      </c>
+      <c r="B25" t="s" s="23">
+        <v>150</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
     </row>
     <row r="26" ht="15.35" customHeight="1">
-      <c r="A26" t="s" s="21">
-        <v>145</v>
-      </c>
-      <c r="B26" t="s" s="22">
-        <v>146</v>
+      <c r="A26" t="s" s="22">
+        <v>151</v>
+      </c>
+      <c r="B26" t="s" s="23">
+        <v>152</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
     </row>
     <row r="27" ht="15.35" customHeight="1">
-      <c r="A27" s="21"/>
-      <c r="B27" s="22"/>
+      <c r="A27" s="22"/>
+      <c r="B27" s="23"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
     </row>
     <row r="28" ht="15.35" customHeight="1">
-      <c r="A28" t="s" s="29">
-        <v>147</v>
-      </c>
-      <c r="B28" t="s" s="29">
-        <v>148</v>
+      <c r="A28" t="s" s="30">
+        <v>153</v>
+      </c>
+      <c r="B28" t="s" s="30">
+        <v>154</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
     </row>
     <row r="29" ht="15.35" customHeight="1">
-      <c r="A29" t="s" s="29">
-        <v>149</v>
-      </c>
-      <c r="B29" t="s" s="29">
-        <v>150</v>
+      <c r="A29" t="s" s="30">
+        <v>155</v>
+      </c>
+      <c r="B29" t="s" s="30">
+        <v>156</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
     </row>
     <row r="30" ht="15.35" customHeight="1">
-      <c r="A30" t="s" s="29">
-        <v>151</v>
-      </c>
-      <c r="B30" t="s" s="29">
-        <v>152</v>
+      <c r="A30" t="s" s="30">
+        <v>157</v>
+      </c>
+      <c r="B30" t="s" s="30">
+        <v>158</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
     </row>
     <row r="31" ht="15.35" customHeight="1">
-      <c r="A31" s="21"/>
-      <c r="B31" s="22"/>
+      <c r="A31" s="22"/>
+      <c r="B31" s="23"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
     </row>
     <row r="32" ht="15.35" customHeight="1">
       <c r="A32" t="s" s="46">
-        <v>153</v>
-      </c>
-      <c r="B32" t="s" s="25">
-        <v>154</v>
+        <v>159</v>
+      </c>
+      <c r="B32" t="s" s="26">
+        <v>160</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
     </row>
     <row r="33" ht="14.6" customHeight="1">
-      <c r="A33" t="s" s="13">
-        <v>155</v>
+      <c r="A33" t="s" s="14">
+        <v>161</v>
       </c>
       <c r="B33" t="s" s="47">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
     </row>
     <row r="34" ht="14.6" customHeight="1">
-      <c r="A34" t="s" s="24">
-        <v>156</v>
-      </c>
-      <c r="B34" t="s" s="25">
-        <v>59</v>
+      <c r="A34" t="s" s="25">
+        <v>162</v>
+      </c>
+      <c r="B34" t="s" s="26">
+        <v>65</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
@@ -12430,11 +12460,11 @@
       <c r="E35" s="8"/>
     </row>
     <row r="36" ht="14.6" customHeight="1">
-      <c r="A36" t="s" s="26">
-        <v>60</v>
-      </c>
-      <c r="B36" t="s" s="27">
-        <v>61</v>
+      <c r="A36" t="s" s="27">
+        <v>66</v>
+      </c>
+      <c r="B36" t="s" s="28">
+        <v>67</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
@@ -12442,28 +12472,28 @@
     </row>
     <row r="37" ht="14.6" customHeight="1">
       <c r="A37" t="s" s="7">
-        <v>52</v>
-      </c>
-      <c r="B37" t="s" s="22">
-        <v>53</v>
+        <v>58</v>
+      </c>
+      <c r="B37" t="s" s="23">
+        <v>59</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
     </row>
     <row r="38" ht="14.6" customHeight="1">
-      <c r="A38" s="29"/>
-      <c r="B38" s="29"/>
+      <c r="A38" s="30"/>
+      <c r="B38" s="30"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
     </row>
     <row r="39" ht="14.6" customHeight="1">
-      <c r="A39" t="s" s="29">
-        <v>129</v>
-      </c>
-      <c r="B39" t="s" s="29">
-        <v>130</v>
+      <c r="A39" t="s" s="30">
+        <v>135</v>
+      </c>
+      <c r="B39" t="s" s="30">
+        <v>136</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
@@ -12478,7 +12508,7 @@
     </row>
     <row r="41" ht="14.6" customHeight="1">
       <c r="A41" t="s" s="52">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B41" s="53">
         <v>0</v>
@@ -12489,7 +12519,7 @@
     </row>
     <row r="42" ht="14.6" customHeight="1">
       <c r="A42" t="s" s="54">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B42" s="55">
         <v>1</v>
@@ -12500,7 +12530,7 @@
     </row>
     <row r="43" ht="14.6" customHeight="1">
       <c r="A43" t="s" s="56">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="B43" s="57">
         <v>2</v>
@@ -12511,7 +12541,7 @@
     </row>
     <row r="44" ht="14.6" customHeight="1">
       <c r="A44" t="s" s="58">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="B44" s="59">
         <v>3</v>
@@ -12522,7 +12552,7 @@
     </row>
     <row r="45" ht="14.6" customHeight="1">
       <c r="A45" t="s" s="60">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B45" s="61">
         <v>4</v>
@@ -12533,7 +12563,7 @@
     </row>
     <row r="46" ht="14.6" customHeight="1">
       <c r="A46" t="s" s="58">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B46" s="59">
         <v>5</v>
@@ -12544,7 +12574,7 @@
     </row>
     <row r="47" ht="14.6" customHeight="1">
       <c r="A47" t="s" s="62">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B47" s="63">
         <v>6</v>
@@ -13568,7 +13598,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -13579,7 +13609,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -13608,7 +13638,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s" s="9">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -13662,44 +13692,44 @@
       <c r="E12" s="8"/>
     </row>
     <row r="13" ht="15.35" customHeight="1">
-      <c r="A13" s="21"/>
-      <c r="B13" s="22"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
     </row>
     <row r="14" ht="15.35" customHeight="1">
-      <c r="A14" t="s" s="29">
-        <v>134</v>
-      </c>
-      <c r="B14" t="s" s="29">
-        <v>167</v>
+      <c r="A14" t="s" s="30">
+        <v>140</v>
+      </c>
+      <c r="B14" t="s" s="30">
+        <v>173</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
     </row>
     <row r="15" ht="15.35" customHeight="1">
-      <c r="A15" t="s" s="21">
-        <v>168</v>
+      <c r="A15" t="s" s="22">
+        <v>174</v>
       </c>
       <c r="B15" t="s" s="7">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
     </row>
     <row r="16" ht="15.35" customHeight="1">
-      <c r="A16" s="21"/>
-      <c r="B16" s="22"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="23"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
     </row>
     <row r="17" ht="15.35" customHeight="1">
       <c r="A17" t="s" s="52">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B17" s="53">
         <v>0</v>
@@ -13710,7 +13740,7 @@
     </row>
     <row r="18" ht="15.35" customHeight="1">
       <c r="A18" t="s" s="54">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B18" s="55">
         <v>1</v>
@@ -13721,7 +13751,7 @@
     </row>
     <row r="19" ht="15.35" customHeight="1">
       <c r="A19" t="s" s="54">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B19" s="57">
         <v>2</v>
@@ -13732,7 +13762,7 @@
     </row>
     <row r="20" ht="15.35" customHeight="1">
       <c r="A20" t="s" s="56">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="B20" s="65">
         <v>3</v>
@@ -13743,7 +13773,7 @@
     </row>
     <row r="21" ht="15.35" customHeight="1">
       <c r="A21" t="s" s="58">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="B21" s="61">
         <v>4</v>
@@ -13754,7 +13784,7 @@
     </row>
     <row r="22" ht="15.35" customHeight="1">
       <c r="A22" t="s" s="60">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B22" s="59">
         <v>5</v>
@@ -13765,7 +13795,7 @@
     </row>
     <row r="23" ht="15.35" customHeight="1">
       <c r="A23" t="s" s="58">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B23" s="63">
         <v>6</v>
@@ -13776,28 +13806,28 @@
     </row>
     <row r="24" ht="15.35" customHeight="1">
       <c r="A24" t="s" s="62">
-        <v>163</v>
-      </c>
-      <c r="B24" t="s" s="22">
-        <v>171</v>
+        <v>169</v>
+      </c>
+      <c r="B24" t="s" s="23">
+        <v>177</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
     </row>
     <row r="25" ht="15.35" customHeight="1">
-      <c r="A25" s="21"/>
-      <c r="B25" s="22"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="23"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
     </row>
     <row r="26" ht="15.35" customHeight="1">
       <c r="A26" t="s" s="9">
-        <v>69</v>
-      </c>
-      <c r="B26" t="s" s="29">
-        <v>70</v>
+        <v>75</v>
+      </c>
+      <c r="B26" t="s" s="30">
+        <v>76</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
@@ -13805,10 +13835,10 @@
     </row>
     <row r="27" ht="15.35" customHeight="1">
       <c r="A27" t="s" s="7">
-        <v>71</v>
-      </c>
-      <c r="B27" t="s" s="29">
-        <v>72</v>
+        <v>77</v>
+      </c>
+      <c r="B27" t="s" s="30">
+        <v>78</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -13816,10 +13846,10 @@
     </row>
     <row r="28" ht="15.35" customHeight="1">
       <c r="A28" t="s" s="7">
-        <v>75</v>
-      </c>
-      <c r="B28" t="s" s="29">
-        <v>76</v>
+        <v>81</v>
+      </c>
+      <c r="B28" t="s" s="30">
+        <v>82</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
@@ -13827,61 +13857,61 @@
     </row>
     <row r="29" ht="15.35" customHeight="1">
       <c r="A29" t="s" s="7">
-        <v>77</v>
-      </c>
-      <c r="B29" t="s" s="29">
-        <v>172</v>
+        <v>83</v>
+      </c>
+      <c r="B29" t="s" s="30">
+        <v>178</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
     </row>
     <row r="30" ht="15.35" customHeight="1">
-      <c r="A30" s="21"/>
-      <c r="B30" s="22"/>
+      <c r="A30" s="22"/>
+      <c r="B30" s="23"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
     </row>
     <row r="31" ht="15.35" customHeight="1">
-      <c r="A31" t="s" s="21">
-        <v>173</v>
-      </c>
-      <c r="B31" t="s" s="22">
-        <v>174</v>
+      <c r="A31" t="s" s="22">
+        <v>179</v>
+      </c>
+      <c r="B31" t="s" s="23">
+        <v>180</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
     </row>
     <row r="32" ht="15.35" customHeight="1">
-      <c r="A32" t="s" s="21">
-        <v>52</v>
-      </c>
-      <c r="B32" t="s" s="29">
-        <v>175</v>
+      <c r="A32" t="s" s="22">
+        <v>58</v>
+      </c>
+      <c r="B32" t="s" s="30">
+        <v>181</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
     </row>
     <row r="33" ht="15.35" customHeight="1">
-      <c r="A33" t="s" s="29">
-        <v>176</v>
-      </c>
-      <c r="B33" t="s" s="29">
-        <v>177</v>
+      <c r="A33" t="s" s="30">
+        <v>182</v>
+      </c>
+      <c r="B33" t="s" s="30">
+        <v>183</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
     </row>
     <row r="34" ht="15.35" customHeight="1">
-      <c r="A34" t="s" s="29">
-        <v>178</v>
-      </c>
-      <c r="B34" t="s" s="29">
-        <v>177</v>
+      <c r="A34" t="s" s="30">
+        <v>184</v>
+      </c>
+      <c r="B34" t="s" s="30">
+        <v>183</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
@@ -13889,39 +13919,39 @@
     </row>
     <row r="35" ht="15.35" customHeight="1">
       <c r="A35" t="s" s="43">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="B35" t="s" s="43">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
     </row>
     <row r="36" ht="15.35" customHeight="1">
-      <c r="A36" t="s" s="29">
-        <v>181</v>
-      </c>
-      <c r="B36" t="s" s="29">
-        <v>182</v>
+      <c r="A36" t="s" s="30">
+        <v>187</v>
+      </c>
+      <c r="B36" t="s" s="30">
+        <v>188</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
     </row>
     <row r="37" ht="15.35" customHeight="1">
-      <c r="A37" s="21"/>
-      <c r="B37" s="22"/>
+      <c r="A37" s="22"/>
+      <c r="B37" s="23"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
     </row>
     <row r="38" ht="15.35" customHeight="1">
       <c r="A38" t="s" s="66">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="B38" t="s" s="67">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
@@ -13929,10 +13959,10 @@
     </row>
     <row r="39" ht="14.6" customHeight="1">
       <c r="A39" t="s" s="68">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="B39" t="s" s="47">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
@@ -13940,10 +13970,10 @@
     </row>
     <row r="40" ht="14.6" customHeight="1">
       <c r="A40" t="s" s="69">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="B40" t="s" s="67">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
@@ -13951,10 +13981,10 @@
     </row>
     <row r="41" ht="14.6" customHeight="1">
       <c r="A41" t="s" s="70">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="B41" t="s" s="71">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
@@ -13962,43 +13992,43 @@
     </row>
     <row r="42" ht="14.6" customHeight="1">
       <c r="A42" t="s" s="72">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B42" t="s" s="73">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
     </row>
     <row r="43" ht="14.6" customHeight="1">
-      <c r="A43" t="s" s="29">
-        <v>192</v>
-      </c>
-      <c r="B43" t="s" s="29">
-        <v>193</v>
+      <c r="A43" t="s" s="30">
+        <v>198</v>
+      </c>
+      <c r="B43" t="s" s="30">
+        <v>199</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
     </row>
     <row r="44" ht="14.6" customHeight="1">
-      <c r="A44" t="s" s="29">
-        <v>194</v>
-      </c>
-      <c r="B44" t="s" s="29">
-        <v>195</v>
+      <c r="A44" t="s" s="30">
+        <v>200</v>
+      </c>
+      <c r="B44" t="s" s="30">
+        <v>201</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
     </row>
     <row r="45" ht="14.6" customHeight="1">
-      <c r="A45" t="s" s="29">
-        <v>196</v>
-      </c>
-      <c r="B45" t="s" s="29">
-        <v>197</v>
+      <c r="A45" t="s" s="30">
+        <v>202</v>
+      </c>
+      <c r="B45" t="s" s="30">
+        <v>203</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
@@ -14006,10 +14036,10 @@
     </row>
     <row r="46" ht="14.6" customHeight="1">
       <c r="A46" t="s" s="69">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B46" t="s" s="67">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
@@ -14017,10 +14047,10 @@
     </row>
     <row r="47" ht="14.6" customHeight="1">
       <c r="A47" t="s" s="74">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="B47" t="s" s="75">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="C47" s="76"/>
       <c r="D47" s="76"/>
@@ -14028,10 +14058,10 @@
     </row>
     <row r="48" ht="14.6" customHeight="1">
       <c r="A48" t="s" s="78">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="B48" t="s" s="79">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="C48" s="80"/>
       <c r="D48" s="80"/>
@@ -15087,7 +15117,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -15098,7 +15128,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -15127,7 +15157,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s" s="9">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -15171,7 +15201,7 @@
     </row>
     <row r="12" ht="14.6" customHeight="1">
       <c r="A12" t="s" s="7">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="B12" t="s" s="7">
         <v>29</v>
@@ -15181,15 +15211,15 @@
       <c r="E12" s="8"/>
     </row>
     <row r="13" ht="15.35" customHeight="1">
-      <c r="A13" s="21"/>
-      <c r="B13" s="22"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
     </row>
     <row r="14" ht="15.35" customHeight="1">
       <c r="A14" t="s" s="52">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B14" s="53">
         <v>0</v>
@@ -15200,7 +15230,7 @@
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" t="s" s="54">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B15" s="57">
         <v>1</v>
@@ -15211,7 +15241,7 @@
     </row>
     <row r="16" ht="15.35" customHeight="1">
       <c r="A16" t="s" s="56">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="B16" s="65">
         <v>2</v>
@@ -15222,7 +15252,7 @@
     </row>
     <row r="17" ht="15.35" customHeight="1">
       <c r="A17" t="s" s="58">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="B17" s="59">
         <v>3</v>
@@ -15233,7 +15263,7 @@
     </row>
     <row r="18" ht="15.35" customHeight="1">
       <c r="A18" t="s" s="60">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B18" s="61">
         <v>4</v>
@@ -15244,7 +15274,7 @@
     </row>
     <row r="19" ht="15.35" customHeight="1">
       <c r="A19" t="s" s="58">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B19" s="59">
         <v>5</v>
@@ -15255,7 +15285,7 @@
     </row>
     <row r="20" ht="15.35" customHeight="1">
       <c r="A20" t="s" s="62">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B20" s="63">
         <v>6</v>
@@ -15265,18 +15295,18 @@
       <c r="E20" s="8"/>
     </row>
     <row r="21" ht="15.35" customHeight="1">
-      <c r="A21" s="21"/>
-      <c r="B21" s="22"/>
+      <c r="A21" s="22"/>
+      <c r="B21" s="23"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
     </row>
     <row r="22" ht="15.35" customHeight="1">
       <c r="A22" t="s" s="9">
-        <v>208</v>
-      </c>
-      <c r="B22" t="s" s="29">
-        <v>186</v>
+        <v>214</v>
+      </c>
+      <c r="B22" t="s" s="30">
+        <v>192</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -15284,56 +15314,56 @@
     </row>
     <row r="23" ht="15.35" customHeight="1">
       <c r="A23" s="7"/>
-      <c r="B23" s="29"/>
+      <c r="B23" s="30"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
     </row>
     <row r="24" ht="15.35" customHeight="1">
       <c r="A24" s="7"/>
-      <c r="B24" s="29"/>
+      <c r="B24" s="30"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
     </row>
     <row r="25" ht="15.35" customHeight="1">
       <c r="A25" s="7"/>
-      <c r="B25" s="29"/>
+      <c r="B25" s="30"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
     </row>
     <row r="26" ht="15.35" customHeight="1">
-      <c r="A26" s="21"/>
-      <c r="B26" s="22"/>
+      <c r="A26" s="22"/>
+      <c r="B26" s="23"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
     </row>
     <row r="27" ht="15.35" customHeight="1">
-      <c r="A27" s="21"/>
-      <c r="B27" s="22"/>
+      <c r="A27" s="22"/>
+      <c r="B27" s="23"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
     </row>
     <row r="28" ht="15.35" customHeight="1">
-      <c r="A28" s="21"/>
-      <c r="B28" s="29"/>
+      <c r="A28" s="22"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
     </row>
     <row r="29" ht="15.35" customHeight="1">
-      <c r="A29" s="29"/>
-      <c r="B29" s="29"/>
+      <c r="A29" s="30"/>
+      <c r="B29" s="30"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
     </row>
     <row r="30" ht="15.35" customHeight="1">
-      <c r="A30" s="29"/>
-      <c r="B30" s="29"/>
+      <c r="A30" s="30"/>
+      <c r="B30" s="30"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
@@ -15346,15 +15376,15 @@
       <c r="E31" s="8"/>
     </row>
     <row r="32" ht="15.35" customHeight="1">
-      <c r="A32" s="29"/>
-      <c r="B32" s="29"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="30"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
     </row>
     <row r="33" ht="15.35" customHeight="1">
-      <c r="A33" s="21"/>
-      <c r="B33" s="22"/>
+      <c r="A33" s="22"/>
+      <c r="B33" s="23"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
@@ -15395,22 +15425,22 @@
       <c r="E38" s="8"/>
     </row>
     <row r="39" ht="14.6" customHeight="1">
-      <c r="A39" s="29"/>
-      <c r="B39" s="29"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="30"/>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
     </row>
     <row r="40" ht="14.6" customHeight="1">
-      <c r="A40" s="29"/>
-      <c r="B40" s="29"/>
+      <c r="A40" s="30"/>
+      <c r="B40" s="30"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
     </row>
     <row r="41" ht="14.6" customHeight="1">
-      <c r="A41" s="29"/>
-      <c r="B41" s="29"/>
+      <c r="A41" s="30"/>
+      <c r="B41" s="30"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>

</xml_diff>

<commit_message>
MGT 7 year Bug
Fixed Duplicate entries for Principal business activities due to date format mismatch in db and date manipulation
</commit_message>
<xml_diff>
--- a/DataExtraction/Input/Config.xlsx
+++ b/DataExtraction/Input/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="252">
   <si>
     <t>Key</t>
   </si>
@@ -98,7 +98,7 @@
     <t>year_field_name</t>
   </si>
   <si>
-    <t>Year</t>
+    <t>year</t>
   </si>
   <si>
     <t>Hold_Sub_Assoc_column_name</t>
@@ -561,9 +561,6 @@
   </si>
   <si>
     <t>year_column_name</t>
-  </si>
-  <si>
-    <t>year</t>
   </si>
   <si>
     <t>stated_on</t>
@@ -4184,7 +4181,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -4195,7 +4192,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -4224,7 +4221,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s" s="9">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -4279,7 +4276,7 @@
     </row>
     <row r="13" ht="14.6" customHeight="1">
       <c r="A13" t="s" s="7">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B13" t="s" s="7">
         <v>29</v>
@@ -4381,10 +4378,10 @@
     </row>
     <row r="23" ht="15.35" customHeight="1">
       <c r="A23" t="s" s="9">
+        <v>217</v>
+      </c>
+      <c r="B23" t="s" s="30">
         <v>218</v>
-      </c>
-      <c r="B23" t="s" s="30">
-        <v>219</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -4392,10 +4389,10 @@
     </row>
     <row r="24" ht="15.35" customHeight="1">
       <c r="A24" t="s" s="30">
+        <v>219</v>
+      </c>
+      <c r="B24" t="s" s="30">
         <v>220</v>
-      </c>
-      <c r="B24" t="s" s="30">
-        <v>221</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -4421,10 +4418,10 @@
     </row>
     <row r="27" ht="15.35" customHeight="1">
       <c r="A27" t="s" s="30">
+        <v>221</v>
+      </c>
+      <c r="B27" t="s" s="30">
         <v>222</v>
-      </c>
-      <c r="B27" t="s" s="30">
-        <v>223</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -4439,10 +4436,10 @@
     </row>
     <row r="29" ht="15.35" customHeight="1">
       <c r="A29" t="s" s="30">
+        <v>223</v>
+      </c>
+      <c r="B29" t="s" s="30">
         <v>224</v>
-      </c>
-      <c r="B29" t="s" s="30">
-        <v>225</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -4450,10 +4447,10 @@
     </row>
     <row r="30" ht="15.35" customHeight="1">
       <c r="A30" t="s" s="30">
+        <v>225</v>
+      </c>
+      <c r="B30" t="s" s="30">
         <v>226</v>
-      </c>
-      <c r="B30" t="s" s="30">
-        <v>227</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -4468,7 +4465,7 @@
     </row>
     <row r="32" ht="15.35" customHeight="1">
       <c r="A32" t="s" s="30">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B32" t="s" s="30">
         <v>96</v>
@@ -4479,7 +4476,7 @@
     </row>
     <row r="33" ht="15.35" customHeight="1">
       <c r="A33" t="s" s="43">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B33" t="s" s="43">
         <v>98</v>
@@ -4497,10 +4494,10 @@
     </row>
     <row r="35" ht="15.35" customHeight="1">
       <c r="A35" t="s" s="97">
+        <v>229</v>
+      </c>
+      <c r="B35" t="s" s="97">
         <v>230</v>
-      </c>
-      <c r="B35" t="s" s="97">
-        <v>231</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -4511,7 +4508,7 @@
         <v>179</v>
       </c>
       <c r="B36" t="s" s="71">
-        <v>180</v>
+        <v>25</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
@@ -4526,10 +4523,10 @@
     </row>
     <row r="38" ht="14.6" customHeight="1">
       <c r="A38" t="s" s="27">
+        <v>231</v>
+      </c>
+      <c r="B38" t="s" s="73">
         <v>232</v>
-      </c>
-      <c r="B38" t="s" s="73">
-        <v>233</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
@@ -4537,10 +4534,10 @@
     </row>
     <row r="39" ht="14.6" customHeight="1">
       <c r="A39" t="s" s="30">
+        <v>233</v>
+      </c>
+      <c r="B39" t="s" s="30">
         <v>234</v>
-      </c>
-      <c r="B39" t="s" s="30">
-        <v>235</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
@@ -4555,10 +4552,10 @@
     </row>
     <row r="41" ht="14.6" customHeight="1">
       <c r="A41" t="s" s="30">
+        <v>235</v>
+      </c>
+      <c r="B41" t="s" s="30">
         <v>236</v>
-      </c>
-      <c r="B41" t="s" s="30">
-        <v>237</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
@@ -4566,10 +4563,10 @@
     </row>
     <row r="42" ht="14.6" customHeight="1">
       <c r="A42" t="s" s="98">
+        <v>237</v>
+      </c>
+      <c r="B42" t="s" s="98">
         <v>238</v>
-      </c>
-      <c r="B42" t="s" s="98">
-        <v>239</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
@@ -4584,10 +4581,10 @@
     </row>
     <row r="44" ht="14.6" customHeight="1">
       <c r="A44" t="s" s="30">
+        <v>239</v>
+      </c>
+      <c r="B44" t="s" s="30">
         <v>240</v>
-      </c>
-      <c r="B44" t="s" s="30">
-        <v>241</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
@@ -4595,10 +4592,10 @@
     </row>
     <row r="45" ht="14.6" customHeight="1">
       <c r="A45" t="s" s="69">
+        <v>241</v>
+      </c>
+      <c r="B45" t="s" s="67">
         <v>242</v>
-      </c>
-      <c r="B45" t="s" s="67">
-        <v>243</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
@@ -4606,10 +4603,10 @@
     </row>
     <row r="46" ht="14.6" customHeight="1">
       <c r="A46" t="s" s="99">
+        <v>243</v>
+      </c>
+      <c r="B46" t="s" s="100">
         <v>244</v>
-      </c>
-      <c r="B46" t="s" s="100">
-        <v>245</v>
       </c>
       <c r="C46" s="101"/>
       <c r="D46" s="101"/>
@@ -4624,10 +4621,10 @@
     </row>
     <row r="48" ht="14.6" customHeight="1">
       <c r="A48" t="s" s="9">
+        <v>245</v>
+      </c>
+      <c r="B48" t="s" s="9">
         <v>246</v>
-      </c>
-      <c r="B48" t="s" s="9">
-        <v>247</v>
       </c>
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
@@ -4635,10 +4632,10 @@
     </row>
     <row r="49" ht="14.6" customHeight="1">
       <c r="A49" t="s" s="7">
+        <v>247</v>
+      </c>
+      <c r="B49" t="s" s="7">
         <v>248</v>
-      </c>
-      <c r="B49" t="s" s="7">
-        <v>249</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
@@ -4646,10 +4643,10 @@
     </row>
     <row r="50" ht="14.6" customHeight="1">
       <c r="A50" t="s" s="9">
+        <v>249</v>
+      </c>
+      <c r="B50" t="s" s="9">
         <v>250</v>
-      </c>
-      <c r="B50" t="s" s="9">
-        <v>251</v>
       </c>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
@@ -5667,7 +5664,7 @@
   <sheetData>
     <row r="1" ht="15.55" customHeight="1">
       <c r="A1" t="s" s="104">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B1" s="104"/>
       <c r="C1" s="104"/>
@@ -13878,7 +13875,7 @@
         <v>179</v>
       </c>
       <c r="B31" t="s" s="23">
-        <v>180</v>
+        <v>25</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
@@ -13889,7 +13886,7 @@
         <v>58</v>
       </c>
       <c r="B32" t="s" s="30">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
@@ -13897,10 +13894,10 @@
     </row>
     <row r="33" ht="15.35" customHeight="1">
       <c r="A33" t="s" s="30">
+        <v>181</v>
+      </c>
+      <c r="B33" t="s" s="30">
         <v>182</v>
-      </c>
-      <c r="B33" t="s" s="30">
-        <v>183</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
@@ -13908,10 +13905,10 @@
     </row>
     <row r="34" ht="15.35" customHeight="1">
       <c r="A34" t="s" s="30">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B34" t="s" s="30">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
@@ -13919,10 +13916,10 @@
     </row>
     <row r="35" ht="15.35" customHeight="1">
       <c r="A35" t="s" s="43">
+        <v>184</v>
+      </c>
+      <c r="B35" t="s" s="43">
         <v>185</v>
-      </c>
-      <c r="B35" t="s" s="43">
-        <v>186</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -13930,10 +13927,10 @@
     </row>
     <row r="36" ht="15.35" customHeight="1">
       <c r="A36" t="s" s="30">
+        <v>186</v>
+      </c>
+      <c r="B36" t="s" s="30">
         <v>187</v>
-      </c>
-      <c r="B36" t="s" s="30">
-        <v>188</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
@@ -13948,10 +13945,10 @@
     </row>
     <row r="38" ht="15.35" customHeight="1">
       <c r="A38" t="s" s="66">
+        <v>188</v>
+      </c>
+      <c r="B38" t="s" s="67">
         <v>189</v>
-      </c>
-      <c r="B38" t="s" s="67">
-        <v>190</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
@@ -13959,10 +13956,10 @@
     </row>
     <row r="39" ht="14.6" customHeight="1">
       <c r="A39" t="s" s="68">
+        <v>190</v>
+      </c>
+      <c r="B39" t="s" s="47">
         <v>191</v>
-      </c>
-      <c r="B39" t="s" s="47">
-        <v>192</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
@@ -13970,10 +13967,10 @@
     </row>
     <row r="40" ht="14.6" customHeight="1">
       <c r="A40" t="s" s="69">
+        <v>192</v>
+      </c>
+      <c r="B40" t="s" s="67">
         <v>193</v>
-      </c>
-      <c r="B40" t="s" s="67">
-        <v>194</v>
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
@@ -13981,7 +13978,7 @@
     </row>
     <row r="41" ht="14.6" customHeight="1">
       <c r="A41" t="s" s="70">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B41" t="s" s="71">
         <v>160</v>
@@ -13992,10 +13989,10 @@
     </row>
     <row r="42" ht="14.6" customHeight="1">
       <c r="A42" t="s" s="72">
+        <v>195</v>
+      </c>
+      <c r="B42" t="s" s="73">
         <v>196</v>
-      </c>
-      <c r="B42" t="s" s="73">
-        <v>197</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
@@ -14003,10 +14000,10 @@
     </row>
     <row r="43" ht="14.6" customHeight="1">
       <c r="A43" t="s" s="30">
+        <v>197</v>
+      </c>
+      <c r="B43" t="s" s="30">
         <v>198</v>
-      </c>
-      <c r="B43" t="s" s="30">
-        <v>199</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
@@ -14014,10 +14011,10 @@
     </row>
     <row r="44" ht="14.6" customHeight="1">
       <c r="A44" t="s" s="30">
+        <v>199</v>
+      </c>
+      <c r="B44" t="s" s="30">
         <v>200</v>
-      </c>
-      <c r="B44" t="s" s="30">
-        <v>201</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
@@ -14025,10 +14022,10 @@
     </row>
     <row r="45" ht="14.6" customHeight="1">
       <c r="A45" t="s" s="30">
+        <v>201</v>
+      </c>
+      <c r="B45" t="s" s="30">
         <v>202</v>
-      </c>
-      <c r="B45" t="s" s="30">
-        <v>203</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
@@ -14036,10 +14033,10 @@
     </row>
     <row r="46" ht="14.6" customHeight="1">
       <c r="A46" t="s" s="69">
+        <v>203</v>
+      </c>
+      <c r="B46" t="s" s="67">
         <v>204</v>
-      </c>
-      <c r="B46" t="s" s="67">
-        <v>205</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
@@ -14047,10 +14044,10 @@
     </row>
     <row r="47" ht="14.6" customHeight="1">
       <c r="A47" t="s" s="74">
+        <v>205</v>
+      </c>
+      <c r="B47" t="s" s="75">
         <v>206</v>
-      </c>
-      <c r="B47" t="s" s="75">
-        <v>207</v>
       </c>
       <c r="C47" s="76"/>
       <c r="D47" s="76"/>
@@ -14058,10 +14055,10 @@
     </row>
     <row r="48" ht="14.6" customHeight="1">
       <c r="A48" t="s" s="78">
+        <v>207</v>
+      </c>
+      <c r="B48" t="s" s="79">
         <v>208</v>
-      </c>
-      <c r="B48" t="s" s="79">
-        <v>209</v>
       </c>
       <c r="C48" s="80"/>
       <c r="D48" s="80"/>
@@ -15117,7 +15114,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -15128,7 +15125,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -15157,7 +15154,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s" s="9">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -15201,7 +15198,7 @@
     </row>
     <row r="12" ht="14.6" customHeight="1">
       <c r="A12" t="s" s="7">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B12" t="s" s="7">
         <v>29</v>
@@ -15303,10 +15300,10 @@
     </row>
     <row r="22" ht="15.35" customHeight="1">
       <c r="A22" t="s" s="9">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B22" t="s" s="30">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>

</xml_diff>

<commit_message>
DIR other than directors Code Dev
</commit_message>
<xml_diff>
--- a/DataExtraction/Input/Config.xlsx
+++ b/DataExtraction/Input/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="274">
   <si>
     <t>Key</t>
   </si>
@@ -434,6 +434,96 @@
     <t>filing_date</t>
   </si>
   <si>
+    <t>age_column_name</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>name_column_name</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>name_first_name_node_name</t>
+  </si>
+  <si>
+    <t>FIRST_NAME</t>
+  </si>
+  <si>
+    <t>name_second_name_node_name</t>
+  </si>
+  <si>
+    <t>MIDDLE_NAME</t>
+  </si>
+  <si>
+    <t>name_last_name_node_name</t>
+  </si>
+  <si>
+    <t>LAST_NAME</t>
+  </si>
+  <si>
+    <t>father_name_column_name</t>
+  </si>
+  <si>
+    <t>father_name</t>
+  </si>
+  <si>
+    <t>father_name_first_name_node_name</t>
+  </si>
+  <si>
+    <t>FIRST_NAME1</t>
+  </si>
+  <si>
+    <t>father_name_second_name_node_name</t>
+  </si>
+  <si>
+    <t>MIDDLE_NAME1</t>
+  </si>
+  <si>
+    <t>father_name_last_name_node_name</t>
+  </si>
+  <si>
+    <t>LAST_NAME1</t>
+  </si>
+  <si>
+    <t>field_name_index</t>
+  </si>
+  <si>
+    <t>xml_type_index</t>
+  </si>
+  <si>
+    <t>single_group_type_index</t>
+  </si>
+  <si>
+    <t>parent_node_index</t>
+  </si>
+  <si>
+    <t>child_nodes_index</t>
+  </si>
+  <si>
+    <t>sql_table_name_index</t>
+  </si>
+  <si>
+    <t>column_name_index</t>
+  </si>
+  <si>
+    <t>column_json_node_index</t>
+  </si>
+  <si>
+    <t>no_of_directors_field_name</t>
+  </si>
+  <si>
+    <t>No_of_directors</t>
+  </si>
+  <si>
+    <t>date_of_birth_column_name</t>
+  </si>
+  <si>
+    <t>date_of_birth</t>
+  </si>
+  <si>
     <t>/Users/gundukalyan/Documents/GitHub/mns-json-prep/DataExtraction/Input/LLP/Form_8_Interim/Form8 (Interim) (1).pdf</t>
   </si>
   <si>
@@ -512,27 +602,9 @@
     <t>charge_sequence_charge_id_column_name</t>
   </si>
   <si>
-    <t>field_name_index</t>
-  </si>
-  <si>
     <t>type_index</t>
   </si>
   <si>
-    <t>parent_node_index</t>
-  </si>
-  <si>
-    <t>child_nodes_index</t>
-  </si>
-  <si>
-    <t>sql_table_name_index</t>
-  </si>
-  <si>
-    <t>column_name_index</t>
-  </si>
-  <si>
-    <t>column_json_node_index</t>
-  </si>
-  <si>
     <t>/Users/gundukalyan/Documents/GitHub/mns-json-prep/DataExtraction/Input/LLP/Form_8_annual/LLP Form8-11012022_signed_1 (1).pdf</t>
   </si>
   <si>
@@ -596,9 +668,6 @@
     <t>auditor_name_column_name</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>membership_number_field_name</t>
   </si>
   <si>
@@ -660,9 +729,6 @@
   </si>
   <si>
     <t>cin_column_name</t>
-  </si>
-  <si>
-    <t>name_column_name</t>
   </si>
   <si>
     <t>/Users/gundukalyan/Documents/GitHub/mns-json-prep/DataExtraction/Input/LLP/Form_11/LLP Form11-08092020for the financial year ending on31.03.2018_5 (1).pdf</t>
@@ -1134,21 +1200,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="17"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="16"/>
       </left>
       <right style="thin">
@@ -1174,6 +1225,36 @@
       </top>
       <bottom style="thin">
         <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1285,21 +1366,6 @@
       </top>
       <bottom style="thin">
         <color indexed="16"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="16"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="16"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1462,7 +1528,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1598,19 +1664,58 @@
     <xf numFmtId="49" fontId="5" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1619,41 +1724,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -1661,7 +1733,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1673,10 +1745,10 @@
     <xf numFmtId="49" fontId="3" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1685,40 +1757,40 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="29" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1730,25 +1802,22 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -4152,10 +4221,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="14.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="48" style="93" customWidth="1"/>
-    <col min="2" max="2" width="61.8516" style="93" customWidth="1"/>
-    <col min="3" max="5" width="16.3516" style="93" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="93" customWidth="1"/>
+    <col min="1" max="1" width="48" style="95" customWidth="1"/>
+    <col min="2" max="2" width="61.8516" style="95" customWidth="1"/>
+    <col min="3" max="5" width="16.3516" style="95" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="95" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
@@ -4181,7 +4250,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>214</v>
+        <v>236</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -4192,7 +4261,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>215</v>
+        <v>237</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -4221,7 +4290,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s" s="9">
-        <v>216</v>
+        <v>238</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -4276,7 +4345,7 @@
     </row>
     <row r="13" ht="14.6" customHeight="1">
       <c r="A13" t="s" s="7">
-        <v>212</v>
+        <v>235</v>
       </c>
       <c r="B13" t="s" s="7">
         <v>29</v>
@@ -4293,10 +4362,10 @@
       <c r="E14" s="8"/>
     </row>
     <row r="15" ht="15.35" customHeight="1">
-      <c r="A15" t="s" s="52">
-        <v>163</v>
-      </c>
-      <c r="B15" s="94">
+      <c r="A15" t="s" s="46">
+        <v>155</v>
+      </c>
+      <c r="B15" s="96">
         <v>0</v>
       </c>
       <c r="C15" s="8"/>
@@ -4304,10 +4373,10 @@
       <c r="E15" s="8"/>
     </row>
     <row r="16" ht="15.35" customHeight="1">
-      <c r="A16" t="s" s="95">
-        <v>164</v>
-      </c>
-      <c r="B16" s="59">
+      <c r="A16" t="s" s="97">
+        <v>193</v>
+      </c>
+      <c r="B16" s="53">
         <v>2</v>
       </c>
       <c r="C16" s="10"/>
@@ -4315,10 +4384,10 @@
       <c r="E16" s="10"/>
     </row>
     <row r="17" ht="15.35" customHeight="1">
-      <c r="A17" t="s" s="96">
-        <v>165</v>
-      </c>
-      <c r="B17" s="59">
+      <c r="A17" t="s" s="52">
+        <v>158</v>
+      </c>
+      <c r="B17" s="53">
         <v>3</v>
       </c>
       <c r="C17" s="8"/>
@@ -4326,10 +4395,10 @@
       <c r="E17" s="8"/>
     </row>
     <row r="18" ht="15.35" customHeight="1">
-      <c r="A18" t="s" s="58">
-        <v>166</v>
-      </c>
-      <c r="B18" s="61">
+      <c r="A18" t="s" s="54">
+        <v>159</v>
+      </c>
+      <c r="B18" s="55">
         <v>4</v>
       </c>
       <c r="C18" s="10"/>
@@ -4337,10 +4406,10 @@
       <c r="E18" s="10"/>
     </row>
     <row r="19" ht="15.35" customHeight="1">
-      <c r="A19" t="s" s="60">
-        <v>167</v>
-      </c>
-      <c r="B19" s="63">
+      <c r="A19" t="s" s="56">
+        <v>160</v>
+      </c>
+      <c r="B19" s="57">
         <v>6</v>
       </c>
       <c r="C19" s="8"/>
@@ -4348,10 +4417,10 @@
       <c r="E19" s="8"/>
     </row>
     <row r="20" ht="15.35" customHeight="1">
-      <c r="A20" t="s" s="58">
-        <v>168</v>
-      </c>
-      <c r="B20" s="59">
+      <c r="A20" t="s" s="54">
+        <v>161</v>
+      </c>
+      <c r="B20" s="53">
         <v>7</v>
       </c>
       <c r="C20" s="10"/>
@@ -4359,10 +4428,10 @@
       <c r="E20" s="10"/>
     </row>
     <row r="21" ht="15.35" customHeight="1">
-      <c r="A21" t="s" s="62">
-        <v>169</v>
-      </c>
-      <c r="B21" s="63">
+      <c r="A21" t="s" s="58">
+        <v>162</v>
+      </c>
+      <c r="B21" s="57">
         <v>8</v>
       </c>
       <c r="C21" s="8"/>
@@ -4378,10 +4447,10 @@
     </row>
     <row r="23" ht="15.35" customHeight="1">
       <c r="A23" t="s" s="9">
-        <v>217</v>
+        <v>239</v>
       </c>
       <c r="B23" t="s" s="30">
-        <v>218</v>
+        <v>240</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -4389,10 +4458,10 @@
     </row>
     <row r="24" ht="15.35" customHeight="1">
       <c r="A24" t="s" s="30">
-        <v>219</v>
+        <v>241</v>
       </c>
       <c r="B24" t="s" s="30">
-        <v>220</v>
+        <v>242</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -4418,10 +4487,10 @@
     </row>
     <row r="27" ht="15.35" customHeight="1">
       <c r="A27" t="s" s="30">
-        <v>221</v>
+        <v>243</v>
       </c>
       <c r="B27" t="s" s="30">
-        <v>222</v>
+        <v>244</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -4436,10 +4505,10 @@
     </row>
     <row r="29" ht="15.35" customHeight="1">
       <c r="A29" t="s" s="30">
-        <v>223</v>
+        <v>245</v>
       </c>
       <c r="B29" t="s" s="30">
-        <v>224</v>
+        <v>246</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -4447,10 +4516,10 @@
     </row>
     <row r="30" ht="15.35" customHeight="1">
       <c r="A30" t="s" s="30">
-        <v>225</v>
+        <v>247</v>
       </c>
       <c r="B30" t="s" s="30">
-        <v>226</v>
+        <v>248</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -4465,7 +4534,7 @@
     </row>
     <row r="32" ht="15.35" customHeight="1">
       <c r="A32" t="s" s="30">
-        <v>227</v>
+        <v>249</v>
       </c>
       <c r="B32" t="s" s="30">
         <v>96</v>
@@ -4476,7 +4545,7 @@
     </row>
     <row r="33" ht="15.35" customHeight="1">
       <c r="A33" t="s" s="43">
-        <v>228</v>
+        <v>250</v>
       </c>
       <c r="B33" t="s" s="43">
         <v>98</v>
@@ -4493,21 +4562,21 @@
       <c r="E34" s="8"/>
     </row>
     <row r="35" ht="15.35" customHeight="1">
-      <c r="A35" t="s" s="97">
-        <v>229</v>
-      </c>
-      <c r="B35" t="s" s="97">
-        <v>230</v>
+      <c r="A35" t="s" s="98">
+        <v>251</v>
+      </c>
+      <c r="B35" t="s" s="98">
+        <v>252</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
     </row>
     <row r="36" ht="14.6" customHeight="1">
-      <c r="A36" t="s" s="70">
-        <v>179</v>
-      </c>
-      <c r="B36" t="s" s="71">
+      <c r="A36" t="s" s="72">
+        <v>203</v>
+      </c>
+      <c r="B36" t="s" s="73">
         <v>25</v>
       </c>
       <c r="C36" s="8"/>
@@ -4515,18 +4584,18 @@
       <c r="E36" s="8"/>
     </row>
     <row r="37" ht="14.6" customHeight="1">
-      <c r="A37" s="48"/>
-      <c r="B37" s="71"/>
+      <c r="A37" s="50"/>
+      <c r="B37" s="73"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
     </row>
     <row r="38" ht="14.6" customHeight="1">
       <c r="A38" t="s" s="27">
-        <v>231</v>
-      </c>
-      <c r="B38" t="s" s="73">
-        <v>232</v>
+        <v>253</v>
+      </c>
+      <c r="B38" t="s" s="75">
+        <v>254</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
@@ -4534,10 +4603,10 @@
     </row>
     <row r="39" ht="14.6" customHeight="1">
       <c r="A39" t="s" s="30">
-        <v>233</v>
+        <v>255</v>
       </c>
       <c r="B39" t="s" s="30">
-        <v>234</v>
+        <v>256</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
@@ -4552,21 +4621,21 @@
     </row>
     <row r="41" ht="14.6" customHeight="1">
       <c r="A41" t="s" s="30">
-        <v>235</v>
+        <v>257</v>
       </c>
       <c r="B41" t="s" s="30">
-        <v>236</v>
+        <v>258</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
     </row>
     <row r="42" ht="14.6" customHeight="1">
-      <c r="A42" t="s" s="98">
-        <v>237</v>
-      </c>
-      <c r="B42" t="s" s="98">
-        <v>238</v>
+      <c r="A42" t="s" s="99">
+        <v>259</v>
+      </c>
+      <c r="B42" t="s" s="99">
+        <v>260</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
@@ -4581,36 +4650,36 @@
     </row>
     <row r="44" ht="14.6" customHeight="1">
       <c r="A44" t="s" s="30">
-        <v>239</v>
+        <v>261</v>
       </c>
       <c r="B44" t="s" s="30">
-        <v>240</v>
+        <v>262</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
     </row>
     <row r="45" ht="14.6" customHeight="1">
-      <c r="A45" t="s" s="69">
-        <v>241</v>
-      </c>
-      <c r="B45" t="s" s="67">
-        <v>242</v>
+      <c r="A45" t="s" s="71">
+        <v>263</v>
+      </c>
+      <c r="B45" t="s" s="69">
+        <v>264</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
     </row>
     <row r="46" ht="14.6" customHeight="1">
-      <c r="A46" t="s" s="99">
-        <v>243</v>
-      </c>
-      <c r="B46" t="s" s="100">
-        <v>244</v>
-      </c>
-      <c r="C46" s="101"/>
-      <c r="D46" s="101"/>
-      <c r="E46" s="102"/>
+      <c r="A46" t="s" s="100">
+        <v>265</v>
+      </c>
+      <c r="B46" t="s" s="101">
+        <v>266</v>
+      </c>
+      <c r="C46" s="102"/>
+      <c r="D46" s="102"/>
+      <c r="E46" s="103"/>
     </row>
     <row r="47" ht="14.6" customHeight="1">
       <c r="A47" s="9"/>
@@ -4621,10 +4690,10 @@
     </row>
     <row r="48" ht="14.6" customHeight="1">
       <c r="A48" t="s" s="9">
-        <v>245</v>
+        <v>267</v>
       </c>
       <c r="B48" t="s" s="9">
-        <v>246</v>
+        <v>268</v>
       </c>
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
@@ -4632,10 +4701,10 @@
     </row>
     <row r="49" ht="14.6" customHeight="1">
       <c r="A49" t="s" s="7">
-        <v>247</v>
+        <v>269</v>
       </c>
       <c r="B49" t="s" s="7">
-        <v>248</v>
+        <v>270</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
@@ -4643,10 +4712,10 @@
     </row>
     <row r="50" ht="14.6" customHeight="1">
       <c r="A50" t="s" s="9">
-        <v>249</v>
+        <v>271</v>
       </c>
       <c r="B50" t="s" s="9">
-        <v>250</v>
+        <v>272</v>
       </c>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
@@ -5658,88 +5727,88 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="14.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="103" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="103" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="104" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="104" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.55" customHeight="1">
-      <c r="A1" t="s" s="104">
-        <v>251</v>
-      </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
+      <c r="A1" t="s" s="105">
+        <v>273</v>
+      </c>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
     </row>
     <row r="2" ht="14.15" customHeight="1">
-      <c r="A2" s="105"/>
-      <c r="B2" s="105"/>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="105"/>
+      <c r="A2" s="106"/>
+      <c r="B2" s="106"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
     </row>
     <row r="3" ht="14.15" customHeight="1">
-      <c r="A3" s="106"/>
-      <c r="B3" s="107"/>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
+      <c r="A3" s="107"/>
+      <c r="B3" s="108"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
     </row>
     <row r="4" ht="13.95" customHeight="1">
-      <c r="A4" s="109"/>
-      <c r="B4" s="110"/>
-      <c r="C4" s="111"/>
-      <c r="D4" s="111"/>
-      <c r="E4" s="111"/>
+      <c r="A4" s="110"/>
+      <c r="B4" s="111"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
     </row>
     <row r="5" ht="13.95" customHeight="1">
-      <c r="A5" s="109"/>
-      <c r="B5" s="110"/>
-      <c r="C5" s="111"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="111"/>
+      <c r="A5" s="110"/>
+      <c r="B5" s="111"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
     </row>
     <row r="6" ht="13.95" customHeight="1">
-      <c r="A6" s="109"/>
-      <c r="B6" s="110"/>
-      <c r="C6" s="111"/>
-      <c r="D6" s="111"/>
-      <c r="E6" s="111"/>
+      <c r="A6" s="110"/>
+      <c r="B6" s="111"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
     </row>
     <row r="7" ht="13.95" customHeight="1">
-      <c r="A7" s="109"/>
-      <c r="B7" s="110"/>
-      <c r="C7" s="111"/>
-      <c r="D7" s="111"/>
-      <c r="E7" s="111"/>
+      <c r="A7" s="110"/>
+      <c r="B7" s="111"/>
+      <c r="C7" s="112"/>
+      <c r="D7" s="112"/>
+      <c r="E7" s="112"/>
     </row>
     <row r="8" ht="13.95" customHeight="1">
-      <c r="A8" s="109"/>
-      <c r="B8" s="110"/>
-      <c r="C8" s="111"/>
-      <c r="D8" s="111"/>
-      <c r="E8" s="111"/>
+      <c r="A8" s="110"/>
+      <c r="B8" s="111"/>
+      <c r="C8" s="112"/>
+      <c r="D8" s="112"/>
+      <c r="E8" s="112"/>
     </row>
     <row r="9" ht="13.95" customHeight="1">
-      <c r="A9" s="109"/>
-      <c r="B9" s="110"/>
-      <c r="C9" s="111"/>
-      <c r="D9" s="111"/>
-      <c r="E9" s="111"/>
+      <c r="A9" s="110"/>
+      <c r="B9" s="111"/>
+      <c r="C9" s="112"/>
+      <c r="D9" s="112"/>
+      <c r="E9" s="112"/>
     </row>
     <row r="10" ht="13.95" customHeight="1">
-      <c r="A10" s="109"/>
-      <c r="B10" s="110"/>
-      <c r="C10" s="111"/>
-      <c r="D10" s="111"/>
-      <c r="E10" s="111"/>
+      <c r="A10" s="110"/>
+      <c r="B10" s="111"/>
+      <c r="C10" s="112"/>
+      <c r="D10" s="112"/>
+      <c r="E10" s="112"/>
     </row>
     <row r="11" ht="13.95" customHeight="1">
-      <c r="A11" s="109"/>
-      <c r="B11" s="110"/>
-      <c r="C11" s="111"/>
-      <c r="D11" s="111"/>
-      <c r="E11" s="111"/>
+      <c r="A11" s="110"/>
+      <c r="B11" s="111"/>
+      <c r="C11" s="112"/>
+      <c r="D11" s="112"/>
+      <c r="E11" s="112"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10766,13 +10835,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E169"/>
+  <dimension ref="A1:E182"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="14.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="28.6719" style="35" customWidth="1"/>
+    <col min="1" max="1" width="36.1875" style="35" customWidth="1"/>
     <col min="2" max="2" width="73.1719" style="35" customWidth="1"/>
     <col min="3" max="5" width="16.3516" style="35" customWidth="1"/>
     <col min="6" max="16384" width="16.3516" style="35" customWidth="1"/>
@@ -10853,10 +10922,10 @@
     </row>
     <row r="8" ht="14.6" customHeight="1">
       <c r="A8" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s" s="7">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="B8" t="s" s="30">
+        <v>12</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -10864,32 +10933,32 @@
     </row>
     <row r="9" ht="14.6" customHeight="1">
       <c r="A9" t="s" s="7">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" ht="14.6" customHeight="1">
+      <c r="A10" t="s" s="7">
         <v>28</v>
       </c>
-      <c r="B9" t="s" s="7">
+      <c r="B10" t="s" s="7">
         <v>29</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" ht="26.6" customHeight="1">
-      <c r="A10" t="s" s="9">
-        <v>95</v>
-      </c>
-      <c r="B10" t="s" s="9">
-        <v>96</v>
-      </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" ht="26.6" customHeight="1">
       <c r="A11" t="s" s="9">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B11" t="s" s="9">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -10897,10 +10966,10 @@
     </row>
     <row r="12" ht="26.6" customHeight="1">
       <c r="A12" t="s" s="9">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B12" t="s" s="9">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -10908,10 +10977,10 @@
     </row>
     <row r="13" ht="26.6" customHeight="1">
       <c r="A13" t="s" s="9">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B13" t="s" s="9">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -10919,10 +10988,10 @@
     </row>
     <row r="14" ht="26.6" customHeight="1">
       <c r="A14" t="s" s="9">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B14" t="s" s="9">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -10930,226 +10999,234 @@
     </row>
     <row r="15" ht="26.6" customHeight="1">
       <c r="A15" t="s" s="9">
-        <v>30</v>
+        <v>103</v>
       </c>
       <c r="B15" t="s" s="9">
-        <v>31</v>
+        <v>104</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
     </row>
-    <row r="16" ht="15.35" customHeight="1">
-      <c r="A16" t="s" s="22">
+    <row r="16" ht="26.6" customHeight="1">
+      <c r="A16" t="s" s="9">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s" s="9">
+        <v>31</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" ht="15.35" customHeight="1">
+      <c r="A17" t="s" s="22">
         <v>105</v>
       </c>
-      <c r="B16" t="s" s="36">
+      <c r="B17" t="s" s="36">
         <v>106</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" ht="14.6" customHeight="1">
-      <c r="A17" t="s" s="7">
-        <v>107</v>
-      </c>
-      <c r="B17" t="s" s="37">
-        <v>108</v>
-      </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
     </row>
     <row r="18" ht="14.6" customHeight="1">
       <c r="A18" t="s" s="7">
-        <v>109</v>
-      </c>
-      <c r="B18" t="s" s="38">
-        <v>110</v>
+        <v>107</v>
+      </c>
+      <c r="B18" t="s" s="37">
+        <v>108</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
     </row>
-    <row r="19" ht="15.35" customHeight="1">
-      <c r="A19" t="s" s="24">
-        <v>111</v>
-      </c>
-      <c r="B19" t="s" s="9">
-        <v>112</v>
+    <row r="19" ht="14.6" customHeight="1">
+      <c r="A19" t="s" s="7">
+        <v>109</v>
+      </c>
+      <c r="B19" t="s" s="38">
+        <v>110</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
     </row>
-    <row r="20" ht="14.6" customHeight="1">
-      <c r="A20" t="s" s="23">
+    <row r="20" ht="15.35" customHeight="1">
+      <c r="A20" t="s" s="24">
+        <v>111</v>
+      </c>
+      <c r="B20" t="s" s="9">
+        <v>112</v>
+      </c>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" ht="14.6" customHeight="1">
+      <c r="A21" t="s" s="23">
         <v>113</v>
       </c>
-      <c r="B20" t="s" s="30">
+      <c r="B21" t="s" s="30">
         <v>114</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-    </row>
-    <row r="21" ht="14.6" customHeight="1">
-      <c r="A21" t="s" s="14">
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" ht="14.6" customHeight="1">
+      <c r="A22" t="s" s="14">
         <v>115</v>
       </c>
-      <c r="B21" t="s" s="39">
+      <c r="B22" t="s" s="39">
         <v>116</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-    </row>
-    <row r="22" ht="15.35" customHeight="1">
-      <c r="A22" t="s" s="9">
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" ht="15.35" customHeight="1">
+      <c r="A23" t="s" s="9">
         <v>117</v>
       </c>
-      <c r="B22" t="s" s="24">
+      <c r="B23" t="s" s="24">
         <v>118</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" ht="15.35" customHeight="1">
-      <c r="A23" t="s" s="7">
-        <v>119</v>
-      </c>
-      <c r="B23" t="s" s="22">
-        <v>108</v>
-      </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
     </row>
     <row r="24" ht="15.35" customHeight="1">
       <c r="A24" t="s" s="7">
+        <v>119</v>
+      </c>
+      <c r="B24" t="s" s="22">
+        <v>108</v>
+      </c>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+    </row>
+    <row r="25" ht="15.35" customHeight="1">
+      <c r="A25" t="s" s="7">
         <v>120</v>
       </c>
-      <c r="B24" t="s" s="22">
+      <c r="B25" t="s" s="22">
         <v>110</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-    </row>
-    <row r="25" ht="15.35" customHeight="1">
-      <c r="A25" t="s" s="9">
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" ht="15.35" customHeight="1">
+      <c r="A26" t="s" s="9">
         <v>121</v>
       </c>
-      <c r="B25" t="s" s="24">
+      <c r="B26" t="s" s="24">
         <v>112</v>
       </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-    </row>
-    <row r="26" ht="14.6" customHeight="1">
-      <c r="A26" t="s" s="25">
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+    </row>
+    <row r="27" ht="14.6" customHeight="1">
+      <c r="A27" t="s" s="25">
         <v>122</v>
       </c>
-      <c r="B26" t="s" s="40">
+      <c r="B27" t="s" s="40">
         <v>123</v>
       </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-    </row>
-    <row r="27" ht="14.6" customHeight="1">
-      <c r="A27" t="s" s="27">
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" ht="14.6" customHeight="1">
+      <c r="A28" t="s" s="27">
         <v>124</v>
       </c>
-      <c r="B27" t="s" s="41">
+      <c r="B28" t="s" s="41">
         <v>104</v>
       </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-    </row>
-    <row r="28" ht="15.35" customHeight="1">
-      <c r="A28" t="s" s="22">
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+    </row>
+    <row r="29" ht="15.35" customHeight="1">
+      <c r="A29" t="s" s="22">
         <v>125</v>
       </c>
-      <c r="B28" t="s" s="22">
+      <c r="B29" t="s" s="22">
         <v>126</v>
       </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-    </row>
-    <row r="29" ht="15.35" customHeight="1">
-      <c r="A29" t="s" s="42">
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" ht="15.35" customHeight="1">
+      <c r="A30" t="s" s="42">
         <v>127</v>
       </c>
-      <c r="B29" t="s" s="24">
+      <c r="B30" t="s" s="24">
         <v>128</v>
       </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-    </row>
-    <row r="30" ht="14.6" customHeight="1">
-      <c r="A30" t="s" s="43">
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+    </row>
+    <row r="31" ht="14.6" customHeight="1">
+      <c r="A31" t="s" s="43">
         <v>129</v>
       </c>
-      <c r="B30" t="s" s="43">
+      <c r="B31" t="s" s="43">
         <v>130</v>
       </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-    </row>
-    <row r="31" ht="14.6" customHeight="1">
-      <c r="A31" t="s" s="44">
-        <v>131</v>
-      </c>
-      <c r="B31" t="s" s="44">
-        <v>132</v>
-      </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
     </row>
     <row r="32" ht="14.6" customHeight="1">
       <c r="A32" t="s" s="44">
+        <v>131</v>
+      </c>
+      <c r="B32" t="s" s="44">
+        <v>132</v>
+      </c>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+    </row>
+    <row r="33" ht="14.6" customHeight="1">
+      <c r="A33" t="s" s="44">
         <v>133</v>
       </c>
-      <c r="B32" t="s" s="43">
+      <c r="B33" t="s" s="43">
         <v>134</v>
       </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-    </row>
-    <row r="33" ht="14.6" customHeight="1">
-      <c r="A33" t="s" s="9">
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" ht="14.6" customHeight="1">
+      <c r="A34" t="s" s="9">
         <v>135</v>
       </c>
-      <c r="B33" t="s" s="9">
+      <c r="B34" t="s" s="9">
         <v>136</v>
       </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-    </row>
-    <row r="34" ht="14.6" customHeight="1">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
     </row>
     <row r="35" ht="14.6" customHeight="1">
-      <c r="A35" s="10"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
+      <c r="A35" t="s" s="7">
+        <v>137</v>
+      </c>
+      <c r="B35" t="s" s="7">
+        <v>138</v>
+      </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
     </row>
     <row r="36" ht="14.6" customHeight="1">
       <c r="A36" s="7"/>
@@ -11159,67 +11236,99 @@
       <c r="E36" s="8"/>
     </row>
     <row r="37" ht="14.6" customHeight="1">
-      <c r="A37" s="9"/>
-      <c r="B37" s="9"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
+      <c r="A37" t="s" s="7">
+        <v>139</v>
+      </c>
+      <c r="B37" t="s" s="7">
+        <v>140</v>
+      </c>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
     </row>
     <row r="38" ht="14.6" customHeight="1">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
+      <c r="A38" t="s" s="7">
+        <v>141</v>
+      </c>
+      <c r="B38" t="s" s="45">
+        <v>142</v>
+      </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
     </row>
     <row r="39" ht="14.6" customHeight="1">
-      <c r="A39" s="9"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
+      <c r="A39" t="s" s="7">
+        <v>143</v>
+      </c>
+      <c r="B39" t="s" s="45">
+        <v>144</v>
+      </c>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
     </row>
     <row r="40" ht="14.6" customHeight="1">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
+      <c r="A40" t="s" s="7">
+        <v>145</v>
+      </c>
+      <c r="B40" t="s" s="45">
+        <v>146</v>
+      </c>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
     </row>
     <row r="41" ht="14.6" customHeight="1">
-      <c r="A41" s="9"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
     </row>
     <row r="42" ht="14.6" customHeight="1">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
+      <c r="A42" t="s" s="7">
+        <v>147</v>
+      </c>
+      <c r="B42" t="s" s="7">
+        <v>148</v>
+      </c>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
     </row>
     <row r="43" ht="14.6" customHeight="1">
-      <c r="A43" s="10"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
+      <c r="A43" t="s" s="7">
+        <v>149</v>
+      </c>
+      <c r="B43" t="s" s="45">
+        <v>150</v>
+      </c>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
     </row>
     <row r="44" ht="14.6" customHeight="1">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
+      <c r="A44" t="s" s="7">
+        <v>151</v>
+      </c>
+      <c r="B44" t="s" s="45">
+        <v>152</v>
+      </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
     </row>
     <row r="45" ht="14.6" customHeight="1">
-      <c r="A45" s="10"/>
-      <c r="B45" s="10"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
+      <c r="A45" t="s" s="7">
+        <v>153</v>
+      </c>
+      <c r="B45" t="s" s="45">
+        <v>154</v>
+      </c>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
     </row>
     <row r="46" ht="14.6" customHeight="1">
       <c r="A46" s="7"/>
@@ -11229,865 +11338,996 @@
       <c r="E46" s="8"/>
     </row>
     <row r="47" ht="14.6" customHeight="1">
-      <c r="A47" s="9"/>
-      <c r="B47" s="9"/>
+      <c r="A47" t="s" s="46">
+        <v>155</v>
+      </c>
+      <c r="B47" s="47">
+        <v>0</v>
+      </c>
       <c r="C47" s="10"/>
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
     </row>
     <row r="48" ht="14.6" customHeight="1">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8"/>
+      <c r="A48" t="s" s="48">
+        <v>156</v>
+      </c>
+      <c r="B48" s="49">
+        <v>1</v>
+      </c>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
     </row>
     <row r="49" ht="14.6" customHeight="1">
-      <c r="A49" s="9"/>
-      <c r="B49" s="9"/>
+      <c r="A49" t="s" s="50">
+        <v>157</v>
+      </c>
+      <c r="B49" s="51">
+        <v>2</v>
+      </c>
       <c r="C49" s="10"/>
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
     </row>
     <row r="50" ht="14.6" customHeight="1">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
+      <c r="A50" t="s" s="52">
+        <v>158</v>
+      </c>
+      <c r="B50" s="53">
+        <v>3</v>
+      </c>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
     </row>
     <row r="51" ht="14.6" customHeight="1">
-      <c r="A51" s="10"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
+      <c r="A51" t="s" s="54">
+        <v>159</v>
+      </c>
+      <c r="B51" s="55">
+        <v>4</v>
+      </c>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
     </row>
     <row r="52" ht="14.6" customHeight="1">
-      <c r="A52" s="8"/>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
+      <c r="A52" t="s" s="56">
+        <v>160</v>
+      </c>
+      <c r="B52" s="53">
+        <v>5</v>
+      </c>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
     </row>
     <row r="53" ht="14.6" customHeight="1">
-      <c r="A53" s="9"/>
-      <c r="B53" s="9"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
+      <c r="A53" t="s" s="54">
+        <v>161</v>
+      </c>
+      <c r="B53" s="57">
+        <v>6</v>
+      </c>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
     </row>
     <row r="54" ht="14.6" customHeight="1">
-      <c r="A54" s="7"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
+      <c r="A54" t="s" s="58">
+        <v>162</v>
+      </c>
+      <c r="B54" s="57">
+        <v>7</v>
+      </c>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
     </row>
     <row r="55" ht="14.6" customHeight="1">
-      <c r="A55" s="9"/>
-      <c r="B55" s="9"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
+      <c r="A55" s="8"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
     </row>
     <row r="56" ht="14.6" customHeight="1">
-      <c r="A56" s="7"/>
-      <c r="B56" s="7"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
+      <c r="A56" t="s" s="9">
+        <v>163</v>
+      </c>
+      <c r="B56" t="s" s="12">
+        <v>164</v>
+      </c>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
     </row>
     <row r="57" ht="14.6" customHeight="1">
-      <c r="A57" s="9"/>
-      <c r="B57" s="9"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10"/>
+      <c r="A57" t="s" s="7">
+        <v>165</v>
+      </c>
+      <c r="B57" t="s" s="45">
+        <v>166</v>
+      </c>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
     </row>
     <row r="58" ht="14.6" customHeight="1">
-      <c r="A58" s="8"/>
-      <c r="B58" s="8"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
+      <c r="A58" s="10"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10"/>
     </row>
     <row r="59" ht="14.6" customHeight="1">
-      <c r="A59" s="9"/>
-      <c r="B59" s="9"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="10"/>
+      <c r="A59" s="7"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
     </row>
     <row r="60" ht="14.6" customHeight="1">
-      <c r="A60" s="7"/>
-      <c r="B60" s="7"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
+      <c r="A60" s="9"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
     </row>
     <row r="61" ht="14.6" customHeight="1">
-      <c r="A61" s="10"/>
-      <c r="B61" s="10"/>
-      <c r="C61" s="10"/>
-      <c r="D61" s="10"/>
-      <c r="E61" s="10"/>
+      <c r="A61" s="8"/>
+      <c r="B61" s="8"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
     </row>
     <row r="62" ht="14.6" customHeight="1">
-      <c r="A62" s="7"/>
-      <c r="B62" s="7"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
+      <c r="A62" s="9"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
     </row>
     <row r="63" ht="14.6" customHeight="1">
-      <c r="A63" s="10"/>
-      <c r="B63" s="10"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="10"/>
+      <c r="A63" s="7"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
     </row>
     <row r="64" ht="14.6" customHeight="1">
-      <c r="A64" s="7"/>
-      <c r="B64" s="7"/>
-      <c r="C64" s="8"/>
-      <c r="D64" s="8"/>
-      <c r="E64" s="8"/>
+      <c r="A64" s="10"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
     </row>
     <row r="65" ht="14.6" customHeight="1">
-      <c r="A65" s="9"/>
-      <c r="B65" s="10"/>
-      <c r="C65" s="10"/>
-      <c r="D65" s="10"/>
-      <c r="E65" s="10"/>
+      <c r="A65" s="8"/>
+      <c r="B65" s="8"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="8"/>
+      <c r="E65" s="8"/>
     </row>
     <row r="66" ht="14.6" customHeight="1">
-      <c r="A66" s="7"/>
-      <c r="B66" s="8"/>
-      <c r="C66" s="8"/>
-      <c r="D66" s="8"/>
-      <c r="E66" s="8"/>
+      <c r="A66" s="9"/>
+      <c r="B66" s="9"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="10"/>
     </row>
     <row r="67" ht="14.6" customHeight="1">
-      <c r="A67" s="9"/>
-      <c r="B67" s="10"/>
-      <c r="C67" s="10"/>
-      <c r="D67" s="10"/>
-      <c r="E67" s="10"/>
+      <c r="A67" s="7"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8"/>
     </row>
     <row r="68" ht="14.6" customHeight="1">
-      <c r="A68" s="8"/>
-      <c r="B68" s="8"/>
-      <c r="C68" s="8"/>
-      <c r="D68" s="8"/>
-      <c r="E68" s="8"/>
+      <c r="A68" s="9"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="10"/>
+      <c r="E68" s="10"/>
     </row>
     <row r="69" ht="14.6" customHeight="1">
-      <c r="A69" s="10"/>
-      <c r="B69" s="10"/>
-      <c r="C69" s="10"/>
-      <c r="D69" s="10"/>
-      <c r="E69" s="10"/>
+      <c r="A69" s="7"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="8"/>
     </row>
     <row r="70" ht="14.6" customHeight="1">
-      <c r="A70" s="7"/>
-      <c r="B70" s="7"/>
-      <c r="C70" s="8"/>
-      <c r="D70" s="8"/>
-      <c r="E70" s="8"/>
+      <c r="A70" s="9"/>
+      <c r="B70" s="9"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="10"/>
     </row>
     <row r="71" ht="14.6" customHeight="1">
-      <c r="A71" s="9"/>
-      <c r="B71" s="9"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
-      <c r="E71" s="10"/>
+      <c r="A71" s="8"/>
+      <c r="B71" s="8"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="8"/>
     </row>
     <row r="72" ht="14.6" customHeight="1">
-      <c r="A72" s="7"/>
-      <c r="B72" s="7"/>
-      <c r="C72" s="8"/>
-      <c r="D72" s="8"/>
-      <c r="E72" s="8"/>
+      <c r="A72" s="9"/>
+      <c r="B72" s="9"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="10"/>
     </row>
     <row r="73" ht="14.6" customHeight="1">
-      <c r="A73" s="9"/>
-      <c r="B73" s="9"/>
-      <c r="C73" s="10"/>
-      <c r="D73" s="10"/>
-      <c r="E73" s="10"/>
+      <c r="A73" s="7"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="8"/>
+      <c r="E73" s="8"/>
     </row>
     <row r="74" ht="14.6" customHeight="1">
-      <c r="A74" s="7"/>
-      <c r="B74" s="7"/>
-      <c r="C74" s="8"/>
-      <c r="D74" s="8"/>
-      <c r="E74" s="8"/>
+      <c r="A74" s="10"/>
+      <c r="B74" s="10"/>
+      <c r="C74" s="10"/>
+      <c r="D74" s="10"/>
+      <c r="E74" s="10"/>
     </row>
     <row r="75" ht="14.6" customHeight="1">
-      <c r="A75" s="9"/>
-      <c r="B75" s="9"/>
-      <c r="C75" s="10"/>
-      <c r="D75" s="10"/>
-      <c r="E75" s="10"/>
+      <c r="A75" s="7"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="8"/>
+      <c r="E75" s="8"/>
     </row>
     <row r="76" ht="14.6" customHeight="1">
-      <c r="A76" s="8"/>
-      <c r="B76" s="8"/>
-      <c r="C76" s="8"/>
-      <c r="D76" s="8"/>
-      <c r="E76" s="8"/>
+      <c r="A76" s="10"/>
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
+      <c r="E76" s="10"/>
     </row>
     <row r="77" ht="14.6" customHeight="1">
-      <c r="A77" s="9"/>
-      <c r="B77" s="9"/>
-      <c r="C77" s="10"/>
-      <c r="D77" s="10"/>
-      <c r="E77" s="10"/>
+      <c r="A77" s="7"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="8"/>
+      <c r="E77" s="8"/>
     </row>
     <row r="78" ht="14.6" customHeight="1">
-      <c r="A78" s="7"/>
-      <c r="B78" s="7"/>
-      <c r="C78" s="8"/>
-      <c r="D78" s="8"/>
-      <c r="E78" s="8"/>
+      <c r="A78" s="9"/>
+      <c r="B78" s="10"/>
+      <c r="C78" s="10"/>
+      <c r="D78" s="10"/>
+      <c r="E78" s="10"/>
     </row>
     <row r="79" ht="14.6" customHeight="1">
-      <c r="A79" s="9"/>
-      <c r="B79" s="9"/>
-      <c r="C79" s="10"/>
-      <c r="D79" s="10"/>
-      <c r="E79" s="10"/>
+      <c r="A79" s="7"/>
+      <c r="B79" s="8"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="8"/>
+      <c r="E79" s="8"/>
     </row>
     <row r="80" ht="14.6" customHeight="1">
-      <c r="A80" s="7"/>
-      <c r="B80" s="7"/>
-      <c r="C80" s="8"/>
-      <c r="D80" s="8"/>
-      <c r="E80" s="8"/>
+      <c r="A80" s="9"/>
+      <c r="B80" s="10"/>
+      <c r="C80" s="10"/>
+      <c r="D80" s="10"/>
+      <c r="E80" s="10"/>
     </row>
     <row r="81" ht="14.6" customHeight="1">
-      <c r="A81" s="9"/>
-      <c r="B81" s="9"/>
-      <c r="C81" s="10"/>
-      <c r="D81" s="10"/>
-      <c r="E81" s="10"/>
+      <c r="A81" s="8"/>
+      <c r="B81" s="8"/>
+      <c r="C81" s="8"/>
+      <c r="D81" s="8"/>
+      <c r="E81" s="8"/>
     </row>
     <row r="82" ht="14.6" customHeight="1">
-      <c r="A82" s="8"/>
-      <c r="B82" s="8"/>
-      <c r="C82" s="8"/>
-      <c r="D82" s="8"/>
-      <c r="E82" s="8"/>
+      <c r="A82" s="10"/>
+      <c r="B82" s="10"/>
+      <c r="C82" s="10"/>
+      <c r="D82" s="10"/>
+      <c r="E82" s="10"/>
     </row>
     <row r="83" ht="14.6" customHeight="1">
-      <c r="A83" s="9"/>
-      <c r="B83" s="9"/>
-      <c r="C83" s="10"/>
-      <c r="D83" s="10"/>
-      <c r="E83" s="10"/>
+      <c r="A83" s="7"/>
+      <c r="B83" s="7"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8"/>
+      <c r="E83" s="8"/>
     </row>
     <row r="84" ht="14.6" customHeight="1">
-      <c r="A84" s="7"/>
-      <c r="B84" s="7"/>
-      <c r="C84" s="8"/>
-      <c r="D84" s="8"/>
-      <c r="E84" s="8"/>
+      <c r="A84" s="9"/>
+      <c r="B84" s="9"/>
+      <c r="C84" s="10"/>
+      <c r="D84" s="10"/>
+      <c r="E84" s="10"/>
     </row>
     <row r="85" ht="14.6" customHeight="1">
-      <c r="A85" s="9"/>
-      <c r="B85" s="9"/>
-      <c r="C85" s="10"/>
-      <c r="D85" s="10"/>
-      <c r="E85" s="10"/>
+      <c r="A85" s="7"/>
+      <c r="B85" s="7"/>
+      <c r="C85" s="8"/>
+      <c r="D85" s="8"/>
+      <c r="E85" s="8"/>
     </row>
     <row r="86" ht="14.6" customHeight="1">
-      <c r="A86" s="7"/>
-      <c r="B86" s="7"/>
-      <c r="C86" s="8"/>
-      <c r="D86" s="8"/>
-      <c r="E86" s="8"/>
+      <c r="A86" s="9"/>
+      <c r="B86" s="9"/>
+      <c r="C86" s="10"/>
+      <c r="D86" s="10"/>
+      <c r="E86" s="10"/>
     </row>
     <row r="87" ht="14.6" customHeight="1">
-      <c r="A87" s="9"/>
-      <c r="B87" s="9"/>
-      <c r="C87" s="10"/>
-      <c r="D87" s="10"/>
-      <c r="E87" s="10"/>
+      <c r="A87" s="7"/>
+      <c r="B87" s="7"/>
+      <c r="C87" s="8"/>
+      <c r="D87" s="8"/>
+      <c r="E87" s="8"/>
     </row>
     <row r="88" ht="14.6" customHeight="1">
-      <c r="A88" s="8"/>
-      <c r="B88" s="8"/>
-      <c r="C88" s="8"/>
-      <c r="D88" s="8"/>
-      <c r="E88" s="8"/>
+      <c r="A88" s="9"/>
+      <c r="B88" s="9"/>
+      <c r="C88" s="10"/>
+      <c r="D88" s="10"/>
+      <c r="E88" s="10"/>
     </row>
     <row r="89" ht="14.6" customHeight="1">
-      <c r="A89" s="9"/>
-      <c r="B89" s="10"/>
-      <c r="C89" s="10"/>
-      <c r="D89" s="10"/>
-      <c r="E89" s="10"/>
+      <c r="A89" s="8"/>
+      <c r="B89" s="8"/>
+      <c r="C89" s="8"/>
+      <c r="D89" s="8"/>
+      <c r="E89" s="8"/>
     </row>
     <row r="90" ht="14.6" customHeight="1">
-      <c r="A90" s="7"/>
-      <c r="B90" s="7"/>
-      <c r="C90" s="8"/>
-      <c r="D90" s="8"/>
-      <c r="E90" s="8"/>
+      <c r="A90" s="9"/>
+      <c r="B90" s="9"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="10"/>
+      <c r="E90" s="10"/>
     </row>
     <row r="91" ht="14.6" customHeight="1">
-      <c r="A91" s="9"/>
-      <c r="B91" s="9"/>
-      <c r="C91" s="10"/>
-      <c r="D91" s="10"/>
-      <c r="E91" s="10"/>
+      <c r="A91" s="7"/>
+      <c r="B91" s="7"/>
+      <c r="C91" s="8"/>
+      <c r="D91" s="8"/>
+      <c r="E91" s="8"/>
     </row>
     <row r="92" ht="14.6" customHeight="1">
-      <c r="A92" s="7"/>
-      <c r="B92" s="7"/>
-      <c r="C92" s="8"/>
-      <c r="D92" s="8"/>
-      <c r="E92" s="8"/>
+      <c r="A92" s="9"/>
+      <c r="B92" s="9"/>
+      <c r="C92" s="10"/>
+      <c r="D92" s="10"/>
+      <c r="E92" s="10"/>
     </row>
     <row r="93" ht="14.6" customHeight="1">
-      <c r="A93" s="9"/>
-      <c r="B93" s="9"/>
-      <c r="C93" s="10"/>
-      <c r="D93" s="10"/>
-      <c r="E93" s="10"/>
+      <c r="A93" s="7"/>
+      <c r="B93" s="7"/>
+      <c r="C93" s="8"/>
+      <c r="D93" s="8"/>
+      <c r="E93" s="8"/>
     </row>
     <row r="94" ht="14.6" customHeight="1">
-      <c r="A94" s="7"/>
-      <c r="B94" s="7"/>
-      <c r="C94" s="8"/>
-      <c r="D94" s="8"/>
-      <c r="E94" s="8"/>
+      <c r="A94" s="9"/>
+      <c r="B94" s="9"/>
+      <c r="C94" s="10"/>
+      <c r="D94" s="10"/>
+      <c r="E94" s="10"/>
     </row>
     <row r="95" ht="14.6" customHeight="1">
-      <c r="A95" s="10"/>
-      <c r="B95" s="10"/>
-      <c r="C95" s="10"/>
-      <c r="D95" s="10"/>
-      <c r="E95" s="10"/>
+      <c r="A95" s="8"/>
+      <c r="B95" s="8"/>
+      <c r="C95" s="8"/>
+      <c r="D95" s="8"/>
+      <c r="E95" s="8"/>
     </row>
     <row r="96" ht="14.6" customHeight="1">
-      <c r="A96" s="7"/>
-      <c r="B96" s="7"/>
-      <c r="C96" s="8"/>
-      <c r="D96" s="8"/>
-      <c r="E96" s="8"/>
+      <c r="A96" s="9"/>
+      <c r="B96" s="9"/>
+      <c r="C96" s="10"/>
+      <c r="D96" s="10"/>
+      <c r="E96" s="10"/>
     </row>
     <row r="97" ht="14.6" customHeight="1">
-      <c r="A97" s="9"/>
-      <c r="B97" s="9"/>
-      <c r="C97" s="10"/>
-      <c r="D97" s="10"/>
-      <c r="E97" s="10"/>
+      <c r="A97" s="7"/>
+      <c r="B97" s="7"/>
+      <c r="C97" s="8"/>
+      <c r="D97" s="8"/>
+      <c r="E97" s="8"/>
     </row>
     <row r="98" ht="14.6" customHeight="1">
-      <c r="A98" s="7"/>
-      <c r="B98" s="7"/>
-      <c r="C98" s="8"/>
-      <c r="D98" s="8"/>
-      <c r="E98" s="8"/>
+      <c r="A98" s="9"/>
+      <c r="B98" s="9"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="10"/>
+      <c r="E98" s="10"/>
     </row>
     <row r="99" ht="14.6" customHeight="1">
-      <c r="A99" s="10"/>
-      <c r="B99" s="10"/>
-      <c r="C99" s="10"/>
-      <c r="D99" s="10"/>
-      <c r="E99" s="10"/>
+      <c r="A99" s="7"/>
+      <c r="B99" s="7"/>
+      <c r="C99" s="8"/>
+      <c r="D99" s="8"/>
+      <c r="E99" s="8"/>
     </row>
     <row r="100" ht="14.6" customHeight="1">
-      <c r="A100" s="7"/>
-      <c r="B100" s="7"/>
-      <c r="C100" s="8"/>
-      <c r="D100" s="8"/>
-      <c r="E100" s="8"/>
+      <c r="A100" s="9"/>
+      <c r="B100" s="9"/>
+      <c r="C100" s="10"/>
+      <c r="D100" s="10"/>
+      <c r="E100" s="10"/>
     </row>
     <row r="101" ht="14.6" customHeight="1">
-      <c r="A101" s="9"/>
-      <c r="B101" s="9"/>
-      <c r="C101" s="10"/>
-      <c r="D101" s="10"/>
-      <c r="E101" s="10"/>
+      <c r="A101" s="8"/>
+      <c r="B101" s="8"/>
+      <c r="C101" s="8"/>
+      <c r="D101" s="8"/>
+      <c r="E101" s="8"/>
     </row>
     <row r="102" ht="14.6" customHeight="1">
-      <c r="A102" s="7"/>
-      <c r="B102" s="7"/>
-      <c r="C102" s="8"/>
-      <c r="D102" s="8"/>
-      <c r="E102" s="8"/>
+      <c r="A102" s="9"/>
+      <c r="B102" s="10"/>
+      <c r="C102" s="10"/>
+      <c r="D102" s="10"/>
+      <c r="E102" s="10"/>
     </row>
     <row r="103" ht="14.6" customHeight="1">
-      <c r="A103" s="9"/>
-      <c r="B103" s="9"/>
-      <c r="C103" s="10"/>
-      <c r="D103" s="10"/>
-      <c r="E103" s="10"/>
+      <c r="A103" s="7"/>
+      <c r="B103" s="7"/>
+      <c r="C103" s="8"/>
+      <c r="D103" s="8"/>
+      <c r="E103" s="8"/>
     </row>
     <row r="104" ht="14.6" customHeight="1">
-      <c r="A104" s="8"/>
-      <c r="B104" s="8"/>
-      <c r="C104" s="8"/>
-      <c r="D104" s="8"/>
-      <c r="E104" s="8"/>
+      <c r="A104" s="9"/>
+      <c r="B104" s="9"/>
+      <c r="C104" s="10"/>
+      <c r="D104" s="10"/>
+      <c r="E104" s="10"/>
     </row>
     <row r="105" ht="14.6" customHeight="1">
-      <c r="A105" s="9"/>
-      <c r="B105" s="9"/>
-      <c r="C105" s="10"/>
-      <c r="D105" s="10"/>
-      <c r="E105" s="10"/>
+      <c r="A105" s="7"/>
+      <c r="B105" s="7"/>
+      <c r="C105" s="8"/>
+      <c r="D105" s="8"/>
+      <c r="E105" s="8"/>
     </row>
     <row r="106" ht="14.6" customHeight="1">
-      <c r="A106" s="7"/>
-      <c r="B106" s="7"/>
-      <c r="C106" s="8"/>
-      <c r="D106" s="8"/>
-      <c r="E106" s="8"/>
+      <c r="A106" s="9"/>
+      <c r="B106" s="9"/>
+      <c r="C106" s="10"/>
+      <c r="D106" s="10"/>
+      <c r="E106" s="10"/>
     </row>
     <row r="107" ht="14.6" customHeight="1">
-      <c r="A107" s="10"/>
-      <c r="B107" s="10"/>
-      <c r="C107" s="10"/>
-      <c r="D107" s="10"/>
-      <c r="E107" s="10"/>
+      <c r="A107" s="7"/>
+      <c r="B107" s="7"/>
+      <c r="C107" s="8"/>
+      <c r="D107" s="8"/>
+      <c r="E107" s="8"/>
     </row>
     <row r="108" ht="14.6" customHeight="1">
-      <c r="A108" s="7"/>
-      <c r="B108" s="7"/>
-      <c r="C108" s="8"/>
-      <c r="D108" s="8"/>
-      <c r="E108" s="8"/>
+      <c r="A108" s="10"/>
+      <c r="B108" s="10"/>
+      <c r="C108" s="10"/>
+      <c r="D108" s="10"/>
+      <c r="E108" s="10"/>
     </row>
     <row r="109" ht="14.6" customHeight="1">
-      <c r="A109" s="9"/>
-      <c r="B109" s="9"/>
-      <c r="C109" s="10"/>
-      <c r="D109" s="10"/>
-      <c r="E109" s="10"/>
+      <c r="A109" s="7"/>
+      <c r="B109" s="7"/>
+      <c r="C109" s="8"/>
+      <c r="D109" s="8"/>
+      <c r="E109" s="8"/>
     </row>
     <row r="110" ht="14.6" customHeight="1">
-      <c r="A110" s="7"/>
-      <c r="B110" s="7"/>
-      <c r="C110" s="8"/>
-      <c r="D110" s="8"/>
-      <c r="E110" s="8"/>
+      <c r="A110" s="9"/>
+      <c r="B110" s="9"/>
+      <c r="C110" s="10"/>
+      <c r="D110" s="10"/>
+      <c r="E110" s="10"/>
     </row>
     <row r="111" ht="14.6" customHeight="1">
-      <c r="A111" s="10"/>
-      <c r="B111" s="10"/>
-      <c r="C111" s="10"/>
-      <c r="D111" s="10"/>
-      <c r="E111" s="10"/>
+      <c r="A111" s="7"/>
+      <c r="B111" s="7"/>
+      <c r="C111" s="8"/>
+      <c r="D111" s="8"/>
+      <c r="E111" s="8"/>
     </row>
     <row r="112" ht="14.6" customHeight="1">
-      <c r="A112" s="7"/>
-      <c r="B112" s="7"/>
-      <c r="C112" s="8"/>
-      <c r="D112" s="8"/>
-      <c r="E112" s="8"/>
+      <c r="A112" s="10"/>
+      <c r="B112" s="10"/>
+      <c r="C112" s="10"/>
+      <c r="D112" s="10"/>
+      <c r="E112" s="10"/>
     </row>
     <row r="113" ht="14.6" customHeight="1">
-      <c r="A113" s="9"/>
-      <c r="B113" s="9"/>
-      <c r="C113" s="10"/>
-      <c r="D113" s="10"/>
-      <c r="E113" s="10"/>
+      <c r="A113" s="7"/>
+      <c r="B113" s="7"/>
+      <c r="C113" s="8"/>
+      <c r="D113" s="8"/>
+      <c r="E113" s="8"/>
     </row>
     <row r="114" ht="14.6" customHeight="1">
-      <c r="A114" s="8"/>
-      <c r="B114" s="8"/>
-      <c r="C114" s="8"/>
-      <c r="D114" s="8"/>
-      <c r="E114" s="8"/>
+      <c r="A114" s="9"/>
+      <c r="B114" s="9"/>
+      <c r="C114" s="10"/>
+      <c r="D114" s="10"/>
+      <c r="E114" s="10"/>
     </row>
     <row r="115" ht="14.6" customHeight="1">
-      <c r="A115" s="9"/>
-      <c r="B115" s="9"/>
-      <c r="C115" s="10"/>
-      <c r="D115" s="10"/>
-      <c r="E115" s="10"/>
+      <c r="A115" s="7"/>
+      <c r="B115" s="7"/>
+      <c r="C115" s="8"/>
+      <c r="D115" s="8"/>
+      <c r="E115" s="8"/>
     </row>
     <row r="116" ht="14.6" customHeight="1">
-      <c r="A116" s="8"/>
-      <c r="B116" s="8"/>
-      <c r="C116" s="8"/>
-      <c r="D116" s="8"/>
-      <c r="E116" s="8"/>
+      <c r="A116" s="9"/>
+      <c r="B116" s="9"/>
+      <c r="C116" s="10"/>
+      <c r="D116" s="10"/>
+      <c r="E116" s="10"/>
     </row>
     <row r="117" ht="14.6" customHeight="1">
-      <c r="A117" s="9"/>
-      <c r="B117" s="9"/>
-      <c r="C117" s="10"/>
-      <c r="D117" s="10"/>
-      <c r="E117" s="10"/>
+      <c r="A117" s="8"/>
+      <c r="B117" s="8"/>
+      <c r="C117" s="8"/>
+      <c r="D117" s="8"/>
+      <c r="E117" s="8"/>
     </row>
     <row r="118" ht="14.6" customHeight="1">
-      <c r="A118" s="7"/>
-      <c r="B118" s="7"/>
-      <c r="C118" s="8"/>
-      <c r="D118" s="8"/>
-      <c r="E118" s="8"/>
+      <c r="A118" s="9"/>
+      <c r="B118" s="9"/>
+      <c r="C118" s="10"/>
+      <c r="D118" s="10"/>
+      <c r="E118" s="10"/>
     </row>
     <row r="119" ht="14.6" customHeight="1">
-      <c r="A119" s="10"/>
-      <c r="B119" s="10"/>
-      <c r="C119" s="10"/>
-      <c r="D119" s="10"/>
-      <c r="E119" s="10"/>
+      <c r="A119" s="7"/>
+      <c r="B119" s="7"/>
+      <c r="C119" s="8"/>
+      <c r="D119" s="8"/>
+      <c r="E119" s="8"/>
     </row>
     <row r="120" ht="14.6" customHeight="1">
-      <c r="A120" s="7"/>
-      <c r="B120" s="7"/>
-      <c r="C120" s="8"/>
-      <c r="D120" s="8"/>
-      <c r="E120" s="8"/>
+      <c r="A120" s="10"/>
+      <c r="B120" s="10"/>
+      <c r="C120" s="10"/>
+      <c r="D120" s="10"/>
+      <c r="E120" s="10"/>
     </row>
     <row r="121" ht="14.6" customHeight="1">
-      <c r="A121" s="9"/>
-      <c r="B121" s="9"/>
-      <c r="C121" s="10"/>
-      <c r="D121" s="10"/>
-      <c r="E121" s="10"/>
+      <c r="A121" s="7"/>
+      <c r="B121" s="7"/>
+      <c r="C121" s="8"/>
+      <c r="D121" s="8"/>
+      <c r="E121" s="8"/>
     </row>
     <row r="122" ht="14.6" customHeight="1">
-      <c r="A122" s="8"/>
-      <c r="B122" s="8"/>
-      <c r="C122" s="8"/>
-      <c r="D122" s="8"/>
-      <c r="E122" s="8"/>
+      <c r="A122" s="9"/>
+      <c r="B122" s="9"/>
+      <c r="C122" s="10"/>
+      <c r="D122" s="10"/>
+      <c r="E122" s="10"/>
     </row>
     <row r="123" ht="14.6" customHeight="1">
-      <c r="A123" s="10"/>
-      <c r="B123" s="10"/>
-      <c r="C123" s="10"/>
-      <c r="D123" s="10"/>
-      <c r="E123" s="10"/>
+      <c r="A123" s="7"/>
+      <c r="B123" s="7"/>
+      <c r="C123" s="8"/>
+      <c r="D123" s="8"/>
+      <c r="E123" s="8"/>
     </row>
     <row r="124" ht="14.6" customHeight="1">
-      <c r="A124" s="7"/>
-      <c r="B124" s="8"/>
-      <c r="C124" s="8"/>
-      <c r="D124" s="8"/>
-      <c r="E124" s="8"/>
+      <c r="A124" s="10"/>
+      <c r="B124" s="10"/>
+      <c r="C124" s="10"/>
+      <c r="D124" s="10"/>
+      <c r="E124" s="10"/>
     </row>
     <row r="125" ht="14.6" customHeight="1">
-      <c r="A125" s="9"/>
-      <c r="B125" s="10"/>
-      <c r="C125" s="10"/>
-      <c r="D125" s="10"/>
-      <c r="E125" s="10"/>
+      <c r="A125" s="7"/>
+      <c r="B125" s="7"/>
+      <c r="C125" s="8"/>
+      <c r="D125" s="8"/>
+      <c r="E125" s="8"/>
     </row>
     <row r="126" ht="14.6" customHeight="1">
-      <c r="A126" s="7"/>
-      <c r="B126" s="7"/>
-      <c r="C126" s="8"/>
-      <c r="D126" s="8"/>
-      <c r="E126" s="8"/>
+      <c r="A126" s="9"/>
+      <c r="B126" s="9"/>
+      <c r="C126" s="10"/>
+      <c r="D126" s="10"/>
+      <c r="E126" s="10"/>
     </row>
     <row r="127" ht="14.6" customHeight="1">
-      <c r="A127" s="10"/>
-      <c r="B127" s="10"/>
-      <c r="C127" s="10"/>
-      <c r="D127" s="10"/>
-      <c r="E127" s="10"/>
+      <c r="A127" s="8"/>
+      <c r="B127" s="8"/>
+      <c r="C127" s="8"/>
+      <c r="D127" s="8"/>
+      <c r="E127" s="8"/>
     </row>
     <row r="128" ht="14.6" customHeight="1">
-      <c r="A128" s="7"/>
-      <c r="B128" s="7"/>
-      <c r="C128" s="8"/>
-      <c r="D128" s="8"/>
-      <c r="E128" s="8"/>
+      <c r="A128" s="9"/>
+      <c r="B128" s="9"/>
+      <c r="C128" s="10"/>
+      <c r="D128" s="10"/>
+      <c r="E128" s="10"/>
     </row>
     <row r="129" ht="14.6" customHeight="1">
-      <c r="A129" s="10"/>
-      <c r="B129" s="10"/>
-      <c r="C129" s="10"/>
-      <c r="D129" s="10"/>
-      <c r="E129" s="10"/>
+      <c r="A129" s="8"/>
+      <c r="B129" s="8"/>
+      <c r="C129" s="8"/>
+      <c r="D129" s="8"/>
+      <c r="E129" s="8"/>
     </row>
     <row r="130" ht="14.6" customHeight="1">
-      <c r="A130" s="8"/>
-      <c r="B130" s="8"/>
-      <c r="C130" s="8"/>
-      <c r="D130" s="8"/>
-      <c r="E130" s="8"/>
+      <c r="A130" s="9"/>
+      <c r="B130" s="9"/>
+      <c r="C130" s="10"/>
+      <c r="D130" s="10"/>
+      <c r="E130" s="10"/>
     </row>
     <row r="131" ht="14.6" customHeight="1">
-      <c r="A131" s="10"/>
-      <c r="B131" s="10"/>
-      <c r="C131" s="10"/>
-      <c r="D131" s="10"/>
-      <c r="E131" s="10"/>
+      <c r="A131" s="7"/>
+      <c r="B131" s="7"/>
+      <c r="C131" s="8"/>
+      <c r="D131" s="8"/>
+      <c r="E131" s="8"/>
     </row>
     <row r="132" ht="14.6" customHeight="1">
-      <c r="A132" s="8"/>
-      <c r="B132" s="8"/>
-      <c r="C132" s="8"/>
-      <c r="D132" s="8"/>
-      <c r="E132" s="8"/>
+      <c r="A132" s="10"/>
+      <c r="B132" s="10"/>
+      <c r="C132" s="10"/>
+      <c r="D132" s="10"/>
+      <c r="E132" s="10"/>
     </row>
     <row r="133" ht="14.6" customHeight="1">
-      <c r="A133" s="9"/>
-      <c r="B133" s="9"/>
-      <c r="C133" s="10"/>
-      <c r="D133" s="10"/>
-      <c r="E133" s="10"/>
+      <c r="A133" s="7"/>
+      <c r="B133" s="7"/>
+      <c r="C133" s="8"/>
+      <c r="D133" s="8"/>
+      <c r="E133" s="8"/>
     </row>
     <row r="134" ht="14.6" customHeight="1">
-      <c r="A134" s="7"/>
-      <c r="B134" s="7"/>
-      <c r="C134" s="8"/>
-      <c r="D134" s="8"/>
-      <c r="E134" s="8"/>
+      <c r="A134" s="9"/>
+      <c r="B134" s="9"/>
+      <c r="C134" s="10"/>
+      <c r="D134" s="10"/>
+      <c r="E134" s="10"/>
     </row>
     <row r="135" ht="14.6" customHeight="1">
-      <c r="A135" s="9"/>
-      <c r="B135" s="9"/>
-      <c r="C135" s="10"/>
-      <c r="D135" s="10"/>
-      <c r="E135" s="10"/>
+      <c r="A135" s="8"/>
+      <c r="B135" s="8"/>
+      <c r="C135" s="8"/>
+      <c r="D135" s="8"/>
+      <c r="E135" s="8"/>
     </row>
     <row r="136" ht="14.6" customHeight="1">
-      <c r="A136" s="7"/>
-      <c r="B136" s="7"/>
-      <c r="C136" s="8"/>
-      <c r="D136" s="8"/>
-      <c r="E136" s="8"/>
+      <c r="A136" s="10"/>
+      <c r="B136" s="10"/>
+      <c r="C136" s="10"/>
+      <c r="D136" s="10"/>
+      <c r="E136" s="10"/>
     </row>
     <row r="137" ht="14.6" customHeight="1">
-      <c r="A137" s="9"/>
-      <c r="B137" s="9"/>
-      <c r="C137" s="10"/>
-      <c r="D137" s="10"/>
-      <c r="E137" s="10"/>
+      <c r="A137" s="7"/>
+      <c r="B137" s="8"/>
+      <c r="C137" s="8"/>
+      <c r="D137" s="8"/>
+      <c r="E137" s="8"/>
     </row>
     <row r="138" ht="14.6" customHeight="1">
-      <c r="A138" s="7"/>
-      <c r="B138" s="7"/>
-      <c r="C138" s="8"/>
-      <c r="D138" s="8"/>
-      <c r="E138" s="8"/>
+      <c r="A138" s="9"/>
+      <c r="B138" s="10"/>
+      <c r="C138" s="10"/>
+      <c r="D138" s="10"/>
+      <c r="E138" s="10"/>
     </row>
     <row r="139" ht="14.6" customHeight="1">
-      <c r="A139" s="9"/>
-      <c r="B139" s="9"/>
-      <c r="C139" s="10"/>
-      <c r="D139" s="10"/>
-      <c r="E139" s="10"/>
+      <c r="A139" s="7"/>
+      <c r="B139" s="7"/>
+      <c r="C139" s="8"/>
+      <c r="D139" s="8"/>
+      <c r="E139" s="8"/>
     </row>
     <row r="140" ht="14.6" customHeight="1">
-      <c r="A140" s="7"/>
-      <c r="B140" s="7"/>
-      <c r="C140" s="8"/>
-      <c r="D140" s="8"/>
-      <c r="E140" s="8"/>
+      <c r="A140" s="10"/>
+      <c r="B140" s="10"/>
+      <c r="C140" s="10"/>
+      <c r="D140" s="10"/>
+      <c r="E140" s="10"/>
     </row>
     <row r="141" ht="14.6" customHeight="1">
-      <c r="A141" s="10"/>
-      <c r="B141" s="10"/>
-      <c r="C141" s="10"/>
-      <c r="D141" s="10"/>
-      <c r="E141" s="10"/>
+      <c r="A141" s="7"/>
+      <c r="B141" s="7"/>
+      <c r="C141" s="8"/>
+      <c r="D141" s="8"/>
+      <c r="E141" s="8"/>
     </row>
     <row r="142" ht="14.6" customHeight="1">
-      <c r="A142" s="7"/>
-      <c r="B142" s="7"/>
-      <c r="C142" s="8"/>
-      <c r="D142" s="8"/>
-      <c r="E142" s="8"/>
+      <c r="A142" s="10"/>
+      <c r="B142" s="10"/>
+      <c r="C142" s="10"/>
+      <c r="D142" s="10"/>
+      <c r="E142" s="10"/>
     </row>
     <row r="143" ht="14.6" customHeight="1">
-      <c r="A143" s="9"/>
-      <c r="B143" s="9"/>
-      <c r="C143" s="10"/>
-      <c r="D143" s="10"/>
-      <c r="E143" s="10"/>
+      <c r="A143" s="8"/>
+      <c r="B143" s="8"/>
+      <c r="C143" s="8"/>
+      <c r="D143" s="8"/>
+      <c r="E143" s="8"/>
     </row>
     <row r="144" ht="14.6" customHeight="1">
-      <c r="A144" s="7"/>
-      <c r="B144" s="7"/>
-      <c r="C144" s="8"/>
-      <c r="D144" s="8"/>
-      <c r="E144" s="8"/>
+      <c r="A144" s="10"/>
+      <c r="B144" s="10"/>
+      <c r="C144" s="10"/>
+      <c r="D144" s="10"/>
+      <c r="E144" s="10"/>
     </row>
     <row r="145" ht="14.6" customHeight="1">
-      <c r="A145" s="9"/>
-      <c r="B145" s="9"/>
-      <c r="C145" s="10"/>
-      <c r="D145" s="10"/>
-      <c r="E145" s="10"/>
+      <c r="A145" s="8"/>
+      <c r="B145" s="8"/>
+      <c r="C145" s="8"/>
+      <c r="D145" s="8"/>
+      <c r="E145" s="8"/>
     </row>
     <row r="146" ht="14.6" customHeight="1">
-      <c r="A146" s="8"/>
-      <c r="B146" s="8"/>
-      <c r="C146" s="8"/>
-      <c r="D146" s="8"/>
-      <c r="E146" s="8"/>
+      <c r="A146" s="9"/>
+      <c r="B146" s="9"/>
+      <c r="C146" s="10"/>
+      <c r="D146" s="10"/>
+      <c r="E146" s="10"/>
     </row>
     <row r="147" ht="14.6" customHeight="1">
-      <c r="A147" s="9"/>
-      <c r="B147" s="9"/>
-      <c r="C147" s="10"/>
-      <c r="D147" s="10"/>
-      <c r="E147" s="10"/>
+      <c r="A147" s="7"/>
+      <c r="B147" s="7"/>
+      <c r="C147" s="8"/>
+      <c r="D147" s="8"/>
+      <c r="E147" s="8"/>
     </row>
     <row r="148" ht="14.6" customHeight="1">
-      <c r="A148" s="7"/>
-      <c r="B148" s="7"/>
-      <c r="C148" s="8"/>
-      <c r="D148" s="8"/>
-      <c r="E148" s="8"/>
+      <c r="A148" s="9"/>
+      <c r="B148" s="9"/>
+      <c r="C148" s="10"/>
+      <c r="D148" s="10"/>
+      <c r="E148" s="10"/>
     </row>
     <row r="149" ht="14.6" customHeight="1">
-      <c r="A149" s="9"/>
-      <c r="B149" s="9"/>
-      <c r="C149" s="10"/>
-      <c r="D149" s="10"/>
-      <c r="E149" s="10"/>
+      <c r="A149" s="7"/>
+      <c r="B149" s="7"/>
+      <c r="C149" s="8"/>
+      <c r="D149" s="8"/>
+      <c r="E149" s="8"/>
     </row>
     <row r="150" ht="14.6" customHeight="1">
-      <c r="A150" s="7"/>
-      <c r="B150" s="7"/>
-      <c r="C150" s="8"/>
-      <c r="D150" s="8"/>
-      <c r="E150" s="8"/>
+      <c r="A150" s="9"/>
+      <c r="B150" s="9"/>
+      <c r="C150" s="10"/>
+      <c r="D150" s="10"/>
+      <c r="E150" s="10"/>
     </row>
     <row r="151" ht="14.6" customHeight="1">
-      <c r="A151" s="9"/>
-      <c r="B151" s="9"/>
-      <c r="C151" s="10"/>
-      <c r="D151" s="10"/>
-      <c r="E151" s="10"/>
+      <c r="A151" s="7"/>
+      <c r="B151" s="7"/>
+      <c r="C151" s="8"/>
+      <c r="D151" s="8"/>
+      <c r="E151" s="8"/>
     </row>
     <row r="152" ht="14.6" customHeight="1">
-      <c r="A152" s="7"/>
-      <c r="B152" s="7"/>
-      <c r="C152" s="8"/>
-      <c r="D152" s="8"/>
-      <c r="E152" s="8"/>
+      <c r="A152" s="9"/>
+      <c r="B152" s="9"/>
+      <c r="C152" s="10"/>
+      <c r="D152" s="10"/>
+      <c r="E152" s="10"/>
     </row>
     <row r="153" ht="14.6" customHeight="1">
-      <c r="A153" s="9"/>
-      <c r="B153" s="9"/>
-      <c r="C153" s="10"/>
-      <c r="D153" s="10"/>
-      <c r="E153" s="10"/>
+      <c r="A153" s="7"/>
+      <c r="B153" s="7"/>
+      <c r="C153" s="8"/>
+      <c r="D153" s="8"/>
+      <c r="E153" s="8"/>
     </row>
     <row r="154" ht="14.6" customHeight="1">
-      <c r="A154" s="8"/>
-      <c r="B154" s="8"/>
-      <c r="C154" s="8"/>
-      <c r="D154" s="8"/>
-      <c r="E154" s="8"/>
+      <c r="A154" s="10"/>
+      <c r="B154" s="10"/>
+      <c r="C154" s="10"/>
+      <c r="D154" s="10"/>
+      <c r="E154" s="10"/>
     </row>
     <row r="155" ht="14.6" customHeight="1">
-      <c r="A155" s="9"/>
-      <c r="B155" s="9"/>
-      <c r="C155" s="10"/>
-      <c r="D155" s="10"/>
-      <c r="E155" s="10"/>
+      <c r="A155" s="7"/>
+      <c r="B155" s="7"/>
+      <c r="C155" s="8"/>
+      <c r="D155" s="8"/>
+      <c r="E155" s="8"/>
     </row>
     <row r="156" ht="14.6" customHeight="1">
-      <c r="A156" s="7"/>
-      <c r="B156" s="7"/>
-      <c r="C156" s="8"/>
-      <c r="D156" s="8"/>
-      <c r="E156" s="8"/>
+      <c r="A156" s="9"/>
+      <c r="B156" s="9"/>
+      <c r="C156" s="10"/>
+      <c r="D156" s="10"/>
+      <c r="E156" s="10"/>
     </row>
     <row r="157" ht="14.6" customHeight="1">
-      <c r="A157" s="9"/>
-      <c r="B157" s="9"/>
-      <c r="C157" s="10"/>
-      <c r="D157" s="10"/>
-      <c r="E157" s="10"/>
+      <c r="A157" s="7"/>
+      <c r="B157" s="7"/>
+      <c r="C157" s="8"/>
+      <c r="D157" s="8"/>
+      <c r="E157" s="8"/>
     </row>
     <row r="158" ht="14.6" customHeight="1">
-      <c r="A158" s="8"/>
-      <c r="B158" s="8"/>
-      <c r="C158" s="8"/>
-      <c r="D158" s="8"/>
-      <c r="E158" s="8"/>
+      <c r="A158" s="9"/>
+      <c r="B158" s="9"/>
+      <c r="C158" s="10"/>
+      <c r="D158" s="10"/>
+      <c r="E158" s="10"/>
     </row>
     <row r="159" ht="14.6" customHeight="1">
-      <c r="A159" s="9"/>
-      <c r="B159" s="9"/>
-      <c r="C159" s="10"/>
-      <c r="D159" s="10"/>
-      <c r="E159" s="10"/>
+      <c r="A159" s="8"/>
+      <c r="B159" s="8"/>
+      <c r="C159" s="8"/>
+      <c r="D159" s="8"/>
+      <c r="E159" s="8"/>
     </row>
     <row r="160" ht="14.6" customHeight="1">
-      <c r="A160" s="7"/>
-      <c r="B160" s="7"/>
-      <c r="C160" s="8"/>
-      <c r="D160" s="8"/>
-      <c r="E160" s="8"/>
+      <c r="A160" s="9"/>
+      <c r="B160" s="9"/>
+      <c r="C160" s="10"/>
+      <c r="D160" s="10"/>
+      <c r="E160" s="10"/>
     </row>
     <row r="161" ht="14.6" customHeight="1">
-      <c r="A161" s="10"/>
-      <c r="B161" s="10"/>
-      <c r="C161" s="10"/>
-      <c r="D161" s="10"/>
-      <c r="E161" s="10"/>
+      <c r="A161" s="7"/>
+      <c r="B161" s="7"/>
+      <c r="C161" s="8"/>
+      <c r="D161" s="8"/>
+      <c r="E161" s="8"/>
     </row>
     <row r="162" ht="14.6" customHeight="1">
-      <c r="A162" s="7"/>
-      <c r="B162" s="7"/>
-      <c r="C162" s="8"/>
-      <c r="D162" s="8"/>
-      <c r="E162" s="8"/>
+      <c r="A162" s="9"/>
+      <c r="B162" s="9"/>
+      <c r="C162" s="10"/>
+      <c r="D162" s="10"/>
+      <c r="E162" s="10"/>
     </row>
     <row r="163" ht="14.6" customHeight="1">
-      <c r="A163" s="9"/>
-      <c r="B163" s="9"/>
-      <c r="C163" s="10"/>
-      <c r="D163" s="10"/>
-      <c r="E163" s="10"/>
+      <c r="A163" s="7"/>
+      <c r="B163" s="7"/>
+      <c r="C163" s="8"/>
+      <c r="D163" s="8"/>
+      <c r="E163" s="8"/>
     </row>
     <row r="164" ht="14.6" customHeight="1">
-      <c r="A164" s="8"/>
-      <c r="B164" s="8"/>
-      <c r="C164" s="8"/>
-      <c r="D164" s="8"/>
-      <c r="E164" s="8"/>
+      <c r="A164" s="9"/>
+      <c r="B164" s="9"/>
+      <c r="C164" s="10"/>
+      <c r="D164" s="10"/>
+      <c r="E164" s="10"/>
     </row>
     <row r="165" ht="14.6" customHeight="1">
-      <c r="A165" s="9"/>
-      <c r="B165" s="9"/>
-      <c r="C165" s="10"/>
-      <c r="D165" s="10"/>
-      <c r="E165" s="10"/>
+      <c r="A165" s="7"/>
+      <c r="B165" s="7"/>
+      <c r="C165" s="8"/>
+      <c r="D165" s="8"/>
+      <c r="E165" s="8"/>
     </row>
     <row r="166" ht="14.6" customHeight="1">
-      <c r="A166" s="7"/>
-      <c r="B166" s="7"/>
-      <c r="C166" s="8"/>
-      <c r="D166" s="8"/>
-      <c r="E166" s="8"/>
+      <c r="A166" s="9"/>
+      <c r="B166" s="9"/>
+      <c r="C166" s="10"/>
+      <c r="D166" s="10"/>
+      <c r="E166" s="10"/>
     </row>
     <row r="167" ht="14.6" customHeight="1">
-      <c r="A167" s="10"/>
-      <c r="B167" s="10"/>
-      <c r="C167" s="10"/>
-      <c r="D167" s="10"/>
-      <c r="E167" s="10"/>
+      <c r="A167" s="8"/>
+      <c r="B167" s="8"/>
+      <c r="C167" s="8"/>
+      <c r="D167" s="8"/>
+      <c r="E167" s="8"/>
     </row>
     <row r="168" ht="14.6" customHeight="1">
-      <c r="A168" s="7"/>
-      <c r="B168" s="7"/>
-      <c r="C168" s="8"/>
-      <c r="D168" s="8"/>
-      <c r="E168" s="8"/>
+      <c r="A168" s="9"/>
+      <c r="B168" s="9"/>
+      <c r="C168" s="10"/>
+      <c r="D168" s="10"/>
+      <c r="E168" s="10"/>
     </row>
     <row r="169" ht="14.6" customHeight="1">
-      <c r="A169" s="9"/>
-      <c r="B169" s="9"/>
-      <c r="C169" s="10"/>
-      <c r="D169" s="10"/>
-      <c r="E169" s="10"/>
+      <c r="A169" s="7"/>
+      <c r="B169" s="7"/>
+      <c r="C169" s="8"/>
+      <c r="D169" s="8"/>
+      <c r="E169" s="8"/>
+    </row>
+    <row r="170" ht="14.6" customHeight="1">
+      <c r="A170" s="9"/>
+      <c r="B170" s="9"/>
+      <c r="C170" s="10"/>
+      <c r="D170" s="10"/>
+      <c r="E170" s="10"/>
+    </row>
+    <row r="171" ht="14.6" customHeight="1">
+      <c r="A171" s="8"/>
+      <c r="B171" s="8"/>
+      <c r="C171" s="8"/>
+      <c r="D171" s="8"/>
+      <c r="E171" s="8"/>
+    </row>
+    <row r="172" ht="14.6" customHeight="1">
+      <c r="A172" s="9"/>
+      <c r="B172" s="9"/>
+      <c r="C172" s="10"/>
+      <c r="D172" s="10"/>
+      <c r="E172" s="10"/>
+    </row>
+    <row r="173" ht="14.6" customHeight="1">
+      <c r="A173" s="7"/>
+      <c r="B173" s="7"/>
+      <c r="C173" s="8"/>
+      <c r="D173" s="8"/>
+      <c r="E173" s="8"/>
+    </row>
+    <row r="174" ht="14.6" customHeight="1">
+      <c r="A174" s="10"/>
+      <c r="B174" s="10"/>
+      <c r="C174" s="10"/>
+      <c r="D174" s="10"/>
+      <c r="E174" s="10"/>
+    </row>
+    <row r="175" ht="14.6" customHeight="1">
+      <c r="A175" s="7"/>
+      <c r="B175" s="7"/>
+      <c r="C175" s="8"/>
+      <c r="D175" s="8"/>
+      <c r="E175" s="8"/>
+    </row>
+    <row r="176" ht="14.6" customHeight="1">
+      <c r="A176" s="9"/>
+      <c r="B176" s="9"/>
+      <c r="C176" s="10"/>
+      <c r="D176" s="10"/>
+      <c r="E176" s="10"/>
+    </row>
+    <row r="177" ht="14.6" customHeight="1">
+      <c r="A177" s="8"/>
+      <c r="B177" s="8"/>
+      <c r="C177" s="8"/>
+      <c r="D177" s="8"/>
+      <c r="E177" s="8"/>
+    </row>
+    <row r="178" ht="14.6" customHeight="1">
+      <c r="A178" s="9"/>
+      <c r="B178" s="9"/>
+      <c r="C178" s="10"/>
+      <c r="D178" s="10"/>
+      <c r="E178" s="10"/>
+    </row>
+    <row r="179" ht="14.6" customHeight="1">
+      <c r="A179" s="7"/>
+      <c r="B179" s="7"/>
+      <c r="C179" s="8"/>
+      <c r="D179" s="8"/>
+      <c r="E179" s="8"/>
+    </row>
+    <row r="180" ht="14.6" customHeight="1">
+      <c r="A180" s="10"/>
+      <c r="B180" s="10"/>
+      <c r="C180" s="10"/>
+      <c r="D180" s="10"/>
+      <c r="E180" s="10"/>
+    </row>
+    <row r="181" ht="14.6" customHeight="1">
+      <c r="A181" s="7"/>
+      <c r="B181" s="7"/>
+      <c r="C181" s="8"/>
+      <c r="D181" s="8"/>
+      <c r="E181" s="8"/>
+    </row>
+    <row r="182" ht="14.6" customHeight="1">
+      <c r="A182" s="9"/>
+      <c r="B182" s="9"/>
+      <c r="C182" s="10"/>
+      <c r="D182" s="10"/>
+      <c r="E182" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -12109,10 +12349,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="14.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="48" style="45" customWidth="1"/>
-    <col min="2" max="2" width="61.8516" style="45" customWidth="1"/>
-    <col min="3" max="5" width="16.3516" style="45" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="45" customWidth="1"/>
+    <col min="1" max="1" width="48" style="59" customWidth="1"/>
+    <col min="2" max="2" width="61.8516" style="59" customWidth="1"/>
+    <col min="3" max="5" width="16.3516" style="59" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="59" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
@@ -12138,7 +12378,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>137</v>
+        <v>167</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -12149,7 +12389,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>138</v>
+        <v>168</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -12178,7 +12418,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s" s="9">
-        <v>139</v>
+        <v>169</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -12240,10 +12480,10 @@
     </row>
     <row r="14" ht="15.35" customHeight="1">
       <c r="A14" t="s" s="30">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="B14" t="s" s="30">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -12251,10 +12491,10 @@
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" t="s" s="22">
-        <v>142</v>
+        <v>172</v>
       </c>
       <c r="B15" t="s" s="7">
-        <v>143</v>
+        <v>173</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -12269,10 +12509,10 @@
     </row>
     <row r="17" ht="15.35" customHeight="1">
       <c r="A17" t="s" s="30">
-        <v>144</v>
+        <v>174</v>
       </c>
       <c r="B17" t="s" s="30">
-        <v>145</v>
+        <v>175</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -12312,7 +12552,7 @@
         <v>68</v>
       </c>
       <c r="B21" t="s" s="23">
-        <v>146</v>
+        <v>176</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -12338,10 +12578,10 @@
     </row>
     <row r="24" ht="15.35" customHeight="1">
       <c r="A24" t="s" s="22">
-        <v>147</v>
+        <v>177</v>
       </c>
       <c r="B24" t="s" s="23">
-        <v>148</v>
+        <v>178</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -12349,10 +12589,10 @@
     </row>
     <row r="25" ht="15.35" customHeight="1">
       <c r="A25" t="s" s="22">
-        <v>149</v>
+        <v>179</v>
       </c>
       <c r="B25" t="s" s="23">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
@@ -12360,10 +12600,10 @@
     </row>
     <row r="26" ht="15.35" customHeight="1">
       <c r="A26" t="s" s="22">
-        <v>151</v>
+        <v>181</v>
       </c>
       <c r="B26" t="s" s="23">
-        <v>152</v>
+        <v>182</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
@@ -12378,10 +12618,10 @@
     </row>
     <row r="28" ht="15.35" customHeight="1">
       <c r="A28" t="s" s="30">
-        <v>153</v>
+        <v>183</v>
       </c>
       <c r="B28" t="s" s="30">
-        <v>154</v>
+        <v>184</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -12389,10 +12629,10 @@
     </row>
     <row r="29" ht="15.35" customHeight="1">
       <c r="A29" t="s" s="30">
-        <v>155</v>
+        <v>185</v>
       </c>
       <c r="B29" t="s" s="30">
-        <v>156</v>
+        <v>186</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -12400,10 +12640,10 @@
     </row>
     <row r="30" ht="15.35" customHeight="1">
       <c r="A30" t="s" s="30">
-        <v>157</v>
+        <v>187</v>
       </c>
       <c r="B30" t="s" s="30">
-        <v>158</v>
+        <v>188</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -12417,11 +12657,11 @@
       <c r="E31" s="8"/>
     </row>
     <row r="32" ht="15.35" customHeight="1">
-      <c r="A32" t="s" s="46">
-        <v>159</v>
+      <c r="A32" t="s" s="60">
+        <v>189</v>
       </c>
       <c r="B32" t="s" s="26">
-        <v>160</v>
+        <v>190</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
@@ -12429,10 +12669,10 @@
     </row>
     <row r="33" ht="14.6" customHeight="1">
       <c r="A33" t="s" s="14">
-        <v>161</v>
-      </c>
-      <c r="B33" t="s" s="47">
-        <v>160</v>
+        <v>191</v>
+      </c>
+      <c r="B33" t="s" s="61">
+        <v>190</v>
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -12440,7 +12680,7 @@
     </row>
     <row r="34" ht="14.6" customHeight="1">
       <c r="A34" t="s" s="25">
-        <v>162</v>
+        <v>192</v>
       </c>
       <c r="B34" t="s" s="26">
         <v>65</v>
@@ -12450,8 +12690,8 @@
       <c r="E34" s="10"/>
     </row>
     <row r="35" ht="14.6" customHeight="1">
-      <c r="A35" s="48"/>
-      <c r="B35" s="49"/>
+      <c r="A35" s="50"/>
+      <c r="B35" s="62"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
@@ -12497,17 +12737,17 @@
       <c r="E39" s="8"/>
     </row>
     <row r="40" ht="14.6" customHeight="1">
-      <c r="A40" s="50"/>
-      <c r="B40" s="51"/>
+      <c r="A40" s="63"/>
+      <c r="B40" s="64"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
     </row>
     <row r="41" ht="14.6" customHeight="1">
-      <c r="A41" t="s" s="52">
-        <v>163</v>
-      </c>
-      <c r="B41" s="53">
+      <c r="A41" t="s" s="46">
+        <v>155</v>
+      </c>
+      <c r="B41" s="47">
         <v>0</v>
       </c>
       <c r="C41" s="8"/>
@@ -12515,10 +12755,10 @@
       <c r="E41" s="8"/>
     </row>
     <row r="42" ht="14.6" customHeight="1">
-      <c r="A42" t="s" s="54">
-        <v>164</v>
-      </c>
-      <c r="B42" s="55">
+      <c r="A42" t="s" s="48">
+        <v>193</v>
+      </c>
+      <c r="B42" s="49">
         <v>1</v>
       </c>
       <c r="C42" s="10"/>
@@ -12526,10 +12766,10 @@
       <c r="E42" s="10"/>
     </row>
     <row r="43" ht="14.6" customHeight="1">
-      <c r="A43" t="s" s="56">
-        <v>165</v>
-      </c>
-      <c r="B43" s="57">
+      <c r="A43" t="s" s="65">
+        <v>158</v>
+      </c>
+      <c r="B43" s="51">
         <v>2</v>
       </c>
       <c r="C43" s="10"/>
@@ -12537,10 +12777,10 @@
       <c r="E43" s="10"/>
     </row>
     <row r="44" ht="14.6" customHeight="1">
-      <c r="A44" t="s" s="58">
-        <v>166</v>
-      </c>
-      <c r="B44" s="59">
+      <c r="A44" t="s" s="54">
+        <v>159</v>
+      </c>
+      <c r="B44" s="53">
         <v>3</v>
       </c>
       <c r="C44" s="8"/>
@@ -12548,10 +12788,10 @@
       <c r="E44" s="8"/>
     </row>
     <row r="45" ht="14.6" customHeight="1">
-      <c r="A45" t="s" s="60">
-        <v>167</v>
-      </c>
-      <c r="B45" s="61">
+      <c r="A45" t="s" s="56">
+        <v>160</v>
+      </c>
+      <c r="B45" s="55">
         <v>4</v>
       </c>
       <c r="C45" s="10"/>
@@ -12559,10 +12799,10 @@
       <c r="E45" s="10"/>
     </row>
     <row r="46" ht="14.6" customHeight="1">
-      <c r="A46" t="s" s="58">
-        <v>168</v>
-      </c>
-      <c r="B46" s="59">
+      <c r="A46" t="s" s="54">
+        <v>161</v>
+      </c>
+      <c r="B46" s="53">
         <v>5</v>
       </c>
       <c r="C46" s="8"/>
@@ -12570,10 +12810,10 @@
       <c r="E46" s="8"/>
     </row>
     <row r="47" ht="14.6" customHeight="1">
-      <c r="A47" t="s" s="62">
-        <v>169</v>
-      </c>
-      <c r="B47" s="63">
+      <c r="A47" t="s" s="58">
+        <v>162</v>
+      </c>
+      <c r="B47" s="57">
         <v>6</v>
       </c>
       <c r="C47" s="10"/>
@@ -13566,10 +13806,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="14.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="48" style="64" customWidth="1"/>
-    <col min="2" max="2" width="61.8516" style="64" customWidth="1"/>
-    <col min="3" max="5" width="16.3516" style="64" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="64" customWidth="1"/>
+    <col min="1" max="1" width="48" style="66" customWidth="1"/>
+    <col min="2" max="2" width="61.8516" style="66" customWidth="1"/>
+    <col min="3" max="5" width="16.3516" style="66" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="66" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
@@ -13595,7 +13835,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>170</v>
+        <v>194</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -13606,7 +13846,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>171</v>
+        <v>195</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -13635,7 +13875,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s" s="9">
-        <v>172</v>
+        <v>196</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -13697,10 +13937,10 @@
     </row>
     <row r="14" ht="15.35" customHeight="1">
       <c r="A14" t="s" s="30">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="B14" t="s" s="30">
-        <v>173</v>
+        <v>197</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -13708,10 +13948,10 @@
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" t="s" s="22">
-        <v>174</v>
+        <v>198</v>
       </c>
       <c r="B15" t="s" s="7">
-        <v>175</v>
+        <v>199</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -13725,10 +13965,10 @@
       <c r="E16" s="8"/>
     </row>
     <row r="17" ht="15.35" customHeight="1">
-      <c r="A17" t="s" s="52">
-        <v>163</v>
-      </c>
-      <c r="B17" s="53">
+      <c r="A17" t="s" s="46">
+        <v>155</v>
+      </c>
+      <c r="B17" s="47">
         <v>0</v>
       </c>
       <c r="C17" s="8"/>
@@ -13736,10 +13976,10 @@
       <c r="E17" s="8"/>
     </row>
     <row r="18" ht="15.35" customHeight="1">
-      <c r="A18" t="s" s="54">
-        <v>164</v>
-      </c>
-      <c r="B18" s="55">
+      <c r="A18" t="s" s="48">
+        <v>193</v>
+      </c>
+      <c r="B18" s="49">
         <v>1</v>
       </c>
       <c r="C18" s="10"/>
@@ -13747,10 +13987,10 @@
       <c r="E18" s="10"/>
     </row>
     <row r="19" ht="15.35" customHeight="1">
-      <c r="A19" t="s" s="54">
-        <v>176</v>
-      </c>
-      <c r="B19" s="57">
+      <c r="A19" t="s" s="48">
+        <v>200</v>
+      </c>
+      <c r="B19" s="51">
         <v>2</v>
       </c>
       <c r="C19" s="10"/>
@@ -13758,10 +13998,10 @@
       <c r="E19" s="10"/>
     </row>
     <row r="20" ht="15.35" customHeight="1">
-      <c r="A20" t="s" s="56">
-        <v>165</v>
-      </c>
-      <c r="B20" s="65">
+      <c r="A20" t="s" s="65">
+        <v>158</v>
+      </c>
+      <c r="B20" s="67">
         <v>3</v>
       </c>
       <c r="C20" s="8"/>
@@ -13769,10 +14009,10 @@
       <c r="E20" s="8"/>
     </row>
     <row r="21" ht="15.35" customHeight="1">
-      <c r="A21" t="s" s="58">
-        <v>166</v>
-      </c>
-      <c r="B21" s="61">
+      <c r="A21" t="s" s="54">
+        <v>159</v>
+      </c>
+      <c r="B21" s="55">
         <v>4</v>
       </c>
       <c r="C21" s="10"/>
@@ -13780,10 +14020,10 @@
       <c r="E21" s="10"/>
     </row>
     <row r="22" ht="15.35" customHeight="1">
-      <c r="A22" t="s" s="60">
-        <v>167</v>
-      </c>
-      <c r="B22" s="59">
+      <c r="A22" t="s" s="56">
+        <v>160</v>
+      </c>
+      <c r="B22" s="53">
         <v>5</v>
       </c>
       <c r="C22" s="8"/>
@@ -13791,10 +14031,10 @@
       <c r="E22" s="8"/>
     </row>
     <row r="23" ht="15.35" customHeight="1">
-      <c r="A23" t="s" s="58">
-        <v>168</v>
-      </c>
-      <c r="B23" s="63">
+      <c r="A23" t="s" s="54">
+        <v>161</v>
+      </c>
+      <c r="B23" s="57">
         <v>6</v>
       </c>
       <c r="C23" s="10"/>
@@ -13802,11 +14042,11 @@
       <c r="E23" s="10"/>
     </row>
     <row r="24" ht="15.35" customHeight="1">
-      <c r="A24" t="s" s="62">
-        <v>169</v>
+      <c r="A24" t="s" s="58">
+        <v>162</v>
       </c>
       <c r="B24" t="s" s="23">
-        <v>177</v>
+        <v>201</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -13857,7 +14097,7 @@
         <v>83</v>
       </c>
       <c r="B29" t="s" s="30">
-        <v>178</v>
+        <v>202</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -13872,7 +14112,7 @@
     </row>
     <row r="31" ht="15.35" customHeight="1">
       <c r="A31" t="s" s="22">
-        <v>179</v>
+        <v>203</v>
       </c>
       <c r="B31" t="s" s="23">
         <v>25</v>
@@ -13886,7 +14126,7 @@
         <v>58</v>
       </c>
       <c r="B32" t="s" s="30">
-        <v>180</v>
+        <v>204</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
@@ -13894,10 +14134,10 @@
     </row>
     <row r="33" ht="15.35" customHeight="1">
       <c r="A33" t="s" s="30">
-        <v>181</v>
+        <v>205</v>
       </c>
       <c r="B33" t="s" s="30">
-        <v>182</v>
+        <v>206</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
@@ -13905,10 +14145,10 @@
     </row>
     <row r="34" ht="15.35" customHeight="1">
       <c r="A34" t="s" s="30">
-        <v>183</v>
+        <v>207</v>
       </c>
       <c r="B34" t="s" s="30">
-        <v>182</v>
+        <v>206</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
@@ -13916,10 +14156,10 @@
     </row>
     <row r="35" ht="15.35" customHeight="1">
       <c r="A35" t="s" s="43">
-        <v>184</v>
+        <v>208</v>
       </c>
       <c r="B35" t="s" s="43">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -13927,10 +14167,10 @@
     </row>
     <row r="36" ht="15.35" customHeight="1">
       <c r="A36" t="s" s="30">
-        <v>186</v>
+        <v>210</v>
       </c>
       <c r="B36" t="s" s="30">
-        <v>187</v>
+        <v>211</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
@@ -13944,55 +14184,55 @@
       <c r="E37" s="8"/>
     </row>
     <row r="38" ht="15.35" customHeight="1">
-      <c r="A38" t="s" s="66">
-        <v>188</v>
-      </c>
-      <c r="B38" t="s" s="67">
-        <v>189</v>
+      <c r="A38" t="s" s="68">
+        <v>212</v>
+      </c>
+      <c r="B38" t="s" s="69">
+        <v>213</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
     </row>
     <row r="39" ht="14.6" customHeight="1">
-      <c r="A39" t="s" s="68">
-        <v>190</v>
-      </c>
-      <c r="B39" t="s" s="47">
-        <v>191</v>
+      <c r="A39" t="s" s="70">
+        <v>214</v>
+      </c>
+      <c r="B39" t="s" s="61">
+        <v>140</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
     </row>
     <row r="40" ht="14.6" customHeight="1">
-      <c r="A40" t="s" s="69">
-        <v>192</v>
-      </c>
-      <c r="B40" t="s" s="67">
-        <v>193</v>
+      <c r="A40" t="s" s="71">
+        <v>215</v>
+      </c>
+      <c r="B40" t="s" s="69">
+        <v>216</v>
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
     </row>
     <row r="41" ht="14.6" customHeight="1">
-      <c r="A41" t="s" s="70">
-        <v>194</v>
-      </c>
-      <c r="B41" t="s" s="71">
-        <v>160</v>
+      <c r="A41" t="s" s="72">
+        <v>217</v>
+      </c>
+      <c r="B41" t="s" s="73">
+        <v>190</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" ht="14.6" customHeight="1">
-      <c r="A42" t="s" s="72">
-        <v>195</v>
-      </c>
-      <c r="B42" t="s" s="73">
-        <v>196</v>
+      <c r="A42" t="s" s="74">
+        <v>218</v>
+      </c>
+      <c r="B42" t="s" s="75">
+        <v>219</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
@@ -14000,10 +14240,10 @@
     </row>
     <row r="43" ht="14.6" customHeight="1">
       <c r="A43" t="s" s="30">
-        <v>197</v>
+        <v>220</v>
       </c>
       <c r="B43" t="s" s="30">
-        <v>198</v>
+        <v>221</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
@@ -14011,10 +14251,10 @@
     </row>
     <row r="44" ht="14.6" customHeight="1">
       <c r="A44" t="s" s="30">
-        <v>199</v>
+        <v>222</v>
       </c>
       <c r="B44" t="s" s="30">
-        <v>200</v>
+        <v>223</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
@@ -14022,82 +14262,82 @@
     </row>
     <row r="45" ht="14.6" customHeight="1">
       <c r="A45" t="s" s="30">
-        <v>201</v>
+        <v>224</v>
       </c>
       <c r="B45" t="s" s="30">
-        <v>202</v>
+        <v>225</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
     </row>
     <row r="46" ht="14.6" customHeight="1">
-      <c r="A46" t="s" s="69">
-        <v>203</v>
-      </c>
-      <c r="B46" t="s" s="67">
-        <v>204</v>
+      <c r="A46" t="s" s="71">
+        <v>226</v>
+      </c>
+      <c r="B46" t="s" s="69">
+        <v>227</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
     </row>
     <row r="47" ht="14.6" customHeight="1">
-      <c r="A47" t="s" s="74">
-        <v>205</v>
-      </c>
-      <c r="B47" t="s" s="75">
-        <v>206</v>
-      </c>
-      <c r="C47" s="76"/>
-      <c r="D47" s="76"/>
-      <c r="E47" s="77"/>
+      <c r="A47" t="s" s="76">
+        <v>228</v>
+      </c>
+      <c r="B47" t="s" s="77">
+        <v>229</v>
+      </c>
+      <c r="C47" s="78"/>
+      <c r="D47" s="78"/>
+      <c r="E47" s="79"/>
     </row>
     <row r="48" ht="14.6" customHeight="1">
-      <c r="A48" t="s" s="78">
-        <v>207</v>
-      </c>
-      <c r="B48" t="s" s="79">
-        <v>208</v>
-      </c>
-      <c r="C48" s="80"/>
-      <c r="D48" s="80"/>
-      <c r="E48" s="81"/>
+      <c r="A48" t="s" s="80">
+        <v>230</v>
+      </c>
+      <c r="B48" t="s" s="81">
+        <v>231</v>
+      </c>
+      <c r="C48" s="82"/>
+      <c r="D48" s="82"/>
+      <c r="E48" s="83"/>
     </row>
     <row r="49" ht="14.6" customHeight="1">
-      <c r="A49" s="82"/>
-      <c r="B49" s="80"/>
-      <c r="C49" s="80"/>
-      <c r="D49" s="80"/>
-      <c r="E49" s="81"/>
+      <c r="A49" s="84"/>
+      <c r="B49" s="82"/>
+      <c r="C49" s="82"/>
+      <c r="D49" s="82"/>
+      <c r="E49" s="83"/>
     </row>
     <row r="50" ht="14.6" customHeight="1">
-      <c r="A50" s="82"/>
-      <c r="B50" s="80"/>
-      <c r="C50" s="80"/>
-      <c r="D50" s="80"/>
-      <c r="E50" s="81"/>
+      <c r="A50" s="84"/>
+      <c r="B50" s="82"/>
+      <c r="C50" s="82"/>
+      <c r="D50" s="82"/>
+      <c r="E50" s="83"/>
     </row>
     <row r="51" ht="14.6" customHeight="1">
-      <c r="A51" s="82"/>
-      <c r="B51" s="80"/>
-      <c r="C51" s="80"/>
-      <c r="D51" s="80"/>
-      <c r="E51" s="81"/>
+      <c r="A51" s="84"/>
+      <c r="B51" s="82"/>
+      <c r="C51" s="82"/>
+      <c r="D51" s="82"/>
+      <c r="E51" s="83"/>
     </row>
     <row r="52" ht="14.6" customHeight="1">
-      <c r="A52" s="82"/>
-      <c r="B52" s="80"/>
-      <c r="C52" s="80"/>
-      <c r="D52" s="80"/>
-      <c r="E52" s="81"/>
+      <c r="A52" s="84"/>
+      <c r="B52" s="82"/>
+      <c r="C52" s="82"/>
+      <c r="D52" s="82"/>
+      <c r="E52" s="83"/>
     </row>
     <row r="53" ht="14.6" customHeight="1">
-      <c r="A53" s="83"/>
-      <c r="B53" s="84"/>
-      <c r="C53" s="84"/>
-      <c r="D53" s="84"/>
-      <c r="E53" s="85"/>
+      <c r="A53" s="85"/>
+      <c r="B53" s="86"/>
+      <c r="C53" s="86"/>
+      <c r="D53" s="86"/>
+      <c r="E53" s="87"/>
     </row>
     <row r="54" ht="14.6" customHeight="1">
       <c r="A54" s="9"/>
@@ -15085,10 +15325,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="14.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="48" style="86" customWidth="1"/>
-    <col min="2" max="2" width="61.8516" style="86" customWidth="1"/>
-    <col min="3" max="5" width="16.3516" style="86" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="86" customWidth="1"/>
+    <col min="1" max="1" width="48" style="88" customWidth="1"/>
+    <col min="2" max="2" width="61.8516" style="88" customWidth="1"/>
+    <col min="3" max="5" width="16.3516" style="88" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="88" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
@@ -15114,7 +15354,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>209</v>
+        <v>232</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -15125,7 +15365,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>210</v>
+        <v>233</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -15154,7 +15394,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s" s="9">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -15198,7 +15438,7 @@
     </row>
     <row r="12" ht="14.6" customHeight="1">
       <c r="A12" t="s" s="7">
-        <v>212</v>
+        <v>235</v>
       </c>
       <c r="B12" t="s" s="7">
         <v>29</v>
@@ -15215,10 +15455,10 @@
       <c r="E13" s="8"/>
     </row>
     <row r="14" ht="15.35" customHeight="1">
-      <c r="A14" t="s" s="52">
-        <v>163</v>
-      </c>
-      <c r="B14" s="53">
+      <c r="A14" t="s" s="46">
+        <v>155</v>
+      </c>
+      <c r="B14" s="47">
         <v>0</v>
       </c>
       <c r="C14" s="8"/>
@@ -15226,10 +15466,10 @@
       <c r="E14" s="8"/>
     </row>
     <row r="15" ht="15.35" customHeight="1">
-      <c r="A15" t="s" s="54">
-        <v>164</v>
-      </c>
-      <c r="B15" s="57">
+      <c r="A15" t="s" s="48">
+        <v>193</v>
+      </c>
+      <c r="B15" s="51">
         <v>1</v>
       </c>
       <c r="C15" s="10"/>
@@ -15237,10 +15477,10 @@
       <c r="E15" s="10"/>
     </row>
     <row r="16" ht="15.35" customHeight="1">
-      <c r="A16" t="s" s="56">
-        <v>165</v>
-      </c>
-      <c r="B16" s="65">
+      <c r="A16" t="s" s="65">
+        <v>158</v>
+      </c>
+      <c r="B16" s="67">
         <v>2</v>
       </c>
       <c r="C16" s="8"/>
@@ -15248,10 +15488,10 @@
       <c r="E16" s="8"/>
     </row>
     <row r="17" ht="15.35" customHeight="1">
-      <c r="A17" t="s" s="58">
-        <v>166</v>
-      </c>
-      <c r="B17" s="59">
+      <c r="A17" t="s" s="54">
+        <v>159</v>
+      </c>
+      <c r="B17" s="53">
         <v>3</v>
       </c>
       <c r="C17" s="10"/>
@@ -15259,10 +15499,10 @@
       <c r="E17" s="10"/>
     </row>
     <row r="18" ht="15.35" customHeight="1">
-      <c r="A18" t="s" s="60">
-        <v>167</v>
-      </c>
-      <c r="B18" s="61">
+      <c r="A18" t="s" s="56">
+        <v>160</v>
+      </c>
+      <c r="B18" s="55">
         <v>4</v>
       </c>
       <c r="C18" s="8"/>
@@ -15270,10 +15510,10 @@
       <c r="E18" s="8"/>
     </row>
     <row r="19" ht="15.35" customHeight="1">
-      <c r="A19" t="s" s="58">
-        <v>168</v>
-      </c>
-      <c r="B19" s="59">
+      <c r="A19" t="s" s="54">
+        <v>161</v>
+      </c>
+      <c r="B19" s="53">
         <v>5</v>
       </c>
       <c r="C19" s="10"/>
@@ -15281,10 +15521,10 @@
       <c r="E19" s="10"/>
     </row>
     <row r="20" ht="15.35" customHeight="1">
-      <c r="A20" t="s" s="62">
-        <v>169</v>
-      </c>
-      <c r="B20" s="63">
+      <c r="A20" t="s" s="58">
+        <v>162</v>
+      </c>
+      <c r="B20" s="57">
         <v>6</v>
       </c>
       <c r="C20" s="8"/>
@@ -15300,10 +15540,10 @@
     </row>
     <row r="22" ht="15.35" customHeight="1">
       <c r="A22" t="s" s="9">
-        <v>213</v>
+        <v>139</v>
       </c>
       <c r="B22" t="s" s="30">
-        <v>191</v>
+        <v>140</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -15387,36 +15627,36 @@
       <c r="E33" s="8"/>
     </row>
     <row r="34" ht="15.35" customHeight="1">
-      <c r="A34" s="66"/>
-      <c r="B34" s="67"/>
+      <c r="A34" s="68"/>
+      <c r="B34" s="69"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
     </row>
     <row r="35" ht="14.6" customHeight="1">
-      <c r="A35" s="68"/>
-      <c r="B35" s="47"/>
+      <c r="A35" s="70"/>
+      <c r="B35" s="61"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
     </row>
     <row r="36" ht="14.6" customHeight="1">
-      <c r="A36" s="69"/>
-      <c r="B36" s="67"/>
+      <c r="A36" s="71"/>
+      <c r="B36" s="69"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
     </row>
     <row r="37" ht="14.6" customHeight="1">
-      <c r="A37" s="70"/>
-      <c r="B37" s="71"/>
+      <c r="A37" s="72"/>
+      <c r="B37" s="73"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
     </row>
     <row r="38" ht="14.6" customHeight="1">
-      <c r="A38" s="72"/>
-      <c r="B38" s="73"/>
+      <c r="A38" s="74"/>
+      <c r="B38" s="75"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
@@ -15443,60 +15683,60 @@
       <c r="E41" s="8"/>
     </row>
     <row r="42" ht="14.6" customHeight="1">
-      <c r="A42" s="87"/>
-      <c r="B42" s="88"/>
+      <c r="A42" s="89"/>
+      <c r="B42" s="90"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
     </row>
     <row r="43" ht="14.6" customHeight="1">
-      <c r="A43" s="89"/>
-      <c r="B43" s="90"/>
-      <c r="C43" s="76"/>
-      <c r="D43" s="76"/>
-      <c r="E43" s="77"/>
+      <c r="A43" s="91"/>
+      <c r="B43" s="92"/>
+      <c r="C43" s="78"/>
+      <c r="D43" s="78"/>
+      <c r="E43" s="79"/>
     </row>
     <row r="44" ht="14.6" customHeight="1">
-      <c r="A44" s="91"/>
-      <c r="B44" s="92"/>
-      <c r="C44" s="80"/>
-      <c r="D44" s="80"/>
-      <c r="E44" s="81"/>
+      <c r="A44" s="93"/>
+      <c r="B44" s="94"/>
+      <c r="C44" s="82"/>
+      <c r="D44" s="82"/>
+      <c r="E44" s="83"/>
     </row>
     <row r="45" ht="14.6" customHeight="1">
-      <c r="A45" s="82"/>
-      <c r="B45" s="80"/>
-      <c r="C45" s="80"/>
-      <c r="D45" s="80"/>
-      <c r="E45" s="81"/>
+      <c r="A45" s="84"/>
+      <c r="B45" s="82"/>
+      <c r="C45" s="82"/>
+      <c r="D45" s="82"/>
+      <c r="E45" s="83"/>
     </row>
     <row r="46" ht="14.6" customHeight="1">
-      <c r="A46" s="82"/>
-      <c r="B46" s="80"/>
-      <c r="C46" s="80"/>
-      <c r="D46" s="80"/>
-      <c r="E46" s="81"/>
+      <c r="A46" s="84"/>
+      <c r="B46" s="82"/>
+      <c r="C46" s="82"/>
+      <c r="D46" s="82"/>
+      <c r="E46" s="83"/>
     </row>
     <row r="47" ht="14.6" customHeight="1">
-      <c r="A47" s="82"/>
-      <c r="B47" s="80"/>
-      <c r="C47" s="80"/>
-      <c r="D47" s="80"/>
-      <c r="E47" s="81"/>
+      <c r="A47" s="84"/>
+      <c r="B47" s="82"/>
+      <c r="C47" s="82"/>
+      <c r="D47" s="82"/>
+      <c r="E47" s="83"/>
     </row>
     <row r="48" ht="14.6" customHeight="1">
-      <c r="A48" s="82"/>
-      <c r="B48" s="80"/>
-      <c r="C48" s="80"/>
-      <c r="D48" s="80"/>
-      <c r="E48" s="81"/>
+      <c r="A48" s="84"/>
+      <c r="B48" s="82"/>
+      <c r="C48" s="82"/>
+      <c r="D48" s="82"/>
+      <c r="E48" s="83"/>
     </row>
     <row r="49" ht="14.6" customHeight="1">
-      <c r="A49" s="83"/>
-      <c r="B49" s="84"/>
-      <c r="C49" s="84"/>
-      <c r="D49" s="84"/>
-      <c r="E49" s="85"/>
+      <c r="A49" s="85"/>
+      <c r="B49" s="86"/>
+      <c r="C49" s="86"/>
+      <c r="D49" s="86"/>
+      <c r="E49" s="87"/>
     </row>
     <row r="50" ht="14.6" customHeight="1">
       <c r="A50" s="9"/>

</xml_diff>

<commit_message>
Form 11 Feedback changes
LLP Table - only update , no insert
</commit_message>
<xml_diff>
--- a/DataExtraction/Input/Config.xlsx
+++ b/DataExtraction/Input/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="273">
   <si>
     <t>Key</t>
   </si>
@@ -758,14 +758,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Company</t>
-    </r>
+    <t>LLP</t>
   </si>
   <si>
     <t>summary_designated_partners_table_name</t>
@@ -835,9 +828,6 @@
   </si>
   <si>
     <t>llp_type_value</t>
-  </si>
-  <si>
-    <t>LLP</t>
   </si>
   <si>
     <t>others_type_value</t>
@@ -4664,7 +4654,7 @@
         <v>263</v>
       </c>
       <c r="B45" t="s" s="69">
-        <v>264</v>
+        <v>240</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
@@ -4672,10 +4662,10 @@
     </row>
     <row r="46" ht="14.6" customHeight="1">
       <c r="A46" t="s" s="100">
+        <v>264</v>
+      </c>
+      <c r="B46" t="s" s="101">
         <v>265</v>
-      </c>
-      <c r="B46" t="s" s="101">
-        <v>266</v>
       </c>
       <c r="C46" s="102"/>
       <c r="D46" s="102"/>
@@ -4690,10 +4680,10 @@
     </row>
     <row r="48" ht="14.6" customHeight="1">
       <c r="A48" t="s" s="9">
+        <v>266</v>
+      </c>
+      <c r="B48" t="s" s="9">
         <v>267</v>
-      </c>
-      <c r="B48" t="s" s="9">
-        <v>268</v>
       </c>
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
@@ -4701,10 +4691,10 @@
     </row>
     <row r="49" ht="14.6" customHeight="1">
       <c r="A49" t="s" s="7">
+        <v>268</v>
+      </c>
+      <c r="B49" t="s" s="7">
         <v>269</v>
-      </c>
-      <c r="B49" t="s" s="7">
-        <v>270</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
@@ -4712,10 +4702,10 @@
     </row>
     <row r="50" ht="14.6" customHeight="1">
       <c r="A50" t="s" s="9">
+        <v>270</v>
+      </c>
+      <c r="B50" t="s" s="9">
         <v>271</v>
-      </c>
-      <c r="B50" t="s" s="9">
-        <v>272</v>
       </c>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
@@ -5704,7 +5694,6 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A23" r:id="rId1" location="" tooltip="" display="Company"/>
-    <hyperlink ref="B23" r:id="rId2" location="" tooltip="" display="Company"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -5733,7 +5722,7 @@
   <sheetData>
     <row r="1" ht="15.55" customHeight="1">
       <c r="A1" t="s" s="105">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B1" s="105"/>
       <c r="C1" s="105"/>

</xml_diff>

<commit_message>
Form 8 Interim Feedback points
1. Form 11 LLP table if exist update, else no insert  - Complete
2. form 8 interim lo property type - values only keys with comma separated - Complete
and replace short form values - Complete
3. status in excel and DB - Status Not Found - Updated config with Capital Letters and updated dict get function default value - Complete
</commit_message>
<xml_diff>
--- a/DataExtraction/Input/Config.xlsx
+++ b/DataExtraction/Input/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="279">
   <si>
     <t>Key</t>
   </si>
@@ -551,7 +551,19 @@
     <t>open_charges</t>
   </si>
   <si>
-    <t>c,MOCH,s</t>
+    <t>C,MOCH,S</t>
+  </si>
+  <si>
+    <t>property_type_abbreviation_list</t>
+  </si>
+  <si>
+    <t>IMPR,SHIP,IIMPR,GDWL,BODB,TRMR,PTNT,FLCH,MVPR,CPRT</t>
+  </si>
+  <si>
+    <t>property_type_list</t>
+  </si>
+  <si>
+    <t>immovable property,ship,any interest in immovable property,goodwill,book debts,trade marks,patent,floating charge,moveable property,copyright or licence under copy right</t>
   </si>
   <si>
     <t>creation_keyword</t>
@@ -602,6 +614,12 @@
     <t>charge_sequence_charge_id_column_name</t>
   </si>
   <si>
+    <t>property_type_column_name</t>
+  </si>
+  <si>
+    <t>property_type</t>
+  </si>
+  <si>
     <t>type_index</t>
   </si>
   <si>
@@ -740,22 +758,7 @@
     <t>/Users/gundukalyan/Documents/GitHub/mns-json-prep/DataExtraction/Output/LLP/Form_11</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Company</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>_table_name</t>
-    </r>
+    <t>company_table_name</t>
   </si>
   <si>
     <t>LLP</t>
@@ -864,7 +867,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -894,6 +897,11 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1518,7 +1526,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1706,6 +1714,12 @@
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -4211,10 +4225,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="14.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="48" style="95" customWidth="1"/>
-    <col min="2" max="2" width="61.8516" style="95" customWidth="1"/>
-    <col min="3" max="5" width="16.3516" style="95" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="95" customWidth="1"/>
+    <col min="1" max="1" width="48" style="97" customWidth="1"/>
+    <col min="2" max="2" width="61.8516" style="97" customWidth="1"/>
+    <col min="3" max="5" width="16.3516" style="97" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="97" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
@@ -4240,7 +4254,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -4251,7 +4265,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -4280,7 +4294,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s" s="9">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -4335,7 +4349,7 @@
     </row>
     <row r="13" ht="14.6" customHeight="1">
       <c r="A13" t="s" s="7">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="B13" t="s" s="7">
         <v>29</v>
@@ -4355,7 +4369,7 @@
       <c r="A15" t="s" s="46">
         <v>155</v>
       </c>
-      <c r="B15" s="96">
+      <c r="B15" s="98">
         <v>0</v>
       </c>
       <c r="C15" s="8"/>
@@ -4363,8 +4377,8 @@
       <c r="E15" s="8"/>
     </row>
     <row r="16" ht="15.35" customHeight="1">
-      <c r="A16" t="s" s="97">
-        <v>193</v>
+      <c r="A16" t="s" s="99">
+        <v>199</v>
       </c>
       <c r="B16" s="53">
         <v>2</v>
@@ -4436,11 +4450,11 @@
       <c r="E22" s="8"/>
     </row>
     <row r="23" ht="15.35" customHeight="1">
-      <c r="A23" t="s" s="9">
-        <v>239</v>
+      <c r="A23" t="s" s="12">
+        <v>245</v>
       </c>
       <c r="B23" t="s" s="30">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -4448,10 +4462,10 @@
     </row>
     <row r="24" ht="15.35" customHeight="1">
       <c r="A24" t="s" s="30">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="B24" t="s" s="30">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -4477,10 +4491,10 @@
     </row>
     <row r="27" ht="15.35" customHeight="1">
       <c r="A27" t="s" s="30">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="B27" t="s" s="30">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -4495,10 +4509,10 @@
     </row>
     <row r="29" ht="15.35" customHeight="1">
       <c r="A29" t="s" s="30">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="B29" t="s" s="30">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -4506,10 +4520,10 @@
     </row>
     <row r="30" ht="15.35" customHeight="1">
       <c r="A30" t="s" s="30">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="B30" t="s" s="30">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -4524,7 +4538,7 @@
     </row>
     <row r="32" ht="15.35" customHeight="1">
       <c r="A32" t="s" s="30">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="B32" t="s" s="30">
         <v>96</v>
@@ -4535,7 +4549,7 @@
     </row>
     <row r="33" ht="15.35" customHeight="1">
       <c r="A33" t="s" s="43">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="B33" t="s" s="43">
         <v>98</v>
@@ -4552,21 +4566,21 @@
       <c r="E34" s="8"/>
     </row>
     <row r="35" ht="15.35" customHeight="1">
-      <c r="A35" t="s" s="98">
-        <v>251</v>
-      </c>
-      <c r="B35" t="s" s="98">
-        <v>252</v>
+      <c r="A35" t="s" s="100">
+        <v>257</v>
+      </c>
+      <c r="B35" t="s" s="100">
+        <v>258</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
     </row>
     <row r="36" ht="14.6" customHeight="1">
-      <c r="A36" t="s" s="72">
-        <v>203</v>
-      </c>
-      <c r="B36" t="s" s="73">
+      <c r="A36" t="s" s="74">
+        <v>209</v>
+      </c>
+      <c r="B36" t="s" s="75">
         <v>25</v>
       </c>
       <c r="C36" s="8"/>
@@ -4575,17 +4589,17 @@
     </row>
     <row r="37" ht="14.6" customHeight="1">
       <c r="A37" s="50"/>
-      <c r="B37" s="73"/>
+      <c r="B37" s="75"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
     </row>
     <row r="38" ht="14.6" customHeight="1">
       <c r="A38" t="s" s="27">
-        <v>253</v>
-      </c>
-      <c r="B38" t="s" s="75">
-        <v>254</v>
+        <v>259</v>
+      </c>
+      <c r="B38" t="s" s="77">
+        <v>260</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
@@ -4593,10 +4607,10 @@
     </row>
     <row r="39" ht="14.6" customHeight="1">
       <c r="A39" t="s" s="30">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="B39" t="s" s="30">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
@@ -4611,21 +4625,21 @@
     </row>
     <row r="41" ht="14.6" customHeight="1">
       <c r="A41" t="s" s="30">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="B41" t="s" s="30">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
     </row>
     <row r="42" ht="14.6" customHeight="1">
-      <c r="A42" t="s" s="99">
-        <v>259</v>
-      </c>
-      <c r="B42" t="s" s="99">
-        <v>260</v>
+      <c r="A42" t="s" s="101">
+        <v>265</v>
+      </c>
+      <c r="B42" t="s" s="101">
+        <v>266</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
@@ -4640,36 +4654,36 @@
     </row>
     <row r="44" ht="14.6" customHeight="1">
       <c r="A44" t="s" s="30">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="B44" t="s" s="30">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
     </row>
     <row r="45" ht="14.6" customHeight="1">
-      <c r="A45" t="s" s="71">
-        <v>263</v>
-      </c>
-      <c r="B45" t="s" s="69">
-        <v>240</v>
+      <c r="A45" t="s" s="73">
+        <v>269</v>
+      </c>
+      <c r="B45" t="s" s="71">
+        <v>246</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
     </row>
     <row r="46" ht="14.6" customHeight="1">
-      <c r="A46" t="s" s="100">
-        <v>264</v>
-      </c>
-      <c r="B46" t="s" s="101">
-        <v>265</v>
-      </c>
-      <c r="C46" s="102"/>
-      <c r="D46" s="102"/>
-      <c r="E46" s="103"/>
+      <c r="A46" t="s" s="102">
+        <v>270</v>
+      </c>
+      <c r="B46" t="s" s="103">
+        <v>271</v>
+      </c>
+      <c r="C46" s="104"/>
+      <c r="D46" s="104"/>
+      <c r="E46" s="105"/>
     </row>
     <row r="47" ht="14.6" customHeight="1">
       <c r="A47" s="9"/>
@@ -4680,10 +4694,10 @@
     </row>
     <row r="48" ht="14.6" customHeight="1">
       <c r="A48" t="s" s="9">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="B48" t="s" s="9">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
@@ -4691,10 +4705,10 @@
     </row>
     <row r="49" ht="14.6" customHeight="1">
       <c r="A49" t="s" s="7">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="B49" t="s" s="7">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
@@ -4702,10 +4716,10 @@
     </row>
     <row r="50" ht="14.6" customHeight="1">
       <c r="A50" t="s" s="9">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="B50" t="s" s="9">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
@@ -5692,9 +5706,6 @@
       <c r="E190" s="10"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A23" r:id="rId1" location="" tooltip="" display="Company"/>
-  </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
@@ -5716,88 +5727,88 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="14.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="104" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="104" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="106" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="106" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.55" customHeight="1">
-      <c r="A1" t="s" s="105">
-        <v>272</v>
-      </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
+      <c r="A1" t="s" s="107">
+        <v>278</v>
+      </c>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
     </row>
     <row r="2" ht="14.15" customHeight="1">
-      <c r="A2" s="106"/>
-      <c r="B2" s="106"/>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
+      <c r="A2" s="108"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
     </row>
     <row r="3" ht="14.15" customHeight="1">
-      <c r="A3" s="107"/>
-      <c r="B3" s="108"/>
-      <c r="C3" s="109"/>
-      <c r="D3" s="109"/>
-      <c r="E3" s="109"/>
+      <c r="A3" s="109"/>
+      <c r="B3" s="110"/>
+      <c r="C3" s="111"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
     </row>
     <row r="4" ht="13.95" customHeight="1">
-      <c r="A4" s="110"/>
-      <c r="B4" s="111"/>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
+      <c r="A4" s="112"/>
+      <c r="B4" s="113"/>
+      <c r="C4" s="114"/>
+      <c r="D4" s="114"/>
+      <c r="E4" s="114"/>
     </row>
     <row r="5" ht="13.95" customHeight="1">
-      <c r="A5" s="110"/>
-      <c r="B5" s="111"/>
-      <c r="C5" s="112"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
+      <c r="A5" s="112"/>
+      <c r="B5" s="113"/>
+      <c r="C5" s="114"/>
+      <c r="D5" s="114"/>
+      <c r="E5" s="114"/>
     </row>
     <row r="6" ht="13.95" customHeight="1">
-      <c r="A6" s="110"/>
-      <c r="B6" s="111"/>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
+      <c r="A6" s="112"/>
+      <c r="B6" s="113"/>
+      <c r="C6" s="114"/>
+      <c r="D6" s="114"/>
+      <c r="E6" s="114"/>
     </row>
     <row r="7" ht="13.95" customHeight="1">
-      <c r="A7" s="110"/>
-      <c r="B7" s="111"/>
-      <c r="C7" s="112"/>
-      <c r="D7" s="112"/>
-      <c r="E7" s="112"/>
+      <c r="A7" s="112"/>
+      <c r="B7" s="113"/>
+      <c r="C7" s="114"/>
+      <c r="D7" s="114"/>
+      <c r="E7" s="114"/>
     </row>
     <row r="8" ht="13.95" customHeight="1">
-      <c r="A8" s="110"/>
-      <c r="B8" s="111"/>
-      <c r="C8" s="112"/>
-      <c r="D8" s="112"/>
-      <c r="E8" s="112"/>
+      <c r="A8" s="112"/>
+      <c r="B8" s="113"/>
+      <c r="C8" s="114"/>
+      <c r="D8" s="114"/>
+      <c r="E8" s="114"/>
     </row>
     <row r="9" ht="13.95" customHeight="1">
-      <c r="A9" s="110"/>
-      <c r="B9" s="111"/>
-      <c r="C9" s="112"/>
-      <c r="D9" s="112"/>
-      <c r="E9" s="112"/>
+      <c r="A9" s="112"/>
+      <c r="B9" s="113"/>
+      <c r="C9" s="114"/>
+      <c r="D9" s="114"/>
+      <c r="E9" s="114"/>
     </row>
     <row r="10" ht="13.95" customHeight="1">
-      <c r="A10" s="110"/>
-      <c r="B10" s="111"/>
-      <c r="C10" s="112"/>
-      <c r="D10" s="112"/>
-      <c r="E10" s="112"/>
+      <c r="A10" s="112"/>
+      <c r="B10" s="113"/>
+      <c r="C10" s="114"/>
+      <c r="D10" s="114"/>
+      <c r="E10" s="114"/>
     </row>
     <row r="11" ht="13.95" customHeight="1">
-      <c r="A11" s="110"/>
-      <c r="B11" s="111"/>
-      <c r="C11" s="112"/>
-      <c r="D11" s="112"/>
-      <c r="E11" s="112"/>
+      <c r="A11" s="112"/>
+      <c r="B11" s="113"/>
+      <c r="C11" s="114"/>
+      <c r="D11" s="114"/>
+      <c r="E11" s="114"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -12332,14 +12343,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E185"/>
+  <dimension ref="A1:E189"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="14.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="48" style="59" customWidth="1"/>
-    <col min="2" max="2" width="61.8516" style="59" customWidth="1"/>
+    <col min="2" max="2" width="141.047" style="59" customWidth="1"/>
     <col min="3" max="5" width="16.3516" style="59" customWidth="1"/>
     <col min="6" max="16384" width="16.3516" style="59" customWidth="1"/>
   </cols>
@@ -12566,50 +12577,50 @@
       <c r="E23" s="10"/>
     </row>
     <row r="24" ht="15.35" customHeight="1">
-      <c r="A24" t="s" s="22">
+      <c r="A24" t="s" s="9">
         <v>177</v>
       </c>
-      <c r="B24" t="s" s="23">
+      <c r="B24" t="s" s="7">
         <v>178</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
     </row>
     <row r="25" ht="15.35" customHeight="1">
-      <c r="A25" t="s" s="22">
+      <c r="A25" t="s" s="7">
         <v>179</v>
       </c>
-      <c r="B25" t="s" s="23">
+      <c r="B25" t="s" s="54">
         <v>180</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
     </row>
     <row r="26" ht="15.35" customHeight="1">
-      <c r="A26" t="s" s="22">
+      <c r="A26" s="7"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+    </row>
+    <row r="27" ht="15.35" customHeight="1">
+      <c r="A27" t="s" s="22">
         <v>181</v>
       </c>
-      <c r="B26" t="s" s="23">
+      <c r="B27" t="s" s="23">
         <v>182</v>
       </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-    </row>
-    <row r="27" ht="15.35" customHeight="1">
-      <c r="A27" s="22"/>
-      <c r="B27" s="23"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
     </row>
     <row r="28" ht="15.35" customHeight="1">
-      <c r="A28" t="s" s="30">
+      <c r="A28" t="s" s="22">
         <v>183</v>
       </c>
-      <c r="B28" t="s" s="30">
+      <c r="B28" t="s" s="23">
         <v>184</v>
       </c>
       <c r="C28" s="8"/>
@@ -12617,10 +12628,10 @@
       <c r="E28" s="8"/>
     </row>
     <row r="29" ht="15.35" customHeight="1">
-      <c r="A29" t="s" s="30">
+      <c r="A29" t="s" s="22">
         <v>185</v>
       </c>
-      <c r="B29" t="s" s="30">
+      <c r="B29" t="s" s="23">
         <v>186</v>
       </c>
       <c r="C29" s="8"/>
@@ -12628,217 +12639,229 @@
       <c r="E29" s="8"/>
     </row>
     <row r="30" ht="15.35" customHeight="1">
-      <c r="A30" t="s" s="30">
-        <v>187</v>
-      </c>
-      <c r="B30" t="s" s="30">
-        <v>188</v>
-      </c>
+      <c r="A30" s="22"/>
+      <c r="B30" s="23"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
     </row>
     <row r="31" ht="15.35" customHeight="1">
-      <c r="A31" s="22"/>
-      <c r="B31" s="23"/>
+      <c r="A31" t="s" s="30">
+        <v>187</v>
+      </c>
+      <c r="B31" t="s" s="30">
+        <v>188</v>
+      </c>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
     </row>
     <row r="32" ht="15.35" customHeight="1">
-      <c r="A32" t="s" s="60">
+      <c r="A32" t="s" s="30">
         <v>189</v>
       </c>
-      <c r="B32" t="s" s="26">
+      <c r="B32" t="s" s="30">
         <v>190</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" ht="14.6" customHeight="1">
-      <c r="A33" t="s" s="14">
+    <row r="33" ht="15.35" customHeight="1">
+      <c r="A33" t="s" s="30">
         <v>191</v>
       </c>
-      <c r="B33" t="s" s="61">
-        <v>190</v>
-      </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-    </row>
-    <row r="34" ht="14.6" customHeight="1">
-      <c r="A34" t="s" s="25">
+      <c r="B33" t="s" s="30">
         <v>192</v>
       </c>
-      <c r="B34" t="s" s="26">
-        <v>65</v>
-      </c>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-    </row>
-    <row r="35" ht="14.6" customHeight="1">
-      <c r="A35" s="50"/>
-      <c r="B35" s="62"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" ht="15.35" customHeight="1">
+      <c r="A34" s="22"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+    </row>
+    <row r="35" ht="15.35" customHeight="1">
+      <c r="A35" t="s" s="60">
+        <v>193</v>
+      </c>
+      <c r="B35" t="s" s="26">
+        <v>194</v>
+      </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
     </row>
     <row r="36" ht="14.6" customHeight="1">
-      <c r="A36" t="s" s="27">
-        <v>66</v>
-      </c>
-      <c r="B36" t="s" s="28">
-        <v>67</v>
-      </c>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
+      <c r="A36" t="s" s="14">
+        <v>195</v>
+      </c>
+      <c r="B36" t="s" s="61">
+        <v>194</v>
+      </c>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
     </row>
     <row r="37" ht="14.6" customHeight="1">
-      <c r="A37" t="s" s="7">
-        <v>58</v>
-      </c>
-      <c r="B37" t="s" s="23">
-        <v>59</v>
+      <c r="A37" t="s" s="25">
+        <v>196</v>
+      </c>
+      <c r="B37" t="s" s="26">
+        <v>65</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
     </row>
     <row r="38" ht="14.6" customHeight="1">
-      <c r="A38" s="30"/>
-      <c r="B38" s="30"/>
+      <c r="A38" s="50"/>
+      <c r="B38" s="62"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
     </row>
     <row r="39" ht="14.6" customHeight="1">
-      <c r="A39" t="s" s="30">
-        <v>135</v>
-      </c>
-      <c r="B39" t="s" s="30">
-        <v>136</v>
+      <c r="A39" t="s" s="27">
+        <v>66</v>
+      </c>
+      <c r="B39" t="s" s="28">
+        <v>67</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
     </row>
     <row r="40" ht="14.6" customHeight="1">
-      <c r="A40" s="63"/>
-      <c r="B40" s="64"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
+      <c r="A40" t="s" s="7">
+        <v>58</v>
+      </c>
+      <c r="B40" t="s" s="23">
+        <v>59</v>
+      </c>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
     </row>
     <row r="41" ht="14.6" customHeight="1">
-      <c r="A41" t="s" s="46">
-        <v>155</v>
-      </c>
-      <c r="B41" s="47">
-        <v>0</v>
-      </c>
+      <c r="A41" s="30"/>
+      <c r="B41" s="30"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" ht="14.6" customHeight="1">
-      <c r="A42" t="s" s="48">
-        <v>193</v>
-      </c>
-      <c r="B42" s="49">
-        <v>1</v>
-      </c>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
+      <c r="A42" t="s" s="30">
+        <v>135</v>
+      </c>
+      <c r="B42" t="s" s="30">
+        <v>136</v>
+      </c>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
     </row>
     <row r="43" ht="14.6" customHeight="1">
-      <c r="A43" t="s" s="65">
-        <v>158</v>
-      </c>
-      <c r="B43" s="51">
-        <v>2</v>
-      </c>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
+      <c r="A43" t="s" s="63">
+        <v>197</v>
+      </c>
+      <c r="B43" t="s" s="64">
+        <v>198</v>
+      </c>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
     </row>
     <row r="44" ht="14.6" customHeight="1">
-      <c r="A44" t="s" s="54">
-        <v>159</v>
-      </c>
-      <c r="B44" s="53">
-        <v>3</v>
-      </c>
+      <c r="A44" s="65"/>
+      <c r="B44" s="66"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
     </row>
     <row r="45" ht="14.6" customHeight="1">
-      <c r="A45" t="s" s="56">
-        <v>160</v>
-      </c>
-      <c r="B45" s="55">
-        <v>4</v>
-      </c>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
+      <c r="A45" t="s" s="46">
+        <v>155</v>
+      </c>
+      <c r="B45" s="47">
+        <v>0</v>
+      </c>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
     </row>
     <row r="46" ht="14.6" customHeight="1">
-      <c r="A46" t="s" s="54">
-        <v>161</v>
-      </c>
-      <c r="B46" s="53">
-        <v>5</v>
-      </c>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
+      <c r="A46" t="s" s="48">
+        <v>199</v>
+      </c>
+      <c r="B46" s="49">
+        <v>1</v>
+      </c>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
     </row>
     <row r="47" ht="14.6" customHeight="1">
-      <c r="A47" t="s" s="58">
-        <v>162</v>
-      </c>
-      <c r="B47" s="57">
-        <v>6</v>
+      <c r="A47" t="s" s="67">
+        <v>158</v>
+      </c>
+      <c r="B47" s="51">
+        <v>2</v>
       </c>
       <c r="C47" s="10"/>
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
     </row>
     <row r="48" ht="14.6" customHeight="1">
-      <c r="A48" s="9"/>
-      <c r="B48" s="7"/>
+      <c r="A48" t="s" s="54">
+        <v>159</v>
+      </c>
+      <c r="B48" s="53">
+        <v>3</v>
+      </c>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
     </row>
     <row r="49" ht="14.6" customHeight="1">
-      <c r="A49" s="9"/>
-      <c r="B49" s="9"/>
+      <c r="A49" t="s" s="56">
+        <v>160</v>
+      </c>
+      <c r="B49" s="55">
+        <v>4</v>
+      </c>
       <c r="C49" s="10"/>
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
     </row>
     <row r="50" ht="14.6" customHeight="1">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
+      <c r="A50" t="s" s="54">
+        <v>161</v>
+      </c>
+      <c r="B50" s="53">
+        <v>5</v>
+      </c>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
     </row>
     <row r="51" ht="14.6" customHeight="1">
-      <c r="A51" s="10"/>
-      <c r="B51" s="10"/>
+      <c r="A51" t="s" s="58">
+        <v>162</v>
+      </c>
+      <c r="B51" s="57">
+        <v>6</v>
+      </c>
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
     </row>
     <row r="52" ht="14.6" customHeight="1">
-      <c r="A52" s="7"/>
+      <c r="A52" s="9"/>
       <c r="B52" s="7"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
@@ -12852,22 +12875,22 @@
       <c r="E53" s="10"/>
     </row>
     <row r="54" ht="14.6" customHeight="1">
-      <c r="A54" s="8"/>
-      <c r="B54" s="8"/>
+      <c r="A54" s="7"/>
+      <c r="B54" s="7"/>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
       <c r="E54" s="8"/>
     </row>
     <row r="55" ht="14.6" customHeight="1">
-      <c r="A55" s="9"/>
-      <c r="B55" s="9"/>
+      <c r="A55" s="10"/>
+      <c r="B55" s="10"/>
       <c r="C55" s="10"/>
       <c r="D55" s="10"/>
       <c r="E55" s="10"/>
     </row>
     <row r="56" ht="14.6" customHeight="1">
-      <c r="A56" s="8"/>
-      <c r="B56" s="8"/>
+      <c r="A56" s="7"/>
+      <c r="B56" s="7"/>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
       <c r="E56" s="8"/>
@@ -12887,50 +12910,50 @@
       <c r="E58" s="8"/>
     </row>
     <row r="59" ht="14.6" customHeight="1">
-      <c r="A59" s="10"/>
-      <c r="B59" s="10"/>
+      <c r="A59" s="9"/>
+      <c r="B59" s="9"/>
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
       <c r="E59" s="10"/>
     </row>
     <row r="60" ht="14.6" customHeight="1">
-      <c r="A60" s="7"/>
-      <c r="B60" s="7"/>
+      <c r="A60" s="8"/>
+      <c r="B60" s="8"/>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
       <c r="E60" s="8"/>
     </row>
     <row r="61" ht="14.6" customHeight="1">
-      <c r="A61" s="10"/>
-      <c r="B61" s="10"/>
+      <c r="A61" s="9"/>
+      <c r="B61" s="9"/>
       <c r="C61" s="10"/>
       <c r="D61" s="10"/>
       <c r="E61" s="10"/>
     </row>
     <row r="62" ht="14.6" customHeight="1">
-      <c r="A62" s="7"/>
-      <c r="B62" s="7"/>
+      <c r="A62" s="8"/>
+      <c r="B62" s="8"/>
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
       <c r="E62" s="8"/>
     </row>
     <row r="63" ht="14.6" customHeight="1">
-      <c r="A63" s="9"/>
-      <c r="B63" s="9"/>
+      <c r="A63" s="10"/>
+      <c r="B63" s="10"/>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
       <c r="E63" s="10"/>
     </row>
     <row r="64" ht="14.6" customHeight="1">
-      <c r="A64" s="8"/>
-      <c r="B64" s="8"/>
+      <c r="A64" s="7"/>
+      <c r="B64" s="7"/>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
       <c r="E64" s="8"/>
     </row>
     <row r="65" ht="14.6" customHeight="1">
-      <c r="A65" s="9"/>
-      <c r="B65" s="9"/>
+      <c r="A65" s="10"/>
+      <c r="B65" s="10"/>
       <c r="C65" s="10"/>
       <c r="D65" s="10"/>
       <c r="E65" s="10"/>
@@ -12943,8 +12966,8 @@
       <c r="E66" s="8"/>
     </row>
     <row r="67" ht="14.6" customHeight="1">
-      <c r="A67" s="10"/>
-      <c r="B67" s="10"/>
+      <c r="A67" s="9"/>
+      <c r="B67" s="9"/>
       <c r="C67" s="10"/>
       <c r="D67" s="10"/>
       <c r="E67" s="10"/>
@@ -12971,15 +12994,15 @@
       <c r="E70" s="8"/>
     </row>
     <row r="71" ht="14.6" customHeight="1">
-      <c r="A71" s="9"/>
-      <c r="B71" s="9"/>
+      <c r="A71" s="10"/>
+      <c r="B71" s="10"/>
       <c r="C71" s="10"/>
       <c r="D71" s="10"/>
       <c r="E71" s="10"/>
     </row>
     <row r="72" ht="14.6" customHeight="1">
-      <c r="A72" s="7"/>
-      <c r="B72" s="7"/>
+      <c r="A72" s="8"/>
+      <c r="B72" s="8"/>
       <c r="C72" s="8"/>
       <c r="D72" s="8"/>
       <c r="E72" s="8"/>
@@ -12992,8 +13015,8 @@
       <c r="E73" s="10"/>
     </row>
     <row r="74" ht="14.6" customHeight="1">
-      <c r="A74" s="8"/>
-      <c r="B74" s="8"/>
+      <c r="A74" s="7"/>
+      <c r="B74" s="7"/>
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
       <c r="E74" s="8"/>
@@ -13013,22 +13036,22 @@
       <c r="E76" s="8"/>
     </row>
     <row r="77" ht="14.6" customHeight="1">
-      <c r="A77" s="10"/>
-      <c r="B77" s="10"/>
+      <c r="A77" s="9"/>
+      <c r="B77" s="9"/>
       <c r="C77" s="10"/>
       <c r="D77" s="10"/>
       <c r="E77" s="10"/>
     </row>
     <row r="78" ht="14.6" customHeight="1">
-      <c r="A78" s="7"/>
-      <c r="B78" s="7"/>
+      <c r="A78" s="8"/>
+      <c r="B78" s="8"/>
       <c r="C78" s="8"/>
       <c r="D78" s="8"/>
       <c r="E78" s="8"/>
     </row>
     <row r="79" ht="14.6" customHeight="1">
-      <c r="A79" s="10"/>
-      <c r="B79" s="10"/>
+      <c r="A79" s="9"/>
+      <c r="B79" s="9"/>
       <c r="C79" s="10"/>
       <c r="D79" s="10"/>
       <c r="E79" s="10"/>
@@ -13041,7 +13064,7 @@
       <c r="E80" s="8"/>
     </row>
     <row r="81" ht="14.6" customHeight="1">
-      <c r="A81" s="9"/>
+      <c r="A81" s="10"/>
       <c r="B81" s="10"/>
       <c r="C81" s="10"/>
       <c r="D81" s="10"/>
@@ -13049,27 +13072,27 @@
     </row>
     <row r="82" ht="14.6" customHeight="1">
       <c r="A82" s="7"/>
-      <c r="B82" s="8"/>
+      <c r="B82" s="7"/>
       <c r="C82" s="8"/>
       <c r="D82" s="8"/>
       <c r="E82" s="8"/>
     </row>
     <row r="83" ht="14.6" customHeight="1">
-      <c r="A83" s="9"/>
+      <c r="A83" s="10"/>
       <c r="B83" s="10"/>
       <c r="C83" s="10"/>
       <c r="D83" s="10"/>
       <c r="E83" s="10"/>
     </row>
     <row r="84" ht="14.6" customHeight="1">
-      <c r="A84" s="8"/>
-      <c r="B84" s="8"/>
+      <c r="A84" s="7"/>
+      <c r="B84" s="7"/>
       <c r="C84" s="8"/>
       <c r="D84" s="8"/>
       <c r="E84" s="8"/>
     </row>
     <row r="85" ht="14.6" customHeight="1">
-      <c r="A85" s="10"/>
+      <c r="A85" s="9"/>
       <c r="B85" s="10"/>
       <c r="C85" s="10"/>
       <c r="D85" s="10"/>
@@ -13077,28 +13100,28 @@
     </row>
     <row r="86" ht="14.6" customHeight="1">
       <c r="A86" s="7"/>
-      <c r="B86" s="7"/>
+      <c r="B86" s="8"/>
       <c r="C86" s="8"/>
       <c r="D86" s="8"/>
       <c r="E86" s="8"/>
     </row>
     <row r="87" ht="14.6" customHeight="1">
       <c r="A87" s="9"/>
-      <c r="B87" s="9"/>
+      <c r="B87" s="10"/>
       <c r="C87" s="10"/>
       <c r="D87" s="10"/>
       <c r="E87" s="10"/>
     </row>
     <row r="88" ht="14.6" customHeight="1">
-      <c r="A88" s="7"/>
-      <c r="B88" s="7"/>
+      <c r="A88" s="8"/>
+      <c r="B88" s="8"/>
       <c r="C88" s="8"/>
       <c r="D88" s="8"/>
       <c r="E88" s="8"/>
     </row>
     <row r="89" ht="14.6" customHeight="1">
-      <c r="A89" s="9"/>
-      <c r="B89" s="9"/>
+      <c r="A89" s="10"/>
+      <c r="B89" s="10"/>
       <c r="C89" s="10"/>
       <c r="D89" s="10"/>
       <c r="E89" s="10"/>
@@ -13118,8 +13141,8 @@
       <c r="E91" s="10"/>
     </row>
     <row r="92" ht="14.6" customHeight="1">
-      <c r="A92" s="8"/>
-      <c r="B92" s="8"/>
+      <c r="A92" s="7"/>
+      <c r="B92" s="7"/>
       <c r="C92" s="8"/>
       <c r="D92" s="8"/>
       <c r="E92" s="8"/>
@@ -13146,8 +13169,8 @@
       <c r="E95" s="10"/>
     </row>
     <row r="96" ht="14.6" customHeight="1">
-      <c r="A96" s="7"/>
-      <c r="B96" s="7"/>
+      <c r="A96" s="8"/>
+      <c r="B96" s="8"/>
       <c r="C96" s="8"/>
       <c r="D96" s="8"/>
       <c r="E96" s="8"/>
@@ -13160,8 +13183,8 @@
       <c r="E97" s="10"/>
     </row>
     <row r="98" ht="14.6" customHeight="1">
-      <c r="A98" s="8"/>
-      <c r="B98" s="8"/>
+      <c r="A98" s="7"/>
+      <c r="B98" s="7"/>
       <c r="C98" s="8"/>
       <c r="D98" s="8"/>
       <c r="E98" s="8"/>
@@ -13188,8 +13211,8 @@
       <c r="E101" s="10"/>
     </row>
     <row r="102" ht="14.6" customHeight="1">
-      <c r="A102" s="7"/>
-      <c r="B102" s="7"/>
+      <c r="A102" s="8"/>
+      <c r="B102" s="8"/>
       <c r="C102" s="8"/>
       <c r="D102" s="8"/>
       <c r="E102" s="8"/>
@@ -13202,15 +13225,15 @@
       <c r="E103" s="10"/>
     </row>
     <row r="104" ht="14.6" customHeight="1">
-      <c r="A104" s="8"/>
-      <c r="B104" s="8"/>
+      <c r="A104" s="7"/>
+      <c r="B104" s="7"/>
       <c r="C104" s="8"/>
       <c r="D104" s="8"/>
       <c r="E104" s="8"/>
     </row>
     <row r="105" ht="14.6" customHeight="1">
       <c r="A105" s="9"/>
-      <c r="B105" s="10"/>
+      <c r="B105" s="9"/>
       <c r="C105" s="10"/>
       <c r="D105" s="10"/>
       <c r="E105" s="10"/>
@@ -13230,15 +13253,15 @@
       <c r="E107" s="10"/>
     </row>
     <row r="108" ht="14.6" customHeight="1">
-      <c r="A108" s="7"/>
-      <c r="B108" s="7"/>
+      <c r="A108" s="8"/>
+      <c r="B108" s="8"/>
       <c r="C108" s="8"/>
       <c r="D108" s="8"/>
       <c r="E108" s="8"/>
     </row>
     <row r="109" ht="14.6" customHeight="1">
       <c r="A109" s="9"/>
-      <c r="B109" s="9"/>
+      <c r="B109" s="10"/>
       <c r="C109" s="10"/>
       <c r="D109" s="10"/>
       <c r="E109" s="10"/>
@@ -13251,8 +13274,8 @@
       <c r="E110" s="8"/>
     </row>
     <row r="111" ht="14.6" customHeight="1">
-      <c r="A111" s="10"/>
-      <c r="B111" s="10"/>
+      <c r="A111" s="9"/>
+      <c r="B111" s="9"/>
       <c r="C111" s="10"/>
       <c r="D111" s="10"/>
       <c r="E111" s="10"/>
@@ -13307,15 +13330,15 @@
       <c r="E118" s="8"/>
     </row>
     <row r="119" ht="14.6" customHeight="1">
-      <c r="A119" s="9"/>
-      <c r="B119" s="9"/>
+      <c r="A119" s="10"/>
+      <c r="B119" s="10"/>
       <c r="C119" s="10"/>
       <c r="D119" s="10"/>
       <c r="E119" s="10"/>
     </row>
     <row r="120" ht="14.6" customHeight="1">
-      <c r="A120" s="8"/>
-      <c r="B120" s="8"/>
+      <c r="A120" s="7"/>
+      <c r="B120" s="7"/>
       <c r="C120" s="8"/>
       <c r="D120" s="8"/>
       <c r="E120" s="8"/>
@@ -13335,15 +13358,15 @@
       <c r="E122" s="8"/>
     </row>
     <row r="123" ht="14.6" customHeight="1">
-      <c r="A123" s="10"/>
-      <c r="B123" s="10"/>
+      <c r="A123" s="9"/>
+      <c r="B123" s="9"/>
       <c r="C123" s="10"/>
       <c r="D123" s="10"/>
       <c r="E123" s="10"/>
     </row>
     <row r="124" ht="14.6" customHeight="1">
-      <c r="A124" s="7"/>
-      <c r="B124" s="7"/>
+      <c r="A124" s="8"/>
+      <c r="B124" s="8"/>
       <c r="C124" s="8"/>
       <c r="D124" s="8"/>
       <c r="E124" s="8"/>
@@ -13384,22 +13407,22 @@
       <c r="E129" s="10"/>
     </row>
     <row r="130" ht="14.6" customHeight="1">
-      <c r="A130" s="8"/>
-      <c r="B130" s="8"/>
+      <c r="A130" s="7"/>
+      <c r="B130" s="7"/>
       <c r="C130" s="8"/>
       <c r="D130" s="8"/>
       <c r="E130" s="8"/>
     </row>
     <row r="131" ht="14.6" customHeight="1">
-      <c r="A131" s="9"/>
-      <c r="B131" s="9"/>
+      <c r="A131" s="10"/>
+      <c r="B131" s="10"/>
       <c r="C131" s="10"/>
       <c r="D131" s="10"/>
       <c r="E131" s="10"/>
     </row>
     <row r="132" ht="14.6" customHeight="1">
-      <c r="A132" s="8"/>
-      <c r="B132" s="8"/>
+      <c r="A132" s="7"/>
+      <c r="B132" s="7"/>
       <c r="C132" s="8"/>
       <c r="D132" s="8"/>
       <c r="E132" s="8"/>
@@ -13412,22 +13435,22 @@
       <c r="E133" s="10"/>
     </row>
     <row r="134" ht="14.6" customHeight="1">
-      <c r="A134" s="7"/>
-      <c r="B134" s="7"/>
+      <c r="A134" s="8"/>
+      <c r="B134" s="8"/>
       <c r="C134" s="8"/>
       <c r="D134" s="8"/>
       <c r="E134" s="8"/>
     </row>
     <row r="135" ht="14.6" customHeight="1">
-      <c r="A135" s="10"/>
-      <c r="B135" s="10"/>
+      <c r="A135" s="9"/>
+      <c r="B135" s="9"/>
       <c r="C135" s="10"/>
       <c r="D135" s="10"/>
       <c r="E135" s="10"/>
     </row>
     <row r="136" ht="14.6" customHeight="1">
-      <c r="A136" s="7"/>
-      <c r="B136" s="7"/>
+      <c r="A136" s="8"/>
+      <c r="B136" s="8"/>
       <c r="C136" s="8"/>
       <c r="D136" s="8"/>
       <c r="E136" s="8"/>
@@ -13440,8 +13463,8 @@
       <c r="E137" s="10"/>
     </row>
     <row r="138" ht="14.6" customHeight="1">
-      <c r="A138" s="8"/>
-      <c r="B138" s="8"/>
+      <c r="A138" s="7"/>
+      <c r="B138" s="7"/>
       <c r="C138" s="8"/>
       <c r="D138" s="8"/>
       <c r="E138" s="8"/>
@@ -13455,21 +13478,21 @@
     </row>
     <row r="140" ht="14.6" customHeight="1">
       <c r="A140" s="7"/>
-      <c r="B140" s="8"/>
+      <c r="B140" s="7"/>
       <c r="C140" s="8"/>
       <c r="D140" s="8"/>
       <c r="E140" s="8"/>
     </row>
     <row r="141" ht="14.6" customHeight="1">
       <c r="A141" s="9"/>
-      <c r="B141" s="10"/>
+      <c r="B141" s="9"/>
       <c r="C141" s="10"/>
       <c r="D141" s="10"/>
       <c r="E141" s="10"/>
     </row>
     <row r="142" ht="14.6" customHeight="1">
-      <c r="A142" s="7"/>
-      <c r="B142" s="7"/>
+      <c r="A142" s="8"/>
+      <c r="B142" s="8"/>
       <c r="C142" s="8"/>
       <c r="D142" s="8"/>
       <c r="E142" s="8"/>
@@ -13483,21 +13506,21 @@
     </row>
     <row r="144" ht="14.6" customHeight="1">
       <c r="A144" s="7"/>
-      <c r="B144" s="7"/>
+      <c r="B144" s="8"/>
       <c r="C144" s="8"/>
       <c r="D144" s="8"/>
       <c r="E144" s="8"/>
     </row>
     <row r="145" ht="14.6" customHeight="1">
-      <c r="A145" s="10"/>
+      <c r="A145" s="9"/>
       <c r="B145" s="10"/>
       <c r="C145" s="10"/>
       <c r="D145" s="10"/>
       <c r="E145" s="10"/>
     </row>
     <row r="146" ht="14.6" customHeight="1">
-      <c r="A146" s="8"/>
-      <c r="B146" s="8"/>
+      <c r="A146" s="7"/>
+      <c r="B146" s="7"/>
       <c r="C146" s="8"/>
       <c r="D146" s="8"/>
       <c r="E146" s="8"/>
@@ -13510,36 +13533,36 @@
       <c r="E147" s="10"/>
     </row>
     <row r="148" ht="14.6" customHeight="1">
-      <c r="A148" s="8"/>
-      <c r="B148" s="8"/>
+      <c r="A148" s="7"/>
+      <c r="B148" s="7"/>
       <c r="C148" s="8"/>
       <c r="D148" s="8"/>
       <c r="E148" s="8"/>
     </row>
     <row r="149" ht="14.6" customHeight="1">
-      <c r="A149" s="9"/>
-      <c r="B149" s="9"/>
+      <c r="A149" s="10"/>
+      <c r="B149" s="10"/>
       <c r="C149" s="10"/>
       <c r="D149" s="10"/>
       <c r="E149" s="10"/>
     </row>
     <row r="150" ht="14.6" customHeight="1">
-      <c r="A150" s="7"/>
-      <c r="B150" s="7"/>
+      <c r="A150" s="8"/>
+      <c r="B150" s="8"/>
       <c r="C150" s="8"/>
       <c r="D150" s="8"/>
       <c r="E150" s="8"/>
     </row>
     <row r="151" ht="14.6" customHeight="1">
-      <c r="A151" s="9"/>
-      <c r="B151" s="9"/>
+      <c r="A151" s="10"/>
+      <c r="B151" s="10"/>
       <c r="C151" s="10"/>
       <c r="D151" s="10"/>
       <c r="E151" s="10"/>
     </row>
     <row r="152" ht="14.6" customHeight="1">
-      <c r="A152" s="7"/>
-      <c r="B152" s="7"/>
+      <c r="A152" s="8"/>
+      <c r="B152" s="8"/>
       <c r="C152" s="8"/>
       <c r="D152" s="8"/>
       <c r="E152" s="8"/>
@@ -13573,8 +13596,8 @@
       <c r="E156" s="8"/>
     </row>
     <row r="157" ht="14.6" customHeight="1">
-      <c r="A157" s="10"/>
-      <c r="B157" s="10"/>
+      <c r="A157" s="9"/>
+      <c r="B157" s="9"/>
       <c r="C157" s="10"/>
       <c r="D157" s="10"/>
       <c r="E157" s="10"/>
@@ -13601,15 +13624,15 @@
       <c r="E160" s="8"/>
     </row>
     <row r="161" ht="14.6" customHeight="1">
-      <c r="A161" s="9"/>
-      <c r="B161" s="9"/>
+      <c r="A161" s="10"/>
+      <c r="B161" s="10"/>
       <c r="C161" s="10"/>
       <c r="D161" s="10"/>
       <c r="E161" s="10"/>
     </row>
     <row r="162" ht="14.6" customHeight="1">
-      <c r="A162" s="8"/>
-      <c r="B162" s="8"/>
+      <c r="A162" s="7"/>
+      <c r="B162" s="7"/>
       <c r="C162" s="8"/>
       <c r="D162" s="8"/>
       <c r="E162" s="8"/>
@@ -13636,8 +13659,8 @@
       <c r="E165" s="10"/>
     </row>
     <row r="166" ht="14.6" customHeight="1">
-      <c r="A166" s="7"/>
-      <c r="B166" s="7"/>
+      <c r="A166" s="8"/>
+      <c r="B166" s="8"/>
       <c r="C166" s="8"/>
       <c r="D166" s="8"/>
       <c r="E166" s="8"/>
@@ -13664,8 +13687,8 @@
       <c r="E169" s="10"/>
     </row>
     <row r="170" ht="14.6" customHeight="1">
-      <c r="A170" s="8"/>
-      <c r="B170" s="8"/>
+      <c r="A170" s="7"/>
+      <c r="B170" s="7"/>
       <c r="C170" s="8"/>
       <c r="D170" s="8"/>
       <c r="E170" s="8"/>
@@ -13713,15 +13736,15 @@
       <c r="E176" s="8"/>
     </row>
     <row r="177" ht="14.6" customHeight="1">
-      <c r="A177" s="10"/>
-      <c r="B177" s="10"/>
+      <c r="A177" s="9"/>
+      <c r="B177" s="9"/>
       <c r="C177" s="10"/>
       <c r="D177" s="10"/>
       <c r="E177" s="10"/>
     </row>
     <row r="178" ht="14.6" customHeight="1">
-      <c r="A178" s="7"/>
-      <c r="B178" s="7"/>
+      <c r="A178" s="8"/>
+      <c r="B178" s="8"/>
       <c r="C178" s="8"/>
       <c r="D178" s="8"/>
       <c r="E178" s="8"/>
@@ -13734,15 +13757,15 @@
       <c r="E179" s="10"/>
     </row>
     <row r="180" ht="14.6" customHeight="1">
-      <c r="A180" s="8"/>
-      <c r="B180" s="8"/>
+      <c r="A180" s="7"/>
+      <c r="B180" s="7"/>
       <c r="C180" s="8"/>
       <c r="D180" s="8"/>
       <c r="E180" s="8"/>
     </row>
     <row r="181" ht="14.6" customHeight="1">
-      <c r="A181" s="9"/>
-      <c r="B181" s="9"/>
+      <c r="A181" s="10"/>
+      <c r="B181" s="10"/>
       <c r="C181" s="10"/>
       <c r="D181" s="10"/>
       <c r="E181" s="10"/>
@@ -13755,15 +13778,15 @@
       <c r="E182" s="8"/>
     </row>
     <row r="183" ht="14.6" customHeight="1">
-      <c r="A183" s="10"/>
-      <c r="B183" s="10"/>
+      <c r="A183" s="9"/>
+      <c r="B183" s="9"/>
       <c r="C183" s="10"/>
       <c r="D183" s="10"/>
       <c r="E183" s="10"/>
     </row>
     <row r="184" ht="14.6" customHeight="1">
-      <c r="A184" s="7"/>
-      <c r="B184" s="7"/>
+      <c r="A184" s="8"/>
+      <c r="B184" s="8"/>
       <c r="C184" s="8"/>
       <c r="D184" s="8"/>
       <c r="E184" s="8"/>
@@ -13774,6 +13797,34 @@
       <c r="C185" s="10"/>
       <c r="D185" s="10"/>
       <c r="E185" s="10"/>
+    </row>
+    <row r="186" ht="14.6" customHeight="1">
+      <c r="A186" s="7"/>
+      <c r="B186" s="7"/>
+      <c r="C186" s="8"/>
+      <c r="D186" s="8"/>
+      <c r="E186" s="8"/>
+    </row>
+    <row r="187" ht="14.6" customHeight="1">
+      <c r="A187" s="10"/>
+      <c r="B187" s="10"/>
+      <c r="C187" s="10"/>
+      <c r="D187" s="10"/>
+      <c r="E187" s="10"/>
+    </row>
+    <row r="188" ht="14.6" customHeight="1">
+      <c r="A188" s="7"/>
+      <c r="B188" s="7"/>
+      <c r="C188" s="8"/>
+      <c r="D188" s="8"/>
+      <c r="E188" s="8"/>
+    </row>
+    <row r="189" ht="14.6" customHeight="1">
+      <c r="A189" s="9"/>
+      <c r="B189" s="9"/>
+      <c r="C189" s="10"/>
+      <c r="D189" s="10"/>
+      <c r="E189" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -13795,10 +13846,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="14.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="48" style="66" customWidth="1"/>
-    <col min="2" max="2" width="61.8516" style="66" customWidth="1"/>
-    <col min="3" max="5" width="16.3516" style="66" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="66" customWidth="1"/>
+    <col min="1" max="1" width="48" style="68" customWidth="1"/>
+    <col min="2" max="2" width="61.8516" style="68" customWidth="1"/>
+    <col min="3" max="5" width="16.3516" style="68" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="68" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
@@ -13824,7 +13875,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -13835,7 +13886,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -13864,7 +13915,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s" s="9">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -13929,7 +13980,7 @@
         <v>170</v>
       </c>
       <c r="B14" t="s" s="30">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -13937,10 +13988,10 @@
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" t="s" s="22">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B15" t="s" s="7">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -13966,7 +14017,7 @@
     </row>
     <row r="18" ht="15.35" customHeight="1">
       <c r="A18" t="s" s="48">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B18" s="49">
         <v>1</v>
@@ -13977,7 +14028,7 @@
     </row>
     <row r="19" ht="15.35" customHeight="1">
       <c r="A19" t="s" s="48">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="B19" s="51">
         <v>2</v>
@@ -13987,10 +14038,10 @@
       <c r="E19" s="10"/>
     </row>
     <row r="20" ht="15.35" customHeight="1">
-      <c r="A20" t="s" s="65">
+      <c r="A20" t="s" s="67">
         <v>158</v>
       </c>
-      <c r="B20" s="67">
+      <c r="B20" s="69">
         <v>3</v>
       </c>
       <c r="C20" s="8"/>
@@ -14035,7 +14086,7 @@
         <v>162</v>
       </c>
       <c r="B24" t="s" s="23">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -14086,7 +14137,7 @@
         <v>83</v>
       </c>
       <c r="B29" t="s" s="30">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -14101,7 +14152,7 @@
     </row>
     <row r="31" ht="15.35" customHeight="1">
       <c r="A31" t="s" s="22">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="B31" t="s" s="23">
         <v>25</v>
@@ -14115,7 +14166,7 @@
         <v>58</v>
       </c>
       <c r="B32" t="s" s="30">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
@@ -14123,10 +14174,10 @@
     </row>
     <row r="33" ht="15.35" customHeight="1">
       <c r="A33" t="s" s="30">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="B33" t="s" s="30">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
@@ -14134,10 +14185,10 @@
     </row>
     <row r="34" ht="15.35" customHeight="1">
       <c r="A34" t="s" s="30">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="B34" t="s" s="30">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
@@ -14145,10 +14196,10 @@
     </row>
     <row r="35" ht="15.35" customHeight="1">
       <c r="A35" t="s" s="43">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="B35" t="s" s="43">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -14156,10 +14207,10 @@
     </row>
     <row r="36" ht="15.35" customHeight="1">
       <c r="A36" t="s" s="30">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="B36" t="s" s="30">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
@@ -14173,19 +14224,19 @@
       <c r="E37" s="8"/>
     </row>
     <row r="38" ht="15.35" customHeight="1">
-      <c r="A38" t="s" s="68">
-        <v>212</v>
-      </c>
-      <c r="B38" t="s" s="69">
-        <v>213</v>
+      <c r="A38" t="s" s="70">
+        <v>218</v>
+      </c>
+      <c r="B38" t="s" s="71">
+        <v>219</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
     </row>
     <row r="39" ht="14.6" customHeight="1">
-      <c r="A39" t="s" s="70">
-        <v>214</v>
+      <c r="A39" t="s" s="72">
+        <v>220</v>
       </c>
       <c r="B39" t="s" s="61">
         <v>140</v>
@@ -14195,33 +14246,33 @@
       <c r="E39" s="10"/>
     </row>
     <row r="40" ht="14.6" customHeight="1">
-      <c r="A40" t="s" s="71">
-        <v>215</v>
-      </c>
-      <c r="B40" t="s" s="69">
-        <v>216</v>
+      <c r="A40" t="s" s="73">
+        <v>221</v>
+      </c>
+      <c r="B40" t="s" s="71">
+        <v>222</v>
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
     </row>
     <row r="41" ht="14.6" customHeight="1">
-      <c r="A41" t="s" s="72">
-        <v>217</v>
-      </c>
-      <c r="B41" t="s" s="73">
-        <v>190</v>
+      <c r="A41" t="s" s="74">
+        <v>223</v>
+      </c>
+      <c r="B41" t="s" s="75">
+        <v>194</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" ht="14.6" customHeight="1">
-      <c r="A42" t="s" s="74">
-        <v>218</v>
-      </c>
-      <c r="B42" t="s" s="75">
-        <v>219</v>
+      <c r="A42" t="s" s="76">
+        <v>224</v>
+      </c>
+      <c r="B42" t="s" s="77">
+        <v>225</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
@@ -14229,10 +14280,10 @@
     </row>
     <row r="43" ht="14.6" customHeight="1">
       <c r="A43" t="s" s="30">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="B43" t="s" s="30">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
@@ -14240,10 +14291,10 @@
     </row>
     <row r="44" ht="14.6" customHeight="1">
       <c r="A44" t="s" s="30">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="B44" t="s" s="30">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
@@ -14251,82 +14302,82 @@
     </row>
     <row r="45" ht="14.6" customHeight="1">
       <c r="A45" t="s" s="30">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="B45" t="s" s="30">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
     </row>
     <row r="46" ht="14.6" customHeight="1">
-      <c r="A46" t="s" s="71">
-        <v>226</v>
-      </c>
-      <c r="B46" t="s" s="69">
-        <v>227</v>
+      <c r="A46" t="s" s="73">
+        <v>232</v>
+      </c>
+      <c r="B46" t="s" s="71">
+        <v>233</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
     </row>
     <row r="47" ht="14.6" customHeight="1">
-      <c r="A47" t="s" s="76">
-        <v>228</v>
-      </c>
-      <c r="B47" t="s" s="77">
-        <v>229</v>
-      </c>
-      <c r="C47" s="78"/>
-      <c r="D47" s="78"/>
-      <c r="E47" s="79"/>
+      <c r="A47" t="s" s="78">
+        <v>234</v>
+      </c>
+      <c r="B47" t="s" s="79">
+        <v>235</v>
+      </c>
+      <c r="C47" s="80"/>
+      <c r="D47" s="80"/>
+      <c r="E47" s="81"/>
     </row>
     <row r="48" ht="14.6" customHeight="1">
-      <c r="A48" t="s" s="80">
-        <v>230</v>
-      </c>
-      <c r="B48" t="s" s="81">
-        <v>231</v>
-      </c>
-      <c r="C48" s="82"/>
-      <c r="D48" s="82"/>
-      <c r="E48" s="83"/>
+      <c r="A48" t="s" s="82">
+        <v>236</v>
+      </c>
+      <c r="B48" t="s" s="83">
+        <v>237</v>
+      </c>
+      <c r="C48" s="84"/>
+      <c r="D48" s="84"/>
+      <c r="E48" s="85"/>
     </row>
     <row r="49" ht="14.6" customHeight="1">
-      <c r="A49" s="84"/>
-      <c r="B49" s="82"/>
-      <c r="C49" s="82"/>
-      <c r="D49" s="82"/>
-      <c r="E49" s="83"/>
+      <c r="A49" s="86"/>
+      <c r="B49" s="84"/>
+      <c r="C49" s="84"/>
+      <c r="D49" s="84"/>
+      <c r="E49" s="85"/>
     </row>
     <row r="50" ht="14.6" customHeight="1">
-      <c r="A50" s="84"/>
-      <c r="B50" s="82"/>
-      <c r="C50" s="82"/>
-      <c r="D50" s="82"/>
-      <c r="E50" s="83"/>
+      <c r="A50" s="86"/>
+      <c r="B50" s="84"/>
+      <c r="C50" s="84"/>
+      <c r="D50" s="84"/>
+      <c r="E50" s="85"/>
     </row>
     <row r="51" ht="14.6" customHeight="1">
-      <c r="A51" s="84"/>
-      <c r="B51" s="82"/>
-      <c r="C51" s="82"/>
-      <c r="D51" s="82"/>
-      <c r="E51" s="83"/>
+      <c r="A51" s="86"/>
+      <c r="B51" s="84"/>
+      <c r="C51" s="84"/>
+      <c r="D51" s="84"/>
+      <c r="E51" s="85"/>
     </row>
     <row r="52" ht="14.6" customHeight="1">
-      <c r="A52" s="84"/>
-      <c r="B52" s="82"/>
-      <c r="C52" s="82"/>
-      <c r="D52" s="82"/>
-      <c r="E52" s="83"/>
+      <c r="A52" s="86"/>
+      <c r="B52" s="84"/>
+      <c r="C52" s="84"/>
+      <c r="D52" s="84"/>
+      <c r="E52" s="85"/>
     </row>
     <row r="53" ht="14.6" customHeight="1">
-      <c r="A53" s="85"/>
-      <c r="B53" s="86"/>
-      <c r="C53" s="86"/>
-      <c r="D53" s="86"/>
-      <c r="E53" s="87"/>
+      <c r="A53" s="87"/>
+      <c r="B53" s="88"/>
+      <c r="C53" s="88"/>
+      <c r="D53" s="88"/>
+      <c r="E53" s="89"/>
     </row>
     <row r="54" ht="14.6" customHeight="1">
       <c r="A54" s="9"/>
@@ -15314,10 +15365,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="14.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="48" style="88" customWidth="1"/>
-    <col min="2" max="2" width="61.8516" style="88" customWidth="1"/>
-    <col min="3" max="5" width="16.3516" style="88" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="88" customWidth="1"/>
+    <col min="1" max="1" width="48" style="90" customWidth="1"/>
+    <col min="2" max="2" width="61.8516" style="90" customWidth="1"/>
+    <col min="3" max="5" width="16.3516" style="90" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="90" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
@@ -15343,7 +15394,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="7">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -15354,7 +15405,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -15383,7 +15434,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s" s="9">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -15427,7 +15478,7 @@
     </row>
     <row r="12" ht="14.6" customHeight="1">
       <c r="A12" t="s" s="7">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="B12" t="s" s="7">
         <v>29</v>
@@ -15456,7 +15507,7 @@
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" t="s" s="48">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B15" s="51">
         <v>1</v>
@@ -15466,10 +15517,10 @@
       <c r="E15" s="10"/>
     </row>
     <row r="16" ht="15.35" customHeight="1">
-      <c r="A16" t="s" s="65">
+      <c r="A16" t="s" s="67">
         <v>158</v>
       </c>
-      <c r="B16" s="67">
+      <c r="B16" s="69">
         <v>2</v>
       </c>
       <c r="C16" s="8"/>
@@ -15616,36 +15667,36 @@
       <c r="E33" s="8"/>
     </row>
     <row r="34" ht="15.35" customHeight="1">
-      <c r="A34" s="68"/>
-      <c r="B34" s="69"/>
+      <c r="A34" s="70"/>
+      <c r="B34" s="71"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
     </row>
     <row r="35" ht="14.6" customHeight="1">
-      <c r="A35" s="70"/>
+      <c r="A35" s="72"/>
       <c r="B35" s="61"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
     </row>
     <row r="36" ht="14.6" customHeight="1">
-      <c r="A36" s="71"/>
-      <c r="B36" s="69"/>
+      <c r="A36" s="73"/>
+      <c r="B36" s="71"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
     </row>
     <row r="37" ht="14.6" customHeight="1">
-      <c r="A37" s="72"/>
-      <c r="B37" s="73"/>
+      <c r="A37" s="74"/>
+      <c r="B37" s="75"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
     </row>
     <row r="38" ht="14.6" customHeight="1">
-      <c r="A38" s="74"/>
-      <c r="B38" s="75"/>
+      <c r="A38" s="76"/>
+      <c r="B38" s="77"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
@@ -15672,60 +15723,60 @@
       <c r="E41" s="8"/>
     </row>
     <row r="42" ht="14.6" customHeight="1">
-      <c r="A42" s="89"/>
-      <c r="B42" s="90"/>
+      <c r="A42" s="91"/>
+      <c r="B42" s="92"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
     </row>
     <row r="43" ht="14.6" customHeight="1">
-      <c r="A43" s="91"/>
-      <c r="B43" s="92"/>
-      <c r="C43" s="78"/>
-      <c r="D43" s="78"/>
-      <c r="E43" s="79"/>
+      <c r="A43" s="93"/>
+      <c r="B43" s="94"/>
+      <c r="C43" s="80"/>
+      <c r="D43" s="80"/>
+      <c r="E43" s="81"/>
     </row>
     <row r="44" ht="14.6" customHeight="1">
-      <c r="A44" s="93"/>
-      <c r="B44" s="94"/>
-      <c r="C44" s="82"/>
-      <c r="D44" s="82"/>
-      <c r="E44" s="83"/>
+      <c r="A44" s="95"/>
+      <c r="B44" s="96"/>
+      <c r="C44" s="84"/>
+      <c r="D44" s="84"/>
+      <c r="E44" s="85"/>
     </row>
     <row r="45" ht="14.6" customHeight="1">
-      <c r="A45" s="84"/>
-      <c r="B45" s="82"/>
-      <c r="C45" s="82"/>
-      <c r="D45" s="82"/>
-      <c r="E45" s="83"/>
+      <c r="A45" s="86"/>
+      <c r="B45" s="84"/>
+      <c r="C45" s="84"/>
+      <c r="D45" s="84"/>
+      <c r="E45" s="85"/>
     </row>
     <row r="46" ht="14.6" customHeight="1">
-      <c r="A46" s="84"/>
-      <c r="B46" s="82"/>
-      <c r="C46" s="82"/>
-      <c r="D46" s="82"/>
-      <c r="E46" s="83"/>
+      <c r="A46" s="86"/>
+      <c r="B46" s="84"/>
+      <c r="C46" s="84"/>
+      <c r="D46" s="84"/>
+      <c r="E46" s="85"/>
     </row>
     <row r="47" ht="14.6" customHeight="1">
-      <c r="A47" s="84"/>
-      <c r="B47" s="82"/>
-      <c r="C47" s="82"/>
-      <c r="D47" s="82"/>
-      <c r="E47" s="83"/>
+      <c r="A47" s="86"/>
+      <c r="B47" s="84"/>
+      <c r="C47" s="84"/>
+      <c r="D47" s="84"/>
+      <c r="E47" s="85"/>
     </row>
     <row r="48" ht="14.6" customHeight="1">
-      <c r="A48" s="84"/>
-      <c r="B48" s="82"/>
-      <c r="C48" s="82"/>
-      <c r="D48" s="82"/>
-      <c r="E48" s="83"/>
+      <c r="A48" s="86"/>
+      <c r="B48" s="84"/>
+      <c r="C48" s="84"/>
+      <c r="D48" s="84"/>
+      <c r="E48" s="85"/>
     </row>
     <row r="49" ht="14.6" customHeight="1">
-      <c r="A49" s="85"/>
-      <c r="B49" s="86"/>
-      <c r="C49" s="86"/>
-      <c r="D49" s="86"/>
-      <c r="E49" s="87"/>
+      <c r="A49" s="87"/>
+      <c r="B49" s="88"/>
+      <c r="C49" s="88"/>
+      <c r="D49" s="88"/>
+      <c r="E49" s="89"/>
     </row>
     <row r="50" ht="14.6" customHeight="1">
       <c r="A50" s="9"/>

</xml_diff>